<commit_message>
Common: Preparing client registration and so
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B0EE36-FFB1-4CC1-BB4F-37D4CCCC6862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967D4434-1CE6-4159-8138-8F2F4DCFD120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1215" yWindow="915" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>cs</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Přihlášení</t>
   </si>
   <si>
-    <t>public.login.title</t>
-  </si>
-  <si>
     <t>public.sign-in.content.title</t>
   </si>
   <si>
@@ -159,6 +156,117 @@
   </si>
   <si>
     <t>A mnoho dalšího, např. nástroje pro výpočty poměrů liquidů, spirálek, Ohmův zákon a další…</t>
+  </si>
+  <si>
+    <t>public.sign-up.menu</t>
+  </si>
+  <si>
+    <t>Registrace</t>
+  </si>
+  <si>
+    <t>public.404.title</t>
+  </si>
+  <si>
+    <t>Tady nic není!</t>
+  </si>
+  <si>
+    <t>I těm nejlepším se to stane…</t>
+  </si>
+  <si>
+    <t>public.404.subtitle</t>
+  </si>
+  <si>
+    <t>public.404.back</t>
+  </si>
+  <si>
+    <t>Bohužel jste narazili na stránku, která neexistuje. Je to divné, ale je to tak.</t>
+  </si>
+  <si>
+    <t>Zpět</t>
+  </si>
+  <si>
+    <t>public.404.home</t>
+  </si>
+  <si>
+    <t>public.development-notice.alert</t>
+  </si>
+  <si>
+    <t>Aplikace je stále ve vývoji a mnoho vychytávek chybí, nicméně je aktivně vyvíjena i používána.</t>
+  </si>
+  <si>
+    <t>public.sign-in.title</t>
+  </si>
+  <si>
+    <t>public.sign-up.title</t>
+  </si>
+  <si>
+    <t>Po registraci získáte okamžitý přístup do aplikace a můžete začít zkoumat zajímavé možnosti, kterými disponuje.</t>
+  </si>
+  <si>
+    <t>user.name.label</t>
+  </si>
+  <si>
+    <t>Vaše jméno</t>
+  </si>
+  <si>
+    <t>user.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Jedná se víceméně o jakékoli jméno, kterým se chcete prezentovat. Pro přihlášení bude použit Váš email.</t>
+  </si>
+  <si>
+    <t>user.password2.label</t>
+  </si>
+  <si>
+    <t>Kontrola hesla</t>
+  </si>
+  <si>
+    <t>public.sign-up.subtitle</t>
+  </si>
+  <si>
+    <t>public.sign-up.form.submit.label</t>
+  </si>
+  <si>
+    <t>Registrovat se</t>
+  </si>
+  <si>
+    <t>user.email.label</t>
+  </si>
+  <si>
+    <t>user.email.label.tooltip</t>
+  </si>
+  <si>
+    <t>Emailová adresa musí být v systému unikátní a slouží dále pro přihlášení do systému.</t>
+  </si>
+  <si>
+    <t>user.password.label.required</t>
+  </si>
+  <si>
+    <t>Bez hesla to bohužel nejde, vyplňte jej prosím.</t>
+  </si>
+  <si>
+    <t>user.password2.label.required</t>
+  </si>
+  <si>
+    <t>Kontrolní heslo je vyžadováno.</t>
+  </si>
+  <si>
+    <t>user.name.label.required</t>
+  </si>
+  <si>
+    <t>Vaše jméno je vyžadováno, vyplňte jej prosím.</t>
+  </si>
+  <si>
+    <t>user.email.label.required</t>
+  </si>
+  <si>
+    <t>E-mailová adresa slouží k přihlášení do systému, je povinná.</t>
+  </si>
+  <si>
+    <t>user.password2.label.mismatch</t>
+  </si>
+  <si>
+    <t>Hesla se neshoduji!</t>
   </si>
 </sst>
 </file>
@@ -522,10 +630,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>21</v>
@@ -606,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,10 +736,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -661,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
@@ -672,10 +780,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -683,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -694,10 +802,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -705,10 +813,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -716,10 +824,230 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Client is building again!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967D4434-1CE6-4159-8138-8F2F4DCFD120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4400C972-4404-48E8-BD79-1EDF352A325A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1215" yWindow="915" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
   <si>
     <t>cs</t>
   </si>
@@ -267,6 +267,30 @@
   </si>
   <si>
     <t>Hesla se neshoduji!</t>
+  </si>
+  <si>
+    <t>public.sign-out.title</t>
+  </si>
+  <si>
+    <t>public.sign-out</t>
+  </si>
+  <si>
+    <t>Odhlašování</t>
+  </si>
+  <si>
+    <t>Probíhá odhlašování z aplikace, prosím vyčkejte…</t>
+  </si>
+  <si>
+    <t>error.Who are you?</t>
+  </si>
+  <si>
+    <t>Je nám líto, ale aplikace vás nepoznává.</t>
+  </si>
+  <si>
+    <t>error.Unknown login</t>
+  </si>
+  <si>
+    <t>Přihlášení selhalo, zkontrolujte si prosím jméno a heslo.</t>
   </si>
 </sst>
 </file>
@@ -630,10 +654,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,6 +1072,50 @@
       </c>
       <c r="C37" s="1" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Soo, some initial stuff looks good
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4400C972-4404-48E8-BD79-1EDF352A325A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F55E12-8A9F-45BA-A253-2E2C9EB8127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="915" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="3675" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="278">
   <si>
     <t>cs</t>
   </si>
@@ -291,6 +291,579 @@
   </si>
   <si>
     <t>Přihlášení selhalo, zkontrolujte si prosím jméno a heslo.</t>
+  </si>
+  <si>
+    <t>translation.check</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>lab.check.user.settings.title</t>
+  </si>
+  <si>
+    <t>Zkontrolujte si prosím nastavejí profilu</t>
+  </si>
+  <si>
+    <t>form-item.settings.language.label</t>
+  </si>
+  <si>
+    <t>Jazyk</t>
+  </si>
+  <si>
+    <t>language.cs</t>
+  </si>
+  <si>
+    <t>Čeština</t>
+  </si>
+  <si>
+    <t>language.translation</t>
+  </si>
+  <si>
+    <t>Překladatelský režim</t>
+  </si>
+  <si>
+    <t>form-item.settings.date.label</t>
+  </si>
+  <si>
+    <t>Formát datumů</t>
+  </si>
+  <si>
+    <t>lab.user.settings.date.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud si zvolíte LL, aplikace se bude snažit odhadnout nastavení z vašeho prohlížeče.</t>
+  </si>
+  <si>
+    <t>form-item.settings.datetime.label</t>
+  </si>
+  <si>
+    <t>Nastavení formátu datumu a času</t>
+  </si>
+  <si>
+    <t>lab.user.settings.datetime.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud si nastavíte LLLL, aplikace se bude snažit odhadnout nastavení z vašeho prohlížeče.</t>
+  </si>
+  <si>
+    <t>lab.user.settings.save</t>
+  </si>
+  <si>
+    <t>Uložit nastavení</t>
+  </si>
+  <si>
+    <t>root.index.title</t>
+  </si>
+  <si>
+    <t>Administrace systému</t>
+  </si>
+  <si>
+    <t>root.home.welcome-title</t>
+  </si>
+  <si>
+    <t>Vítejte v administraci systému</t>
+  </si>
+  <si>
+    <t>root.home.welcome-subtitle</t>
+  </si>
+  <si>
+    <t>V této části aplikace máte božský přístup všude a lze dělat všechno. Proto prosím dávtejte opravdu velký pozor na co klikáte, poněvadž překlepy zde se neodpouští.</t>
+  </si>
+  <si>
+    <t>root.home.menu</t>
+  </si>
+  <si>
+    <t>root.settings.menu</t>
+  </si>
+  <si>
+    <t>Nastavení</t>
+  </si>
+  <si>
+    <t>root.import.index.menu</t>
+  </si>
+  <si>
+    <t>Importy</t>
+  </si>
+  <si>
+    <t>root.import.index.title</t>
+  </si>
+  <si>
+    <t>root.import.index.page-menu</t>
+  </si>
+  <si>
+    <t>Obecné</t>
+  </si>
+  <si>
+    <t>root.import.import.page-menu</t>
+  </si>
+  <si>
+    <t>root.import.upload-template.page-menu</t>
+  </si>
+  <si>
+    <t>Nahrát šablonu</t>
+  </si>
+  <si>
+    <t>root.import.upload-template.title</t>
+  </si>
+  <si>
+    <t>root.import.template.upload.name.label</t>
+  </si>
+  <si>
+    <t>Jméno šablony</t>
+  </si>
+  <si>
+    <t>root.import.template.name</t>
+  </si>
+  <si>
+    <t>Nastavené jméno šablony</t>
+  </si>
+  <si>
+    <t>root.import.template.upload.submit.label</t>
+  </si>
+  <si>
+    <t>Nastavit</t>
+  </si>
+  <si>
+    <t>root.import.template.upload</t>
+  </si>
+  <si>
+    <t>Nahrání šablony</t>
+  </si>
+  <si>
+    <t>root.import.template.upload.hint</t>
+  </si>
+  <si>
+    <t>Zde je možné nahrát importní šablonu, kterou pak ostatní uživatelé mohou použít jako základní kámen pro vlastní importy.</t>
+  </si>
+  <si>
+    <t>root.import.template.page-menu</t>
+  </si>
+  <si>
+    <t>Seznam šablon</t>
+  </si>
+  <si>
+    <t>root.import.index.subtitle</t>
+  </si>
+  <si>
+    <t>Zde je možné spustit importy a spravovat šablony importů.</t>
+  </si>
+  <si>
+    <t>root.common.import.title</t>
+  </si>
+  <si>
+    <t>shared.import.create.title</t>
+  </si>
+  <si>
+    <t>Spustit import</t>
+  </si>
+  <si>
+    <t>shared.import.create.subtitle</t>
+  </si>
+  <si>
+    <t>Zde je možné spouštět veškeré importy, které aplikace podporuje.</t>
+  </si>
+  <si>
+    <t>form-item.file.label</t>
+  </si>
+  <si>
+    <t>Soubor</t>
+  </si>
+  <si>
+    <t>shared.import.upload</t>
+  </si>
+  <si>
+    <t>Nahrajte soubor</t>
+  </si>
+  <si>
+    <t>shared.import.submit</t>
+  </si>
+  <si>
+    <t>shared.import.import.tab.title</t>
+  </si>
+  <si>
+    <t>shared.import.table.tab.title</t>
+  </si>
+  <si>
+    <t>Úlohy</t>
+  </si>
+  <si>
+    <t>shared.job.column.status.label</t>
+  </si>
+  <si>
+    <t>Stav</t>
+  </si>
+  <si>
+    <t>shared.job.column.service.label</t>
+  </si>
+  <si>
+    <t>Služba</t>
+  </si>
+  <si>
+    <t>shared.job.column.progress.label</t>
+  </si>
+  <si>
+    <t>Průběh</t>
+  </si>
+  <si>
+    <t>shared.job.column.stats.label</t>
+  </si>
+  <si>
+    <t>shared.job.column.runtime.label</t>
+  </si>
+  <si>
+    <t>Doba běhu</t>
+  </si>
+  <si>
+    <t>common.nothing-found</t>
+  </si>
+  <si>
+    <t>Žádná data</t>
+  </si>
+  <si>
+    <t>shared.import.success</t>
+  </si>
+  <si>
+    <t>Import byl úspěšně spuštěn.</t>
+  </si>
+  <si>
+    <t>job.status.6</t>
+  </si>
+  <si>
+    <t>Ke kontrole</t>
+  </si>
+  <si>
+    <t>shared.job.commit.success</t>
+  </si>
+  <si>
+    <t>Úloha byla potvrzena</t>
+  </si>
+  <si>
+    <t>job.status.3</t>
+  </si>
+  <si>
+    <t>Hotovo</t>
+  </si>
+  <si>
+    <t>job.status.0</t>
+  </si>
+  <si>
+    <t>Vytvořeno</t>
+  </si>
+  <si>
+    <t>job.status.1</t>
+  </si>
+  <si>
+    <t>Naplánováno</t>
+  </si>
+  <si>
+    <t>job.status.2</t>
+  </si>
+  <si>
+    <t>Probíhá</t>
+  </si>
+  <si>
+    <t>job.status.4</t>
+  </si>
+  <si>
+    <t>Selhání</t>
+  </si>
+  <si>
+    <t>job.status.5</t>
+  </si>
+  <si>
+    <t>Přerušeno</t>
+  </si>
+  <si>
+    <t>job-service.Edde\Excel\ExcelImportService</t>
+  </si>
+  <si>
+    <t>Import Excelu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>shared.import.tool.commit.button</t>
+  </si>
+  <si>
+    <t>Potvrdit všechny úlohy</t>
+  </si>
+  <si>
+    <t>shared.import.tool.interrupt.button</t>
+  </si>
+  <si>
+    <t>Přerušit všechny úlohy</t>
+  </si>
+  <si>
+    <t>shared.import.tool.clear.button</t>
+  </si>
+  <si>
+    <t>Odstranit úlohy</t>
+  </si>
+  <si>
+    <t>shared.import.commit.confirm.title</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete potvrdit všechny úlohy?</t>
+  </si>
+  <si>
+    <t>shared.import.interrupt.confirm.title</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete přerušit všechny běžící úlohy?</t>
+  </si>
+  <si>
+    <t>shared.import.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit všechny (neběžící) úlohy?</t>
+  </si>
+  <si>
+    <t>shared.job.delete-all.success</t>
+  </si>
+  <si>
+    <t>Úlohy byly úspěšně odstraněny.</t>
+  </si>
+  <si>
+    <t>shared.job.commit-all.success</t>
+  </si>
+  <si>
+    <t>Úlohy byly úspěšně potvrzeny.</t>
+  </si>
+  <si>
+    <t>shared.job.interrupt-all.success</t>
+  </si>
+  <si>
+    <t>Úlohy byly úspěšně přerušeny.</t>
+  </si>
+  <si>
+    <t>shared.file.column.name</t>
+  </si>
+  <si>
+    <t>Název souboru</t>
+  </si>
+  <si>
+    <t>shared.file.column.size</t>
+  </si>
+  <si>
+    <t>Velikost</t>
+  </si>
+  <si>
+    <t>shared.file.column.user</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>shared.file.force-gc.title</t>
+  </si>
+  <si>
+    <t>Odstranit zastaralé soubory</t>
+  </si>
+  <si>
+    <t>shared.file.gc.success</t>
+  </si>
+  <si>
+    <t>Čištění souborů bylo úspěšné. Počet odstraněných záznamů: {{data.records}}, počet odstraněných souborů {{data.files}}, čas běhu {{data.runtime}}.</t>
+  </si>
+  <si>
+    <t>root.import.template.title</t>
+  </si>
+  <si>
+    <t>Šablony pro import</t>
+  </si>
+  <si>
+    <t>root.job.index.menu</t>
+  </si>
+  <si>
+    <t>root.common.index.menu</t>
+  </si>
+  <si>
+    <t>root.upgrade.index.menu</t>
+  </si>
+  <si>
+    <t>Aktualizace</t>
+  </si>
+  <si>
+    <t>root.file.menu</t>
+  </si>
+  <si>
+    <t>Soubory</t>
+  </si>
+  <si>
+    <t>root.profiler.menu</t>
+  </si>
+  <si>
+    <t>Profiler</t>
+  </si>
+  <si>
+    <t>root.user.menu</t>
+  </si>
+  <si>
+    <t>Uživatelé</t>
+  </si>
+  <si>
+    <t>root.sites.menu</t>
+  </si>
+  <si>
+    <t>Aplikace</t>
+  </si>
+  <si>
+    <t>root.external.menu</t>
+  </si>
+  <si>
+    <t>Externí nástroje</t>
+  </si>
+  <si>
+    <t>root.download-sdk.menu</t>
+  </si>
+  <si>
+    <t>SDK</t>
+  </si>
+  <si>
+    <t>root.discovery.menu</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
+    <t>root.lab.menu</t>
+  </si>
+  <si>
+    <t>Laboratoř</t>
+  </si>
+  <si>
+    <t>root.public.menu</t>
+  </si>
+  <si>
+    <t>Veřejný web</t>
+  </si>
+  <si>
+    <t>lab.home.title</t>
+  </si>
+  <si>
+    <t>lab.home.welcome-title</t>
+  </si>
+  <si>
+    <t>Vítejte v Laboratoři!</t>
+  </si>
+  <si>
+    <t>lab.home.welcome-subtitle</t>
+  </si>
+  <si>
+    <t>V této aplikaci naleznete plno zajímavých nástrojů, které vám pomohou zlepšit požitek z vapování!</t>
+  </si>
+  <si>
+    <t>lab.build.menu</t>
+  </si>
+  <si>
+    <t>Buildy</t>
+  </si>
+  <si>
+    <t>lab.home.menu</t>
+  </si>
+  <si>
+    <t>lab.user.profile.tooltip</t>
+  </si>
+  <si>
+    <t>Váš profil</t>
+  </si>
+  <si>
+    <t>common.sign-out.tooltip</t>
+  </si>
+  <si>
+    <t>Odhlásit se</t>
+  </si>
+  <si>
+    <t>shared.job.preview.common</t>
+  </si>
+  <si>
+    <t>shared.job.preview.job-log</t>
+  </si>
+  <si>
+    <t>Deník</t>
+  </si>
+  <si>
+    <t>shared.job.preview.result</t>
+  </si>
+  <si>
+    <t>Výstup</t>
+  </si>
+  <si>
+    <t>shared.job-log.table.message</t>
+  </si>
+  <si>
+    <t>Zpráva</t>
+  </si>
+  <si>
+    <t>shared.job-log.table.reference</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>shared.job-log.table.level</t>
+  </si>
+  <si>
+    <t>Úroveň</t>
+  </si>
+  <si>
+    <t>shared.job-log.table.type</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>shared.log.type.common</t>
+  </si>
+  <si>
+    <t>shared.job.preview.progress</t>
+  </si>
+  <si>
+    <t>shared.job.preview.status</t>
+  </si>
+  <si>
+    <t>shared.job.preview.service</t>
+  </si>
+  <si>
+    <t>shared.job.preview.user</t>
+  </si>
+  <si>
+    <t>shared.job.preview.ratio</t>
+  </si>
+  <si>
+    <t>Úspěšnost</t>
+  </si>
+  <si>
+    <t>shared.job.preview.stats</t>
+  </si>
+  <si>
+    <t>Úspěšné/Selhání</t>
+  </si>
+  <si>
+    <t>shared.job.preview.runtime</t>
+  </si>
+  <si>
+    <t>shared.job.preview.performance</t>
+  </si>
+  <si>
+    <t>Relativní výkon</t>
+  </si>
+  <si>
+    <t>shared.job.preview.created</t>
+  </si>
+  <si>
+    <t>shared.job.preview.done</t>
+  </si>
+  <si>
+    <t>Dokončeno</t>
+  </si>
+  <si>
+    <t>shared.job.preview.params</t>
+  </si>
+  <si>
+    <t>Parametry</t>
   </si>
 </sst>
 </file>
@@ -654,10 +1227,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,6 +1689,1161 @@
       </c>
       <c r="C41" s="1" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added some new translations
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F55E12-8A9F-45BA-A253-2E2C9EB8127A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09C176-B5E0-4DDE-9364-3ECEFB35D62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="3675" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="342">
   <si>
     <t>cs</t>
   </si>
@@ -864,6 +864,198 @@
   </si>
   <si>
     <t>Parametry</t>
+  </si>
+  <si>
+    <t>root.common.index.title</t>
+  </si>
+  <si>
+    <t>Obecné nástroje</t>
+  </si>
+  <si>
+    <t>root.common.index.subtitle</t>
+  </si>
+  <si>
+    <t>Sada nástrojů, u kterých se nevědělo, kam s nimi (zatím).</t>
+  </si>
+  <si>
+    <t>root.common.logs.menu</t>
+  </si>
+  <si>
+    <t>Logy</t>
+  </si>
+  <si>
+    <t>root.common.utils.menu</t>
+  </si>
+  <si>
+    <t>Nástroje</t>
+  </si>
+  <si>
+    <t>root.upgrade.index.title</t>
+  </si>
+  <si>
+    <t>root.upgrade.index.subtitle</t>
+  </si>
+  <si>
+    <t>Aplikace by se měla držet aktualizovaná sama, nicméně aktuální stav je možné vidět zde.</t>
+  </si>
+  <si>
+    <t>root.upgrade.run.menu</t>
+  </si>
+  <si>
+    <t>Aktualizovat</t>
+  </si>
+  <si>
+    <t>root.upgrade.list.menu</t>
+  </si>
+  <si>
+    <t>Seznam aktualizací</t>
+  </si>
+  <si>
+    <t>root.upgrade.list.title</t>
+  </si>
+  <si>
+    <t>root.upgrade.table.active.title</t>
+  </si>
+  <si>
+    <t>Instalováno</t>
+  </si>
+  <si>
+    <t>root.upgrade.table.version.title</t>
+  </si>
+  <si>
+    <t>Verze</t>
+  </si>
+  <si>
+    <t>root.upgrade.table.name.title</t>
+  </si>
+  <si>
+    <t>Název</t>
+  </si>
+  <si>
+    <t>root.upgrade.run.title</t>
+  </si>
+  <si>
+    <t>Spustit aktualizaci</t>
+  </si>
+  <si>
+    <t>root.upgrade.run.button</t>
+  </si>
+  <si>
+    <t>Spustit</t>
+  </si>
+  <si>
+    <t>root.job.index.title</t>
+  </si>
+  <si>
+    <t>Ulohy</t>
+  </si>
+  <si>
+    <t>root.job.index.subtitle</t>
+  </si>
+  <si>
+    <t>Správa úloh na pozadí.</t>
+  </si>
+  <si>
+    <t>root.job.index.page-menu</t>
+  </si>
+  <si>
+    <t>root.job.list.page-menu</t>
+  </si>
+  <si>
+    <t>root.job.list.title</t>
+  </si>
+  <si>
+    <t>Seznam úloh</t>
+  </si>
+  <si>
+    <t>root.file.list.title</t>
+  </si>
+  <si>
+    <t>Seznam souborů</t>
+  </si>
+  <si>
+    <t>shared.file.column.path</t>
+  </si>
+  <si>
+    <t>Cesta</t>
+  </si>
+  <si>
+    <t>shared.file.column.native</t>
+  </si>
+  <si>
+    <t>Umístění</t>
+  </si>
+  <si>
+    <t>shared.file.column.mime</t>
+  </si>
+  <si>
+    <t>Mime</t>
+  </si>
+  <si>
+    <t>shared.file.column.ttl</t>
+  </si>
+  <si>
+    <t>Čas vypřšení</t>
+  </si>
+  <si>
+    <t>shared.file.column.created</t>
+  </si>
+  <si>
+    <t>Vytvořen</t>
+  </si>
+  <si>
+    <t>shared.file.column.updated</t>
+  </si>
+  <si>
+    <t>Aktualizován</t>
+  </si>
+  <si>
+    <t>root.file.list.menu</t>
+  </si>
+  <si>
+    <t>root.file.upload.menu</t>
+  </si>
+  <si>
+    <t>Nahrát soubor</t>
+  </si>
+  <si>
+    <t>root.file.upload.title</t>
+  </si>
+  <si>
+    <t>shared.file.upload.path.label</t>
+  </si>
+  <si>
+    <t>shared.file.upload.replace.label</t>
+  </si>
+  <si>
+    <t>shared.file.upload.submit.label</t>
+  </si>
+  <si>
+    <t>shared.file.upload.name.label</t>
+  </si>
+  <si>
+    <t>Nahradit?</t>
+  </si>
+  <si>
+    <t>root.file.path</t>
+  </si>
+  <si>
+    <t>root.file.name</t>
+  </si>
+  <si>
+    <t>root.file.replace</t>
+  </si>
+  <si>
+    <t>root.file.upload</t>
+  </si>
+  <si>
+    <t>Nahrání souboru</t>
+  </si>
+  <si>
+    <t>root.file.upload.hint</t>
+  </si>
+  <si>
+    <t>Zde je možné nahrát libovolný soubor do systému.</t>
   </si>
 </sst>
 </file>
@@ -1227,10 +1419,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,6 +3036,435 @@
       </c>
       <c r="C146" s="1" t="s">
         <v>277</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing wizard stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFFF8B-3CAF-4779-88DA-7140C94F198A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8154C-C6D4-42BF-B623-A1484BAF3C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="351">
   <si>
     <t>cs</t>
   </si>
@@ -1062,6 +1062,27 @@
   </si>
   <si>
     <t>Průvodci</t>
+  </si>
+  <si>
+    <t>lab.wizard.title</t>
+  </si>
+  <si>
+    <t>lab.wizard.subtitle</t>
+  </si>
+  <si>
+    <t>Veškeré užitečné postupy v aplikaci jsou řešené pomocí průvodců; tady je najdete.</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.title</t>
+  </si>
+  <si>
+    <t>Průvodce novým buildem</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.subtitle</t>
+  </si>
+  <si>
+    <t>Tento průvodce vám pomůže zaevidovat nový build.</t>
   </si>
 </sst>
 </file>
@@ -1425,10 +1446,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,6 +3503,50 @@
       </c>
       <c r="C186" s="1" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial wizard UI stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8154C-C6D4-42BF-B623-A1484BAF3C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A647C93B-B831-471F-86CD-DD632E1F6170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="370">
   <si>
     <t>cs</t>
   </si>
@@ -1073,16 +1073,73 @@
     <t>Veškeré užitečné postupy v aplikaci jsou řešené pomocí průvodců; tady je najdete.</t>
   </si>
   <si>
-    <t>lab.wizard.build.title</t>
-  </si>
-  <si>
     <t>Průvodce novým buildem</t>
   </si>
   <si>
-    <t>lab.wizard.build.subtitle</t>
-  </si>
-  <si>
     <t>Tento průvodce vám pomůže zaevidovat nový build.</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.first.title</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.first.subtitle</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.first.tab.label</t>
+  </si>
+  <si>
+    <t>Úvod</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.first.tab.description</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.coil.tab.label</t>
+  </si>
+  <si>
+    <t>Spirálka</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.coil.tab.description</t>
+  </si>
+  <si>
+    <t>Vyberte prosím použitou spirálku</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.atomizer.tab.label</t>
+  </si>
+  <si>
+    <t>Atomizér</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.atomizer.tab.description</t>
+  </si>
+  <si>
+    <t>Vyberte prosím použitý atomizér</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.cotton.tab.label</t>
+  </si>
+  <si>
+    <t>Vata</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.cotton.tab.description</t>
+  </si>
+  <si>
+    <t>Vyberte prosím vatu</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.build.tab.label</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>lab.wizard.build.build.tab.description</t>
+  </si>
+  <si>
+    <t>Doplňující informace o buildu</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1503,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,10 +3589,10 @@
         <v>0</v>
       </c>
       <c r="B189" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C189" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3543,10 +3600,120 @@
         <v>0</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial form for build
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A647C93B-B831-471F-86CD-DD632E1F6170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46A14B8-A333-CE49-9F15-600A3E61EA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="385">
   <si>
     <t>cs</t>
   </si>
@@ -1140,6 +1140,51 @@
   </si>
   <si>
     <t>Doplňující informace o buildu</t>
+  </si>
+  <si>
+    <t>Seznam buildů</t>
+  </si>
+  <si>
+    <t>V této sekci je možné spravovat a vytvářet buildy.</t>
+  </si>
+  <si>
+    <t>lab.build.index.menu</t>
+  </si>
+  <si>
+    <t>lab.build.create.menu</t>
+  </si>
+  <si>
+    <t>Nový build</t>
+  </si>
+  <si>
+    <t>lab.build.list.menu</t>
+  </si>
+  <si>
+    <t>lab.build.title</t>
+  </si>
+  <si>
+    <t>lab.build.subtitle</t>
+  </si>
+  <si>
+    <t>lab.build.create.title</t>
+  </si>
+  <si>
+    <t>lab.build.create.subtitle</t>
+  </si>
+  <si>
+    <t>lab.build.name.label</t>
+  </si>
+  <si>
+    <t>Jméno</t>
+  </si>
+  <si>
+    <t>lab.build.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Jméno buildu musí být unikátní; později bude možné ho použít pro evidenci požitků (vapování).</t>
+  </si>
+  <si>
+    <t>lab.build.atomizerId.label</t>
   </si>
 </sst>
 </file>
@@ -1503,20 +1548,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B193" sqref="B193"/>
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1527,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1571,7 +1616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1582,7 +1627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1626,7 +1671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1715,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1759,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1792,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +1803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1791,7 +1836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1847,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1813,7 +1858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -1824,7 +1869,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1835,7 +1880,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1846,7 +1891,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1913,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1890,7 +1935,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -1901,7 +1946,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1968,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1979,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1990,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1956,7 +2001,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +2012,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1978,7 +2023,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +2034,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2000,7 +2045,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -2011,7 +2056,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2033,7 +2078,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -2055,7 +2100,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -2066,7 +2111,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +2133,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2099,7 +2144,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -2110,7 +2155,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2177,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -2143,7 +2188,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2199,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -2165,7 +2210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +2221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -2187,7 +2232,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2243,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -2209,7 +2254,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2265,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2276,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2287,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -2253,7 +2298,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -2264,7 +2309,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -2275,7 +2320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -2286,7 +2331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -2297,7 +2342,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -2308,7 +2353,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2364,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2375,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -2341,7 +2386,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -2352,7 +2397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2408,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2419,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -2385,7 +2430,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +2441,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2452,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -2418,7 +2463,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -2429,7 +2474,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -2440,7 +2485,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -2451,7 +2496,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +2507,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -2473,7 +2518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2529,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2540,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -2506,7 +2551,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -2517,7 +2562,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
@@ -2528,7 +2573,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -2539,7 +2584,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2595,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2606,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -2572,7 +2617,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2628,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -2594,7 +2639,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2650,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -2616,7 +2661,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -2627,7 +2672,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2683,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2694,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -2660,7 +2705,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2716,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2727,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -2693,7 +2738,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -2704,7 +2749,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -2715,7 +2760,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -2726,7 +2771,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2782,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +2793,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +2804,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +2815,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -2781,7 +2826,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +2837,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +2848,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -2814,7 +2859,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2870,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -2836,7 +2881,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +2892,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +2903,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +2914,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +2925,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -2891,7 +2936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +2947,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -2913,7 +2958,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -2924,7 +2969,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -2935,7 +2980,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -2946,7 +2991,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>0</v>
       </c>
@@ -2957,7 +3002,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +3013,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -2979,7 +3024,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
@@ -2990,7 +3035,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -3001,7 +3046,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3057,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +3068,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -3034,7 +3079,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3090,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -3056,7 +3101,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -3067,7 +3112,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>0</v>
       </c>
@@ -3078,7 +3123,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>0</v>
       </c>
@@ -3089,7 +3134,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>0</v>
       </c>
@@ -3100,7 +3145,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -3111,7 +3156,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>0</v>
       </c>
@@ -3122,7 +3167,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>0</v>
       </c>
@@ -3133,7 +3178,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>0</v>
       </c>
@@ -3144,7 +3189,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>0</v>
       </c>
@@ -3155,7 +3200,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>0</v>
       </c>
@@ -3166,7 +3211,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>0</v>
       </c>
@@ -3177,7 +3222,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3233,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -3199,7 +3244,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -3210,7 +3255,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
@@ -3221,7 +3266,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>0</v>
       </c>
@@ -3232,7 +3277,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>0</v>
       </c>
@@ -3243,7 +3288,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3299,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>0</v>
       </c>
@@ -3265,7 +3310,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
@@ -3276,7 +3321,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>0</v>
       </c>
@@ -3287,7 +3332,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>0</v>
       </c>
@@ -3298,7 +3343,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -3309,7 +3354,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
@@ -3320,7 +3365,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -3331,7 +3376,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>0</v>
       </c>
@@ -3342,7 +3387,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>0</v>
       </c>
@@ -3353,7 +3398,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>0</v>
       </c>
@@ -3364,7 +3409,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>0</v>
       </c>
@@ -3375,7 +3420,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>0</v>
       </c>
@@ -3386,7 +3431,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -3397,7 +3442,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>0</v>
       </c>
@@ -3408,7 +3453,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>0</v>
       </c>
@@ -3419,7 +3464,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>0</v>
       </c>
@@ -3430,7 +3475,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>0</v>
       </c>
@@ -3441,7 +3486,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3497,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>0</v>
       </c>
@@ -3463,7 +3508,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>0</v>
       </c>
@@ -3474,7 +3519,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>0</v>
       </c>
@@ -3485,7 +3530,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>0</v>
       </c>
@@ -3496,7 +3541,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>0</v>
       </c>
@@ -3507,7 +3552,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>0</v>
       </c>
@@ -3518,7 +3563,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>0</v>
       </c>
@@ -3529,7 +3574,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>0</v>
       </c>
@@ -3540,7 +3585,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>0</v>
       </c>
@@ -3551,7 +3596,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>0</v>
       </c>
@@ -3562,7 +3607,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>0</v>
       </c>
@@ -3573,7 +3618,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3629,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>0</v>
       </c>
@@ -3595,7 +3640,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>0</v>
       </c>
@@ -3606,7 +3651,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>0</v>
       </c>
@@ -3617,7 +3662,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>0</v>
       </c>
@@ -3628,7 +3673,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>0</v>
       </c>
@@ -3639,7 +3684,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>0</v>
       </c>
@@ -3650,7 +3695,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>0</v>
       </c>
@@ -3661,7 +3706,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>0</v>
       </c>
@@ -3672,7 +3717,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +3728,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>0</v>
       </c>
@@ -3694,7 +3739,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>0</v>
       </c>
@@ -3705,7 +3750,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>0</v>
       </c>
@@ -3714,6 +3759,116 @@
       </c>
       <c r="C200" s="1" t="s">
         <v>369</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3732,13 +3887,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -3746,7 +3901,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3767,13 +3922,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -3781,7 +3936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3789,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3797,7 +3952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Common: Preparing support for cascaded object creation
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46A14B8-A333-CE49-9F15-600A3E61EA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73A8F39-C1CF-2349-982A-0C30C2A7C317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="399">
   <si>
     <t>cs</t>
   </si>
@@ -1185,6 +1185,48 @@
   </si>
   <si>
     <t>lab.build.atomizerId.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.tooltip.create</t>
+  </si>
+  <si>
+    <t>Přidat atomizér</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.title</t>
+  </si>
+  <si>
+    <t>Vytvořit atomizér</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.subtitle</t>
+  </si>
+  <si>
+    <t>Přidejte nový atomizér, který tak bude přístupný ostatních a v buildech.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.name.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.vendorId.label</t>
+  </si>
+  <si>
+    <t>Výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.tooltip.create</t>
+  </si>
+  <si>
+    <t>Založit výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.subtitle</t>
+  </si>
+  <si>
+    <t>Výrobci jsou dostupní přes celou aplikaci, např. u atomizérů, modů, drátů a dalšího.</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.title</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1590,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3869,6 +3911,94 @@
       </c>
       <c r="C210" s="1" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So, initial cascade works!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73A8F39-C1CF-2349-982A-0C30C2A7C317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DB405D-2AD2-DE4D-A88C-F452E8CBE7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="417">
   <si>
     <t>cs</t>
   </si>
@@ -1227,6 +1227,60 @@
   </si>
   <si>
     <t>lab.vendor.create.title</t>
+  </si>
+  <si>
+    <t>lab.vendor.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Při zadávání jména výrobce se prosím snažte držet přesného názvu, včetně velikosti písmen a cizích znaků.</t>
+  </si>
+  <si>
+    <t>lab.vendor.name.label</t>
+  </si>
+  <si>
+    <t>Jméno výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.submit</t>
+  </si>
+  <si>
+    <t>lab.vendor.name.label.required</t>
+  </si>
+  <si>
+    <t>Jméno výrobce je povinné</t>
+  </si>
+  <si>
+    <t>lab.atomizer.name.label.required</t>
+  </si>
+  <si>
+    <t>Jméno atomizéru je povinné</t>
+  </si>
+  <si>
+    <t>lab.build.name.label.required</t>
+  </si>
+  <si>
+    <t>Jméno buildu je povinné</t>
+  </si>
+  <si>
+    <t>lab.build.create.submit</t>
+  </si>
+  <si>
+    <t>lab.vendor.create.success</t>
+  </si>
+  <si>
+    <t>Výrobce [{{data.name}}] byl úspěšně vytvořen.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.create.success</t>
+  </si>
+  <si>
+    <t>Atomizér [{{data.name}}] byl úspěšně vytvořen.</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3999,6 +4053,116 @@
       </c>
       <c r="C218" s="1" t="s">
         <v>397</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: First quite complex cascade works!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275A30D9-49F5-D44D-B131-C42260960CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C741F88-A39A-F74C-BBEE-BFF871BE8673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="457">
   <si>
     <t>cs</t>
   </si>
@@ -1308,6 +1308,99 @@
   </si>
   <si>
     <t>Odporový drát</t>
+  </si>
+  <si>
+    <t>lab.coil.ohm.label</t>
+  </si>
+  <si>
+    <t>Odpor spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.ohm.label.tooltip</t>
+  </si>
+  <si>
+    <t>Odporem spirálky je v tomto případě míněn odpor v základně atomizéru.</t>
+  </si>
+  <si>
+    <t>lab.coil.wraps.label.tooltip</t>
+  </si>
+  <si>
+    <t>Počet otoček</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uveďte prosím finální počet otoček (tzn. tolik, v kolika bude spirálka umístěna do atomizéru). </t>
+  </si>
+  <si>
+    <t>lab.coil.code.label</t>
+  </si>
+  <si>
+    <t>Kód spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Kód bude užitečný v importech, exportech a vůbec v identifikaci spirálky člověkěm. Musí být unikátní.</t>
+  </si>
+  <si>
+    <t>lab.coil.wraps.label</t>
+  </si>
+  <si>
+    <t>lab.wire.name.label</t>
+  </si>
+  <si>
+    <t>Název drátu</t>
+  </si>
+  <si>
+    <t>lab.wire.tooltip.create</t>
+  </si>
+  <si>
+    <t>Vytvořit drát</t>
+  </si>
+  <si>
+    <t>lab.wire.create.title</t>
+  </si>
+  <si>
+    <t>Nový drát</t>
+  </si>
+  <si>
+    <t>lab.wire.create.subtitle</t>
+  </si>
+  <si>
+    <t>Dráty se používají k tvorbě spirálek.</t>
+  </si>
+  <si>
+    <t>lab.wire.description.label</t>
+  </si>
+  <si>
+    <t>Popis</t>
+  </si>
+  <si>
+    <t>lab.wire.ga.label</t>
+  </si>
+  <si>
+    <t>Tloušťka (GA)</t>
+  </si>
+  <si>
+    <t>lab.wire.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.wire.create.submit</t>
+  </si>
+  <si>
+    <t>lab.coil.create.submit</t>
+  </si>
+  <si>
+    <t>lab.coil.create.success</t>
+  </si>
+  <si>
+    <t>Spirálka byla vytvoředna.</t>
+  </si>
+  <si>
+    <t>lab.wire.create.success</t>
+  </si>
+  <si>
+    <t>Drát byl uložen.</t>
   </si>
 </sst>
 </file>
@@ -1671,10 +1764,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
+    <sheetView tabSelected="1" topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4245,6 +4338,215 @@
       </c>
       <c r="C233" s="1" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Whoho, it's possible to create a build!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C741F88-A39A-F74C-BBEE-BFF871BE8673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF062426-4DB2-E341-B13A-2DF6D761F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="486">
   <si>
     <t>cs</t>
   </si>
@@ -1401,6 +1401,93 @@
   </si>
   <si>
     <t>Drát byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.cotton.name.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.build.cottonId.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.tooltip.create</t>
+  </si>
+  <si>
+    <t>Přidat vatu</t>
+  </si>
+  <si>
+    <t>lab.cotton.create.title</t>
+  </si>
+  <si>
+    <t>lab.cotton.create.subtitle</t>
+  </si>
+  <si>
+    <t>Přidejte vatu pro použití v buildech.</t>
+  </si>
+  <si>
+    <t>lab.cotton.description.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit vatu</t>
+  </si>
+  <si>
+    <t>lab.cotton.create.success</t>
+  </si>
+  <si>
+    <t>Vata byla uložena.</t>
+  </si>
+  <si>
+    <t>lab.build.coils.label</t>
+  </si>
+  <si>
+    <t>Počet spirálek</t>
+  </si>
+  <si>
+    <t>lab.build.coil.label</t>
+  </si>
+  <si>
+    <t>Pozice spirálky</t>
+  </si>
+  <si>
+    <t>lab.build.coil.label.tooltip</t>
+  </si>
+  <si>
+    <t>Pozice spirálky je relativní umístění proti vzduchu, kdy přesné umístění je nula, umístění výše je kladné číslo a umístění níže záporné číslo. Smyslem je napovědět, jak byla spirálka umístěna a jaký byl výsledný vliv na požitek.</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.label</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.label.tooltip</t>
+  </si>
+  <si>
+    <t>Množství vaty</t>
+  </si>
+  <si>
+    <t>Množství vaty je relativní množství, kdy nula znamená optimální usazení ve spirálce, kladná čísla znamenají větší množství vaty a záporná naopak menší množství vaty. Smyslem je napovědět, jak který atomizér snáží jaké množství vaty.</t>
+  </si>
+  <si>
+    <t>lab.build.common.title</t>
+  </si>
+  <si>
+    <t>lab.build.coil.title</t>
+  </si>
+  <si>
+    <t>lab.build.cotton.title</t>
+  </si>
+  <si>
+    <t>lab.build.description.label</t>
+  </si>
+  <si>
+    <t>lab.build.ohm.label</t>
+  </si>
+  <si>
+    <t>Odpor buildu</t>
   </si>
 </sst>
 </file>
@@ -1764,10 +1851,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C252"/>
+  <dimension ref="A1:C271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4547,6 +4634,215 @@
       </c>
       <c r="C252" s="1" t="s">
         <v>456</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A bit improved some stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF062426-4DB2-E341-B13A-2DF6D761F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0EDDB9-22C6-6D4B-A5BF-F4C05E10F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="487">
   <si>
     <t>cs</t>
   </si>
@@ -1137,6 +1137,9 @@
   </si>
   <si>
     <t>Doplňující informace o buildu</t>
+  </si>
+  <si>
+    <t>lab.build.list.title</t>
   </si>
   <si>
     <t>Seznam buildů</t>
@@ -1851,10 +1854,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C271"/>
+  <dimension ref="A1:C272"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B261" sqref="B261"/>
+      <selection activeCell="B264" sqref="B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1902,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -4069,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>241</v>
@@ -4080,10 +4083,10 @@
         <v>0</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
@@ -4091,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>119</v>
@@ -4102,10 +4105,10 @@
         <v>0</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
@@ -4113,10 +4116,10 @@
         <v>0</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -4124,10 +4127,10 @@
         <v>0</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
@@ -4135,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>182</v>
@@ -4146,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
@@ -4157,10 +4160,10 @@
         <v>0</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -4168,7 +4171,7 @@
         <v>0</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>358</v>
@@ -4179,10 +4182,10 @@
         <v>0</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -4190,10 +4193,10 @@
         <v>0</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
@@ -4201,10 +4204,10 @@
         <v>0</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
@@ -4212,10 +4215,10 @@
         <v>0</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
@@ -4223,10 +4226,10 @@
         <v>0</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -4234,10 +4237,10 @@
         <v>0</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
@@ -4245,10 +4248,10 @@
         <v>0</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
@@ -4256,10 +4259,10 @@
         <v>0</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -4267,10 +4270,10 @@
         <v>0</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
@@ -4278,10 +4281,10 @@
         <v>0</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
@@ -4289,10 +4292,10 @@
         <v>0</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
@@ -4300,10 +4303,10 @@
         <v>0</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
@@ -4311,10 +4314,10 @@
         <v>0</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
@@ -4322,10 +4325,10 @@
         <v>0</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
@@ -4333,10 +4336,10 @@
         <v>0</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
@@ -4344,10 +4347,10 @@
         <v>0</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
@@ -4355,10 +4358,10 @@
         <v>0</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
@@ -4366,10 +4369,10 @@
         <v>0</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
@@ -4377,7 +4380,7 @@
         <v>0</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>354</v>
@@ -4388,10 +4391,10 @@
         <v>0</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
@@ -4399,10 +4402,10 @@
         <v>0</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
@@ -4410,10 +4413,10 @@
         <v>0</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
@@ -4421,10 +4424,10 @@
         <v>0</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
@@ -4432,10 +4435,10 @@
         <v>0</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
@@ -4443,10 +4446,10 @@
         <v>0</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
@@ -4454,10 +4457,10 @@
         <v>0</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
@@ -4465,10 +4468,10 @@
         <v>0</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
@@ -4476,10 +4479,10 @@
         <v>0</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
@@ -4487,10 +4490,10 @@
         <v>0</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
@@ -4498,10 +4501,10 @@
         <v>0</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
@@ -4509,10 +4512,10 @@
         <v>0</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
@@ -4520,10 +4523,10 @@
         <v>0</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
@@ -4531,10 +4534,10 @@
         <v>0</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -4542,10 +4545,10 @@
         <v>0</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
@@ -4553,10 +4556,10 @@
         <v>0</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
@@ -4564,10 +4567,10 @@
         <v>0</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
@@ -4575,10 +4578,10 @@
         <v>0</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
@@ -4586,10 +4589,10 @@
         <v>0</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
@@ -4597,10 +4600,10 @@
         <v>0</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
@@ -4608,10 +4611,10 @@
         <v>0</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
@@ -4619,10 +4622,10 @@
         <v>0</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
@@ -4630,10 +4633,10 @@
         <v>0</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
@@ -4641,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>298</v>
@@ -4652,10 +4655,10 @@
         <v>0</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
@@ -4663,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>362</v>
@@ -4674,10 +4677,10 @@
         <v>0</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,10 +4688,10 @@
         <v>0</v>
       </c>
       <c r="B257" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
@@ -4696,10 +4699,10 @@
         <v>0</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
@@ -4707,10 +4710,10 @@
         <v>0</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
@@ -4718,10 +4721,10 @@
         <v>0</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
@@ -4729,10 +4732,10 @@
         <v>0</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
@@ -4740,10 +4743,10 @@
         <v>0</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
@@ -4751,10 +4754,10 @@
         <v>0</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -4762,10 +4765,10 @@
         <v>0</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
@@ -4773,10 +4776,10 @@
         <v>0</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -4784,10 +4787,10 @@
         <v>0</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
@@ -4795,7 +4798,7 @@
         <v>0</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>119</v>
@@ -4806,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>354</v>
@@ -4817,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>362</v>
@@ -4828,10 +4831,10 @@
         <v>0</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
@@ -4839,10 +4842,21 @@
         <v>0</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A lot of small fixes/improvements
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0EDDB9-22C6-6D4B-A5BF-F4C05E10F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC05712-36AE-4329-8FD9-9B4524AA4702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="505">
   <si>
     <t>cs</t>
   </si>
@@ -1491,6 +1491,60 @@
   </si>
   <si>
     <t>Odpor buildu</t>
+  </si>
+  <si>
+    <t>lab.vape.menu</t>
+  </si>
+  <si>
+    <t>Vapování</t>
+  </si>
+  <si>
+    <t>lab.liquid.menu</t>
+  </si>
+  <si>
+    <t>Liquidy</t>
+  </si>
+  <si>
+    <t>lab.atomizer.menu</t>
+  </si>
+  <si>
+    <t>Atomizéry</t>
+  </si>
+  <si>
+    <t>lab.mod.menu</t>
+  </si>
+  <si>
+    <t>Mody</t>
+  </si>
+  <si>
+    <t>lab.cell.menu</t>
+  </si>
+  <si>
+    <t>Články</t>
+  </si>
+  <si>
+    <t>lab.vendor.menu</t>
+  </si>
+  <si>
+    <t>Výrobci</t>
+  </si>
+  <si>
+    <t>lab.cotton.menu</t>
+  </si>
+  <si>
+    <t>Vaty</t>
+  </si>
+  <si>
+    <t>lab.wire.menu</t>
+  </si>
+  <si>
+    <t>Dráty</t>
+  </si>
+  <si>
+    <t>lab.coil.menu</t>
+  </si>
+  <si>
+    <t>Spirálky</t>
   </si>
 </sst>
 </file>
@@ -1854,20 +1908,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C272"/>
+  <dimension ref="A1:C281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B264" sqref="B264"/>
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="72.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="72.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -1878,7 +1932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1889,7 +1943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1900,7 +1954,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +1987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1944,7 +1998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +2009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +2020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +2031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1999,7 +2053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2010,7 +2064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2043,7 +2097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2108,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2065,7 +2119,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2076,7 +2130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2152,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2163,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2185,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2196,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2153,7 +2207,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2175,7 +2229,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2186,7 +2240,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2197,7 +2251,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2208,7 +2262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2219,7 +2273,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2284,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2241,7 +2295,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +2306,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2263,7 +2317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2274,7 +2328,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2339,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2296,7 +2350,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2361,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2318,7 +2372,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2394,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2405,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,7 +2416,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +2427,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -2384,7 +2438,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -2395,7 +2449,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2460,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -2417,7 +2471,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -2428,7 +2482,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +2493,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -2450,7 +2504,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +2515,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -2483,7 +2537,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -2494,7 +2548,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2505,7 +2559,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2570,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -2527,7 +2581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2592,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2603,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -2560,7 +2614,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2625,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -2582,7 +2636,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -2593,7 +2647,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -2604,7 +2658,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -2615,7 +2669,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2680,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -2648,7 +2702,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -2659,7 +2713,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2724,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +2735,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -2692,7 +2746,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -2703,7 +2757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -2725,7 +2779,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +2790,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -2747,7 +2801,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2812,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -2769,7 +2823,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -2780,7 +2834,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -2791,7 +2845,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2856,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -2813,7 +2867,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -2824,7 +2878,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
@@ -2835,7 +2889,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
@@ -2846,7 +2900,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -2857,7 +2911,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>0</v>
       </c>
@@ -2868,7 +2922,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>0</v>
       </c>
@@ -2879,7 +2933,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +2944,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2955,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2966,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>0</v>
       </c>
@@ -2923,7 +2977,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -2934,7 +2988,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +2999,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -2956,7 +3010,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -2967,7 +3021,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3032,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -2989,7 +3043,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -3000,7 +3054,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -3011,7 +3065,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -3022,7 +3076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -3033,7 +3087,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3098,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>0</v>
       </c>
@@ -3055,7 +3109,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -3066,7 +3120,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3131,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +3142,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
@@ -3099,7 +3153,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>0</v>
       </c>
@@ -3110,7 +3164,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
@@ -3121,7 +3175,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -3132,7 +3186,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -3143,7 +3197,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -3154,7 +3208,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -3165,7 +3219,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3230,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -3187,7 +3241,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -3198,7 +3252,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>0</v>
       </c>
@@ -3209,7 +3263,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -3220,7 +3274,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3285,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -3242,7 +3296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3307,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -3264,7 +3318,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -3275,7 +3329,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>0</v>
       </c>
@@ -3286,7 +3340,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>0</v>
       </c>
@@ -3297,7 +3351,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>0</v>
       </c>
@@ -3308,7 +3362,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>0</v>
       </c>
@@ -3319,7 +3373,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
@@ -3330,7 +3384,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>0</v>
       </c>
@@ -3341,7 +3395,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3406,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>0</v>
       </c>
@@ -3363,7 +3417,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>0</v>
       </c>
@@ -3374,7 +3428,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -3385,7 +3439,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3450,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>0</v>
       </c>
@@ -3407,7 +3461,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>0</v>
       </c>
@@ -3418,7 +3472,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>0</v>
       </c>
@@ -3429,7 +3483,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>0</v>
       </c>
@@ -3440,7 +3494,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>0</v>
       </c>
@@ -3451,7 +3505,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>0</v>
       </c>
@@ -3462,7 +3516,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>0</v>
       </c>
@@ -3473,7 +3527,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>0</v>
       </c>
@@ -3484,7 +3538,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>0</v>
       </c>
@@ -3495,7 +3549,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>0</v>
       </c>
@@ -3506,7 +3560,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>0</v>
       </c>
@@ -3517,7 +3571,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>0</v>
       </c>
@@ -3528,7 +3582,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3593,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -3550,7 +3604,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -3561,7 +3615,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3626,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>0</v>
       </c>
@@ -3583,7 +3637,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>0</v>
       </c>
@@ -3594,7 +3648,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>0</v>
       </c>
@@ -3605,7 +3659,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>0</v>
       </c>
@@ -3616,7 +3670,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
@@ -3627,7 +3681,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>0</v>
       </c>
@@ -3638,7 +3692,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>0</v>
       </c>
@@ -3649,7 +3703,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -3660,7 +3714,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
@@ -3671,7 +3725,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -3682,7 +3736,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>0</v>
       </c>
@@ -3693,7 +3747,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>0</v>
       </c>
@@ -3704,7 +3758,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>0</v>
       </c>
@@ -3715,7 +3769,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>0</v>
       </c>
@@ -3726,7 +3780,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>0</v>
       </c>
@@ -3737,7 +3791,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -3748,7 +3802,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>0</v>
       </c>
@@ -3759,7 +3813,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>0</v>
       </c>
@@ -3770,7 +3824,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>0</v>
       </c>
@@ -3781,7 +3835,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>0</v>
       </c>
@@ -3792,7 +3846,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>0</v>
       </c>
@@ -3803,7 +3857,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>0</v>
       </c>
@@ -3814,7 +3868,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>0</v>
       </c>
@@ -3825,7 +3879,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>0</v>
       </c>
@@ -3836,7 +3890,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>0</v>
       </c>
@@ -3847,7 +3901,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>0</v>
       </c>
@@ -3858,7 +3912,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>0</v>
       </c>
@@ -3869,7 +3923,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>0</v>
       </c>
@@ -3880,7 +3934,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3945,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3956,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>0</v>
       </c>
@@ -3913,7 +3967,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>0</v>
       </c>
@@ -3924,7 +3978,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>0</v>
       </c>
@@ -3935,7 +3989,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>0</v>
       </c>
@@ -3946,7 +4000,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>0</v>
       </c>
@@ -3957,7 +4011,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>0</v>
       </c>
@@ -3968,7 +4022,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>0</v>
       </c>
@@ -3979,7 +4033,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>0</v>
       </c>
@@ -3990,7 +4044,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>0</v>
       </c>
@@ -4001,7 +4055,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>0</v>
       </c>
@@ -4012,7 +4066,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +4077,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4088,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>0</v>
       </c>
@@ -4045,7 +4099,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>0</v>
       </c>
@@ -4056,7 +4110,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>0</v>
       </c>
@@ -4067,7 +4121,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>0</v>
       </c>
@@ -4078,7 +4132,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>0</v>
       </c>
@@ -4089,7 +4143,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>0</v>
       </c>
@@ -4100,7 +4154,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>0</v>
       </c>
@@ -4111,7 +4165,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>0</v>
       </c>
@@ -4122,7 +4176,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>0</v>
       </c>
@@ -4133,7 +4187,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>0</v>
       </c>
@@ -4144,7 +4198,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>0</v>
       </c>
@@ -4155,7 +4209,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>0</v>
       </c>
@@ -4166,7 +4220,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>0</v>
       </c>
@@ -4177,7 +4231,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>0</v>
       </c>
@@ -4188,7 +4242,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>0</v>
       </c>
@@ -4199,7 +4253,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>0</v>
       </c>
@@ -4210,7 +4264,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>0</v>
       </c>
@@ -4221,7 +4275,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>0</v>
       </c>
@@ -4232,7 +4286,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>0</v>
       </c>
@@ -4243,7 +4297,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>0</v>
       </c>
@@ -4254,7 +4308,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>0</v>
       </c>
@@ -4265,7 +4319,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>0</v>
       </c>
@@ -4276,7 +4330,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>0</v>
       </c>
@@ -4287,7 +4341,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>0</v>
       </c>
@@ -4298,7 +4352,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>0</v>
       </c>
@@ -4309,7 +4363,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>0</v>
       </c>
@@ -4320,7 +4374,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>0</v>
       </c>
@@ -4331,7 +4385,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>0</v>
       </c>
@@ -4342,7 +4396,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4407,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>0</v>
       </c>
@@ -4364,7 +4418,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>0</v>
       </c>
@@ -4375,7 +4429,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>0</v>
       </c>
@@ -4386,7 +4440,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>0</v>
       </c>
@@ -4397,7 +4451,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>0</v>
       </c>
@@ -4408,7 +4462,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>0</v>
       </c>
@@ -4419,7 +4473,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>0</v>
       </c>
@@ -4430,7 +4484,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>0</v>
       </c>
@@ -4441,7 +4495,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>0</v>
       </c>
@@ -4452,7 +4506,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>0</v>
       </c>
@@ -4463,7 +4517,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>0</v>
       </c>
@@ -4474,7 +4528,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>0</v>
       </c>
@@ -4485,7 +4539,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>0</v>
       </c>
@@ -4496,7 +4550,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>0</v>
       </c>
@@ -4507,7 +4561,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>0</v>
       </c>
@@ -4518,7 +4572,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4583,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>0</v>
       </c>
@@ -4540,7 +4594,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>0</v>
       </c>
@@ -4551,7 +4605,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>0</v>
       </c>
@@ -4562,7 +4616,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>0</v>
       </c>
@@ -4573,7 +4627,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>0</v>
       </c>
@@ -4584,7 +4638,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>0</v>
       </c>
@@ -4595,7 +4649,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>0</v>
       </c>
@@ -4606,7 +4660,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>0</v>
       </c>
@@ -4617,7 +4671,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>0</v>
       </c>
@@ -4628,7 +4682,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>0</v>
       </c>
@@ -4639,7 +4693,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>0</v>
       </c>
@@ -4650,7 +4704,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>0</v>
       </c>
@@ -4661,7 +4715,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>0</v>
       </c>
@@ -4672,7 +4726,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>0</v>
       </c>
@@ -4683,7 +4737,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>0</v>
       </c>
@@ -4694,7 +4748,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>0</v>
       </c>
@@ -4705,7 +4759,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>0</v>
       </c>
@@ -4716,7 +4770,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>0</v>
       </c>
@@ -4727,7 +4781,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>0</v>
       </c>
@@ -4738,7 +4792,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>0</v>
       </c>
@@ -4749,7 +4803,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>0</v>
       </c>
@@ -4760,7 +4814,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>0</v>
       </c>
@@ -4771,7 +4825,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>0</v>
       </c>
@@ -4782,7 +4836,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>0</v>
       </c>
@@ -4793,7 +4847,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>0</v>
       </c>
@@ -4804,7 +4858,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>0</v>
       </c>
@@ -4815,7 +4869,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>0</v>
       </c>
@@ -4826,7 +4880,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>0</v>
       </c>
@@ -4837,7 +4891,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>0</v>
       </c>
@@ -4848,7 +4902,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>0</v>
       </c>
@@ -4857,6 +4911,105 @@
       </c>
       <c r="C272" s="1" t="s">
         <v>370</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -4875,13 +5028,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="51.5" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -4889,7 +5042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -4910,13 +5063,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -4924,7 +5077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4932,7 +5085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4940,7 +5093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Common: Some new menu icons
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC05712-36AE-4329-8FD9-9B4524AA4702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323B1817-2846-4CD5-89B0-45141E92DD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="508">
   <si>
     <t>cs</t>
   </si>
@@ -1545,6 +1545,15 @@
   </si>
   <si>
     <t>Spirálky</t>
+  </si>
+  <si>
+    <t>lab.tool.menu</t>
+  </si>
+  <si>
+    <t>lab.steep.menu</t>
+  </si>
+  <si>
+    <t>Zrání</t>
   </si>
 </sst>
 </file>
@@ -1908,10 +1917,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C281"/>
+  <dimension ref="A1:C283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B277" sqref="B277"/>
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5010,6 +5019,28 @@
       </c>
       <c r="C281" s="1" t="s">
         <v>504</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Updated build table
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323B1817-2846-4CD5-89B0-45141E92DD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82665D11-6B33-4F16-B213-7DFEED5EE9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="512">
   <si>
     <t>cs</t>
   </si>
@@ -1554,6 +1554,18 @@
   </si>
   <si>
     <t>Zrání</t>
+  </si>
+  <si>
+    <t>lab.build.button.create</t>
+  </si>
+  <si>
+    <t>lab.build.button.list</t>
+  </si>
+  <si>
+    <t>Nejnovější buildy</t>
+  </si>
+  <si>
+    <t>lab.build.latest.title</t>
   </si>
 </sst>
 </file>
@@ -1917,10 +1929,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C283"/>
+  <dimension ref="A1:C286"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B278" sqref="B278"/>
+      <selection activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5041,6 +5053,39 @@
       </c>
       <c r="C283" s="1" t="s">
         <v>507</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So initial listing works
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82665D11-6B33-4F16-B213-7DFEED5EE9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9491B186-5910-4F4C-BEEE-4DA378B310D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="526">
   <si>
     <t>cs</t>
   </si>
@@ -1566,6 +1566,48 @@
   </si>
   <si>
     <t>lab.build.latest.title</t>
+  </si>
+  <si>
+    <t>error.Duplicate entry [z_build_name_unique] of [z_build].</t>
+  </si>
+  <si>
+    <t>Tento název buildu jste již použili; zvolte prosím jiný.</t>
+  </si>
+  <si>
+    <t>lab.build.table.name</t>
+  </si>
+  <si>
+    <t>Jméno buildu</t>
+  </si>
+  <si>
+    <t>lab.build.table.atomizer</t>
+  </si>
+  <si>
+    <t>lab.build.table.cotton</t>
+  </si>
+  <si>
+    <t>lab.build.table.coil</t>
+  </si>
+  <si>
+    <t>lab.build.table.ohm</t>
+  </si>
+  <si>
+    <t>lab.build.table.coils</t>
+  </si>
+  <si>
+    <t>lab.build.table.created</t>
+  </si>
+  <si>
+    <t>lab.build.created.message</t>
+  </si>
+  <si>
+    <t>Build [{{data.name}}] byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.build.table.coilOffset</t>
+  </si>
+  <si>
+    <t>lab.build.table.cottonOffset</t>
   </si>
 </sst>
 </file>
@@ -1929,10 +1971,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C286"/>
+  <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B279" sqref="B279"/>
+    <sheetView tabSelected="1" topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B297" sqref="B297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5086,6 +5128,127 @@
       </c>
       <c r="C286" s="1" t="s">
         <v>510</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved build form
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC63BCD-745A-4D30-84AE-16B7248E82E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E5AC6-FAC2-47CB-9557-A231C6D815EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="532">
   <si>
     <t>cs</t>
   </si>
@@ -1496,9 +1496,6 @@
     <t>lab.vape.menu</t>
   </si>
   <si>
-    <t>Vapování</t>
-  </si>
-  <si>
     <t>lab.liquid.menu</t>
   </si>
   <si>
@@ -1620,6 +1617,15 @@
   </si>
   <si>
     <t>Detail buildu</t>
+  </si>
+  <si>
+    <t>Vape</t>
+  </si>
+  <si>
+    <t>lab.build.advanced.title</t>
+  </si>
+  <si>
+    <t>Pokročilé</t>
   </si>
 </sst>
 </file>
@@ -1983,9 +1989,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C299"/>
+  <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B297" sqref="B297"/>
     </sheetView>
   </sheetViews>
@@ -4996,7 +5002,7 @@
         <v>487</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>488</v>
+        <v>529</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5004,10 +5010,10 @@
         <v>0</v>
       </c>
       <c r="B274" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C274" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5015,10 +5021,10 @@
         <v>0</v>
       </c>
       <c r="B275" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -5026,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="B276" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C276" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C276" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5037,10 +5043,10 @@
         <v>0</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -5048,10 +5054,10 @@
         <v>0</v>
       </c>
       <c r="B278" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C278" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5059,10 +5065,10 @@
         <v>0</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>499</v>
-      </c>
-      <c r="C279" s="1" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,10 +5076,10 @@
         <v>0</v>
       </c>
       <c r="B280" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C280" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -5081,10 +5087,10 @@
         <v>0</v>
       </c>
       <c r="B281" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -5092,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>284</v>
@@ -5103,10 +5109,10 @@
         <v>0</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="C283" s="1" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>374</v>
@@ -5125,7 +5131,7 @@
         <v>0</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>370</v>
@@ -5136,10 +5142,10 @@
         <v>0</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -5147,10 +5153,10 @@
         <v>0</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="C287" s="1" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -5158,10 +5164,10 @@
         <v>0</v>
       </c>
       <c r="B288" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C288" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>358</v>
@@ -5180,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>362</v>
@@ -5191,7 +5197,7 @@
         <v>0</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>354</v>
@@ -5202,7 +5208,7 @@
         <v>0</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>486</v>
@@ -5213,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>472</v>
@@ -5224,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>322</v>
@@ -5235,10 +5241,10 @@
         <v>0</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="C295" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -5246,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>474</v>
@@ -5257,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>479</v>
@@ -5268,10 +5274,10 @@
         <v>0</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C298" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -5279,10 +5285,21 @@
         <v>0</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>529</v>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added some boirelplate stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E5AC6-FAC2-47CB-9557-A231C6D815EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE595669-34EE-405A-80C2-057311C2AAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="557">
   <si>
     <t>cs</t>
   </si>
@@ -1626,6 +1626,81 @@
   </si>
   <si>
     <t>Pokročilé</t>
+  </si>
+  <si>
+    <t>lab.mixture.menu</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>lab.mixture.title</t>
+  </si>
+  <si>
+    <t>Mixy</t>
+  </si>
+  <si>
+    <t>lab.mixture.subtitle</t>
+  </si>
+  <si>
+    <t>Každý požitek potřebuje liquid a tato sekce slouží pro správu namíchaných liquidů (včetně hotových); tyto mixy se pak dále používají ve vapování pro trasování, jak který mix chutnal.</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.create</t>
+  </si>
+  <si>
+    <t>Nový mix</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.list</t>
+  </si>
+  <si>
+    <t>Seznam mixů</t>
+  </si>
+  <si>
+    <t>lab.mixture.create.title</t>
+  </si>
+  <si>
+    <t>lab.mixture.create.subtitle</t>
+  </si>
+  <si>
+    <t>Mix vám pomůže sledovat složení liquidu, množství nikotinu a jeho stáří (tzn. zrání).</t>
+  </si>
+  <si>
+    <t>lab.mixture.list.title</t>
+  </si>
+  <si>
+    <t>lab.vape.title</t>
+  </si>
+  <si>
+    <t>lab.vape.subtitle</t>
+  </si>
+  <si>
+    <t>Toto je nejzajímavější část aplikace, kde si můžete trasovat zážitky z vapování, které vám tak umožní zjistit, jaké spirálky, nastavení vzduchu, liquidy (a jejich stáří) vám vyhovují nejvíce.</t>
+  </si>
+  <si>
+    <t>lab.vape.button.create</t>
+  </si>
+  <si>
+    <t>Nový vape</t>
+  </si>
+  <si>
+    <t>lab.vape.button.list</t>
+  </si>
+  <si>
+    <t>Seznam vapů</t>
+  </si>
+  <si>
+    <t>lab.vape.create.title</t>
+  </si>
+  <si>
+    <t>lab.vape.create.subtitle</t>
+  </si>
+  <si>
+    <t>Vape je základní stavební kámen pro záznam chutě a požitku z vapování.</t>
+  </si>
+  <si>
+    <t>lab.vape.list.title</t>
   </si>
 </sst>
 </file>
@@ -1989,10 +2064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C300"/>
+  <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B297" sqref="B297"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B310" sqref="B310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,6 +5375,171 @@
       </c>
       <c r="C300" s="1" t="s">
         <v>531</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed translation loading stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE595669-34EE-405A-80C2-057311C2AAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ADB086-CA42-4B4D-A61B-9D62748E9780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2066,8 +2066,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B310" sqref="B310"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B279" sqref="B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Huge amount of quite not interesting things
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ADB086-CA42-4B4D-A61B-9D62748E9780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EF4AD7-93E1-4EDE-B6EC-0E958B3C0435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="589">
   <si>
     <t>cs</t>
   </si>
@@ -1701,6 +1701,102 @@
   </si>
   <si>
     <t>lab.vape.list.title</t>
+  </si>
+  <si>
+    <t>lab.mixture.name.label</t>
+  </si>
+  <si>
+    <t>Název mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.code.label</t>
+  </si>
+  <si>
+    <t>Kód</t>
+  </si>
+  <si>
+    <t>lab.mixture.code.label.tooltip</t>
+  </si>
+  <si>
+    <t>Myšlenka kódu je možnost si ho fyzicky napsat na lahvičku; měl by být snadno zapamatovatelný a zároveň unikátní.</t>
+  </si>
+  <si>
+    <t>lab.mixture.steep.label</t>
+  </si>
+  <si>
+    <t>Doba zrání</t>
+  </si>
+  <si>
+    <t>lab.mixture.steep.label.tooltip</t>
+  </si>
+  <si>
+    <t>lab.mixture.pg.label</t>
+  </si>
+  <si>
+    <t>Poměr PG</t>
+  </si>
+  <si>
+    <t>lab.mixture.vg.label</t>
+  </si>
+  <si>
+    <t>Poměr VG</t>
+  </si>
+  <si>
+    <t>lab.mixture.nicotine.label</t>
+  </si>
+  <si>
+    <t>Obsah nikotinu</t>
+  </si>
+  <si>
+    <t>lab.mixture.volume.label</t>
+  </si>
+  <si>
+    <t>Celkový objem</t>
+  </si>
+  <si>
+    <t>lab.mixture.mixed.label</t>
+  </si>
+  <si>
+    <t>Datum mixování</t>
+  </si>
+  <si>
+    <t>lab.mixture.expires.label</t>
+  </si>
+  <si>
+    <t>Expirace</t>
+  </si>
+  <si>
+    <t>lab.mixture.expires.label.tooltip</t>
+  </si>
+  <si>
+    <t>Datum expirace je napsaný na lahvičce; pokud jej vyplníte, aplikace vám pohlídá liquidy, které by už nemuselo být vhodné použít.</t>
+  </si>
+  <si>
+    <t>lab.mixture.liquidId.label</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>lab.mixture.baseId.label</t>
+  </si>
+  <si>
+    <t>Báze</t>
+  </si>
+  <si>
+    <t>lab.mixture.boosterId.label</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>Doporučená doba zrání (v dnech); neplatí pro již hotové liquidy.</t>
+  </si>
+  <si>
+    <t>lab.mixture.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit mix</t>
   </si>
 </sst>
 </file>
@@ -2064,10 +2160,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C315"/>
+  <dimension ref="A1:C331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B279" sqref="B279"/>
+    <sheetView tabSelected="1" topLeftCell="A316" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B326" sqref="B326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,6 +5636,182 @@
       </c>
       <c r="C315" s="1" t="s">
         <v>552</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial mixture stuff works
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EF4AD7-93E1-4EDE-B6EC-0E958B3C0435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26AB7A1-D176-4582-B053-2669A2062A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="591">
   <si>
     <t>cs</t>
   </si>
@@ -1797,6 +1797,12 @@
   </si>
   <si>
     <t>Vytvořit mix</t>
+  </si>
+  <si>
+    <t>lab.mixture.created.message</t>
+  </si>
+  <si>
+    <t>Mix byl úspěšně uložen.</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2166,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C331"/>
+  <dimension ref="A1:C332"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B326" sqref="B326"/>
@@ -5812,6 +5818,17 @@
       </c>
       <c r="C331" s="1" t="s">
         <v>588</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added liquid stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26AB7A1-D176-4582-B053-2669A2062A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ED3297-8C93-4BE2-8E3C-38895C1D010D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="609">
   <si>
     <t>cs</t>
   </si>
@@ -1803,6 +1803,60 @@
   </si>
   <si>
     <t>Mix byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.liquid.tooltip.create</t>
+  </si>
+  <si>
+    <t>Nový liquid</t>
+  </si>
+  <si>
+    <t>Vytvořit liquid</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.subtitle</t>
+  </si>
+  <si>
+    <t>Liquidy je možné použít pro míchání mixů k vapování.</t>
+  </si>
+  <si>
+    <t>lab.liquid.name.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.description.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.pg.label</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>lab.liquid.vg.label</t>
+  </si>
+  <si>
+    <t>VG</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.submit</t>
+  </si>
+  <si>
+    <t>lab.liquid.volume.label</t>
+  </si>
+  <si>
+    <t>Objem</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.success</t>
+  </si>
+  <si>
+    <t>Liquid [{{data.name}}] byl uložen.</t>
   </si>
 </sst>
 </file>
@@ -2166,10 +2220,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C332"/>
+  <dimension ref="A1:C344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B326" sqref="B326"/>
+    <sheetView tabSelected="1" topLeftCell="A328" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B342" sqref="B342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5829,6 +5883,138 @@
       </c>
       <c r="C332" s="1" t="s">
         <v>590</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added more cool stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ED3297-8C93-4BE2-8E3C-38895C1D010D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A0EDD-5E20-4B83-955E-98790BDCDF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="623">
   <si>
     <t>cs</t>
   </si>
@@ -1857,6 +1857,48 @@
   </si>
   <si>
     <t>Liquid [{{data.name}}] byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.base.tooltip.create</t>
+  </si>
+  <si>
+    <t>Nová báze</t>
+  </si>
+  <si>
+    <t>lab.base.create.title</t>
+  </si>
+  <si>
+    <t>lab.base.create.subtitle</t>
+  </si>
+  <si>
+    <t>Báze je užitečná v mixech.</t>
+  </si>
+  <si>
+    <t>lab.base.name.label</t>
+  </si>
+  <si>
+    <t>Název báze</t>
+  </si>
+  <si>
+    <t>lab.base.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.base.pg.label</t>
+  </si>
+  <si>
+    <t>lab.base.vg.label</t>
+  </si>
+  <si>
+    <t>lab.base.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit bázi</t>
+  </si>
+  <si>
+    <t>lab.base.create.success</t>
+  </si>
+  <si>
+    <t>Báze [{{data.name}}] byla uložena.</t>
   </si>
 </sst>
 </file>
@@ -2220,10 +2262,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C344"/>
+  <dimension ref="A1:C354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B342" sqref="B342"/>
+    <sheetView tabSelected="1" topLeftCell="A337" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B353" sqref="B353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6015,6 +6057,116 @@
       </c>
       <c r="C344" s="1" t="s">
         <v>608</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Finally! Booster are online!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45A0EDD-5E20-4B83-955E-98790BDCDF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09023BA-837C-428D-9396-7AD84E531B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="638">
   <si>
     <t>cs</t>
   </si>
@@ -1899,6 +1899,51 @@
   </si>
   <si>
     <t>Báze [{{data.name}}] byla uložena.</t>
+  </si>
+  <si>
+    <t>lab.booster.tooltip.create</t>
+  </si>
+  <si>
+    <t>Vytvořit booster</t>
+  </si>
+  <si>
+    <t>lab.booster.create.title</t>
+  </si>
+  <si>
+    <t>Nový booster</t>
+  </si>
+  <si>
+    <t>lab.booster.create.subtitle</t>
+  </si>
+  <si>
+    <t>Boostery jsou užitečné pro tvorbu mixů.</t>
+  </si>
+  <si>
+    <t>lab.booster.name.label</t>
+  </si>
+  <si>
+    <t>lab.booster.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.booster.nicotine.label</t>
+  </si>
+  <si>
+    <t>lab.booster.volume.label</t>
+  </si>
+  <si>
+    <t>lab.booster.create.submit</t>
+  </si>
+  <si>
+    <t>lab.booster.create.success</t>
+  </si>
+  <si>
+    <t>Booster [{{data.name}}] vytvořen.</t>
+  </si>
+  <si>
+    <t>lab.booster.pg.label</t>
+  </si>
+  <si>
+    <t>lab.booster.vg.label</t>
   </si>
 </sst>
 </file>
@@ -2262,10 +2307,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C354"/>
+  <dimension ref="A1:C365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B353" sqref="B353"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B360" sqref="B360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6167,6 +6212,127 @@
       </c>
       <c r="C354" s="1" t="s">
         <v>622</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared a lot of interesting stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09023BA-837C-428D-9396-7AD84E531B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097A45B1-D6CD-4506-B1EA-77233B7BBCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="653">
   <si>
     <t>cs</t>
   </si>
@@ -1850,6 +1850,9 @@
     <t>lab.liquid.volume.label</t>
   </si>
   <si>
+    <t>Obsah</t>
+  </si>
+  <si>
     <t>Objem</t>
   </si>
   <si>
@@ -1944,6 +1947,48 @@
   </si>
   <si>
     <t>lab.booster.vg.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.name</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.code</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.steep</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.pgvg</t>
+  </si>
+  <si>
+    <t>PG/VG</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.nicotine</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.mixed</t>
+  </si>
+  <si>
+    <t>Datum mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.volume</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.liquid</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.booster</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.base</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.expires</t>
+  </si>
+  <si>
+    <t>Datum expirace</t>
   </si>
 </sst>
 </file>
@@ -2307,10 +2352,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C365"/>
+  <dimension ref="A1:C376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B360" sqref="B360"/>
+    <sheetView tabSelected="1" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B372" sqref="B372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6090,7 +6135,7 @@
         <v>605</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -6098,10 +6143,10 @@
         <v>0</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -6109,10 +6154,10 @@
         <v>0</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -6120,10 +6165,10 @@
         <v>0</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -6131,10 +6176,10 @@
         <v>0</v>
       </c>
       <c r="B347" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C347" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="C347" s="1" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -6142,10 +6187,10 @@
         <v>0</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -6153,10 +6198,10 @@
         <v>0</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -6164,7 +6209,7 @@
         <v>0</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>393</v>
@@ -6175,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>601</v>
@@ -6186,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>603</v>
@@ -6197,10 +6242,10 @@
         <v>0</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -6208,10 +6253,10 @@
         <v>0</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -6219,10 +6264,10 @@
         <v>0</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -6230,10 +6275,10 @@
         <v>0</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -6241,10 +6286,10 @@
         <v>0</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -6252,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>298</v>
@@ -6263,7 +6308,7 @@
         <v>0</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>393</v>
@@ -6274,7 +6319,7 @@
         <v>0</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>571</v>
@@ -6285,10 +6330,10 @@
         <v>0</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -6296,10 +6341,10 @@
         <v>0</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -6307,10 +6352,10 @@
         <v>0</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -6318,7 +6363,7 @@
         <v>0</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>601</v>
@@ -6329,10 +6374,131 @@
         <v>0</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>603</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A375" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A376" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Adding new setup and list of setups, yaay!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097A45B1-D6CD-4506-B1EA-77233B7BBCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD157329-74D2-44B6-8147-40E5608F6F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="711">
   <si>
     <t>cs</t>
   </si>
@@ -1989,6 +1989,180 @@
   </si>
   <si>
     <t>Datum expirace</t>
+  </si>
+  <si>
+    <t>lab.setup.menu</t>
+  </si>
+  <si>
+    <t>Setupy</t>
+  </si>
+  <si>
+    <t>lab.setup.title</t>
+  </si>
+  <si>
+    <t>lab.setup.subtitle</t>
+  </si>
+  <si>
+    <t>Setup je složení fyzických zařízení použitých pro vapování.</t>
+  </si>
+  <si>
+    <t>lab.setup.button.create</t>
+  </si>
+  <si>
+    <t>Nový setup</t>
+  </si>
+  <si>
+    <t>lab.setup.button.list</t>
+  </si>
+  <si>
+    <t>Seznam setupů</t>
+  </si>
+  <si>
+    <t>lab.setup.create.title</t>
+  </si>
+  <si>
+    <t>lab.setup.create.subtitle</t>
+  </si>
+  <si>
+    <t>Setup je poslední součást, která je potřebná pro sledování požitků z vapingu.</t>
+  </si>
+  <si>
+    <t>lab.setup.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit setup</t>
+  </si>
+  <si>
+    <t>lab.setup.name.label</t>
+  </si>
+  <si>
+    <t>Název setupu</t>
+  </si>
+  <si>
+    <t>lab.setup.description.label</t>
+  </si>
+  <si>
+    <t>lab.setup.driptipId.label</t>
+  </si>
+  <si>
+    <t>Náústek</t>
+  </si>
+  <si>
+    <t>lab.setup.buildId.label</t>
+  </si>
+  <si>
+    <t>lab.setup.modId.label</t>
+  </si>
+  <si>
+    <t>Mod</t>
+  </si>
+  <si>
+    <t>lab.driptip.tooltip.create</t>
+  </si>
+  <si>
+    <t>Vytvořit náústek</t>
+  </si>
+  <si>
+    <t>lab.driptip.create.title</t>
+  </si>
+  <si>
+    <t>Nový náústek</t>
+  </si>
+  <si>
+    <t>lab.driptip.create.subtitle</t>
+  </si>
+  <si>
+    <t>Nezdá se to, ale náústky jsou také důležité.</t>
+  </si>
+  <si>
+    <t>lab.driptip.code.label</t>
+  </si>
+  <si>
+    <t>lab.driptip.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.driptip.create.submit</t>
+  </si>
+  <si>
+    <t>lab.driptip.created.message</t>
+  </si>
+  <si>
+    <t>Náústek [{{data.code}}] byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.build.tooltip.create</t>
+  </si>
+  <si>
+    <t>Vytvořit build</t>
+  </si>
+  <si>
+    <t>lab.mod.tooltip.create</t>
+  </si>
+  <si>
+    <t>Vytvořit mod</t>
+  </si>
+  <si>
+    <t>lab.mod.create.title</t>
+  </si>
+  <si>
+    <t>Nový mod</t>
+  </si>
+  <si>
+    <t>lab.mod.create.subtitle</t>
+  </si>
+  <si>
+    <t>Mod obecně zastupuje zařízení, ze kterého lze vapovat.</t>
+  </si>
+  <si>
+    <t>lab.mod.name.label</t>
+  </si>
+  <si>
+    <t>Název modu</t>
+  </si>
+  <si>
+    <t>lab.mod.power.label</t>
+  </si>
+  <si>
+    <t>Výkon (watty)</t>
+  </si>
+  <si>
+    <t>lab.mod.vendorId.label</t>
+  </si>
+  <si>
+    <t>error.Duplicate entry [z_setup_name_unique] of [z_setup].</t>
+  </si>
+  <si>
+    <t>Jméno tohoto setupu je již obsazené, použijte prosím jiné.</t>
+  </si>
+  <si>
+    <t>lab.setup.created.message</t>
+  </si>
+  <si>
+    <t>Setup [{{data.name}}] byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.setup.list.title</t>
+  </si>
+  <si>
+    <t>lab.setup.table.name</t>
+  </si>
+  <si>
+    <t>lab.setup.table.driptip</t>
+  </si>
+  <si>
+    <t>lab.setup.table.build</t>
+  </si>
+  <si>
+    <t>lab.setup.table.mod</t>
+  </si>
+  <si>
+    <t>lab.build.inline.atomizer.tooltip</t>
+  </si>
+  <si>
+    <t>lab.build.inline.wraps.tooltip</t>
+  </si>
+  <si>
+    <t>Počet otoček na spirálce</t>
   </si>
 </sst>
 </file>
@@ -2352,10 +2526,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C376"/>
+  <dimension ref="A1:C412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B372" sqref="B372"/>
+    <sheetView tabSelected="1" topLeftCell="A373" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B401" sqref="B401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6499,6 +6673,402 @@
       </c>
       <c r="C376" s="1" t="s">
         <v>652</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A409" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A411" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A412" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Renamed driptip code to name
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC93FC-5B07-4C4B-9361-2DD909EB710D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D893E4F-80AA-4ADC-A585-7B40015D5CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="715">
   <si>
     <t>cs</t>
   </si>
@@ -2169,6 +2169,12 @@
   </si>
   <si>
     <t>Build [{{data.name}}] byl vytvořen.</t>
+  </si>
+  <si>
+    <t>lab.driptip.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Jméno použijte libovolné pro popis náústku.</t>
   </si>
 </sst>
 </file>
@@ -2532,10 +2538,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C413"/>
+  <dimension ref="A1:C414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B400" sqref="B400"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B412" sqref="B412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7086,6 +7092,17 @@
       </c>
       <c r="C413" s="1" t="s">
         <v>712</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A414" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared vape form
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61E253A-F468-4AD6-B668-F54684D12F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C56BA-2BB4-4381-9485-F6C4A984C5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="802">
   <si>
     <t>cs</t>
   </si>
@@ -2175,6 +2175,267 @@
   </si>
   <si>
     <t>public.home.welcome.subtitle</t>
+  </si>
+  <si>
+    <t>lab.vape.setupId.label</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>lab.vape.create.submit</t>
+  </si>
+  <si>
+    <t>Vytvořit vape</t>
+  </si>
+  <si>
+    <t>lab.setup.tooltip.create</t>
+  </si>
+  <si>
+    <t>lab.vape.mixtureId.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.tooltip.create</t>
+  </si>
+  <si>
+    <t>lab.mixture.create.success</t>
+  </si>
+  <si>
+    <t>Mix [{{data.name}}] byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.setup.create.success</t>
+  </si>
+  <si>
+    <t>Setup [{{data.name}}] byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.vape.driptipId.label</t>
+  </si>
+  <si>
+    <t>lab.driptip.name.label</t>
+  </si>
+  <si>
+    <t>lab.driptip.create.success</t>
+  </si>
+  <si>
+    <t>Náústek [{{data.name}}] byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.vape.common.title</t>
+  </si>
+  <si>
+    <t>lab.vape.rating.title</t>
+  </si>
+  <si>
+    <t>Celkové hodnocení</t>
+  </si>
+  <si>
+    <t>lab.vape.rating.label</t>
+  </si>
+  <si>
+    <t>lab.vape.rating.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato hodnota by měla reprezentovat celkový pocit z vapingu, včetně setupu, bublání atomizéru, chuti, prostě všeho.</t>
+  </si>
+  <si>
+    <t>lab.vape.taste.label</t>
+  </si>
+  <si>
+    <t>Chuťový projev</t>
+  </si>
+  <si>
+    <t>lab.vape.taste.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato hodnota sleduje pouze dojem z chuťového projevu buildu. Hlavní tedy je, jak moc je projev blízko očekávání.</t>
+  </si>
+  <si>
+    <t>lab.vape.rating-advanced.title</t>
+  </si>
+  <si>
+    <t>Rozborka chuťového projevu</t>
+  </si>
+  <si>
+    <t>lab.vape.fruits.label</t>
+  </si>
+  <si>
+    <t>Ovocné tóny</t>
+  </si>
+  <si>
+    <t>lab.vape.fruits.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato položka sleduje, jak dobře vybraný build podává ovocné složky; např. v daném nastavení se mohou lépe projevovat citronové tóny, ale chuť buchty může být v pozadí.</t>
+  </si>
+  <si>
+    <t>lab.vape.tobacco.label</t>
+  </si>
+  <si>
+    <t>Tabák</t>
+  </si>
+  <si>
+    <t>lab.vape.tobacco.label.tooltip</t>
+  </si>
+  <si>
+    <t>Hodnocení tabákového projevu daného liquidu.</t>
+  </si>
+  <si>
+    <t>lab.vape.cakes.label</t>
+  </si>
+  <si>
+    <t>Buchty</t>
+  </si>
+  <si>
+    <t>lab.vape.cakes.label.tooltip</t>
+  </si>
+  <si>
+    <t>Hodnocení kvality podání chuti buchet.</t>
+  </si>
+  <si>
+    <t>lab.vape.complex.label</t>
+  </si>
+  <si>
+    <t>Komplexní</t>
+  </si>
+  <si>
+    <t>lab.vape.complex.label.tooltip</t>
+  </si>
+  <si>
+    <t>Toto hodnocení celkově sleduje komplexitu podání chuti u liquidů, kde není dominantní položka (např. pouze jablko); lze tak také určit, jak dobře daný build podává komplikovanější příchutě (např. tabák s tóny bourbonu).</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.label</t>
+  </si>
+  <si>
+    <t>Větrnost</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.label.tooltip</t>
+  </si>
+  <si>
+    <t>Liquidy, které obsahují mátu nebo jsou jinak větravé, nejsou vždy příjemné; toto hodnocení je reverzní - vyšší číslo udává větší míru "ice" efektu, kdy nejvyšší reprezentuje již nepříjemný zážitek.</t>
+  </si>
+  <si>
+    <t>lab.vape.vape.title</t>
+  </si>
+  <si>
+    <t>Hodnocení vapingu</t>
+  </si>
+  <si>
+    <t>lab.vape.settings.title</t>
+  </si>
+  <si>
+    <t>lab.vape.power.label</t>
+  </si>
+  <si>
+    <t>Použitý výkon</t>
+  </si>
+  <si>
+    <t>lab.vape.power.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zde si zaznamenejte výkon, který máte nastavený pro daný setup v průměrném použití; je možné takto zaznamenat i příliš vysoké hodnoty nebo naopak velmi nízké. Pokud vyjde hodnocení vapu dobře, aplikace bude schopna určit optimální výkon pro ten či onen build.</t>
+  </si>
+  <si>
+    <t>lab.vape.tc.label</t>
+  </si>
+  <si>
+    <t>lab.vape.tc.label.tooltip</t>
+  </si>
+  <si>
+    <t>Teplota</t>
+  </si>
+  <si>
+    <t>Pokud máte spirálku, která podporuje režim teploty, je možné si zde zaznamenat vliv teploty na chuť a vůbec zážitek z vapování, včetně těch nepříjemných.</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.label</t>
+  </si>
+  <si>
+    <t>Airflow</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.label.tooltip</t>
+  </si>
+  <si>
+    <t>Jedná se o nastavení airflow na atomizéru (pokud jej umí); nula je úplně zavřeno nebo velmi tuhé MTL, pětka je plně otevřeno na velmi volné DL.</t>
+  </si>
+  <si>
+    <t>lab.vape.juice.label</t>
+  </si>
+  <si>
+    <t>Juice flow</t>
+  </si>
+  <si>
+    <t>lab.vape.juice.label.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud atomizér podporuje juice flow, je možné si zde poznamenat optimální nastavení, aby nedocházelo k únikům. Nula je takřka zavřeno, pět je plně otevřeno.</t>
+  </si>
+  <si>
+    <t>DL/MTL</t>
+  </si>
+  <si>
+    <t>lab.vape.mtl.label</t>
+  </si>
+  <si>
+    <t>Hodnocení MTL</t>
+  </si>
+  <si>
+    <t>lab.vape.mtl.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zde se jedná o kombinaci hodnocení chuťového projevu v MTL; čím vyšší hodnocení, tím lépe build funguje v MTL.</t>
+  </si>
+  <si>
+    <t>lab.vape.dl.label</t>
+  </si>
+  <si>
+    <t>Hodnocení DL</t>
+  </si>
+  <si>
+    <t>lab.vape.dl.label.tooltip</t>
+  </si>
+  <si>
+    <t>Hodnocení buildu pro DL; čím vyšší hodnocení, tím lépe build funguje v DL.</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.label</t>
+  </si>
+  <si>
+    <t>Oblaka</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.label.tooltip</t>
+  </si>
+  <si>
+    <t>Prosté hodnocení generovaných oblak; nízké hodnocení je komorní MTL mezi lidi, maximální hodnocení je prasostroj někde venku. Nebo mezi vapery.</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.label</t>
+  </si>
+  <si>
+    <t>Úniky</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.label.tooltip</t>
+  </si>
+  <si>
+    <t>Touto hodnotou je míněno, jakou tendenci má liquid unikat; toto je obecně nežádoucí - čím vyšší číslo, tím více má tank tendenci protékat. Nula naopak znamená žádné protečení.</t>
+  </si>
+  <si>
+    <t>lab.vape.dryhit.label</t>
+  </si>
+  <si>
+    <t>Dryhit</t>
+  </si>
+  <si>
+    <t>lab.vape.dryhit.label.tooltip</t>
+  </si>
+  <si>
+    <t>Touto hodnotou je míněno, jak moc je možné atomizér trápit, než se dostaví dryhit; vyšší hodnota obecně znamená stabilnější dodávání liquidu a bezproblémové bafání za sebou, nižší naopak vyžaduje střídmější a hodnoty k nule znamenají, že je něco špatně.</t>
   </si>
 </sst>
 </file>
@@ -2538,10 +2799,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C414"/>
+  <dimension ref="A1:C462"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B460" sqref="B460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7103,6 +7364,534 @@
       </c>
       <c r="C414" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A415" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A420" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A421" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A422" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A423" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A424" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A425" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A426" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A427" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A429" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A430" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A431" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A432" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A433" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A435" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A437" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A438" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A439" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A441" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A442" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A445" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A447" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A448" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A449" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A450" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A451" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A452" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A453" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A457" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A458" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A459" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A460" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A461" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A462" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: It's possible to save a vape, yaay!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543C56BA-2BB4-4381-9485-F6C4A984C5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C7118-5B78-403C-A11C-958AEE80BED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="804">
   <si>
     <t>cs</t>
   </si>
@@ -2436,6 +2436,12 @@
   </si>
   <si>
     <t>Touto hodnotou je míněno, jak moc je možné atomizér trápit, než se dostaví dryhit; vyšší hodnota obecně znamená stabilnější dodávání liquidu a bezproblémové bafání za sebou, nižší naopak vyžaduje střídmější a hodnoty k nule znamenají, že je něco špatně.</t>
+  </si>
+  <si>
+    <t>lab.vape.created.message</t>
+  </si>
+  <si>
+    <t>Vape byl uložen.</t>
   </si>
 </sst>
 </file>
@@ -2799,7 +2805,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C462"/>
+  <dimension ref="A1:C463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B460" sqref="B460"/>
@@ -7892,6 +7898,17 @@
       </c>
       <c r="C462" s="1" t="s">
         <v>801</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A463" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Somehow polished some pieces of UI
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181C7118-5B78-403C-A11C-958AEE80BED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B37AF-4DE5-4095-ADCE-2491B784F81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="839">
   <si>
     <t>cs</t>
   </si>
@@ -2442,6 +2442,111 @@
   </si>
   <si>
     <t>Vape byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.vape.table.setup</t>
+  </si>
+  <si>
+    <t>lab.vape.table.mixture</t>
+  </si>
+  <si>
+    <t>lab.vape.table.rating</t>
+  </si>
+  <si>
+    <t>Hodnocení</t>
+  </si>
+  <si>
+    <t>lab.vape.table.taste</t>
+  </si>
+  <si>
+    <t>Chuť</t>
+  </si>
+  <si>
+    <t>lab.vape.table.power</t>
+  </si>
+  <si>
+    <t>Výkon</t>
+  </si>
+  <si>
+    <t>lab.vape.table.tc</t>
+  </si>
+  <si>
+    <t>Hodnocení chuti</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.setup</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.mixture</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.driptip</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.leaks</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.dryhit</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.rating</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.taste</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.power</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.tc</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.airflow</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.juice</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.mtl</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.dl</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.clouds</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.fruits</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.tobacco</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.cakes</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.complex</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.fresh</t>
+  </si>
+  <si>
+    <t>Dryhity</t>
+  </si>
+  <si>
+    <t>MTL</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.atomizer</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.coil</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.mod</t>
   </si>
 </sst>
 </file>
@@ -2805,10 +2910,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C463"/>
+  <dimension ref="A1:C491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B460" sqref="B460"/>
+    <sheetView tabSelected="1" topLeftCell="A478" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B485" sqref="B485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7909,6 +8014,314 @@
       </c>
       <c r="C463" s="1" t="s">
         <v>803</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A464" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A467" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A468" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A469" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C469" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A470" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C470" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A471" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A472" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A473" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C473" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A474" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A475" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A476" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A477" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C477" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A478" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C478" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A479" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C479" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A480" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B480" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A481" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A483" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C483" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A484" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C484" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C485" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A486" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C486" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A487" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C487" s="1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C488" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A489" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C489" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A490" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C490" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C491" s="1" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Dropped unique key on name on mixture
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA25BA7F-E744-4EBC-824C-41DC952461CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56267609-465F-41B5-83E4-468F0A5697A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="846">
   <si>
     <t>cs</t>
   </si>
@@ -2562,6 +2562,12 @@
   </si>
   <si>
     <t>Touto hodnotou je míněno, jak moc je možné atomizér trápit, než se dostaví dryhit; nižší hodnota obecně znamená stabilnější dodávání liquidu a bezproblémové bafání za sebou, vyšší naopak vyžaduje střídmější a nejvyšší hodnoty znamenají, že je něco špatně.</t>
+  </si>
+  <si>
+    <t>error.Duplicate entry [z_mixture_code_unique] of [z_mixture].</t>
+  </si>
+  <si>
+    <t>Kód mixu je již použitý; vyberte prosím jiný.</t>
   </si>
 </sst>
 </file>
@@ -2925,10 +2931,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C495"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A483" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B491" sqref="B491"/>
+      <selection activeCell="B490" sqref="B490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8370,6 +8376,17 @@
       </c>
       <c r="C494" s="1" t="s">
         <v>816</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A495" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C495" s="1" t="s">
+        <v>845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added some initial mix detail
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56267609-465F-41B5-83E4-468F0A5697A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B92949-A402-4B30-9BA8-84E5FB9A9EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="857">
   <si>
     <t>cs</t>
   </si>
@@ -2568,6 +2568,39 @@
   </si>
   <si>
     <t>Kód mixu je již použitý; vyberte prosím jiný.</t>
+  </si>
+  <si>
+    <t>lab.mixture.index.title</t>
+  </si>
+  <si>
+    <t>Detail mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.index.preview.title</t>
+  </si>
+  <si>
+    <t>Náhled mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Zde můžete spravovat vybraný mix.</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.name</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.liquid</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.nicotine</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.base</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.booster</t>
   </si>
 </sst>
 </file>
@@ -2931,10 +2964,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C495"/>
+  <dimension ref="A1:C503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A483" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B490" sqref="B490"/>
+    <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B498" sqref="B498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8387,6 +8420,94 @@
       </c>
       <c r="C495" s="1" t="s">
         <v>845</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C496" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C497" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A498" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A499" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C500" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A501" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A502" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A503" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improving UI and UX
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B92949-A402-4B30-9BA8-84E5FB9A9EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28142904-4D48-4643-AE8C-8F6C5EA95E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="864">
   <si>
     <t>cs</t>
   </si>
@@ -2601,6 +2601,27 @@
   </si>
   <si>
     <t>lab.mixture.preview.booster</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit</t>
+  </si>
+  <si>
+    <t>lab.mixture.edit.title</t>
+  </si>
+  <si>
+    <t>Editace mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud je třeba mix upravit, zde je to správné místo.</t>
+  </si>
+  <si>
+    <t>lab.mixture.link.button</t>
   </si>
 </sst>
 </file>
@@ -2964,10 +2985,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C503"/>
+  <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B498" sqref="B498"/>
+      <selection activeCell="B497" sqref="B497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8508,6 +8529,50 @@
       </c>
       <c r="C503" s="1" t="s">
         <v>585</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A505" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C506" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A507" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="C507" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Mixture patch works
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28142904-4D48-4643-AE8C-8F6C5EA95E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F74A4-2AF4-4403-B3B1-8AA1A143194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="866">
   <si>
     <t>cs</t>
   </si>
@@ -2622,6 +2622,12 @@
   </si>
   <si>
     <t>lab.mixture.link.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.update.submit</t>
+  </si>
+  <si>
+    <t>lab.mixture.update.success</t>
   </si>
 </sst>
 </file>
@@ -2985,10 +2991,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C507"/>
+  <dimension ref="A1:C509"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B497" sqref="B497"/>
+      <selection activeCell="B502" sqref="B502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8573,6 +8579,28 @@
       </c>
       <c r="C507" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A508" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C508" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C509" s="1" t="s">
+        <v>724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Build edit works
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77F74A4-2AF4-4403-B3B1-8AA1A143194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8794D9C-339E-45ED-A745-2DB21184431B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="880">
   <si>
     <t>cs</t>
   </si>
@@ -2628,6 +2628,48 @@
   </si>
   <si>
     <t>lab.mixture.update.success</t>
+  </si>
+  <si>
+    <t>lab.build.index.title</t>
+  </si>
+  <si>
+    <t>lab.build.index.preview.title</t>
+  </si>
+  <si>
+    <t>lab.build.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Zde můžete spravovat vybraný build.</t>
+  </si>
+  <si>
+    <t>lab.build.button.edit</t>
+  </si>
+  <si>
+    <t>lab.build.preview.name</t>
+  </si>
+  <si>
+    <t>lab.build.edit.title</t>
+  </si>
+  <si>
+    <t>Editace buildu</t>
+  </si>
+  <si>
+    <t>lab.build.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Místo, kde je možné upravit build.</t>
+  </si>
+  <si>
+    <t>lab.build.update.submit</t>
+  </si>
+  <si>
+    <t>lab.build.update.success</t>
+  </si>
+  <si>
+    <t>Build [{{data.name}}] byl aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.build.link.button</t>
   </si>
 </sst>
 </file>
@@ -2991,10 +3033,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C509"/>
+  <dimension ref="A1:C519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B502" sqref="B502"/>
+    <sheetView tabSelected="1" topLeftCell="A498" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B514" sqref="B514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8601,6 +8643,116 @@
       </c>
       <c r="C509" s="1" t="s">
         <v>724</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A512" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A513" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A514" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A515" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A516" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A517" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A518" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A519" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added vape edit
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8794D9C-339E-45ED-A745-2DB21184431B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC51538-65C4-4447-AF59-8F58A0657FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="894">
   <si>
     <t>cs</t>
   </si>
@@ -2670,6 +2670,48 @@
   </si>
   <si>
     <t>lab.build.link.button</t>
+  </si>
+  <si>
+    <t>lab.vape.edit.title</t>
+  </si>
+  <si>
+    <t>Editace vapu</t>
+  </si>
+  <si>
+    <t>lab.vape.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Každý se někdy překlepne, zde je možné upravit vape.</t>
+  </si>
+  <si>
+    <t>lab.vape.link.button</t>
+  </si>
+  <si>
+    <t>lab.vape.update.submit</t>
+  </si>
+  <si>
+    <t>lab.vape.update.success</t>
+  </si>
+  <si>
+    <t>Vape byl aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.vape.index.title</t>
+  </si>
+  <si>
+    <t>lab.vape.button.edit</t>
+  </si>
+  <si>
+    <t>Editovat</t>
+  </si>
+  <si>
+    <t>lab.vape.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Správa vybraného vapu</t>
+  </si>
+  <si>
+    <t>lab.vape.index.preview.title</t>
   </si>
 </sst>
 </file>
@@ -3033,10 +3075,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C519"/>
+  <dimension ref="A1:C528"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A498" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B514" sqref="B514"/>
+    <sheetView tabSelected="1" topLeftCell="A510" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B524" sqref="B524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8753,6 +8795,105 @@
       </c>
       <c r="C519" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A520" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A521" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A522" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A523" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A524" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A525" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="C525" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A526" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C526" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A527" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C527" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A528" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="C528" s="1" t="s">
+        <v>814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added build age in vapes and builds
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC51538-65C4-4447-AF59-8F58A0657FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463454E-F2DE-48BE-9261-F95CD7F31406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="7620" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="897">
   <si>
     <t>cs</t>
   </si>
@@ -2712,6 +2712,15 @@
   </si>
   <si>
     <t>lab.vape.index.preview.title</t>
+  </si>
+  <si>
+    <t>lab.vape.table.age</t>
+  </si>
+  <si>
+    <t>Stáří buildu</t>
+  </si>
+  <si>
+    <t>lab.build.table.age</t>
   </si>
 </sst>
 </file>
@@ -3075,10 +3084,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C528"/>
+  <dimension ref="A1:C530"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A510" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B524" sqref="B524"/>
+      <selection activeCell="B523" sqref="B523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8894,6 +8903,28 @@
       </c>
       <c r="C528" s="1" t="s">
         <v>814</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A529" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="C529" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A530" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved vape table
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463454E-F2DE-48BE-9261-F95CD7F31406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AE931-FC41-464E-A3B4-AE9659AF5794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="899">
   <si>
     <t>cs</t>
   </si>
@@ -2721,6 +2721,12 @@
   </si>
   <si>
     <t>lab.build.table.age</t>
+  </si>
+  <si>
+    <t>lab.vape.preview</t>
+  </si>
+  <si>
+    <t>Náhled</t>
   </si>
 </sst>
 </file>
@@ -3084,10 +3090,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C530"/>
+  <dimension ref="A1:C531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A510" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B523" sqref="B523"/>
+    <sheetView tabSelected="1" topLeftCell="A516" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B527" sqref="B527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8925,6 +8931,17 @@
       </c>
       <c r="C530" s="1" t="s">
         <v>895</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A531" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved mixture table
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8AE931-FC41-464E-A3B4-AE9659AF5794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C663895F-F740-4164-9B38-37FA8258CD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="913">
   <si>
     <t>cs</t>
   </si>
@@ -2727,6 +2727,48 @@
   </si>
   <si>
     <t>Náhled</t>
+  </si>
+  <si>
+    <t>lab.vape.button.all.list</t>
+  </si>
+  <si>
+    <t>Všechny vapy</t>
+  </si>
+  <si>
+    <t>lab.vape.latest.title</t>
+  </si>
+  <si>
+    <t>Nejnovější vapy</t>
+  </si>
+  <si>
+    <t>lab.vape.button.clone</t>
+  </si>
+  <si>
+    <t>Klonovat</t>
+  </si>
+  <si>
+    <t>lab.vape.button.index</t>
+  </si>
+  <si>
+    <t>Detail vapu</t>
+  </si>
+  <si>
+    <t>lab.vape.clone.title</t>
+  </si>
+  <si>
+    <t>Klon vapu</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.age</t>
+  </si>
+  <si>
+    <t>Stáří mixu</t>
+  </si>
+  <si>
+    <t>lab.mixture.steep.done</t>
+  </si>
+  <si>
+    <t>Zrání dokončeno</t>
   </si>
 </sst>
 </file>
@@ -3090,10 +3132,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C531"/>
+  <dimension ref="A1:C539"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A516" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B527" sqref="B527"/>
+      <selection activeCell="B528" sqref="B528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8942,6 +8984,94 @@
       </c>
       <c r="C531" s="1" t="s">
         <v>898</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A533" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A535" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A536" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A537" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A538" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A539" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added an ability to clone builds and vapes
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C663895F-F740-4164-9B38-37FA8258CD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7405FD7C-FA9A-4C22-B3F5-C25B87BE39C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="931">
   <si>
     <t>cs</t>
   </si>
@@ -2769,6 +2769,60 @@
   </si>
   <si>
     <t>Zrání dokončeno</t>
+  </si>
+  <si>
+    <t>lab.build.preview.description</t>
+  </si>
+  <si>
+    <t>lab.build.preview.atomizer</t>
+  </si>
+  <si>
+    <t>lab.build.preview.coil</t>
+  </si>
+  <si>
+    <t>lab.build.preview.cotton</t>
+  </si>
+  <si>
+    <t>lab.build.preview.ohm</t>
+  </si>
+  <si>
+    <t>Odpor</t>
+  </si>
+  <si>
+    <t>lab.build.preview.coilOffset</t>
+  </si>
+  <si>
+    <t>lab.build.preview.cottonOffset</t>
+  </si>
+  <si>
+    <t>lab.build.preview.coils</t>
+  </si>
+  <si>
+    <t>lab.build.button.clone</t>
+  </si>
+  <si>
+    <t>lab.build.button.index</t>
+  </si>
+  <si>
+    <t>lab.build.preview</t>
+  </si>
+  <si>
+    <t>Náhled buildu</t>
+  </si>
+  <si>
+    <t>lab.build.preview.preview.title</t>
+  </si>
+  <si>
+    <t>lab.build.preview.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Zde vidíte veškeré dostupné informace o buildu.</t>
+  </si>
+  <si>
+    <t>lab.build.clone.title</t>
+  </si>
+  <si>
+    <t>Klon buildu</t>
   </si>
 </sst>
 </file>
@@ -3132,10 +3186,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C539"/>
+  <dimension ref="A1:C553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B528" sqref="B528"/>
+    <sheetView tabSelected="1" topLeftCell="A534" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B548" sqref="B548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9072,6 +9126,160 @@
       </c>
       <c r="C539" s="1" t="s">
         <v>912</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A540" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A541" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A542" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A543" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A544" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A545" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A546" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A547" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A548" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A549" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="C549" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A550" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A551" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="C551" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A552" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C552" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A553" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C553" s="1" t="s">
+        <v>930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added an ability to remove a vape
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7405FD7C-FA9A-4C22-B3F5-C25B87BE39C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF65BBE8-7DC6-42EF-B9C3-F4478762901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="941">
   <si>
     <t>cs</t>
   </si>
@@ -2823,6 +2823,36 @@
   </si>
   <si>
     <t>Klon buildu</t>
+  </si>
+  <si>
+    <t>lab.vape.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný vape? Touto akcí ovlivníte statistiky pro buildy, atomizéry a další, které jsou postavené na datech o vapování.</t>
+  </si>
+  <si>
+    <t>lab.vape.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>Odstranit vape</t>
+  </si>
+  <si>
+    <t>common.cancel</t>
+  </si>
+  <si>
+    <t>Zrušit</t>
+  </si>
+  <si>
+    <t>lab.vape.button.delete</t>
+  </si>
+  <si>
+    <t>lab.vape.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.vape.deleted.success</t>
+  </si>
+  <si>
+    <t>Vape byl úspěšně odstraněn.</t>
   </si>
 </sst>
 </file>
@@ -3186,10 +3216,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C553"/>
+  <dimension ref="A1:C559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A534" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B548" sqref="B548"/>
+    <sheetView tabSelected="1" topLeftCell="A540" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B554" sqref="B554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9280,6 +9310,72 @@
       </c>
       <c r="C553" s="1" t="s">
         <v>930</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A554" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C554" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A555" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C555" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A556" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A557" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A558" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A559" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added build creation time into a form
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1AB0B3-06D8-43F4-8AFA-7FAACDFE3701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550376D-DA35-475A-B66E-91FCBC37EF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="944">
   <si>
     <t>cs</t>
   </si>
@@ -2853,6 +2853,15 @@
   </si>
   <si>
     <t>Vape byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.build.created.label</t>
+  </si>
+  <si>
+    <t>Datum vytvoření</t>
+  </si>
+  <si>
+    <t>lab.build.preview.created</t>
   </si>
 </sst>
 </file>
@@ -3216,10 +3225,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C561"/>
+  <dimension ref="A1:C563"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A540" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B553" sqref="B553"/>
+      <selection activeCell="B555" sqref="B555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9398,6 +9407,28 @@
       </c>
       <c r="C561" s="1" t="s">
         <v>847</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A562" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="C562" s="1" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added throathit value
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550376D-DA35-475A-B66E-91FCBC37EF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD54E31-DE47-42DF-9F63-1D579C1BF2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="951">
   <si>
     <t>cs</t>
   </si>
@@ -2862,6 +2862,27 @@
   </si>
   <si>
     <t>lab.build.preview.created</t>
+  </si>
+  <si>
+    <t>job-service.Edde\Phinx\UpgradeJobService</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.throathit</t>
+  </si>
+  <si>
+    <t>Throat hit</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.label</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato hodnota reprezentuje, jak velký kopanec (nikotinu) vape dává; vyšší hodnoty znamenají méně příjemný požitek a nejvyšší už jsou zabijáci.</t>
   </si>
 </sst>
 </file>
@@ -3225,10 +3246,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C563"/>
+  <dimension ref="A1:C567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A540" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B555" sqref="B555"/>
+    <sheetView tabSelected="1" topLeftCell="A546" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9429,6 +9450,50 @@
       </c>
       <c r="C563" s="1" t="s">
         <v>942</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A565" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A567" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Finished mix detail
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD54E31-DE47-42DF-9F63-1D579C1BF2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A323BE26-EBD1-4D6B-A05D-ADF9A47ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="962">
   <si>
     <t>cs</t>
   </si>
@@ -2883,6 +2883,39 @@
   </si>
   <si>
     <t>Tato hodnota reprezentuje, jak velký kopanec (nikotinu) vape dává; vyšší hodnoty znamenají méně příjemný požitek a nejvyšší už jsou zabijáci.</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.pgvg</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.age</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.steep</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.mixed</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.expires</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.volume</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.preview.title</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Přehled všech dostupných dat o vybraném mixu.</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.index</t>
   </si>
 </sst>
 </file>
@@ -3246,10 +3279,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C567"/>
+  <dimension ref="A1:C577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A546" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+    <sheetView tabSelected="1" topLeftCell="A558" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B570" sqref="B570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9494,6 +9527,116 @@
       </c>
       <c r="C567" s="1" t="s">
         <v>950</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A568" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C568" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C569" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A570" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A571" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A573" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A574" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A575" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="C575" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A576" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A577" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved setup stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A323BE26-EBD1-4D6B-A05D-ADF9A47ABF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5683C3A-0BDE-42E5-B6F6-78F970F37305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="7515" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="993">
   <si>
     <t>cs</t>
   </si>
@@ -2916,6 +2916,99 @@
   </si>
   <si>
     <t>lab.mixture.button.index</t>
+  </si>
+  <si>
+    <t>lab.setup.preview</t>
+  </si>
+  <si>
+    <t>Náhled setupu</t>
+  </si>
+  <si>
+    <t>lab.setup.deleted.success</t>
+  </si>
+  <si>
+    <t>Setup byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.setup.button.index</t>
+  </si>
+  <si>
+    <t>Detail setupu</t>
+  </si>
+  <si>
+    <t>lab.setup.button.edit</t>
+  </si>
+  <si>
+    <t>lab.setup.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit setup</t>
+  </si>
+  <si>
+    <t>lab.setup.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.setup.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>lab.setup.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.preview.title</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Zde naleznete veškeré informace o vybraném setupu.</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.name</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.description</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.atomizer</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.mod</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.coil</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.cotton</t>
+  </si>
+  <si>
+    <t>lab.setup.preview.ohm</t>
+  </si>
+  <si>
+    <t>lab.setup.index.title</t>
+  </si>
+  <si>
+    <t>lab.setup.index.preview.title</t>
+  </si>
+  <si>
+    <t>lab.setup.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>lab.setup.edit.title</t>
+  </si>
+  <si>
+    <t>Editace setupu</t>
+  </si>
+  <si>
+    <t>lab.setup.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud je třeba něco poladit…</t>
+  </si>
+  <si>
+    <t>lab.setup.link.button</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný setup? Tímto odstraníte veškerá data s ním spojená, můžete tak změnit i statistiky vapování a další vedlejší efekty. Použijte pouze pokud jste si naprosto jisti, co děláte; tuto akci nelze vzít zpět.</t>
   </si>
 </sst>
 </file>
@@ -3279,10 +3372,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C577"/>
+  <dimension ref="A1:C600"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A558" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B570" sqref="B570"/>
+    <sheetView tabSelected="1" topLeftCell="A579" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C585" sqref="C585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9637,6 +9730,259 @@
       </c>
       <c r="C577" s="1" t="s">
         <v>847</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A578" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A579" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A580" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A581" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A582" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A583" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A584" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A585" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A586" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A587" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A588" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A589" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A590" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A591" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A592" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A593" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A594" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A595" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A596" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A597" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A598" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A599" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A600" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: It's possible to activate/deactivate build
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5683C3A-0BDE-42E5-B6F6-78F970F37305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D7239A-C457-425C-8CC3-2440E5393B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1006">
   <si>
     <t>cs</t>
   </si>
@@ -3009,6 +3009,45 @@
   </si>
   <si>
     <t>Opravdu si přejete odstranit vybraný setup? Tímto odstraníte veškerá data s ním spojená, můžete tak změnit i statistiky vapování a další vedlejší efekty. Použijte pouze pokud jste si naprosto jisti, co děláte; tuto akci nelze vzít zpět.</t>
+  </si>
+  <si>
+    <t>root.common.utils.title</t>
+  </si>
+  <si>
+    <t>root.cache.drop.label</t>
+  </si>
+  <si>
+    <t>Smazat cache</t>
+  </si>
+  <si>
+    <t>root.cache.drop.success</t>
+  </si>
+  <si>
+    <t>Cache byla smazána</t>
+  </si>
+  <si>
+    <t>lab.build.button.deactivate</t>
+  </si>
+  <si>
+    <t>Deaktivovat build</t>
+  </si>
+  <si>
+    <t>lab.build.button.activate</t>
+  </si>
+  <si>
+    <t>Aktivovat build</t>
+  </si>
+  <si>
+    <t>lab.build.deactivated.success</t>
+  </si>
+  <si>
+    <t>Build [{{data.name}}] byl deaktivován; přestane se nabízet v různých nabídkách napříč aplikací.</t>
+  </si>
+  <si>
+    <t>lab.build.activated.success</t>
+  </si>
+  <si>
+    <t>Build [{{data.name}}] byl aktivován; bude se opět nabízet v nabídkách napříč aplikací.</t>
   </si>
 </sst>
 </file>
@@ -3372,10 +3411,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C600"/>
+  <dimension ref="A1:C607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A579" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C585" sqref="C585"/>
+    <sheetView tabSelected="1" topLeftCell="A591" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B601" sqref="B601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9983,6 +10022,83 @@
       </c>
       <c r="C600" s="1" t="s">
         <v>967</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A601" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B601" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A602" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A603" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A604" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B604" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A605" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B605" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A606" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A607" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B607" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>1005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial attempts with filter
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D7239A-C457-425C-8CC3-2440E5393B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06802099-B415-4BFD-8465-3B7DB0E2C300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="1013">
   <si>
     <t>cs</t>
   </si>
@@ -3048,6 +3048,27 @@
   </si>
   <si>
     <t>Build [{{data.name}}] byl aktivován; bude se opět nabízet v nabídkách napříč aplikací.</t>
+  </si>
+  <si>
+    <t>lab.vape.filter.title</t>
+  </si>
+  <si>
+    <t>Nastavení filtru</t>
+  </si>
+  <si>
+    <t>Filtrovat</t>
+  </si>
+  <si>
+    <t>common.filter.clear</t>
+  </si>
+  <si>
+    <t>Zrušit filtr</t>
+  </si>
+  <si>
+    <t>common.filter.submit</t>
+  </si>
+  <si>
+    <t>lab.vape.atomizerId.label</t>
   </si>
 </sst>
 </file>
@@ -3411,10 +3432,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C607"/>
+  <dimension ref="A1:C611"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A591" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B601" sqref="B601"/>
+      <selection activeCell="B605" sqref="B605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10099,6 +10120,50 @@
       </c>
       <c r="C607" s="1" t="s">
         <v>1005</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A608" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A609" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A610" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A611" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added initial filter for vapes
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06802099-B415-4BFD-8465-3B7DB0E2C300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA190AB-773A-46D7-8CC6-0C5729CDFE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="1013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="1015">
   <si>
     <t>cs</t>
   </si>
@@ -3069,6 +3069,12 @@
   </si>
   <si>
     <t>lab.vape.atomizerId.label</t>
+  </si>
+  <si>
+    <t>lab.mod.create.submit</t>
+  </si>
+  <si>
+    <t>lab.vape.modId.label</t>
   </si>
 </sst>
 </file>
@@ -3432,10 +3438,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C611"/>
+  <dimension ref="A1:C613"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A591" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B605" sqref="B605"/>
+      <selection activeCell="B606" sqref="B606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10164,6 +10170,28 @@
       </c>
       <c r="C611" s="1" t="s">
         <v>358</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A612" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A613" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added some more filters
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA190AB-773A-46D7-8CC6-0C5729CDFE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B724E5C-9243-4E84-B7B2-42F5F219D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1016">
   <si>
     <t>cs</t>
   </si>
@@ -3075,6 +3075,9 @@
   </si>
   <si>
     <t>lab.vape.modId.label</t>
+  </si>
+  <si>
+    <t>lab.vape.coilId.label</t>
   </si>
 </sst>
 </file>
@@ -3438,10 +3441,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C613"/>
+  <dimension ref="A1:C614"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A591" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B606" sqref="B606"/>
+      <selection activeCell="B608" sqref="B608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10192,6 +10195,17 @@
       </c>
       <c r="C613" s="1" t="s">
         <v>674</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A614" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B614" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed build edit form
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B724E5C-9243-4E84-B7B2-42F5F219D74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBE5A46-E5E1-4DDC-B80D-4301046C05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1022">
   <si>
     <t>cs</t>
   </si>
@@ -3078,6 +3078,24 @@
   </si>
   <si>
     <t>lab.vape.coilId.label</t>
+  </si>
+  <si>
+    <t>lab.build.build.title</t>
+  </si>
+  <si>
+    <t>lab.build.active.label</t>
+  </si>
+  <si>
+    <t>Aktivní?</t>
+  </si>
+  <si>
+    <t>lab.build.active.label.tooltip</t>
+  </si>
+  <si>
+    <t>Aktivním buildem je míněn takový, který je stále v použití; pokud je již vyřazen (nahrazen), lze jej označit jako neaktivní, čímž se přestane nabízet v různých seznamech.</t>
+  </si>
+  <si>
+    <t>lab.build.preview.active</t>
   </si>
 </sst>
 </file>
@@ -3441,10 +3459,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C614"/>
+  <dimension ref="A1:C618"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A591" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B608" sqref="B608"/>
+    <sheetView tabSelected="1" topLeftCell="A597" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B614" sqref="B614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10206,6 +10224,50 @@
       </c>
       <c r="C614" s="1" t="s">
         <v>354</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A615" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A616" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A617" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A618" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B618" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>1018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added recent mixes
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBE5A46-E5E1-4DDC-B80D-4301046C05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31C24C4-F290-4BF7-9E3D-DE28F8B8BAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1030">
   <si>
     <t>cs</t>
   </si>
@@ -3096,6 +3096,30 @@
   </si>
   <si>
     <t>lab.build.preview.active</t>
+  </si>
+  <si>
+    <t>lab.mixture.common.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.mixture.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.content.label</t>
+  </si>
+  <si>
+    <t>Složení</t>
+  </si>
+  <si>
+    <t>lab.mixture.latest.title</t>
+  </si>
+  <si>
+    <t>Poslední mixy</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.all.list</t>
+  </si>
+  <si>
+    <t>Všechny mixy</t>
   </si>
 </sst>
 </file>
@@ -3459,10 +3483,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C618"/>
+  <dimension ref="A1:C623"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A597" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B614" sqref="B614"/>
+    <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B617" sqref="B617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10268,6 +10292,61 @@
       </c>
       <c r="C618" s="1" t="s">
         <v>1018</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A619" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A620" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A621" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A622" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A623" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>1029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added mixture age
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31C24C4-F290-4BF7-9E3D-DE28F8B8BAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DA511-525D-4439-A6C8-372EE91F1ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1031">
   <si>
     <t>cs</t>
   </si>
@@ -3120,6 +3120,9 @@
   </si>
   <si>
     <t>Všechny mixy</t>
+  </si>
+  <si>
+    <t>lab.vape.table.mixture.age</t>
   </si>
 </sst>
 </file>
@@ -3483,10 +3486,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C623"/>
+  <dimension ref="A1:C624"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B617" sqref="B617"/>
+      <selection activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10347,6 +10350,17 @@
       </c>
       <c r="C623" s="1" t="s">
         <v>1029</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A624" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improving mobile version
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DA511-525D-4439-A6C8-372EE91F1ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049506DB-DE17-46B0-8F9A-7EA87CC69B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1032">
   <si>
     <t>cs</t>
   </si>
@@ -3123,6 +3123,9 @@
   </si>
   <si>
     <t>lab.vape.table.mixture.age</t>
+  </si>
+  <si>
+    <t>lab.setup.update.submit</t>
   </si>
 </sst>
 </file>
@@ -3486,10 +3489,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C624"/>
+  <dimension ref="A1:C625"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B616" sqref="B616"/>
+      <selection activeCell="B620" sqref="B620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10361,6 +10364,17 @@
       </c>
       <c r="C624" s="1" t="s">
         <v>910</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Simplified repository stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049506DB-DE17-46B0-8F9A-7EA87CC69B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9604621-9153-40BC-8E20-8AD807A33C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1033">
   <si>
     <t>cs</t>
   </si>
@@ -3126,6 +3126,9 @@
   </si>
   <si>
     <t>lab.setup.update.submit</t>
+  </si>
+  <si>
+    <t>lab.vape.liquidId.label</t>
   </si>
 </sst>
 </file>
@@ -3489,9 +3492,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C625"/>
+  <dimension ref="A1:C626"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A615" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B620" sqref="B620"/>
     </sheetView>
   </sheetViews>
@@ -10375,6 +10378,17 @@
       </c>
       <c r="C625" s="1" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B626" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C626" s="1" t="s">
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved filter UI a bit
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9604621-9153-40BC-8E20-8AD807A33C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2918BA-03EA-4239-95C0-4290EEB34723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3053,9 +3053,6 @@
     <t>lab.vape.filter.title</t>
   </si>
   <si>
-    <t>Nastavení filtru</t>
-  </si>
-  <si>
     <t>Filtrovat</t>
   </si>
   <si>
@@ -3129,6 +3126,9 @@
   </si>
   <si>
     <t>lab.vape.liquidId.label</t>
+  </si>
+  <si>
+    <t>Filtrování</t>
   </si>
 </sst>
 </file>
@@ -3494,8 +3494,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C626"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A615" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B620" sqref="B620"/>
+    <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C609" sqref="C609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10190,7 +10190,7 @@
         <v>1006</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1007</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -10198,10 +10198,10 @@
         <v>0</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
@@ -10209,10 +10209,10 @@
         <v>0</v>
       </c>
       <c r="B610" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C610" s="1" t="s">
         <v>1009</v>
-      </c>
-      <c r="C610" s="1" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.25">
@@ -10220,7 +10220,7 @@
         <v>0</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>358</v>
@@ -10231,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C612" s="1" t="s">
         <v>689</v>
@@ -10242,7 +10242,7 @@
         <v>0</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C613" s="1" t="s">
         <v>674</v>
@@ -10253,7 +10253,7 @@
         <v>0</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C614" s="1" t="s">
         <v>354</v>
@@ -10264,7 +10264,7 @@
         <v>0</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C615" s="1" t="s">
         <v>366</v>
@@ -10275,10 +10275,10 @@
         <v>0</v>
       </c>
       <c r="B616" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C616" s="1" t="s">
         <v>1017</v>
-      </c>
-      <c r="C616" s="1" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="617" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10286,10 +10286,10 @@
         <v>0</v>
       </c>
       <c r="B617" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C617" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="C617" s="1" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
@@ -10297,10 +10297,10 @@
         <v>0</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.25">
@@ -10308,7 +10308,7 @@
         <v>0</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C619" s="1" t="s">
         <v>119</v>
@@ -10319,7 +10319,7 @@
         <v>0</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C620" s="1" t="s">
         <v>533</v>
@@ -10330,10 +10330,10 @@
         <v>0</v>
       </c>
       <c r="B621" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C621" s="1" t="s">
         <v>1024</v>
-      </c>
-      <c r="C621" s="1" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
@@ -10341,10 +10341,10 @@
         <v>0</v>
       </c>
       <c r="B622" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C622" s="1" t="s">
         <v>1026</v>
-      </c>
-      <c r="C622" s="1" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
@@ -10352,10 +10352,10 @@
         <v>0</v>
       </c>
       <c r="B623" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C623" s="1" t="s">
         <v>1028</v>
-      </c>
-      <c r="C623" s="1" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
@@ -10363,7 +10363,7 @@
         <v>0</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C624" s="1" t="s">
         <v>910</v>
@@ -10374,7 +10374,7 @@
         <v>0</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C625" s="1" t="s">
         <v>289</v>
@@ -10385,7 +10385,7 @@
         <v>0</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C626" s="1" t="s">
         <v>581</v>

</xml_diff>

<commit_message>
Common: A lot of small improvements; added glow and active flag
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2918BA-03EA-4239-95C0-4290EEB34723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C0A0E-638D-45AD-A3A0-56E3CC4AEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1048">
   <si>
     <t>cs</t>
   </si>
@@ -3129,6 +3129,51 @@
   </si>
   <si>
     <t>Filtrování</t>
+  </si>
+  <si>
+    <t>Žhavení</t>
+  </si>
+  <si>
+    <t>lab.build.glow.label</t>
+  </si>
+  <si>
+    <t>lab.build.glow.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato hodnota udává rychlost žhavení; čím vyšší číslo, tím rychleji se spirálka rozžhaví; smyslem je poskytnout náhled, jak moc "divoký" build je.</t>
+  </si>
+  <si>
+    <t>lab.build.table.glow</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.activate</t>
+  </si>
+  <si>
+    <t>Aktivovat mix</t>
+  </si>
+  <si>
+    <t>lab.mixture.button.deactivate</t>
+  </si>
+  <si>
+    <t>Deaktivovat mix</t>
+  </si>
+  <si>
+    <t>lab.mixture.deactivated.success</t>
+  </si>
+  <si>
+    <t>Mix [{{data.name}}] byl úspěšně deaktivován.</t>
+  </si>
+  <si>
+    <t>lab.mixture.activated.success</t>
+  </si>
+  <si>
+    <t>Mix [{{data.name}}] byl úspěšně aktivován.</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.active</t>
+  </si>
+  <si>
+    <t>Aktivní</t>
   </si>
 </sst>
 </file>
@@ -3492,10 +3537,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C626"/>
+  <dimension ref="A1:C634"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A606" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C609" sqref="C609"/>
+    <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B629" sqref="B629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10389,6 +10434,94 @@
       </c>
       <c r="C626" s="1" t="s">
         <v>581</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B627" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A628" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B628" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A631" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B631" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C631" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A632" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C632" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A633" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C633" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A634" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B634" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C634" s="1" t="s">
+        <v>1047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved mobile version of vape
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C0A0E-638D-45AD-A3A0-56E3CC4AEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6C087E-5164-4ED5-9CD4-2D6052EE3240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1052">
   <si>
     <t>cs</t>
   </si>
@@ -3174,6 +3174,18 @@
   </si>
   <si>
     <t>Aktivní</t>
+  </si>
+  <si>
+    <t>lab.vape.build.title</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.build</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.liquid</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.created</t>
   </si>
 </sst>
 </file>
@@ -3537,10 +3549,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C634"/>
+  <dimension ref="A1:C638"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B629" sqref="B629"/>
+      <selection activeCell="B632" sqref="B632"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10522,6 +10534,50 @@
       </c>
       <c r="C634" s="1" t="s">
         <v>1047</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A635" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C635" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A636" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C636" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A637" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B637" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C637" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A638" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B638" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C638" s="1" t="s">
+        <v>942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved vape preview
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6C087E-5164-4ED5-9CD4-2D6052EE3240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5816CD-E7D0-4D68-824F-C1E9CA9DD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1053">
   <si>
     <t>cs</t>
   </si>
@@ -3186,6 +3186,9 @@
   </si>
   <si>
     <t>lab.vape.preview.created</t>
+  </si>
+  <si>
+    <t>lab.vape.preview.mixture.age</t>
   </si>
 </sst>
 </file>
@@ -3549,7 +3552,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C638"/>
+  <dimension ref="A1:C639"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B632" sqref="B632"/>
@@ -10578,6 +10581,17 @@
       </c>
       <c r="C638" s="1" t="s">
         <v>942</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A639" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B639" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C639" s="1" t="s">
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added whole coil section
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5816CD-E7D0-4D68-824F-C1E9CA9DD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9570A687-8ED8-4562-A65C-84C50A06BF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="6465" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="600" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1093">
   <si>
     <t>cs</t>
   </si>
@@ -3189,6 +3189,126 @@
   </si>
   <si>
     <t>lab.vape.preview.mixture.age</t>
+  </si>
+  <si>
+    <t>lab.coil.title</t>
+  </si>
+  <si>
+    <t>lab.coil.subtitle</t>
+  </si>
+  <si>
+    <t>V této sekci se nachází správa veškerých spirálek, které jste kdy vytvořili.</t>
+  </si>
+  <si>
+    <t>lab.coil.button.create</t>
+  </si>
+  <si>
+    <t>lab.coil.button.list</t>
+  </si>
+  <si>
+    <t>Seznam spirálek</t>
+  </si>
+  <si>
+    <t>lab.coil.list.title</t>
+  </si>
+  <si>
+    <t>lab.coil.table.wire</t>
+  </si>
+  <si>
+    <t>Drát</t>
+  </si>
+  <si>
+    <t>lab.coil.table.wraps</t>
+  </si>
+  <si>
+    <t>lab.coil.table.ohm</t>
+  </si>
+  <si>
+    <t>lab.coil.filter.title</t>
+  </si>
+  <si>
+    <t>Filtrovat spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.preview</t>
+  </si>
+  <si>
+    <t>Náhled spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.preview.title</t>
+  </si>
+  <si>
+    <t>Detail spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Přehled dostupných dat o vybrané spirálce.</t>
+  </si>
+  <si>
+    <t>lab.coil.button.index</t>
+  </si>
+  <si>
+    <t>Klonovat spirálku</t>
+  </si>
+  <si>
+    <t>lab.coil.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit spirálku</t>
+  </si>
+  <si>
+    <t>lab.coil.button.clone</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.wire</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.wraps</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.ohm</t>
+  </si>
+  <si>
+    <t>lab.coil.edit.title</t>
+  </si>
+  <si>
+    <t>Editace spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Upravte vlastnosti vybrané spirálky.</t>
+  </si>
+  <si>
+    <t>lab.coil.update.submit</t>
+  </si>
+  <si>
+    <t>lab.coil.update.message</t>
+  </si>
+  <si>
+    <t>Spirálka byla úspěšně aktualizována.</t>
+  </si>
+  <si>
+    <t>lab.coil.index.title</t>
+  </si>
+  <si>
+    <t>lab.coil.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>lab.coil.index.preview.title</t>
+  </si>
+  <si>
+    <t>lab.coil.clone.title</t>
+  </si>
+  <si>
+    <t>Klon spirálky</t>
+  </si>
+  <si>
+    <t>lab.coil.link.button</t>
   </si>
 </sst>
 </file>
@@ -3552,10 +3672,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C639"/>
+  <dimension ref="A1:C668"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A621" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B632" sqref="B632"/>
+    <sheetView tabSelected="1" topLeftCell="A642" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B658" sqref="B658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10592,6 +10712,325 @@
       </c>
       <c r="C639" s="1" t="s">
         <v>910</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A640" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B640" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C640" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A641" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B641" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C641" s="1" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A642" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B642" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C642" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A643" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B643" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C643" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A644" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B644" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C644" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A645" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B645" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C645" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A646" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B646" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C646" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A647" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B647" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C647" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A648" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C648" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A649" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B649" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C649" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A650" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B650" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C650" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A651" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B651" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C651" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A652" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B652" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C652" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A653" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B653" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C653" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A654" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B654" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C654" s="1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A655" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B655" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C655" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="656" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A656" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B656" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C656" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A657" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B657" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C657" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A658" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B658" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C658" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A659" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B659" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C659" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A660" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B660" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C660" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A661" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B661" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C661" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A662" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B662" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C662" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A663" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B663" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C663" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A664" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B664" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C664" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A665" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B665" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C665" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A666" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B666" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C666" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A667" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B667" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C667" s="1" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A668" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B668" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C668" s="1" t="s">
+        <v>1069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Coil stuff done
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9570A687-8ED8-4562-A65C-84C50A06BF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282AB5CC-DE71-47AB-87E0-A3E97BAE6D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="600" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1101">
   <si>
     <t>cs</t>
   </si>
@@ -3309,6 +3309,30 @@
   </si>
   <si>
     <t>lab.coil.link.button</t>
+  </si>
+  <si>
+    <t>lab.coil.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit spirálku</t>
+  </si>
+  <si>
+    <t>lab.coil.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.coil.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybranou spirálku? Tato nebezpečná akce může mít vliv na ostatní data, kdy může dojít k odmazání např. vapů nebo buildů, které tuto spirálku využívají. Použijte prosím s velkým rozmyslem.</t>
+  </si>
+  <si>
+    <t>lab.coil.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.coil.deleted.success</t>
+  </si>
+  <si>
+    <t>Spirálka byla úspěšně odstraněna. Bůh s vámi!</t>
   </si>
 </sst>
 </file>
@@ -3672,10 +3696,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C668"/>
+  <dimension ref="A1:C673"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A642" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B658" sqref="B658"/>
+      <selection activeCell="B664" sqref="B664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11031,6 +11055,61 @@
       </c>
       <c r="C668" s="1" t="s">
         <v>1069</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A669" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B669" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C669" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A670" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B670" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C670" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A671" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B671" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C671" s="1" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A672" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B672" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C672" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A673" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B673" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C673" s="1" t="s">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed coil stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282AB5CC-DE71-47AB-87E0-A3E97BAE6D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20002D6A-FA95-4715-972E-08A2CC2DC508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="600" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="1103">
   <si>
     <t>cs</t>
   </si>
@@ -3333,6 +3333,12 @@
   </si>
   <si>
     <t>Spirálka byla úspěšně odstraněna. Bůh s vámi!</t>
+  </si>
+  <si>
+    <t>error.Duplicate entry [z_coil_coil_unique] of [z_coil].</t>
+  </si>
+  <si>
+    <t>Spirálka s vybranými vlastnostmi již existuje (tzn. drát, počet otoček a odpor je stejný).</t>
   </si>
 </sst>
 </file>
@@ -3696,10 +3702,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C673"/>
+  <dimension ref="A1:C674"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A642" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B664" sqref="B664"/>
+      <selection activeCell="B666" sqref="B666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11110,6 +11116,17 @@
       </c>
       <c r="C673" s="1" t="s">
         <v>1100</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A674" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B674" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C674" s="1" t="s">
+        <v>1102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved stuff 'round
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFA961D-33BD-41FE-9677-8472E0E2DE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F72F91-556E-42FA-A149-B5394906A0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="600" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="1108">
   <si>
     <t>cs</t>
   </si>
@@ -3342,6 +3342,18 @@
   </si>
   <si>
     <t>Aktualizace aplikace</t>
+  </si>
+  <si>
+    <t>lab.vape.table.atomizer</t>
+  </si>
+  <si>
+    <t>lab.vape.buildId.label</t>
+  </si>
+  <si>
+    <t>lab.vape.table.mod</t>
+  </si>
+  <si>
+    <t>lab.build.button.vape.create</t>
   </si>
 </sst>
 </file>
@@ -3705,10 +3717,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C675"/>
+  <dimension ref="A1:C679"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A642" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B670" sqref="B670"/>
+      <selection activeCell="B667" sqref="B667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11141,6 +11153,50 @@
       </c>
       <c r="C675" s="1" t="s">
         <v>1103</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A676" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B676" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C676" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A677" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B677" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C677" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A678" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B678" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C678" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A679" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B679" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C679" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added build filter
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14951AD6-4F80-48DE-A475-FF659D76DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0F784E-3E01-4E9B-9761-0CA46588794E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="600" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="1117">
   <si>
     <t>cs</t>
   </si>
@@ -3366,6 +3366,21 @@
   </si>
   <si>
     <t>Build byl uložen.</t>
+  </si>
+  <si>
+    <t>lab.build.filter.title</t>
+  </si>
+  <si>
+    <t>Filtr</t>
+  </si>
+  <si>
+    <t>Filtr buildů</t>
+  </si>
+  <si>
+    <t>lab.build.modId.label</t>
+  </si>
+  <si>
+    <t>lab.build.wireId.label</t>
   </si>
 </sst>
 </file>
@@ -3729,10 +3744,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C681"/>
+  <dimension ref="A1:C685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+    <sheetView tabSelected="1" topLeftCell="A662" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B682" sqref="B682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11231,6 +11246,50 @@
       </c>
       <c r="C681" s="1" t="s">
         <v>1110</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A682" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B682" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C682" s="1" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A683" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B683" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C683" s="1" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A684" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B684" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C684" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A685" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B685" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C685" s="1" t="s">
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added an ability to remove a build
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50203386-2A2A-804D-8262-46C28B4274E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0ED873-2B14-F14B-BC8A-E7CC467C8379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="600" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="1126">
   <si>
     <t>cs</t>
   </si>
@@ -3384,6 +3384,30 @@
   </si>
   <si>
     <t>lab.vape.table.coil</t>
+  </si>
+  <si>
+    <t>lab.build.button.delete</t>
+  </si>
+  <si>
+    <t>Ostranit build</t>
+  </si>
+  <si>
+    <t>lab.build.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.build.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.build.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný build? Tato akce může odstranit velké množství zajímavých dat, zejména pak záznamů vapování. Buďte prosím velmi obezřetní, ponevadž tuto akci nelze vzít zpět. Hodně štěstí.</t>
+  </si>
+  <si>
+    <t>lab.build.deleted.success</t>
+  </si>
+  <si>
+    <t>Build byl úspěšně odstraněn. Škoda dat. </t>
   </si>
 </sst>
 </file>
@@ -3747,10 +3771,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C686"/>
+  <dimension ref="A1:C691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A671" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B680" sqref="B680"/>
+    <sheetView tabSelected="1" topLeftCell="A677" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B682" sqref="B682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11304,6 +11328,61 @@
       </c>
       <c r="C686" s="1" t="s">
         <v>354</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A687" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B687" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A688" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B688" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C688" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A689" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B689" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A690" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B690" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C690" s="1" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="691" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A691" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B691" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C691" s="1" t="s">
+        <v>1125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added coil size
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0ED873-2B14-F14B-BC8A-E7CC467C8379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C331CDC-A135-F145-8C76-54BAA669C9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="600" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="1127">
   <si>
     <t>cs</t>
   </si>
@@ -3408,6 +3408,9 @@
   </si>
   <si>
     <t>Build byl úspěšně odstraněn. Škoda dat. </t>
+  </si>
+  <si>
+    <t>lab.coil.size.label</t>
   </si>
 </sst>
 </file>
@@ -3771,10 +3774,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C691"/>
+  <dimension ref="A1:C692"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A677" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B682" sqref="B682"/>
+      <selection activeCell="B688" sqref="B688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11383,6 +11386,17 @@
       </c>
       <c r="C691" s="1" t="s">
         <v>1125</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A692" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B692" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C692" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared base comment
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E96B093-CD16-B54C-9288-7C21D59E3319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2904D8F6-40EC-C647-9099-D8EABE556B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="600" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="1130">
   <si>
     <t>cs</t>
   </si>
@@ -3414,6 +3414,12 @@
   </si>
   <si>
     <t>lab.build.age.label</t>
+  </si>
+  <si>
+    <t>lab.build.comment.create</t>
+  </si>
+  <si>
+    <t> Přidat komentář</t>
   </si>
 </sst>
 </file>
@@ -3777,10 +3783,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C693"/>
+  <dimension ref="A1:C694"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A677" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B690" sqref="B690"/>
+      <selection activeCell="B691" sqref="B691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11411,6 +11417,17 @@
       </c>
       <c r="C693" s="1" t="s">
         <v>894</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A694" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B694" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C694" s="1" t="s">
+        <v>1129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added liquid section
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F71739F-FD8F-4CCA-AE82-0DFF260A773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E27228D-6E82-4888-9DBC-5DE8A6938179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="5055" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2475" yWindow="6525" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="1201">
   <si>
     <t>cs</t>
   </si>
@@ -3519,6 +3519,120 @@
   </si>
   <si>
     <t>Výchozí řazení</t>
+  </si>
+  <si>
+    <t>lab.liquid.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.subtitle</t>
+  </si>
+  <si>
+    <t>Tato sekce slouží pro správu liquidů.</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.create</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.list</t>
+  </si>
+  <si>
+    <t>Seznam liquidů</t>
+  </si>
+  <si>
+    <t>lab.liquid.list.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview</t>
+  </si>
+  <si>
+    <t>Náhled liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.index</t>
+  </si>
+  <si>
+    <t>Detail liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.edit</t>
+  </si>
+  <si>
+    <t>Editace liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit liquid</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Tuto akci si prosím velmi rozvažte, poněvadž může mít hluboký dopad na celou aplikaci, hlavně pak statistická data o vapování. Smazání liquidu obecně není doporučeno, proto prosím postupujte s maximální obezřetností, protože není cesty zpět. Vážně.</t>
+  </si>
+  <si>
+    <t>lab.liquid.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.liquid.deleted.success</t>
+  </si>
+  <si>
+    <t>Liquid [{{data.name}}] (a možná i hromada jiných dat) byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.liquid.table.name</t>
+  </si>
+  <si>
+    <t>lab.liquid.table.pgvg</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.preview.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.preview.subtitle</t>
+  </si>
+  <si>
+    <t>Zde jsou veškeré dostupné informace o vybraném liquidu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.name</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.pgvg</t>
+  </si>
+  <si>
+    <t>lab.liquid.edit.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.edit.subtitle</t>
+  </si>
+  <si>
+    <t>Uprava údajů o vybraném liquidu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.update.submit</t>
+  </si>
+  <si>
+    <t>lab.liquid.updated.message</t>
+  </si>
+  <si>
+    <t>Liquid [{{data.name}}] byl aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.liquid.index.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.index.preview.title</t>
+  </si>
+  <si>
+    <t>lab.liquid.index.preview.subtitle</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.volume</t>
   </si>
 </sst>
 </file>
@@ -3882,10 +3996,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C712"/>
+  <dimension ref="A1:C739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A689" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B707" sqref="B707"/>
+    <sheetView tabSelected="1" topLeftCell="A722" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B738" sqref="B738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11725,6 +11839,303 @@
       </c>
       <c r="C712" s="1" t="s">
         <v>1162</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A713" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B713" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C713" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="714" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A714" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B714" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C714" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="715" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A715" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B715" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C715" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="716" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A716" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B716" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C716" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A717" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B717" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C717" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A718" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B718" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C718" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A719" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B719" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C719" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A720" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B720" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C720" s="1" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A721" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B721" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C721" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A722" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B722" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C722" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A723" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B723" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C723" s="1" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A724" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B724" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C724" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A725" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B725" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C725" s="1" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A726" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B726" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C726" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A727" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B727" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C727" s="1" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A728" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B728" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C728" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A729" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B729" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C729" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A730" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B730" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C730" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A731" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B731" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C731" s="1" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="732" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A732" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B732" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C732" s="1" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="733" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A733" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B733" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C733" s="1" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="734" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A734" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B734" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C734" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="735" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A735" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B735" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C735" s="1" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A736" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B736" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C736" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="737" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A737" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B737" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C737" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="738" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A738" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B738" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C738" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="739" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A739" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B739" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C739" s="1" t="s">
+        <v>606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added filter for liquids
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E27228D-6E82-4888-9DBC-5DE8A6938179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B9E8DA-1BB3-42CC-8F86-AF11FAD375C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="6525" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1203">
   <si>
     <t>cs</t>
   </si>
@@ -3633,6 +3633,12 @@
   </si>
   <si>
     <t>lab.liquid.preview.volume</t>
+  </si>
+  <si>
+    <t>lab.liquid.filter.title</t>
+  </si>
+  <si>
+    <t>Filtrovat liquidy</t>
   </si>
 </sst>
 </file>
@@ -3996,10 +4002,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C739"/>
+  <dimension ref="A1:C740"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A722" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B738" sqref="B738"/>
+      <selection activeCell="B731" sqref="B731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12136,6 +12142,17 @@
       </c>
       <c r="C739" s="1" t="s">
         <v>606</v>
+      </c>
+    </row>
+    <row r="740" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A740" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B740" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C740" s="1" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added build rating
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B9E8DA-1BB3-42CC-8F86-AF11FAD375C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93825AF-E734-47E7-BCA9-CC6407C0E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="6525" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="1209">
   <si>
     <t>cs</t>
   </si>
@@ -3639,6 +3639,24 @@
   </si>
   <si>
     <t>Filtrovat liquidy</t>
+  </si>
+  <si>
+    <t>lab.build.rating.label</t>
+  </si>
+  <si>
+    <t>Hodnocení buildu</t>
+  </si>
+  <si>
+    <t>lab.build.rating.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tato hodnota má napovědět. Jak moc se build obecně povedl - jestli je zábavný, nebo z něj chutná, nebo všechno, nebo jestli se k němu už nevracet. V komentářích pak lze dopsat případné poznámky i v průběhu využívání buildu.</t>
+  </si>
+  <si>
+    <t>lab.build.preview.rating</t>
+  </si>
+  <si>
+    <t>lab.build.table.rating</t>
   </si>
 </sst>
 </file>
@@ -4002,10 +4020,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C740"/>
+  <dimension ref="A1:C744"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A722" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B731" sqref="B731"/>
+      <selection activeCell="B738" sqref="B738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12153,6 +12171,50 @@
       </c>
       <c r="C740" s="1" t="s">
         <v>1202</v>
+      </c>
+    </row>
+    <row r="741" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A741" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B741" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C741" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="742" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A742" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B742" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C742" s="1" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="743" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A743" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B743" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C743" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="744" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A744" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B744" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C744" s="1" t="s">
+        <v>806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved UI a bit II
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B0FB44-A84D-41EB-B6CF-0A8488A1671E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0102BA-3FF9-4B6F-BED8-3607BCBD932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="1217">
   <si>
     <t>cs</t>
   </si>
@@ -3669,6 +3669,18 @@
   </si>
   <si>
     <t>lab.vape.common.tab</t>
+  </si>
+  <si>
+    <t>lab.mixture.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.mixture.common.tab</t>
+  </si>
+  <si>
+    <t>lab.liquid.common.tab</t>
+  </si>
+  <si>
+    <t>lab.liquid.comments.tab</t>
   </si>
 </sst>
 </file>
@@ -4032,10 +4044,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C748"/>
+  <dimension ref="A1:C752"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A731" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B746" sqref="B746"/>
+      <selection activeCell="B742" sqref="B742"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12271,6 +12283,50 @@
       </c>
       <c r="C748" s="1" t="s">
         <v>528</v>
+      </c>
+    </row>
+    <row r="749" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A749" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B749" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C749" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="750" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A750" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B750" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C750" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="751" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A751" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B751" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C751" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="752" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A752" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B752" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C752" s="1" t="s">
+        <v>1136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing image upload
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0102BA-3FF9-4B6F-BED8-3607BCBD932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56667F66-4599-4226-96C4-1DBA4CFE36B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="1230">
   <si>
     <t>cs</t>
   </si>
@@ -3681,6 +3681,45 @@
   </si>
   <si>
     <t>lab.liquid.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.build.images.tab</t>
+  </si>
+  <si>
+    <t>Obrázky</t>
+  </si>
+  <si>
+    <t>lab.build.image.upload</t>
+  </si>
+  <si>
+    <t>Nahrát obrázek</t>
+  </si>
+  <si>
+    <t>lab.build.image.upload.hint</t>
+  </si>
+  <si>
+    <t>Obrázky jsou fajn, tady je možné jej nahrát.</t>
+  </si>
+  <si>
+    <t>lab.build.upload.tab</t>
+  </si>
+  <si>
+    <t>common.error.file-too-large</t>
+  </si>
+  <si>
+    <t>Vybraný soubor je příliš velký.</t>
+  </si>
+  <si>
+    <t>lab.build.image.upload.started</t>
+  </si>
+  <si>
+    <t>Upload byl zahájen.</t>
+  </si>
+  <si>
+    <t>lab.build.image.upload.success</t>
+  </si>
+  <si>
+    <t>Upload obrázku byl úspěšný.</t>
   </si>
 </sst>
 </file>
@@ -4044,10 +4083,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C752"/>
+  <dimension ref="A1:C759"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A731" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B742" sqref="B742"/>
+    <sheetView tabSelected="1" topLeftCell="A737" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B752" sqref="B752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12327,6 +12366,83 @@
       </c>
       <c r="C752" s="1" t="s">
         <v>1136</v>
+      </c>
+    </row>
+    <row r="753" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A753" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B753" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C753" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="754" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A754" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B754" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C754" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="755" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A755" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B755" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C755" s="1" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="756" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A756" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B756" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C756" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A757" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B757" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C757" s="1" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="758" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A758" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B758" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C758" s="1" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="759" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A759" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B759" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C759" s="1" t="s">
+        <v>1229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Very first support for gallery
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56667F66-4599-4226-96C4-1DBA4CFE36B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A385A03-4FFD-490F-9196-271878C65B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="1245">
   <si>
     <t>cs</t>
   </si>
@@ -3720,6 +3720,51 @@
   </si>
   <si>
     <t>Upload obrázku byl úspěšný.</t>
+  </si>
+  <si>
+    <t>lab.build.image.cancel.upload</t>
+  </si>
+  <si>
+    <t>Zrušit nahrávání</t>
+  </si>
+  <si>
+    <t>lab.liquid.upload.tab</t>
+  </si>
+  <si>
+    <t>Nejsou dostupné žádné obrázky.</t>
+  </si>
+  <si>
+    <t>lab.liquid.images.tab</t>
+  </si>
+  <si>
+    <t>common.gallery.no-images</t>
+  </si>
+  <si>
+    <t>lab.liquid.image.upload</t>
+  </si>
+  <si>
+    <t>Nahrajte obrázek liquidu</t>
+  </si>
+  <si>
+    <t>lab.liquid.image.upload.hint</t>
+  </si>
+  <si>
+    <t>Obrázek pomůže snadno identifikovat, o jaký liquid se jedná.</t>
+  </si>
+  <si>
+    <t>lab.liquid.image.upload.started</t>
+  </si>
+  <si>
+    <t>Nahrávání bylo zahájeno.</t>
+  </si>
+  <si>
+    <t>Obrázek byl úspěšně nahrán.</t>
+  </si>
+  <si>
+    <t>lab.liquid.image.cancel.upload</t>
+  </si>
+  <si>
+    <t>lab.liquid.image.upload.success</t>
   </si>
 </sst>
 </file>
@@ -4083,10 +4128,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C759"/>
+  <dimension ref="A1:C768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A737" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B752" sqref="B752"/>
+    <sheetView tabSelected="1" topLeftCell="A749" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B764" sqref="B764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12443,6 +12488,105 @@
       </c>
       <c r="C759" s="1" t="s">
         <v>1229</v>
+      </c>
+    </row>
+    <row r="760" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A760" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B760" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C760" s="1" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="761" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A761" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B761" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C761" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="762" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A762" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B762" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C762" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="763" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A763" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B763" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C763" s="1" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="764" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A764" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B764" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C764" s="1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="765" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A765" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B765" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C765" s="1" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="766" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A766" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B766" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C766" s="1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="767" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A767" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B767" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C767" s="1" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="768" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A768" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B768" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C768" s="1" t="s">
+        <v>1231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Very first experimental gallery implementation
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A385A03-4FFD-490F-9196-271878C65B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23698EF4-0306-4620-ACD3-16AD55A38657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="1245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="1247">
   <si>
     <t>cs</t>
   </si>
@@ -3765,6 +3765,12 @@
   </si>
   <si>
     <t>lab.liquid.image.upload.success</t>
+  </si>
+  <si>
+    <t>common.show-gallery.button</t>
+  </si>
+  <si>
+    <t>Zobrazit obrázky</t>
   </si>
 </sst>
 </file>
@@ -4128,7 +4134,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C768"/>
+  <dimension ref="A1:C769"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A749" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B764" sqref="B764"/>
@@ -12587,6 +12593,17 @@
       </c>
       <c r="C768" s="1" t="s">
         <v>1231</v>
+      </c>
+    </row>
+    <row r="769" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A769" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B769" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C769" s="1" t="s">
+        <v>1246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added mixture rating
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23698EF4-0306-4620-ACD3-16AD55A38657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347457D-74B9-4BCD-B1F1-0672DDCFDC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="1247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1257">
   <si>
     <t>cs</t>
   </si>
@@ -2201,9 +2201,6 @@
     <t>lab.mixture.create.success</t>
   </si>
   <si>
-    <t>Mix [{{data.name}}] byl úspěšně uložen.</t>
-  </si>
-  <si>
     <t>lab.setup.create.success</t>
   </si>
   <si>
@@ -3158,15 +3155,9 @@
     <t>lab.mixture.deactivated.success</t>
   </si>
   <si>
-    <t>Mix [{{data.name}}] byl úspěšně deaktivován.</t>
-  </si>
-  <si>
     <t>lab.mixture.activated.success</t>
   </si>
   <si>
-    <t>Mix [{{data.name}}] byl úspěšně aktivován.</t>
-  </si>
-  <si>
     <t>lab.mixture.preview.active</t>
   </si>
   <si>
@@ -3771,6 +3762,45 @@
   </si>
   <si>
     <t>Zobrazit obrázky</t>
+  </si>
+  <si>
+    <t>lab.mixture.filter.title</t>
+  </si>
+  <si>
+    <t>Filtr mixů</t>
+  </si>
+  <si>
+    <t>lab.mixture.rating.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.active.label</t>
+  </si>
+  <si>
+    <t>Mix byl úspěšně aktualizován.</t>
+  </si>
+  <si>
+    <t>Mix byl úspěšně deaktivován.</t>
+  </si>
+  <si>
+    <t>Mix byl úspěšně aktivován.</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.code</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.rating</t>
+  </si>
+  <si>
+    <t>lab.mixture.rating.label.tooltip</t>
+  </si>
+  <si>
+    <t>Hodnocení mixu - mimo jiné vypovídá o tom, zda stojí za to si jej případně pořídit znovu (např. deset hvězd) nebo zda stojí za bačkoru a měl by shořet v pekle (jedna hvezda).</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.rating</t>
   </si>
 </sst>
 </file>
@@ -4134,10 +4164,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C769"/>
+  <dimension ref="A1:C777"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A749" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B764" sqref="B764"/>
+    <sheetView tabSelected="1" topLeftCell="A766" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B773" sqref="B773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7378,7 +7408,7 @@
         <v>521</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -8764,7 +8794,7 @@
         <v>722</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>723</v>
+        <v>589</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
@@ -8772,10 +8802,10 @@
         <v>0</v>
       </c>
       <c r="B421" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C421" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="C421" s="1" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
@@ -8783,7 +8813,7 @@
         <v>0</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>670</v>
@@ -8794,7 +8824,7 @@
         <v>0</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>381</v>
@@ -8805,10 +8835,10 @@
         <v>0</v>
       </c>
       <c r="B424" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C424" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C424" s="1" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -8816,7 +8846,7 @@
         <v>0</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>119</v>
@@ -8827,10 +8857,10 @@
         <v>0</v>
       </c>
       <c r="B426" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C426" s="1" t="s">
         <v>731</v>
-      </c>
-      <c r="C426" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -8838,10 +8868,10 @@
         <v>0</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -8849,10 +8879,10 @@
         <v>0</v>
       </c>
       <c r="B428" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C428" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="C428" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -8860,10 +8890,10 @@
         <v>0</v>
       </c>
       <c r="B429" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C429" s="1" t="s">
         <v>736</v>
-      </c>
-      <c r="C429" s="1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -8871,10 +8901,10 @@
         <v>0</v>
       </c>
       <c r="B430" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="C430" s="1" t="s">
         <v>738</v>
-      </c>
-      <c r="C430" s="1" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -8882,10 +8912,10 @@
         <v>0</v>
       </c>
       <c r="B431" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C431" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -8893,10 +8923,10 @@
         <v>0</v>
       </c>
       <c r="B432" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="C432" s="1" t="s">
         <v>742</v>
-      </c>
-      <c r="C432" s="1" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -8904,10 +8934,10 @@
         <v>0</v>
       </c>
       <c r="B433" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C433" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="C433" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -8915,10 +8945,10 @@
         <v>0</v>
       </c>
       <c r="B434" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="C434" s="1" t="s">
         <v>746</v>
-      </c>
-      <c r="C434" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
@@ -8926,10 +8956,10 @@
         <v>0</v>
       </c>
       <c r="B435" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="C435" s="1" t="s">
         <v>748</v>
-      </c>
-      <c r="C435" s="1" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
@@ -8937,10 +8967,10 @@
         <v>0</v>
       </c>
       <c r="B436" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C436" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
@@ -8948,10 +8978,10 @@
         <v>0</v>
       </c>
       <c r="B437" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C437" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="C437" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -8959,10 +8989,10 @@
         <v>0</v>
       </c>
       <c r="B438" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C438" s="1" t="s">
         <v>754</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="439" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -8970,10 +9000,10 @@
         <v>0</v>
       </c>
       <c r="B439" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C439" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="C439" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
@@ -8981,10 +9011,10 @@
         <v>0</v>
       </c>
       <c r="B440" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="C440" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="C440" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -8992,10 +9022,10 @@
         <v>0</v>
       </c>
       <c r="B441" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C441" s="1" t="s">
         <v>760</v>
-      </c>
-      <c r="C441" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
@@ -9003,10 +9033,10 @@
         <v>0</v>
       </c>
       <c r="B442" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C442" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="C442" s="1" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
@@ -9014,7 +9044,7 @@
         <v>0</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>114</v>
@@ -9025,10 +9055,10 @@
         <v>0</v>
       </c>
       <c r="B444" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C444" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="C444" s="1" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
@@ -9036,10 +9066,10 @@
         <v>0</v>
       </c>
       <c r="B445" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C445" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -9047,10 +9077,10 @@
         <v>0</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C446" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9058,10 +9088,10 @@
         <v>0</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C447" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -9069,10 +9099,10 @@
         <v>0</v>
       </c>
       <c r="B448" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="C448" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="C448" s="1" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="449" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9080,10 +9110,10 @@
         <v>0</v>
       </c>
       <c r="B449" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C449" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="C449" s="1" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
@@ -9091,10 +9121,10 @@
         <v>0</v>
       </c>
       <c r="B450" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C450" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="C450" s="1" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9102,10 +9132,10 @@
         <v>0</v>
       </c>
       <c r="B451" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="C451" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="C451" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
@@ -9113,10 +9143,10 @@
         <v>0</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
@@ -9124,10 +9154,10 @@
         <v>0</v>
       </c>
       <c r="B453" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C453" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="C453" s="1" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="454" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9135,10 +9165,10 @@
         <v>0</v>
       </c>
       <c r="B454" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="C454" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
@@ -9146,10 +9176,10 @@
         <v>0</v>
       </c>
       <c r="B455" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="C455" s="1" t="s">
         <v>786</v>
-      </c>
-      <c r="C455" s="1" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
@@ -9157,10 +9187,10 @@
         <v>0</v>
       </c>
       <c r="B456" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="C456" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="C456" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
@@ -9168,10 +9198,10 @@
         <v>0</v>
       </c>
       <c r="B457" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="C457" s="1" t="s">
         <v>790</v>
-      </c>
-      <c r="C457" s="1" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="458" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9179,10 +9209,10 @@
         <v>0</v>
       </c>
       <c r="B458" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C458" s="1" t="s">
         <v>792</v>
-      </c>
-      <c r="C458" s="1" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
@@ -9190,10 +9220,10 @@
         <v>0</v>
       </c>
       <c r="B459" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="C459" s="1" t="s">
         <v>794</v>
-      </c>
-      <c r="C459" s="1" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9201,10 +9231,10 @@
         <v>0</v>
       </c>
       <c r="B460" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="C460" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="C460" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -9212,10 +9242,10 @@
         <v>0</v>
       </c>
       <c r="B461" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C461" s="1" t="s">
         <v>798</v>
-      </c>
-      <c r="C461" s="1" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="462" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9223,10 +9253,10 @@
         <v>0</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C462" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
@@ -9234,10 +9264,10 @@
         <v>0</v>
       </c>
       <c r="B463" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C463" s="1" t="s">
         <v>801</v>
-      </c>
-      <c r="C463" s="1" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
@@ -9245,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>716</v>
@@ -9256,7 +9286,7 @@
         <v>0</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>532</v>
@@ -9267,10 +9297,10 @@
         <v>0</v>
       </c>
       <c r="B466" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C466" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="C466" s="1" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -9278,10 +9308,10 @@
         <v>0</v>
       </c>
       <c r="B467" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C467" s="1" t="s">
         <v>807</v>
-      </c>
-      <c r="C467" s="1" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
@@ -9289,10 +9319,10 @@
         <v>0</v>
       </c>
       <c r="B468" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="C468" s="1" t="s">
         <v>809</v>
-      </c>
-      <c r="C468" s="1" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -9300,10 +9330,10 @@
         <v>0</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
@@ -9311,7 +9341,7 @@
         <v>0</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>716</v>
@@ -9322,7 +9352,7 @@
         <v>0</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>532</v>
@@ -9333,7 +9363,7 @@
         <v>0</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>670</v>
@@ -9344,10 +9374,10 @@
         <v>0</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
@@ -9355,10 +9385,10 @@
         <v>0</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
@@ -9366,10 +9396,10 @@
         <v>0</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C475" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
@@ -9377,10 +9407,10 @@
         <v>0</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C476" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
@@ -9388,7 +9418,7 @@
         <v>0</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>696</v>
@@ -9399,10 +9429,10 @@
         <v>0</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
@@ -9410,10 +9440,10 @@
         <v>0</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C479" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
@@ -9421,10 +9451,10 @@
         <v>0</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C480" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
@@ -9432,10 +9462,10 @@
         <v>0</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C481" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
@@ -9443,10 +9473,10 @@
         <v>0</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C482" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
@@ -9454,10 +9484,10 @@
         <v>0</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C483" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
@@ -9465,10 +9495,10 @@
         <v>0</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C484" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
@@ -9476,10 +9506,10 @@
         <v>0</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
@@ -9487,10 +9517,10 @@
         <v>0</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C486" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
@@ -9498,10 +9528,10 @@
         <v>0</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C487" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
@@ -9509,10 +9539,10 @@
         <v>0</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C488" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
@@ -9520,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C489" s="1" t="s">
         <v>358</v>
@@ -9531,7 +9561,7 @@
         <v>0</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C490" s="1" t="s">
         <v>354</v>
@@ -9542,7 +9572,7 @@
         <v>0</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C491" s="1" t="s">
         <v>673</v>
@@ -9564,10 +9594,10 @@
         <v>0</v>
       </c>
       <c r="B493" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="C493" s="1" t="s">
         <v>812</v>
-      </c>
-      <c r="C493" s="1" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
@@ -9575,10 +9605,10 @@
         <v>0</v>
       </c>
       <c r="B494" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C494" s="1" t="s">
         <v>814</v>
-      </c>
-      <c r="C494" s="1" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
@@ -9586,10 +9616,10 @@
         <v>0</v>
       </c>
       <c r="B495" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C495" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="C495" s="1" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
@@ -9597,10 +9627,10 @@
         <v>0</v>
       </c>
       <c r="B496" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="C496" s="1" t="s">
         <v>845</v>
-      </c>
-      <c r="C496" s="1" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -9608,10 +9638,10 @@
         <v>0</v>
       </c>
       <c r="B497" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C497" s="1" t="s">
         <v>847</v>
-      </c>
-      <c r="C497" s="1" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
@@ -9619,10 +9649,10 @@
         <v>0</v>
       </c>
       <c r="B498" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C498" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="C498" s="1" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
@@ -9630,7 +9660,7 @@
         <v>0</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C499" s="1" t="s">
         <v>298</v>
@@ -9641,7 +9671,7 @@
         <v>0</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C500" s="1" t="s">
         <v>580</v>
@@ -9652,7 +9682,7 @@
         <v>0</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C501" s="1" t="s">
         <v>570</v>
@@ -9663,7 +9693,7 @@
         <v>0</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>582</v>
@@ -9674,7 +9704,7 @@
         <v>0</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C503" s="1" t="s">
         <v>584</v>
@@ -9685,10 +9715,10 @@
         <v>0</v>
       </c>
       <c r="B504" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C504" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="C504" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
@@ -9696,10 +9726,10 @@
         <v>0</v>
       </c>
       <c r="B505" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C505" s="1" t="s">
         <v>858</v>
-      </c>
-      <c r="C505" s="1" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
@@ -9707,10 +9737,10 @@
         <v>0</v>
       </c>
       <c r="B506" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C506" s="1" t="s">
         <v>860</v>
-      </c>
-      <c r="C506" s="1" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.25">
@@ -9718,7 +9748,7 @@
         <v>0</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C507" s="1" t="s">
         <v>49</v>
@@ -9729,7 +9759,7 @@
         <v>0</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C508" s="1" t="s">
         <v>289</v>
@@ -9740,10 +9770,10 @@
         <v>0</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>723</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
@@ -9751,7 +9781,7 @@
         <v>0</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C510" s="1" t="s">
         <v>527</v>
@@ -9762,7 +9792,7 @@
         <v>0</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C511" s="1" t="s">
         <v>527</v>
@@ -9773,10 +9803,10 @@
         <v>0</v>
       </c>
       <c r="B512" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="C512" s="1" t="s">
         <v>867</v>
-      </c>
-      <c r="C512" s="1" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
@@ -9784,10 +9814,10 @@
         <v>0</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
@@ -9795,7 +9825,7 @@
         <v>0</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>381</v>
@@ -9806,10 +9836,10 @@
         <v>0</v>
       </c>
       <c r="B515" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="C515" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="C515" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
@@ -9817,10 +9847,10 @@
         <v>0</v>
       </c>
       <c r="B516" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C516" s="1" t="s">
         <v>873</v>
-      </c>
-      <c r="C516" s="1" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
@@ -9828,7 +9858,7 @@
         <v>0</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C517" s="1" t="s">
         <v>289</v>
@@ -9839,10 +9869,10 @@
         <v>0</v>
       </c>
       <c r="B518" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C518" s="1" t="s">
         <v>876</v>
-      </c>
-      <c r="C518" s="1" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -9850,7 +9880,7 @@
         <v>0</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C519" s="1" t="s">
         <v>49</v>
@@ -9861,10 +9891,10 @@
         <v>0</v>
       </c>
       <c r="B520" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="C520" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="C520" s="1" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -9872,10 +9902,10 @@
         <v>0</v>
       </c>
       <c r="B521" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="C521" s="1" t="s">
         <v>881</v>
-      </c>
-      <c r="C521" s="1" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
@@ -9883,7 +9913,7 @@
         <v>0</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C522" s="1" t="s">
         <v>49</v>
@@ -9894,7 +9924,7 @@
         <v>0</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C523" s="1" t="s">
         <v>289</v>
@@ -9905,10 +9935,10 @@
         <v>0</v>
       </c>
       <c r="B524" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C524" s="1" t="s">
         <v>885</v>
-      </c>
-      <c r="C524" s="1" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
@@ -9916,10 +9946,10 @@
         <v>0</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
@@ -9927,10 +9957,10 @@
         <v>0</v>
       </c>
       <c r="B526" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="C526" s="1" t="s">
         <v>888</v>
-      </c>
-      <c r="C526" s="1" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
@@ -9938,10 +9968,10 @@
         <v>0</v>
       </c>
       <c r="B527" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C527" s="1" t="s">
         <v>890</v>
-      </c>
-      <c r="C527" s="1" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
@@ -9949,10 +9979,10 @@
         <v>0</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
@@ -9960,10 +9990,10 @@
         <v>0</v>
       </c>
       <c r="B529" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="C529" s="1" t="s">
         <v>893</v>
-      </c>
-      <c r="C529" s="1" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.25">
@@ -9971,10 +10001,10 @@
         <v>0</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C530" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
@@ -9982,10 +10012,10 @@
         <v>0</v>
       </c>
       <c r="B531" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C531" s="1" t="s">
         <v>896</v>
-      </c>
-      <c r="C531" s="1" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
@@ -9993,10 +10023,10 @@
         <v>0</v>
       </c>
       <c r="B532" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C532" s="1" t="s">
         <v>898</v>
-      </c>
-      <c r="C532" s="1" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
@@ -10004,10 +10034,10 @@
         <v>0</v>
       </c>
       <c r="B533" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C533" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="C533" s="1" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
@@ -10015,10 +10045,10 @@
         <v>0</v>
       </c>
       <c r="B534" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C534" s="1" t="s">
         <v>902</v>
-      </c>
-      <c r="C534" s="1" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.25">
@@ -10026,10 +10056,10 @@
         <v>0</v>
       </c>
       <c r="B535" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C535" s="1" t="s">
         <v>904</v>
-      </c>
-      <c r="C535" s="1" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.25">
@@ -10037,10 +10067,10 @@
         <v>0</v>
       </c>
       <c r="B536" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C536" s="1" t="s">
         <v>906</v>
-      </c>
-      <c r="C536" s="1" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
@@ -10048,7 +10078,7 @@
         <v>0</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C537" s="1" t="s">
         <v>527</v>
@@ -10059,10 +10089,10 @@
         <v>0</v>
       </c>
       <c r="B538" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C538" s="1" t="s">
         <v>908</v>
-      </c>
-      <c r="C538" s="1" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.25">
@@ -10070,10 +10100,10 @@
         <v>0</v>
       </c>
       <c r="B539" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="C539" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="C539" s="1" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
@@ -10081,7 +10111,7 @@
         <v>0</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C540" s="1" t="s">
         <v>448</v>
@@ -10092,7 +10122,7 @@
         <v>0</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C541" s="1" t="s">
         <v>358</v>
@@ -10103,7 +10133,7 @@
         <v>0</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C542" s="1" t="s">
         <v>354</v>
@@ -10114,7 +10144,7 @@
         <v>0</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C543" s="1" t="s">
         <v>362</v>
@@ -10125,10 +10155,10 @@
         <v>0</v>
       </c>
       <c r="B544" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C544" s="1" t="s">
         <v>916</v>
-      </c>
-      <c r="C544" s="1" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
@@ -10136,7 +10166,7 @@
         <v>0</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C545" s="1" t="s">
         <v>474</v>
@@ -10147,7 +10177,7 @@
         <v>0</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C546" s="1" t="s">
         <v>479</v>
@@ -10158,7 +10188,7 @@
         <v>0</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C547" s="1" t="s">
         <v>472</v>
@@ -10169,10 +10199,10 @@
         <v>0</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
@@ -10180,7 +10210,7 @@
         <v>0</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C549" s="1" t="s">
         <v>527</v>
@@ -10191,10 +10221,10 @@
         <v>0</v>
       </c>
       <c r="B550" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="C550" s="1" t="s">
         <v>923</v>
-      </c>
-      <c r="C550" s="1" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.25">
@@ -10202,10 +10232,10 @@
         <v>0</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
@@ -10213,10 +10243,10 @@
         <v>0</v>
       </c>
       <c r="B552" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C552" s="1" t="s">
         <v>926</v>
-      </c>
-      <c r="C552" s="1" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
@@ -10224,10 +10254,10 @@
         <v>0</v>
       </c>
       <c r="B553" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C553" s="1" t="s">
         <v>928</v>
-      </c>
-      <c r="C553" s="1" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="554" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10235,10 +10265,10 @@
         <v>0</v>
       </c>
       <c r="B554" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C554" s="1" t="s">
         <v>930</v>
-      </c>
-      <c r="C554" s="1" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.25">
@@ -10246,10 +10276,10 @@
         <v>0</v>
       </c>
       <c r="B555" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C555" s="1" t="s">
         <v>932</v>
-      </c>
-      <c r="C555" s="1" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.25">
@@ -10257,10 +10287,10 @@
         <v>0</v>
       </c>
       <c r="B556" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C556" s="1" t="s">
         <v>934</v>
-      </c>
-      <c r="C556" s="1" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.25">
@@ -10268,10 +10298,10 @@
         <v>0</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C557" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.25">
@@ -10279,10 +10309,10 @@
         <v>0</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.25">
@@ -10290,10 +10320,10 @@
         <v>0</v>
       </c>
       <c r="B559" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C559" s="1" t="s">
         <v>938</v>
-      </c>
-      <c r="C559" s="1" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.25">
@@ -10301,10 +10331,10 @@
         <v>0</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.25">
@@ -10312,10 +10342,10 @@
         <v>0</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
@@ -10323,10 +10353,10 @@
         <v>0</v>
       </c>
       <c r="B562" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C562" s="1" t="s">
         <v>940</v>
-      </c>
-      <c r="C562" s="1" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.25">
@@ -10334,10 +10364,10 @@
         <v>0</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.25">
@@ -10345,10 +10375,10 @@
         <v>0</v>
       </c>
       <c r="B564" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C564" s="1" t="s">
         <v>943</v>
-      </c>
-      <c r="C564" s="1" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
@@ -10356,10 +10386,10 @@
         <v>0</v>
       </c>
       <c r="B565" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C565" s="1" t="s">
         <v>945</v>
-      </c>
-      <c r="C565" s="1" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.25">
@@ -10367,10 +10397,10 @@
         <v>0</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C566" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="567" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10378,10 +10408,10 @@
         <v>0</v>
       </c>
       <c r="B567" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C567" s="1" t="s">
         <v>948</v>
-      </c>
-      <c r="C567" s="1" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
@@ -10389,7 +10419,7 @@
         <v>0</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C568" s="1" t="s">
         <v>642</v>
@@ -10400,10 +10430,10 @@
         <v>0</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
@@ -10411,7 +10441,7 @@
         <v>0</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>563</v>
@@ -10422,7 +10452,7 @@
         <v>0</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>645</v>
@@ -10433,7 +10463,7 @@
         <v>0</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>576</v>
@@ -10444,7 +10474,7 @@
         <v>0</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>606</v>
@@ -10455,10 +10485,10 @@
         <v>0</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
@@ -10466,10 +10496,10 @@
         <v>0</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
@@ -10477,10 +10507,10 @@
         <v>0</v>
       </c>
       <c r="B576" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C576" s="1" t="s">
         <v>958</v>
-      </c>
-      <c r="C576" s="1" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
@@ -10488,10 +10518,10 @@
         <v>0</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
@@ -10499,10 +10529,10 @@
         <v>0</v>
       </c>
       <c r="B578" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="C578" s="1" t="s">
         <v>961</v>
-      </c>
-      <c r="C578" s="1" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.25">
@@ -10510,10 +10540,10 @@
         <v>0</v>
       </c>
       <c r="B579" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="C579" s="1" t="s">
         <v>963</v>
-      </c>
-      <c r="C579" s="1" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
@@ -10521,10 +10551,10 @@
         <v>0</v>
       </c>
       <c r="B580" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="C580" s="1" t="s">
         <v>965</v>
-      </c>
-      <c r="C580" s="1" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.25">
@@ -10532,10 +10562,10 @@
         <v>0</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
@@ -10543,10 +10573,10 @@
         <v>0</v>
       </c>
       <c r="B582" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="C582" s="1" t="s">
         <v>968</v>
-      </c>
-      <c r="C582" s="1" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
@@ -10554,10 +10584,10 @@
         <v>0</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="584" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -10565,10 +10595,10 @@
         <v>0</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C584" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.25">
@@ -10576,10 +10606,10 @@
         <v>0</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.25">
@@ -10587,10 +10617,10 @@
         <v>0</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.25">
@@ -10598,10 +10628,10 @@
         <v>0</v>
       </c>
       <c r="B587" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C587" s="1" t="s">
         <v>974</v>
-      </c>
-      <c r="C587" s="1" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.25">
@@ -10609,7 +10639,7 @@
         <v>0</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C588" s="1" t="s">
         <v>381</v>
@@ -10620,7 +10650,7 @@
         <v>0</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C589" s="1" t="s">
         <v>448</v>
@@ -10631,7 +10661,7 @@
         <v>0</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C590" s="1" t="s">
         <v>358</v>
@@ -10642,7 +10672,7 @@
         <v>0</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C591" s="1" t="s">
         <v>673</v>
@@ -10653,7 +10683,7 @@
         <v>0</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>354</v>
@@ -10664,7 +10694,7 @@
         <v>0</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>362</v>
@@ -10675,10 +10705,10 @@
         <v>0</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.25">
@@ -10686,10 +10716,10 @@
         <v>0</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.25">
@@ -10697,10 +10727,10 @@
         <v>0</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.25">
@@ -10708,10 +10738,10 @@
         <v>0</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.25">
@@ -10719,10 +10749,10 @@
         <v>0</v>
       </c>
       <c r="B598" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C598" s="1" t="s">
         <v>986</v>
-      </c>
-      <c r="C598" s="1" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
@@ -10730,10 +10760,10 @@
         <v>0</v>
       </c>
       <c r="B599" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C599" s="1" t="s">
         <v>988</v>
-      </c>
-      <c r="C599" s="1" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
@@ -10741,10 +10771,10 @@
         <v>0</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.25">
@@ -10752,7 +10782,7 @@
         <v>0</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C601" s="1" t="s">
         <v>284</v>
@@ -10763,10 +10793,10 @@
         <v>0</v>
       </c>
       <c r="B602" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C602" s="1" t="s">
         <v>993</v>
-      </c>
-      <c r="C602" s="1" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.25">
@@ -10774,10 +10804,10 @@
         <v>0</v>
       </c>
       <c r="B603" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="C603" s="1" t="s">
         <v>995</v>
-      </c>
-      <c r="C603" s="1" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.25">
@@ -10785,10 +10815,10 @@
         <v>0</v>
       </c>
       <c r="B604" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C604" s="1" t="s">
         <v>997</v>
-      </c>
-      <c r="C604" s="1" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.25">
@@ -10796,10 +10826,10 @@
         <v>0</v>
       </c>
       <c r="B605" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="C605" s="1" t="s">
         <v>999</v>
-      </c>
-      <c r="C605" s="1" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="606" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10807,10 +10837,10 @@
         <v>0</v>
       </c>
       <c r="B606" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C606" s="1" t="s">
         <v>1001</v>
-      </c>
-      <c r="C606" s="1" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.25">
@@ -10818,10 +10848,10 @@
         <v>0</v>
       </c>
       <c r="B607" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C607" s="1" t="s">
         <v>1003</v>
-      </c>
-      <c r="C607" s="1" t="s">
-        <v>1004</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
@@ -10829,10 +10859,10 @@
         <v>0</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -10840,10 +10870,10 @@
         <v>0</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
@@ -10851,10 +10881,10 @@
         <v>0</v>
       </c>
       <c r="B610" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C610" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="C610" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.25">
@@ -10862,7 +10892,7 @@
         <v>0</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>358</v>
@@ -10873,7 +10903,7 @@
         <v>0</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C612" s="1" t="s">
         <v>688</v>
@@ -10884,7 +10914,7 @@
         <v>0</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C613" s="1" t="s">
         <v>673</v>
@@ -10895,7 +10925,7 @@
         <v>0</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C614" s="1" t="s">
         <v>354</v>
@@ -10906,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C615" s="1" t="s">
         <v>366</v>
@@ -10917,10 +10947,10 @@
         <v>0</v>
       </c>
       <c r="B616" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C616" s="1" t="s">
         <v>1015</v>
-      </c>
-      <c r="C616" s="1" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="617" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10928,10 +10958,10 @@
         <v>0</v>
       </c>
       <c r="B617" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C617" s="1" t="s">
         <v>1017</v>
-      </c>
-      <c r="C617" s="1" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
@@ -10939,10 +10969,10 @@
         <v>0</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.25">
@@ -10950,7 +10980,7 @@
         <v>0</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C619" s="1" t="s">
         <v>119</v>
@@ -10961,7 +10991,7 @@
         <v>0</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C620" s="1" t="s">
         <v>532</v>
@@ -10972,10 +11002,10 @@
         <v>0</v>
       </c>
       <c r="B621" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C621" s="1" t="s">
         <v>1022</v>
-      </c>
-      <c r="C621" s="1" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
@@ -10983,10 +11013,10 @@
         <v>0</v>
       </c>
       <c r="B622" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C622" s="1" t="s">
         <v>1024</v>
-      </c>
-      <c r="C622" s="1" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
@@ -10994,10 +11024,10 @@
         <v>0</v>
       </c>
       <c r="B623" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C623" s="1" t="s">
         <v>1026</v>
-      </c>
-      <c r="C623" s="1" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
@@ -11005,10 +11035,10 @@
         <v>0</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C624" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.25">
@@ -11016,7 +11046,7 @@
         <v>0</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C625" s="1" t="s">
         <v>289</v>
@@ -11027,7 +11057,7 @@
         <v>0</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C626" s="1" t="s">
         <v>580</v>
@@ -11038,10 +11068,10 @@
         <v>0</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C627" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="628" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -11049,10 +11079,10 @@
         <v>0</v>
       </c>
       <c r="B628" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C628" s="1" t="s">
         <v>1034</v>
-      </c>
-      <c r="C628" s="1" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.25">
@@ -11060,10 +11090,10 @@
         <v>0</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C629" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.25">
@@ -11071,10 +11101,10 @@
         <v>0</v>
       </c>
       <c r="B630" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C630" s="1" t="s">
         <v>1037</v>
-      </c>
-      <c r="C630" s="1" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.25">
@@ -11082,10 +11112,10 @@
         <v>0</v>
       </c>
       <c r="B631" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C631" s="1" t="s">
         <v>1039</v>
-      </c>
-      <c r="C631" s="1" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
@@ -11093,10 +11123,10 @@
         <v>0</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>1042</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.25">
@@ -11104,10 +11134,10 @@
         <v>0</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>1044</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.25">
@@ -11115,10 +11145,10 @@
         <v>0</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.25">
@@ -11126,7 +11156,7 @@
         <v>0</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="C635" s="1" t="s">
         <v>366</v>
@@ -11137,7 +11167,7 @@
         <v>0</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="C636" s="1" t="s">
         <v>366</v>
@@ -11148,7 +11178,7 @@
         <v>0</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="C637" s="1" t="s">
         <v>580</v>
@@ -11159,10 +11189,10 @@
         <v>0</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.25">
@@ -11170,10 +11200,10 @@
         <v>0</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.25">
@@ -11181,7 +11211,7 @@
         <v>0</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="C640" s="1" t="s">
         <v>503</v>
@@ -11192,10 +11222,10 @@
         <v>0</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.25">
@@ -11203,7 +11233,7 @@
         <v>0</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="C642" s="1" t="s">
         <v>422</v>
@@ -11214,10 +11244,10 @@
         <v>0</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.25">
@@ -11225,10 +11255,10 @@
         <v>0</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.25">
@@ -11236,10 +11266,10 @@
         <v>0</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.25">
@@ -11247,7 +11277,7 @@
         <v>0</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C646" s="1" t="s">
         <v>432</v>
@@ -11258,10 +11288,10 @@
         <v>0</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.25">
@@ -11269,10 +11299,10 @@
         <v>0</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
@@ -11283,7 +11313,7 @@
         <v>425</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.25">
@@ -11291,10 +11321,10 @@
         <v>0</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
@@ -11302,10 +11332,10 @@
         <v>0</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -11313,10 +11343,10 @@
         <v>0</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.25">
@@ -11324,10 +11354,10 @@
         <v>0</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.25">
@@ -11335,10 +11365,10 @@
         <v>0</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.25">
@@ -11346,10 +11376,10 @@
         <v>0</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.25">
@@ -11357,10 +11387,10 @@
         <v>0</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.25">
@@ -11368,10 +11398,10 @@
         <v>0</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.25">
@@ -11379,7 +11409,7 @@
         <v>0</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="C658" s="1" t="s">
         <v>432</v>
@@ -11390,10 +11420,10 @@
         <v>0</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.25">
@@ -11401,10 +11431,10 @@
         <v>0</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.25">
@@ -11412,10 +11442,10 @@
         <v>0</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.25">
@@ -11423,7 +11453,7 @@
         <v>0</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="C662" s="1" t="s">
         <v>289</v>
@@ -11434,10 +11464,10 @@
         <v>0</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.25">
@@ -11445,10 +11475,10 @@
         <v>0</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -11456,10 +11486,10 @@
         <v>0</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
@@ -11467,10 +11497,10 @@
         <v>0</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -11478,10 +11508,10 @@
         <v>0</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.25">
@@ -11489,10 +11519,10 @@
         <v>0</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
@@ -11500,10 +11530,10 @@
         <v>0</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
@@ -11511,10 +11541,10 @@
         <v>0</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="671" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -11522,10 +11552,10 @@
         <v>0</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.25">
@@ -11533,10 +11563,10 @@
         <v>0</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.25">
@@ -11544,10 +11574,10 @@
         <v>0</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -11555,10 +11585,10 @@
         <v>0</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.25">
@@ -11566,10 +11596,10 @@
         <v>0</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
@@ -11577,7 +11607,7 @@
         <v>0</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="C676" s="1" t="s">
         <v>358</v>
@@ -11588,7 +11618,7 @@
         <v>0</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>366</v>
@@ -11599,7 +11629,7 @@
         <v>0</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>673</v>
@@ -11610,7 +11640,7 @@
         <v>0</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="C679" s="1" t="s">
         <v>549</v>
@@ -11621,10 +11651,10 @@
         <v>0</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="681" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -11632,10 +11662,10 @@
         <v>0</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
@@ -11643,10 +11673,10 @@
         <v>0</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.25">
@@ -11654,10 +11684,10 @@
         <v>0</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
@@ -11665,7 +11695,7 @@
         <v>0</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C684" s="1" t="s">
         <v>673</v>
@@ -11676,10 +11706,10 @@
         <v>0</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
@@ -11687,7 +11717,7 @@
         <v>0</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>354</v>
@@ -11698,10 +11728,10 @@
         <v>0</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
@@ -11709,10 +11739,10 @@
         <v>0</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
@@ -11720,10 +11750,10 @@
         <v>0</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="690" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -11731,10 +11761,10 @@
         <v>0</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -11742,10 +11772,10 @@
         <v>0</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
@@ -11753,7 +11783,7 @@
         <v>0</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>204</v>
@@ -11764,10 +11794,10 @@
         <v>0</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="694" spans="1:3" x14ac:dyDescent="0.25">
@@ -11775,10 +11805,10 @@
         <v>0</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
@@ -11786,10 +11816,10 @@
         <v>0</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.25">
@@ -11797,10 +11827,10 @@
         <v>0</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="697" spans="1:3" x14ac:dyDescent="0.25">
@@ -11808,10 +11838,10 @@
         <v>0</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="698" spans="1:3" x14ac:dyDescent="0.25">
@@ -11819,10 +11849,10 @@
         <v>0</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="699" spans="1:3" x14ac:dyDescent="0.25">
@@ -11830,10 +11860,10 @@
         <v>0</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.25">
@@ -11841,10 +11871,10 @@
         <v>0</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.25">
@@ -11852,10 +11882,10 @@
         <v>0</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.25">
@@ -11863,10 +11893,10 @@
         <v>0</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.25">
@@ -11874,10 +11904,10 @@
         <v>0</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.25">
@@ -11885,7 +11915,7 @@
         <v>0</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="C704" s="1" t="s">
         <v>289</v>
@@ -11896,10 +11926,10 @@
         <v>0</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.25">
@@ -11907,10 +11937,10 @@
         <v>0</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.25">
@@ -11918,10 +11948,10 @@
         <v>0</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.25">
@@ -11929,10 +11959,10 @@
         <v>0</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.25">
@@ -11940,10 +11970,10 @@
         <v>0</v>
       </c>
       <c r="B709" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C709" s="1" t="s">
         <v>1155</v>
-      </c>
-      <c r="C709" s="1" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.25">
@@ -11951,10 +11981,10 @@
         <v>0</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.25">
@@ -11962,10 +11992,10 @@
         <v>0</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.25">
@@ -11973,10 +12003,10 @@
         <v>0</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="C712" s="1" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.25">
@@ -11984,7 +12014,7 @@
         <v>0</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="C713" s="1" t="s">
         <v>489</v>
@@ -11995,10 +12025,10 @@
         <v>0</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.25">
@@ -12006,7 +12036,7 @@
         <v>0</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>591</v>
@@ -12017,10 +12047,10 @@
         <v>0</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.25">
@@ -12028,10 +12058,10 @@
         <v>0</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.25">
@@ -12039,10 +12069,10 @@
         <v>0</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="719" spans="1:3" x14ac:dyDescent="0.25">
@@ -12050,10 +12080,10 @@
         <v>0</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="720" spans="1:3" x14ac:dyDescent="0.25">
@@ -12061,10 +12091,10 @@
         <v>0</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="721" spans="1:3" x14ac:dyDescent="0.25">
@@ -12072,10 +12102,10 @@
         <v>0</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.25">
@@ -12083,10 +12113,10 @@
         <v>0</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="C722" s="1" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="723" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -12094,10 +12124,10 @@
         <v>0</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="C723" s="1" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.25">
@@ -12105,10 +12135,10 @@
         <v>0</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="C724" s="1" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.25">
@@ -12116,10 +12146,10 @@
         <v>0</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="C725" s="1" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="726" spans="1:3" x14ac:dyDescent="0.25">
@@ -12127,7 +12157,7 @@
         <v>0</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>298</v>
@@ -12138,7 +12168,7 @@
         <v>0</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>642</v>
@@ -12149,10 +12179,10 @@
         <v>0</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="C728" s="1" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.25">
@@ -12160,10 +12190,10 @@
         <v>0</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="C729" s="1" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.25">
@@ -12171,7 +12201,7 @@
         <v>0</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="C730" s="1" t="s">
         <v>381</v>
@@ -12182,7 +12212,7 @@
         <v>0</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>642</v>
@@ -12193,10 +12223,10 @@
         <v>0</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="C732" s="1" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.25">
@@ -12204,10 +12234,10 @@
         <v>0</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.25">
@@ -12215,7 +12245,7 @@
         <v>0</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>289</v>
@@ -12226,10 +12256,10 @@
         <v>0</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.25">
@@ -12237,10 +12267,10 @@
         <v>0</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.25">
@@ -12248,10 +12278,10 @@
         <v>0</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
@@ -12259,10 +12289,10 @@
         <v>0</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.25">
@@ -12270,7 +12300,7 @@
         <v>0</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="C739" s="1" t="s">
         <v>606</v>
@@ -12281,10 +12311,10 @@
         <v>0</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.25">
@@ -12292,10 +12322,10 @@
         <v>0</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="742" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -12303,10 +12333,10 @@
         <v>0</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.25">
@@ -12314,10 +12344,10 @@
         <v>0</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.25">
@@ -12325,10 +12355,10 @@
         <v>0</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.25">
@@ -12336,7 +12366,7 @@
         <v>0</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="C745" s="1" t="s">
         <v>366</v>
@@ -12347,10 +12377,10 @@
         <v>0</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.25">
@@ -12358,10 +12388,10 @@
         <v>0</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.25">
@@ -12369,7 +12399,7 @@
         <v>0</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="C748" s="1" t="s">
         <v>528</v>
@@ -12380,10 +12410,10 @@
         <v>0</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.25">
@@ -12391,7 +12421,7 @@
         <v>0</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="C750" s="1" t="s">
         <v>532</v>
@@ -12402,7 +12432,7 @@
         <v>0</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="C751" s="1" t="s">
         <v>580</v>
@@ -12413,10 +12443,10 @@
         <v>0</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.25">
@@ -12424,10 +12454,10 @@
         <v>0</v>
       </c>
       <c r="B753" s="1" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="C753" s="1" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.25">
@@ -12435,10 +12465,10 @@
         <v>0</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
@@ -12446,10 +12476,10 @@
         <v>0</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
@@ -12457,10 +12487,10 @@
         <v>0</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
@@ -12468,10 +12498,10 @@
         <v>0</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="C757" s="1" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.25">
@@ -12479,10 +12509,10 @@
         <v>0</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.25">
@@ -12490,10 +12520,10 @@
         <v>0</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.25">
@@ -12501,10 +12531,10 @@
         <v>0</v>
       </c>
       <c r="B760" s="1" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
@@ -12512,10 +12542,10 @@
         <v>0</v>
       </c>
       <c r="B761" s="1" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="C761" s="1" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
@@ -12523,10 +12553,10 @@
         <v>0</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
@@ -12534,10 +12564,10 @@
         <v>0</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.25">
@@ -12545,10 +12575,10 @@
         <v>0</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
@@ -12556,10 +12586,10 @@
         <v>0</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.25">
@@ -12567,10 +12597,10 @@
         <v>0</v>
       </c>
       <c r="B766" s="1" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
@@ -12578,10 +12608,10 @@
         <v>0</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
@@ -12589,10 +12619,10 @@
         <v>0</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
@@ -12600,10 +12630,98 @@
         <v>0</v>
       </c>
       <c r="B769" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C769" s="1" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="770" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A770" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B770" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C770" s="1" t="s">
         <v>1245</v>
       </c>
-      <c r="C769" s="1" t="s">
+    </row>
+    <row r="771" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A771" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B771" s="1" t="s">
         <v>1246</v>
+      </c>
+      <c r="C771" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="772" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A772" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B772" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C772" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="773" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A773" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B773" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C773" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="774" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A774" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B774" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C774" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="775" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A775" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B775" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C775" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="776" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A776" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B776" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C776" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="777" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A777" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B777" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C777" s="1" t="s">
+        <v>805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved UI, a lot
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347457D-74B9-4BCD-B1F1-0672DDCFDC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37B33A0-0B57-4D0D-9A97-18727560A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="1293">
   <si>
     <t>cs</t>
   </si>
@@ -3801,6 +3801,114 @@
   </si>
   <si>
     <t>lab.mixture.table.rating</t>
+  </si>
+  <si>
+    <t>lab.mixture.preview.vendor</t>
+  </si>
+  <si>
+    <t>lab.mixture.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.list.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.create.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.edit.label</t>
+  </si>
+  <si>
+    <t>lab.mixture.index.label</t>
+  </si>
+  <si>
+    <t>Editace</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Seznam</t>
+  </si>
+  <si>
+    <t>Nový</t>
+  </si>
+  <si>
+    <t>lab.build.label</t>
+  </si>
+  <si>
+    <t>lab.build.list.label</t>
+  </si>
+  <si>
+    <t>lab.build.create.label</t>
+  </si>
+  <si>
+    <t>lab.build.clone.label</t>
+  </si>
+  <si>
+    <t>Klon</t>
+  </si>
+  <si>
+    <t>lab.build.index.label</t>
+  </si>
+  <si>
+    <t>lab.build.edit.label</t>
+  </si>
+  <si>
+    <t>lab.vape.label</t>
+  </si>
+  <si>
+    <t>Vapy</t>
+  </si>
+  <si>
+    <t>lab.vape.list.label</t>
+  </si>
+  <si>
+    <t>lab.vape.create.label</t>
+  </si>
+  <si>
+    <t>lab.vape.index.label</t>
+  </si>
+  <si>
+    <t>lab.vape.clone.label</t>
+  </si>
+  <si>
+    <t>lab.vape.edit.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.list.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.edit.label</t>
+  </si>
+  <si>
+    <t>lab.liquid.index.label</t>
+  </si>
+  <si>
+    <t>lab.coil.label</t>
+  </si>
+  <si>
+    <t>lab.coil.list.label</t>
+  </si>
+  <si>
+    <t>lab.coil.create.label</t>
+  </si>
+  <si>
+    <t>Nová</t>
+  </si>
+  <si>
+    <t>lab.coil.index.label</t>
+  </si>
+  <si>
+    <t>lab.coil.edit.label</t>
+  </si>
+  <si>
+    <t>lab.coil.clone.label</t>
   </si>
 </sst>
 </file>
@@ -4164,10 +4272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C777"/>
+  <dimension ref="A1:C806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A766" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B773" sqref="B773"/>
+    <sheetView tabSelected="1" topLeftCell="A790" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B798" sqref="B798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12722,6 +12830,325 @@
       </c>
       <c r="C777" s="1" t="s">
         <v>805</v>
+      </c>
+    </row>
+    <row r="778" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A778" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B778" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C778" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="779" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A779" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B779" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C779" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="780" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A780" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B780" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C780" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="781" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A781" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B781" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C781" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="782" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A782" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B782" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C782" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="783" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A783" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B783" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C783" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="784" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A784" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B784" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C784" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="785" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A785" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B785" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C785" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A786" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B786" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C786" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="787" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A787" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B787" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C787" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="788" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A788" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B788" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C788" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="789" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A789" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B789" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C789" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A790" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B790" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C790" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="791" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A791" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B791" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C791" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="792" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A792" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B792" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C792" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="793" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A793" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B793" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C793" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="794" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A794" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B794" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C794" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="795" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A795" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C795" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A796" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B796" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C796" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="797" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A797" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B797" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C797" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="798" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A798" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B798" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C798" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="799" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A799" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B799" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C799" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="800" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A800" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B800" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C800" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A801" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B801" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C801" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A802" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B802" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C802" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A803" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B803" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C803" s="1" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="804" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A804" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B804" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C804" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A805" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B805" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C805" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A806" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B806" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C806" s="1" t="s">
+        <v>1271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added external rating for vapes
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37B33A0-0B57-4D0D-9A97-18727560A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932CD130-FA4B-4C33-B5A0-D9C2F87424F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="6840" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="8205" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1306">
   <si>
     <t>cs</t>
   </si>
@@ -2165,9 +2165,6 @@
     <t>lab.build.create.success</t>
   </si>
   <si>
-    <t>Build [{{data.name}}] byl vytvořen.</t>
-  </si>
-  <si>
     <t>lab.driptip.name.label.tooltip</t>
   </si>
   <si>
@@ -2660,9 +2657,6 @@
     <t>lab.build.update.success</t>
   </si>
   <si>
-    <t>Build [{{data.name}}] byl aktualizován.</t>
-  </si>
-  <si>
     <t>lab.build.link.button</t>
   </si>
   <si>
@@ -3035,15 +3029,9 @@
     <t>lab.build.deactivated.success</t>
   </si>
   <si>
-    <t>Build [{{data.name}}] byl deaktivován; přestane se nabízet v různých nabídkách napříč aplikací.</t>
-  </si>
-  <si>
     <t>lab.build.activated.success</t>
   </si>
   <si>
-    <t>Build [{{data.name}}] byl aktivován; bude se opět nabízet v nabídkách napříč aplikací.</t>
-  </si>
-  <si>
     <t>lab.vape.filter.title</t>
   </si>
   <si>
@@ -3909,6 +3897,57 @@
   </si>
   <si>
     <t>lab.coil.clone.label</t>
+  </si>
+  <si>
+    <t>lab.vape.rate.button</t>
+  </si>
+  <si>
+    <t>Hodnocení vapu</t>
+  </si>
+  <si>
+    <t>lab.vape.rate.submit</t>
+  </si>
+  <si>
+    <t>Uložit hodnocení</t>
+  </si>
+  <si>
+    <t>lab.vape.rate.update.success</t>
+  </si>
+  <si>
+    <t>Hodnocení vapu bylo uloženo.</t>
+  </si>
+  <si>
+    <t>Build byl vytvořen.</t>
+  </si>
+  <si>
+    <t>Build byl aktualizován.</t>
+  </si>
+  <si>
+    <t>Build byl deaktivován; přestane se nabízet v různých nabídkách napříč aplikací.</t>
+  </si>
+  <si>
+    <t>Build byl aktivován; bude se opět nabízet v nabídkách napříč aplikací.</t>
+  </si>
+  <si>
+    <t>lab.vape.rate.label</t>
+  </si>
+  <si>
+    <t>lab.vape.unrated.unrated</t>
+  </si>
+  <si>
+    <t>Neohodnoceno</t>
+  </si>
+  <si>
+    <t>lab.vape.unrated.rated</t>
+  </si>
+  <si>
+    <t>S hodnocením</t>
+  </si>
+  <si>
+    <t>lab.vape.unrated.all</t>
+  </si>
+  <si>
+    <t>Všechny</t>
   </si>
 </sst>
 </file>
@@ -4272,10 +4311,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C806"/>
+  <dimension ref="A1:C813"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A790" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B798" sqref="B798"/>
+    <sheetView tabSelected="1" topLeftCell="A796" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B811" sqref="B811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7516,7 +7555,7 @@
         <v>521</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -8814,7 +8853,7 @@
         <v>710</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>711</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -8822,10 +8861,10 @@
         <v>0</v>
       </c>
       <c r="B413" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C413" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="C413" s="1" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -8833,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C414" s="1" t="s">
         <v>18</v>
@@ -8844,10 +8883,10 @@
         <v>0</v>
       </c>
       <c r="B415" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="C415" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="C415" s="1" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
@@ -8855,10 +8894,10 @@
         <v>0</v>
       </c>
       <c r="B416" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C416" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="C416" s="1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -8866,7 +8905,7 @@
         <v>0</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C417" s="1" t="s">
         <v>665</v>
@@ -8877,7 +8916,7 @@
         <v>0</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>532</v>
@@ -8888,7 +8927,7 @@
         <v>0</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>587</v>
@@ -8899,7 +8938,7 @@
         <v>0</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>589</v>
@@ -8910,10 +8949,10 @@
         <v>0</v>
       </c>
       <c r="B421" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C421" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="C421" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
@@ -8921,7 +8960,7 @@
         <v>0</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>670</v>
@@ -8932,7 +8971,7 @@
         <v>0</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>381</v>
@@ -8943,10 +8982,10 @@
         <v>0</v>
       </c>
       <c r="B424" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C424" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="C424" s="1" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -8954,7 +8993,7 @@
         <v>0</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>119</v>
@@ -8965,10 +9004,10 @@
         <v>0</v>
       </c>
       <c r="B426" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="C426" s="1" t="s">
         <v>730</v>
-      </c>
-      <c r="C426" s="1" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -8976,10 +9015,10 @@
         <v>0</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -8987,10 +9026,10 @@
         <v>0</v>
       </c>
       <c r="B428" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="C428" s="1" t="s">
         <v>733</v>
-      </c>
-      <c r="C428" s="1" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -8998,10 +9037,10 @@
         <v>0</v>
       </c>
       <c r="B429" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C429" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="C429" s="1" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9009,10 +9048,10 @@
         <v>0</v>
       </c>
       <c r="B430" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="C430" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="C430" s="1" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -9020,10 +9059,10 @@
         <v>0</v>
       </c>
       <c r="B431" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="C431" s="1" t="s">
         <v>739</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -9031,10 +9070,10 @@
         <v>0</v>
       </c>
       <c r="B432" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C432" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="C432" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9042,10 +9081,10 @@
         <v>0</v>
       </c>
       <c r="B433" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C433" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="C433" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -9053,10 +9092,10 @@
         <v>0</v>
       </c>
       <c r="B434" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C434" s="1" t="s">
         <v>745</v>
-      </c>
-      <c r="C434" s="1" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
@@ -9064,10 +9103,10 @@
         <v>0</v>
       </c>
       <c r="B435" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="C435" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="C435" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
@@ -9075,10 +9114,10 @@
         <v>0</v>
       </c>
       <c r="B436" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="C436" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
@@ -9086,10 +9125,10 @@
         <v>0</v>
       </c>
       <c r="B437" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="C437" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="C437" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -9097,10 +9136,10 @@
         <v>0</v>
       </c>
       <c r="B438" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C438" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="439" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9108,10 +9147,10 @@
         <v>0</v>
       </c>
       <c r="B439" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="C439" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="C439" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
@@ -9119,10 +9158,10 @@
         <v>0</v>
       </c>
       <c r="B440" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C440" s="1" t="s">
         <v>757</v>
-      </c>
-      <c r="C440" s="1" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9130,10 +9169,10 @@
         <v>0</v>
       </c>
       <c r="B441" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C441" s="1" t="s">
         <v>759</v>
-      </c>
-      <c r="C441" s="1" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
@@ -9141,10 +9180,10 @@
         <v>0</v>
       </c>
       <c r="B442" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="C442" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="C442" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
@@ -9152,7 +9191,7 @@
         <v>0</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>114</v>
@@ -9163,10 +9202,10 @@
         <v>0</v>
       </c>
       <c r="B444" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C444" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="C444" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
@@ -9174,10 +9213,10 @@
         <v>0</v>
       </c>
       <c r="B445" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C445" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -9185,10 +9224,10 @@
         <v>0</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C446" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9196,10 +9235,10 @@
         <v>0</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C447" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -9207,10 +9246,10 @@
         <v>0</v>
       </c>
       <c r="B448" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="C448" s="1" t="s">
         <v>772</v>
-      </c>
-      <c r="C448" s="1" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="449" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9218,10 +9257,10 @@
         <v>0</v>
       </c>
       <c r="B449" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="C449" s="1" t="s">
         <v>774</v>
-      </c>
-      <c r="C449" s="1" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
@@ -9229,10 +9268,10 @@
         <v>0</v>
       </c>
       <c r="B450" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="C450" s="1" t="s">
         <v>776</v>
-      </c>
-      <c r="C450" s="1" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9240,10 +9279,10 @@
         <v>0</v>
       </c>
       <c r="B451" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C451" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="C451" s="1" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
@@ -9251,10 +9290,10 @@
         <v>0</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
@@ -9262,10 +9301,10 @@
         <v>0</v>
       </c>
       <c r="B453" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C453" s="1" t="s">
         <v>781</v>
-      </c>
-      <c r="C453" s="1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="454" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9273,10 +9312,10 @@
         <v>0</v>
       </c>
       <c r="B454" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="C454" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
@@ -9284,10 +9323,10 @@
         <v>0</v>
       </c>
       <c r="B455" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="C455" s="1" t="s">
         <v>785</v>
-      </c>
-      <c r="C455" s="1" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
@@ -9295,10 +9334,10 @@
         <v>0</v>
       </c>
       <c r="B456" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="C456" s="1" t="s">
         <v>787</v>
-      </c>
-      <c r="C456" s="1" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
@@ -9306,10 +9345,10 @@
         <v>0</v>
       </c>
       <c r="B457" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="C457" s="1" t="s">
         <v>789</v>
-      </c>
-      <c r="C457" s="1" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="458" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -9317,10 +9356,10 @@
         <v>0</v>
       </c>
       <c r="B458" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="C458" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="C458" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
@@ -9328,10 +9367,10 @@
         <v>0</v>
       </c>
       <c r="B459" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C459" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="C459" s="1" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9339,10 +9378,10 @@
         <v>0</v>
       </c>
       <c r="B460" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C460" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="C460" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -9350,10 +9389,10 @@
         <v>0</v>
       </c>
       <c r="B461" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C461" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="C461" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="462" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -9361,10 +9400,10 @@
         <v>0</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C462" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
@@ -9372,10 +9411,10 @@
         <v>0</v>
       </c>
       <c r="B463" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="C463" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="C463" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
@@ -9383,10 +9422,10 @@
         <v>0</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C464" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
@@ -9394,7 +9433,7 @@
         <v>0</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>532</v>
@@ -9405,10 +9444,10 @@
         <v>0</v>
       </c>
       <c r="B466" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="C466" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="C466" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -9416,10 +9455,10 @@
         <v>0</v>
       </c>
       <c r="B467" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C467" s="1" t="s">
         <v>806</v>
-      </c>
-      <c r="C467" s="1" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
@@ -9427,10 +9466,10 @@
         <v>0</v>
       </c>
       <c r="B468" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C468" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="C468" s="1" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -9438,10 +9477,10 @@
         <v>0</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
@@ -9449,10 +9488,10 @@
         <v>0</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C470" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
@@ -9460,7 +9499,7 @@
         <v>0</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>532</v>
@@ -9471,7 +9510,7 @@
         <v>0</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>670</v>
@@ -9482,10 +9521,10 @@
         <v>0</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
@@ -9493,10 +9532,10 @@
         <v>0</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
@@ -9504,10 +9543,10 @@
         <v>0</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C475" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
@@ -9515,10 +9554,10 @@
         <v>0</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C476" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
@@ -9526,7 +9565,7 @@
         <v>0</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>696</v>
@@ -9537,10 +9576,10 @@
         <v>0</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
@@ -9548,10 +9587,10 @@
         <v>0</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C479" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
@@ -9559,10 +9598,10 @@
         <v>0</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C480" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
@@ -9570,10 +9609,10 @@
         <v>0</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C481" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
@@ -9581,10 +9620,10 @@
         <v>0</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C482" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
@@ -9592,10 +9631,10 @@
         <v>0</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C483" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
@@ -9603,10 +9642,10 @@
         <v>0</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C484" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
@@ -9614,10 +9653,10 @@
         <v>0</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
@@ -9625,10 +9664,10 @@
         <v>0</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C486" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
@@ -9636,10 +9675,10 @@
         <v>0</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C487" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
@@ -9647,10 +9686,10 @@
         <v>0</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C488" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
@@ -9658,7 +9697,7 @@
         <v>0</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C489" s="1" t="s">
         <v>358</v>
@@ -9669,7 +9708,7 @@
         <v>0</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C490" s="1" t="s">
         <v>354</v>
@@ -9680,7 +9719,7 @@
         <v>0</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C491" s="1" t="s">
         <v>673</v>
@@ -9702,10 +9741,10 @@
         <v>0</v>
       </c>
       <c r="B493" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C493" s="1" t="s">
         <v>811</v>
-      </c>
-      <c r="C493" s="1" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
@@ -9713,10 +9752,10 @@
         <v>0</v>
       </c>
       <c r="B494" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="C494" s="1" t="s">
         <v>813</v>
-      </c>
-      <c r="C494" s="1" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
@@ -9724,10 +9763,10 @@
         <v>0</v>
       </c>
       <c r="B495" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C495" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="C495" s="1" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
@@ -9735,10 +9774,10 @@
         <v>0</v>
       </c>
       <c r="B496" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C496" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="C496" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -9746,10 +9785,10 @@
         <v>0</v>
       </c>
       <c r="B497" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C497" s="1" t="s">
         <v>846</v>
-      </c>
-      <c r="C497" s="1" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
@@ -9757,10 +9796,10 @@
         <v>0</v>
       </c>
       <c r="B498" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C498" s="1" t="s">
         <v>848</v>
-      </c>
-      <c r="C498" s="1" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
@@ -9768,7 +9807,7 @@
         <v>0</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C499" s="1" t="s">
         <v>298</v>
@@ -9779,7 +9818,7 @@
         <v>0</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C500" s="1" t="s">
         <v>580</v>
@@ -9790,7 +9829,7 @@
         <v>0</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C501" s="1" t="s">
         <v>570</v>
@@ -9801,7 +9840,7 @@
         <v>0</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>582</v>
@@ -9812,7 +9851,7 @@
         <v>0</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C503" s="1" t="s">
         <v>584</v>
@@ -9823,10 +9862,10 @@
         <v>0</v>
       </c>
       <c r="B504" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C504" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="C504" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
@@ -9834,10 +9873,10 @@
         <v>0</v>
       </c>
       <c r="B505" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="C505" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="C505" s="1" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
@@ -9845,10 +9884,10 @@
         <v>0</v>
       </c>
       <c r="B506" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C506" s="1" t="s">
         <v>859</v>
-      </c>
-      <c r="C506" s="1" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.25">
@@ -9856,7 +9895,7 @@
         <v>0</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C507" s="1" t="s">
         <v>49</v>
@@ -9867,7 +9906,7 @@
         <v>0</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C508" s="1" t="s">
         <v>289</v>
@@ -9878,10 +9917,10 @@
         <v>0</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
@@ -9889,7 +9928,7 @@
         <v>0</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C510" s="1" t="s">
         <v>527</v>
@@ -9900,7 +9939,7 @@
         <v>0</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C511" s="1" t="s">
         <v>527</v>
@@ -9911,10 +9950,10 @@
         <v>0</v>
       </c>
       <c r="B512" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C512" s="1" t="s">
         <v>866</v>
-      </c>
-      <c r="C512" s="1" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
@@ -9922,10 +9961,10 @@
         <v>0</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
@@ -9933,7 +9972,7 @@
         <v>0</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>381</v>
@@ -9944,10 +9983,10 @@
         <v>0</v>
       </c>
       <c r="B515" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C515" s="1" t="s">
         <v>870</v>
-      </c>
-      <c r="C515" s="1" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
@@ -9955,10 +9994,10 @@
         <v>0</v>
       </c>
       <c r="B516" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C516" s="1" t="s">
         <v>872</v>
-      </c>
-      <c r="C516" s="1" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
@@ -9966,7 +10005,7 @@
         <v>0</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C517" s="1" t="s">
         <v>289</v>
@@ -9977,10 +10016,10 @@
         <v>0</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>876</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -9988,7 +10027,7 @@
         <v>0</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C519" s="1" t="s">
         <v>49</v>
@@ -9999,10 +10038,10 @@
         <v>0</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -10010,10 +10049,10 @@
         <v>0</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
@@ -10021,7 +10060,7 @@
         <v>0</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C522" s="1" t="s">
         <v>49</v>
@@ -10032,7 +10071,7 @@
         <v>0</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C523" s="1" t="s">
         <v>289</v>
@@ -10043,10 +10082,10 @@
         <v>0</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
@@ -10054,10 +10093,10 @@
         <v>0</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
@@ -10065,10 +10104,10 @@
         <v>0</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C526" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
@@ -10076,10 +10115,10 @@
         <v>0</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C527" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
@@ -10087,10 +10126,10 @@
         <v>0</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
@@ -10098,10 +10137,10 @@
         <v>0</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.25">
@@ -10109,10 +10148,10 @@
         <v>0</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C530" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
@@ -10120,10 +10159,10 @@
         <v>0</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
@@ -10131,10 +10170,10 @@
         <v>0</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C532" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
@@ -10142,10 +10181,10 @@
         <v>0</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C533" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
@@ -10153,10 +10192,10 @@
         <v>0</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C534" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.25">
@@ -10164,10 +10203,10 @@
         <v>0</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.25">
@@ -10175,10 +10214,10 @@
         <v>0</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
@@ -10186,7 +10225,7 @@
         <v>0</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C537" s="1" t="s">
         <v>527</v>
@@ -10197,10 +10236,10 @@
         <v>0</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C538" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.25">
@@ -10208,10 +10247,10 @@
         <v>0</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
@@ -10219,7 +10258,7 @@
         <v>0</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C540" s="1" t="s">
         <v>448</v>
@@ -10230,7 +10269,7 @@
         <v>0</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C541" s="1" t="s">
         <v>358</v>
@@ -10241,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C542" s="1" t="s">
         <v>354</v>
@@ -10252,7 +10291,7 @@
         <v>0</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C543" s="1" t="s">
         <v>362</v>
@@ -10263,10 +10302,10 @@
         <v>0</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
@@ -10274,7 +10313,7 @@
         <v>0</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C545" s="1" t="s">
         <v>474</v>
@@ -10285,7 +10324,7 @@
         <v>0</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C546" s="1" t="s">
         <v>479</v>
@@ -10296,7 +10335,7 @@
         <v>0</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C547" s="1" t="s">
         <v>472</v>
@@ -10307,10 +10346,10 @@
         <v>0</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
@@ -10318,7 +10357,7 @@
         <v>0</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C549" s="1" t="s">
         <v>527</v>
@@ -10329,10 +10368,10 @@
         <v>0</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C550" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.25">
@@ -10340,10 +10379,10 @@
         <v>0</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
@@ -10351,10 +10390,10 @@
         <v>0</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
@@ -10362,10 +10401,10 @@
         <v>0</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C553" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="554" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10373,10 +10412,10 @@
         <v>0</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C554" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.25">
@@ -10384,10 +10423,10 @@
         <v>0</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.25">
@@ -10395,10 +10434,10 @@
         <v>0</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C556" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.25">
@@ -10406,10 +10445,10 @@
         <v>0</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C557" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.25">
@@ -10417,10 +10456,10 @@
         <v>0</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.25">
@@ -10428,10 +10467,10 @@
         <v>0</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.25">
@@ -10439,10 +10478,10 @@
         <v>0</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.25">
@@ -10450,10 +10489,10 @@
         <v>0</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
@@ -10461,10 +10500,10 @@
         <v>0</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.25">
@@ -10472,10 +10511,10 @@
         <v>0</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.25">
@@ -10483,10 +10522,10 @@
         <v>0</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C564" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
@@ -10494,10 +10533,10 @@
         <v>0</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C565" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.25">
@@ -10505,10 +10544,10 @@
         <v>0</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C566" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="567" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -10516,10 +10555,10 @@
         <v>0</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C567" s="1" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
@@ -10527,7 +10566,7 @@
         <v>0</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C568" s="1" t="s">
         <v>642</v>
@@ -10538,10 +10577,10 @@
         <v>0</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
@@ -10549,7 +10588,7 @@
         <v>0</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>563</v>
@@ -10560,7 +10599,7 @@
         <v>0</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>645</v>
@@ -10571,7 +10610,7 @@
         <v>0</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>576</v>
@@ -10582,7 +10621,7 @@
         <v>0</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>606</v>
@@ -10593,10 +10632,10 @@
         <v>0</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
@@ -10604,10 +10643,10 @@
         <v>0</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
@@ -10615,10 +10654,10 @@
         <v>0</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
@@ -10626,10 +10665,10 @@
         <v>0</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
@@ -10637,10 +10676,10 @@
         <v>0</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.25">
@@ -10648,10 +10687,10 @@
         <v>0</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
@@ -10659,10 +10698,10 @@
         <v>0</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C580" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.25">
@@ -10670,10 +10709,10 @@
         <v>0</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
@@ -10681,10 +10720,10 @@
         <v>0</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
@@ -10692,10 +10731,10 @@
         <v>0</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="584" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -10703,10 +10742,10 @@
         <v>0</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C584" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.25">
@@ -10714,10 +10753,10 @@
         <v>0</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.25">
@@ -10725,10 +10764,10 @@
         <v>0</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.25">
@@ -10736,10 +10775,10 @@
         <v>0</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="588" spans="1:3" x14ac:dyDescent="0.25">
@@ -10747,7 +10786,7 @@
         <v>0</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C588" s="1" t="s">
         <v>381</v>
@@ -10758,7 +10797,7 @@
         <v>0</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C589" s="1" t="s">
         <v>448</v>
@@ -10769,7 +10808,7 @@
         <v>0</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C590" s="1" t="s">
         <v>358</v>
@@ -10780,7 +10819,7 @@
         <v>0</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C591" s="1" t="s">
         <v>673</v>
@@ -10791,7 +10830,7 @@
         <v>0</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>354</v>
@@ -10802,7 +10841,7 @@
         <v>0</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>362</v>
@@ -10813,10 +10852,10 @@
         <v>0</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.25">
@@ -10824,10 +10863,10 @@
         <v>0</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.25">
@@ -10835,10 +10874,10 @@
         <v>0</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.25">
@@ -10846,10 +10885,10 @@
         <v>0</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.25">
@@ -10857,10 +10896,10 @@
         <v>0</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
@@ -10868,10 +10907,10 @@
         <v>0</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
@@ -10879,10 +10918,10 @@
         <v>0</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.25">
@@ -10890,7 +10929,7 @@
         <v>0</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C601" s="1" t="s">
         <v>284</v>
@@ -10901,10 +10940,10 @@
         <v>0</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.25">
@@ -10912,10 +10951,10 @@
         <v>0</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.25">
@@ -10923,10 +10962,10 @@
         <v>0</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C604" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.25">
@@ -10934,21 +10973,21 @@
         <v>0</v>
       </c>
       <c r="B605" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A606" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B606" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="C605" s="1" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="606" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A606" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B606" s="1" t="s">
-        <v>1000</v>
-      </c>
       <c r="C606" s="1" t="s">
-        <v>1001</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.25">
@@ -10956,10 +10995,10 @@
         <v>0</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>1003</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
@@ -10967,10 +11006,10 @@
         <v>0</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -10978,10 +11017,10 @@
         <v>0</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
@@ -10989,10 +11028,10 @@
         <v>0</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="C610" s="1" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.25">
@@ -11000,7 +11039,7 @@
         <v>0</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>358</v>
@@ -11011,7 +11050,7 @@
         <v>0</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="C612" s="1" t="s">
         <v>688</v>
@@ -11022,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="C613" s="1" t="s">
         <v>673</v>
@@ -11033,7 +11072,7 @@
         <v>0</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="C614" s="1" t="s">
         <v>354</v>
@@ -11044,7 +11083,7 @@
         <v>0</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="C615" s="1" t="s">
         <v>366</v>
@@ -11055,10 +11094,10 @@
         <v>0</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="617" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -11066,10 +11105,10 @@
         <v>0</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="C617" s="1" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
@@ -11077,10 +11116,10 @@
         <v>0</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.25">
@@ -11088,7 +11127,7 @@
         <v>0</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="C619" s="1" t="s">
         <v>119</v>
@@ -11099,7 +11138,7 @@
         <v>0</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="C620" s="1" t="s">
         <v>532</v>
@@ -11110,10 +11149,10 @@
         <v>0</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
@@ -11121,10 +11160,10 @@
         <v>0</v>
       </c>
       <c r="B622" s="1" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
@@ -11132,10 +11171,10 @@
         <v>0</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
@@ -11143,10 +11182,10 @@
         <v>0</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="C624" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.25">
@@ -11154,7 +11193,7 @@
         <v>0</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="C625" s="1" t="s">
         <v>289</v>
@@ -11165,7 +11204,7 @@
         <v>0</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="C626" s="1" t="s">
         <v>580</v>
@@ -11176,10 +11215,10 @@
         <v>0</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="C627" s="1" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="628" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -11187,10 +11226,10 @@
         <v>0</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="C628" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.25">
@@ -11198,10 +11237,10 @@
         <v>0</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="C629" s="1" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.25">
@@ -11209,10 +11248,10 @@
         <v>0</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="C630" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.25">
@@ -11220,10 +11259,10 @@
         <v>0</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
@@ -11231,10 +11270,10 @@
         <v>0</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.25">
@@ -11242,10 +11281,10 @@
         <v>0</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.25">
@@ -11253,10 +11292,10 @@
         <v>0</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.25">
@@ -11264,7 +11303,7 @@
         <v>0</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="C635" s="1" t="s">
         <v>366</v>
@@ -11275,7 +11314,7 @@
         <v>0</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="C636" s="1" t="s">
         <v>366</v>
@@ -11286,7 +11325,7 @@
         <v>0</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="C637" s="1" t="s">
         <v>580</v>
@@ -11297,10 +11336,10 @@
         <v>0</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.25">
@@ -11308,10 +11347,10 @@
         <v>0</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.25">
@@ -11319,7 +11358,7 @@
         <v>0</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="C640" s="1" t="s">
         <v>503</v>
@@ -11330,10 +11369,10 @@
         <v>0</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.25">
@@ -11341,7 +11380,7 @@
         <v>0</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="C642" s="1" t="s">
         <v>422</v>
@@ -11352,10 +11391,10 @@
         <v>0</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.25">
@@ -11363,10 +11402,10 @@
         <v>0</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.25">
@@ -11374,10 +11413,10 @@
         <v>0</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.25">
@@ -11385,7 +11424,7 @@
         <v>0</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="C646" s="1" t="s">
         <v>432</v>
@@ -11396,10 +11435,10 @@
         <v>0</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.25">
@@ -11407,10 +11446,10 @@
         <v>0</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
@@ -11421,7 +11460,7 @@
         <v>425</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.25">
@@ -11429,10 +11468,10 @@
         <v>0</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
@@ -11440,10 +11479,10 @@
         <v>0</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
@@ -11451,10 +11490,10 @@
         <v>0</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.25">
@@ -11462,10 +11501,10 @@
         <v>0</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.25">
@@ -11473,10 +11512,10 @@
         <v>0</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.25">
@@ -11484,10 +11523,10 @@
         <v>0</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.25">
@@ -11495,10 +11534,10 @@
         <v>0</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.25">
@@ -11506,10 +11545,10 @@
         <v>0</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.25">
@@ -11517,7 +11556,7 @@
         <v>0</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="C658" s="1" t="s">
         <v>432</v>
@@ -11528,10 +11567,10 @@
         <v>0</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.25">
@@ -11539,10 +11578,10 @@
         <v>0</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.25">
@@ -11550,10 +11589,10 @@
         <v>0</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.25">
@@ -11561,7 +11600,7 @@
         <v>0</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="C662" s="1" t="s">
         <v>289</v>
@@ -11572,10 +11611,10 @@
         <v>0</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.25">
@@ -11583,10 +11622,10 @@
         <v>0</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
@@ -11594,10 +11633,10 @@
         <v>0</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
@@ -11605,10 +11644,10 @@
         <v>0</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
@@ -11616,10 +11655,10 @@
         <v>0</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.25">
@@ -11627,10 +11666,10 @@
         <v>0</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
@@ -11638,10 +11677,10 @@
         <v>0</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
@@ -11649,10 +11688,10 @@
         <v>0</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="671" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -11660,10 +11699,10 @@
         <v>0</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.25">
@@ -11671,10 +11710,10 @@
         <v>0</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.25">
@@ -11682,10 +11721,10 @@
         <v>0</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -11693,10 +11732,10 @@
         <v>0</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.25">
@@ -11704,10 +11743,10 @@
         <v>0</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
@@ -11715,7 +11754,7 @@
         <v>0</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C676" s="1" t="s">
         <v>358</v>
@@ -11726,7 +11765,7 @@
         <v>0</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>366</v>
@@ -11737,7 +11776,7 @@
         <v>0</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>673</v>
@@ -11748,7 +11787,7 @@
         <v>0</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="C679" s="1" t="s">
         <v>549</v>
@@ -11759,10 +11798,10 @@
         <v>0</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="681" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -11770,10 +11809,10 @@
         <v>0</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
@@ -11781,10 +11820,10 @@
         <v>0</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.25">
@@ -11792,10 +11831,10 @@
         <v>0</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
@@ -11803,7 +11842,7 @@
         <v>0</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C684" s="1" t="s">
         <v>673</v>
@@ -11814,10 +11853,10 @@
         <v>0</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
@@ -11825,7 +11864,7 @@
         <v>0</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>354</v>
@@ -11836,10 +11875,10 @@
         <v>0</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
@@ -11847,10 +11886,10 @@
         <v>0</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
@@ -11858,10 +11897,10 @@
         <v>0</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="690" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -11869,10 +11908,10 @@
         <v>0</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
@@ -11880,10 +11919,10 @@
         <v>0</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="C691" s="1" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
@@ -11891,7 +11930,7 @@
         <v>0</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>204</v>
@@ -11902,10 +11941,10 @@
         <v>0</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="694" spans="1:3" x14ac:dyDescent="0.25">
@@ -11913,10 +11952,10 @@
         <v>0</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
@@ -11924,10 +11963,10 @@
         <v>0</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.25">
@@ -11935,10 +11974,10 @@
         <v>0</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="697" spans="1:3" x14ac:dyDescent="0.25">
@@ -11946,10 +11985,10 @@
         <v>0</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="698" spans="1:3" x14ac:dyDescent="0.25">
@@ -11957,10 +11996,10 @@
         <v>0</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="699" spans="1:3" x14ac:dyDescent="0.25">
@@ -11968,10 +12007,10 @@
         <v>0</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.25">
@@ -11979,10 +12018,10 @@
         <v>0</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.25">
@@ -11990,10 +12029,10 @@
         <v>0</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.25">
@@ -12001,10 +12040,10 @@
         <v>0</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.25">
@@ -12012,10 +12051,10 @@
         <v>0</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.25">
@@ -12023,7 +12062,7 @@
         <v>0</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="C704" s="1" t="s">
         <v>289</v>
@@ -12034,10 +12073,10 @@
         <v>0</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.25">
@@ -12045,10 +12084,10 @@
         <v>0</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.25">
@@ -12056,10 +12095,10 @@
         <v>0</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.25">
@@ -12067,10 +12106,10 @@
         <v>0</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.25">
@@ -12078,10 +12117,10 @@
         <v>0</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="C709" s="1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.25">
@@ -12089,10 +12128,10 @@
         <v>0</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.25">
@@ -12100,10 +12139,10 @@
         <v>0</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.25">
@@ -12111,10 +12150,10 @@
         <v>0</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="C712" s="1" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.25">
@@ -12122,7 +12161,7 @@
         <v>0</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="C713" s="1" t="s">
         <v>489</v>
@@ -12133,10 +12172,10 @@
         <v>0</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.25">
@@ -12144,7 +12183,7 @@
         <v>0</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>591</v>
@@ -12155,10 +12194,10 @@
         <v>0</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.25">
@@ -12166,10 +12205,10 @@
         <v>0</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.25">
@@ -12177,10 +12216,10 @@
         <v>0</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="719" spans="1:3" x14ac:dyDescent="0.25">
@@ -12188,10 +12227,10 @@
         <v>0</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="720" spans="1:3" x14ac:dyDescent="0.25">
@@ -12199,10 +12238,10 @@
         <v>0</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="721" spans="1:3" x14ac:dyDescent="0.25">
@@ -12210,10 +12249,10 @@
         <v>0</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="C721" s="1" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.25">
@@ -12221,10 +12260,10 @@
         <v>0</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="C722" s="1" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="723" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -12232,10 +12271,10 @@
         <v>0</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="C723" s="1" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.25">
@@ -12243,10 +12282,10 @@
         <v>0</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="C724" s="1" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.25">
@@ -12254,10 +12293,10 @@
         <v>0</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="C725" s="1" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="726" spans="1:3" x14ac:dyDescent="0.25">
@@ -12265,7 +12304,7 @@
         <v>0</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>298</v>
@@ -12276,7 +12315,7 @@
         <v>0</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>642</v>
@@ -12287,10 +12326,10 @@
         <v>0</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C728" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.25">
@@ -12298,10 +12337,10 @@
         <v>0</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="C729" s="1" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.25">
@@ -12309,7 +12348,7 @@
         <v>0</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="C730" s="1" t="s">
         <v>381</v>
@@ -12320,7 +12359,7 @@
         <v>0</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>642</v>
@@ -12331,10 +12370,10 @@
         <v>0</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="C732" s="1" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.25">
@@ -12342,10 +12381,10 @@
         <v>0</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.25">
@@ -12353,7 +12392,7 @@
         <v>0</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>289</v>
@@ -12364,10 +12403,10 @@
         <v>0</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.25">
@@ -12375,10 +12414,10 @@
         <v>0</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.25">
@@ -12386,10 +12425,10 @@
         <v>0</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="C737" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
@@ -12397,10 +12436,10 @@
         <v>0</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="C738" s="1" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.25">
@@ -12408,7 +12447,7 @@
         <v>0</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="C739" s="1" t="s">
         <v>606</v>
@@ -12419,10 +12458,10 @@
         <v>0</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C740" s="1" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.25">
@@ -12430,10 +12469,10 @@
         <v>0</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="C741" s="1" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="742" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -12441,10 +12480,10 @@
         <v>0</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="C742" s="1" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.25">
@@ -12452,10 +12491,10 @@
         <v>0</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="C743" s="1" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.25">
@@ -12463,10 +12502,10 @@
         <v>0</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.25">
@@ -12474,7 +12513,7 @@
         <v>0</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="C745" s="1" t="s">
         <v>366</v>
@@ -12485,10 +12524,10 @@
         <v>0</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.25">
@@ -12496,10 +12535,10 @@
         <v>0</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.25">
@@ -12507,7 +12546,7 @@
         <v>0</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C748" s="1" t="s">
         <v>528</v>
@@ -12518,10 +12557,10 @@
         <v>0</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.25">
@@ -12529,7 +12568,7 @@
         <v>0</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="C750" s="1" t="s">
         <v>532</v>
@@ -12540,7 +12579,7 @@
         <v>0</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="C751" s="1" t="s">
         <v>580</v>
@@ -12551,10 +12590,10 @@
         <v>0</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.25">
@@ -12562,10 +12601,10 @@
         <v>0</v>
       </c>
       <c r="B753" s="1" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="C753" s="1" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.25">
@@ -12573,10 +12612,10 @@
         <v>0</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C754" s="1" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
@@ -12584,10 +12623,10 @@
         <v>0</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="C755" s="1" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
@@ -12595,10 +12634,10 @@
         <v>0</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="C756" s="1" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
@@ -12606,10 +12645,10 @@
         <v>0</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="C757" s="1" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.25">
@@ -12617,10 +12656,10 @@
         <v>0</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="C758" s="1" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.25">
@@ -12628,10 +12667,10 @@
         <v>0</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="C759" s="1" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.25">
@@ -12639,10 +12678,10 @@
         <v>0</v>
       </c>
       <c r="B760" s="1" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="C760" s="1" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
@@ -12650,10 +12689,10 @@
         <v>0</v>
       </c>
       <c r="B761" s="1" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="C761" s="1" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
@@ -12661,10 +12700,10 @@
         <v>0</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
@@ -12672,10 +12711,10 @@
         <v>0</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.25">
@@ -12683,10 +12722,10 @@
         <v>0</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
@@ -12694,10 +12733,10 @@
         <v>0</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.25">
@@ -12705,10 +12744,10 @@
         <v>0</v>
       </c>
       <c r="B766" s="1" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
@@ -12716,10 +12755,10 @@
         <v>0</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
@@ -12727,10 +12766,10 @@
         <v>0</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
@@ -12738,10 +12777,10 @@
         <v>0</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C769" s="1" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
@@ -12749,10 +12788,10 @@
         <v>0</v>
       </c>
       <c r="B770" s="1" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="C770" s="1" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.25">
@@ -12760,10 +12799,10 @@
         <v>0</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="C771" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.25">
@@ -12771,7 +12810,7 @@
         <v>0</v>
       </c>
       <c r="B772" s="1" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="C772" s="1" t="s">
         <v>393</v>
@@ -12782,10 +12821,10 @@
         <v>0</v>
       </c>
       <c r="B773" s="1" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
@@ -12793,7 +12832,7 @@
         <v>0</v>
       </c>
       <c r="B774" s="1" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="C774" s="1" t="s">
         <v>559</v>
@@ -12804,10 +12843,10 @@
         <v>0</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="C775" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="776" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -12815,10 +12854,10 @@
         <v>0</v>
       </c>
       <c r="B776" s="1" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="C776" s="1" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
@@ -12826,10 +12865,10 @@
         <v>0</v>
       </c>
       <c r="B777" s="1" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="C777" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
@@ -12837,7 +12876,7 @@
         <v>0</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="C778" s="1" t="s">
         <v>393</v>
@@ -12848,7 +12887,7 @@
         <v>0</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="C779" s="1" t="s">
         <v>534</v>
@@ -12859,10 +12898,10 @@
         <v>0</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
@@ -12870,10 +12909,10 @@
         <v>0</v>
       </c>
       <c r="B781" s="1" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
       <c r="C781" s="1" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
@@ -12881,10 +12920,10 @@
         <v>0</v>
       </c>
       <c r="B782" s="1" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.25">
@@ -12892,10 +12931,10 @@
         <v>0</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="C783" s="1" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
@@ -12903,7 +12942,7 @@
         <v>0</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="C784" s="1" t="s">
         <v>241</v>
@@ -12914,10 +12953,10 @@
         <v>0</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="C785" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.25">
@@ -12925,10 +12964,10 @@
         <v>0</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="C786" s="1" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
@@ -12936,10 +12975,10 @@
         <v>0</v>
       </c>
       <c r="B787" s="1" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="C787" s="1" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
@@ -12947,7 +12986,7 @@
         <v>0</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="C788" s="1" t="s">
         <v>366</v>
@@ -12958,10 +12997,10 @@
         <v>0</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="C789" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.25">
@@ -12969,10 +13008,10 @@
         <v>0</v>
       </c>
       <c r="B790" s="1" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="C790" s="1" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.25">
@@ -12980,10 +13019,10 @@
         <v>0</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="C791" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
@@ -12991,10 +13030,10 @@
         <v>0</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="C792" s="1" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
@@ -13002,7 +13041,7 @@
         <v>0</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="C793" s="1" t="s">
         <v>528</v>
@@ -13013,10 +13052,10 @@
         <v>0</v>
       </c>
       <c r="B794" s="1" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="C794" s="1" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
@@ -13024,10 +13063,10 @@
         <v>0</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.25">
@@ -13035,7 +13074,7 @@
         <v>0</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>489</v>
@@ -13046,10 +13085,10 @@
         <v>0</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.25">
@@ -13057,10 +13096,10 @@
         <v>0</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
@@ -13068,7 +13107,7 @@
         <v>0</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>580</v>
@@ -13079,10 +13118,10 @@
         <v>0</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
@@ -13090,7 +13129,7 @@
         <v>0</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>503</v>
@@ -13101,10 +13140,10 @@
         <v>0</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.25">
@@ -13112,10 +13151,10 @@
         <v>0</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="C803" s="1" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
@@ -13123,7 +13162,7 @@
         <v>0</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>354</v>
@@ -13134,10 +13173,10 @@
         <v>0</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="C805" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="806" spans="1:3" x14ac:dyDescent="0.25">
@@ -13145,10 +13184,87 @@
         <v>0</v>
       </c>
       <c r="B806" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C806" s="1" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A807" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B807" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C807" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A808" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B808" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C808" s="1" t="s">
         <v>1292</v>
       </c>
-      <c r="C806" s="1" t="s">
-        <v>1271</v>
+    </row>
+    <row r="809" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A809" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B809" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C809" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A810" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B810" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C810" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A811" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B811" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C811" s="1" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A812" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B812" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C812" s="1" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A813" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B813" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C813" s="1" t="s">
+        <v>1305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Experiment with graphs
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932CD130-FA4B-4C33-B5A0-D9C2F87424F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882C07E9-C2D9-4D00-A2E9-22044DA6D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="705" yWindow="8205" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="1308">
   <si>
     <t>cs</t>
   </si>
@@ -3948,6 +3948,12 @@
   </si>
   <si>
     <t>Všechny</t>
+  </si>
+  <si>
+    <t>lab.build.graph.tab</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -4311,10 +4317,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C813"/>
+  <dimension ref="A1:C814"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A796" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B811" sqref="B811"/>
+      <selection activeCell="B807" sqref="B807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13265,6 +13271,17 @@
       </c>
       <c r="C813" s="1" t="s">
         <v>1305</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A814" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B814" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C814" s="1" t="s">
+        <v>1307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some experiments with graphs
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882C07E9-C2D9-4D00-A2E9-22044DA6D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6C8E3C-43A8-4484-A353-4153B7D5AF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="8205" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2505" uniqueCount="1332">
   <si>
     <t>cs</t>
   </si>
@@ -3954,6 +3954,78 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.min.label</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.max.label</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.average.label</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.median.label</t>
+  </si>
+  <si>
+    <t>Nejhorší</t>
+  </si>
+  <si>
+    <t>Nejlepší</t>
+  </si>
+  <si>
+    <t>Průměr</t>
+  </si>
+  <si>
+    <t>Medián</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.count.label</t>
+  </si>
+  <si>
+    <t>Počet hodnocení</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.rating.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.taste.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.fruits.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.complex.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.tobacco.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.fresh.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.mtl.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.dl.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.throathit.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.cakes.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.clouds.column</t>
+  </si>
+  <si>
+    <t>Mraky</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.title</t>
+  </si>
+  <si>
+    <t>Přehled hodnocení vapování</t>
   </si>
 </sst>
 </file>
@@ -4317,10 +4389,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C814"/>
+  <dimension ref="A1:C831"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A796" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B807" sqref="B807"/>
+    <sheetView tabSelected="1" topLeftCell="A808" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B825" sqref="B825"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13282,6 +13354,193 @@
       </c>
       <c r="C814" s="1" t="s">
         <v>1307</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A815" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B815" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C815" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A816" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B816" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C816" s="1" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A817" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B817" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C817" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A818" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B818" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C818" s="1" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A819" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B819" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C819" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A820" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B820" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C820" s="1" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A821" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B821" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C821" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A822" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B822" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C822" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A823" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B823" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C823" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A824" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B824" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C824" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A825" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B825" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C825" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A826" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B826" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C826" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A827" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B827" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C827" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A828" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B828" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C828" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A829" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B829" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C829" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A830" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B830" s="1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C830" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A831" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B831" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C831" s="1" t="s">
+        <v>1331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A lot of small improvements
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6C8E3C-43A8-4484-A353-4153B7D5AF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCAA7AA-0856-496C-A6C4-77724F6889F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2505" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="1335">
   <si>
     <t>cs</t>
   </si>
@@ -3950,12 +3950,6 @@
     <t>Všechny</t>
   </si>
   <si>
-    <t>lab.build.graph.tab</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>lab.vape.plot.min.label</t>
   </si>
   <si>
@@ -4026,6 +4020,21 @@
   </si>
   <si>
     <t>Přehled hodnocení vapování</t>
+  </si>
+  <si>
+    <t>lab.build.vape.plot.tab</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.no-data.title</t>
+  </si>
+  <si>
+    <t>Nejsou dostupná žádná data o vapování</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.no-data.subtitle</t>
+  </si>
+  <si>
+    <t>Pokud chcete sledovat tyto velice zajímavé údaje, vytvořte prosím zážitek z vapování s tímto buildem a přidejte k němu hodnocení.</t>
   </si>
 </sst>
 </file>
@@ -4389,10 +4398,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C831"/>
+  <dimension ref="A1:C833"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A808" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B825" sqref="B825"/>
+      <selection activeCell="C833" sqref="C833"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13350,10 +13359,10 @@
         <v>0</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>1306</v>
+        <v>1330</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>1307</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.25">
@@ -13361,10 +13370,10 @@
         <v>0</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.25">
@@ -13372,10 +13381,10 @@
         <v>0</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.25">
@@ -13383,10 +13392,10 @@
         <v>0</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.25">
@@ -13394,10 +13403,10 @@
         <v>0</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.25">
@@ -13405,10 +13414,10 @@
         <v>0</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.25">
@@ -13416,7 +13425,7 @@
         <v>0</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C820" s="1" t="s">
         <v>730</v>
@@ -13427,7 +13436,7 @@
         <v>0</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C821" s="1" t="s">
         <v>806</v>
@@ -13438,7 +13447,7 @@
         <v>0</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C822" s="1" t="s">
         <v>741</v>
@@ -13449,7 +13458,7 @@
         <v>0</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>753</v>
@@ -13460,7 +13469,7 @@
         <v>0</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>745</v>
@@ -13471,7 +13480,7 @@
         <v>0</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C825" s="1" t="s">
         <v>757</v>
@@ -13482,7 +13491,7 @@
         <v>0</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>835</v>
@@ -13493,7 +13502,7 @@
         <v>0</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C827" s="1" t="s">
         <v>836</v>
@@ -13504,7 +13513,7 @@
         <v>0</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="C828" s="1" t="s">
         <v>943</v>
@@ -13515,7 +13524,7 @@
         <v>0</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C829" s="1" t="s">
         <v>749</v>
@@ -13526,10 +13535,10 @@
         <v>0</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.25">
@@ -13537,10 +13546,32 @@
         <v>0</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="C831" s="1" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A832" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B832" s="1" t="s">
         <v>1331</v>
+      </c>
+      <c r="C832" s="1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A833" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B833" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C833" s="1" t="s">
+        <v>1334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So finished first quite nice upgrade of the UI, filtering, graphs and so
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCAA7AA-0856-496C-A6C4-77724F6889F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC0B264-54C3-4F8F-B9EB-8CF81C0A36A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="1335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1338">
   <si>
     <t>cs</t>
   </si>
@@ -4035,6 +4035,15 @@
   </si>
   <si>
     <t>Pokud chcete sledovat tyto velice zajímavé údaje, vytvořte prosím zážitek z vapování s tímto buildem a přidejte k němu hodnocení.</t>
+  </si>
+  <si>
+    <t>lab.mixture.vape.plot.tab</t>
+  </si>
+  <si>
+    <t>Hodnocení vapování</t>
+  </si>
+  <si>
+    <t>lab.liquid.vape.plot.tab</t>
   </si>
 </sst>
 </file>
@@ -4398,10 +4407,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C833"/>
+  <dimension ref="A1:C835"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A808" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C833" sqref="C833"/>
+    <sheetView tabSelected="1" topLeftCell="A814" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B832" sqref="B832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13572,6 +13581,28 @@
       </c>
       <c r="C833" s="1" t="s">
         <v>1334</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A834" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B834" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C834" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A835" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B835" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C835" s="1" t="s">
+        <v>1336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved internal stuff a lot
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50671D40-A99A-470E-9738-897287B44B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6BB7FE-42E9-4194-AD8E-42788A6C9446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="1349">
   <si>
     <t>cs</t>
   </si>
@@ -4071,6 +4071,12 @@
   </si>
   <si>
     <t>Počet vapů [{{data.total}}]</t>
+  </si>
+  <si>
+    <t>lab.build.table.footer.label</t>
+  </si>
+  <si>
+    <t>Počet buildů [{{data.total}}]</t>
   </si>
 </sst>
 </file>
@@ -4434,10 +4440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C840"/>
+  <dimension ref="A1:C841"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A823" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C840" sqref="C840"/>
+      <selection activeCell="B836" sqref="B836"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13685,6 +13691,17 @@
       </c>
       <c r="C840" s="1" t="s">
         <v>1346</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A841" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C841" s="1" t="s">
+        <v>1348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite an improvement
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B444427-5328-4AD3-BAA8-982B8BC21F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D10EAE-B9DF-45F4-AB74-339E890BD063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="1369">
   <si>
     <t>cs</t>
   </si>
@@ -4125,6 +4125,18 @@
   </si>
   <si>
     <t>lab.liquid.button.plot</t>
+  </si>
+  <si>
+    <t>lab.build.comments.build.tab</t>
+  </si>
+  <si>
+    <t>Komentáře k buildu</t>
+  </si>
+  <si>
+    <t>lab.build.comments.vape.tab</t>
+  </si>
+  <si>
+    <t>Komentáře k vapování</t>
   </si>
 </sst>
 </file>
@@ -4488,10 +4500,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C852"/>
+  <dimension ref="A1:C854"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A829" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B843" sqref="B843"/>
+      <selection activeCell="B844" sqref="B844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13871,6 +13883,28 @@
       </c>
       <c r="C852" s="1" t="s">
         <v>1335</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A853" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B853" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C853" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A854" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B854" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C854" s="1" t="s">
+        <v>1368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added vape plot
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D10EAE-B9DF-45F4-AB74-339E890BD063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC305D-72BD-4D78-B293-A7FE3047AF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="1371">
   <si>
     <t>cs</t>
   </si>
@@ -4137,6 +4137,12 @@
   </si>
   <si>
     <t>Komentáře k vapování</t>
+  </si>
+  <si>
+    <t>lab.vape.button.plot</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.label</t>
   </si>
 </sst>
 </file>
@@ -4500,10 +4506,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C854"/>
+  <dimension ref="A1:C856"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A829" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B844" sqref="B844"/>
+    <sheetView tabSelected="1" topLeftCell="A838" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C856" sqref="C856"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13905,6 +13911,28 @@
       </c>
       <c r="C854" s="1" t="s">
         <v>1368</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A855" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B855" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C855" s="1" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A856" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B856" s="1" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C856" s="1" t="s">
+        <v>1343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Experimental improvement of the forms
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC305D-72BD-4D78-B293-A7FE3047AF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CAEC4-7CB3-4147-B46F-E26E493DE828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="1371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1403">
   <si>
     <t>cs</t>
   </si>
@@ -4143,6 +4143,102 @@
   </si>
   <si>
     <t>lab.vape.plot.label</t>
+  </si>
+  <si>
+    <t>lab.build.coilOffset.-2</t>
+  </si>
+  <si>
+    <t>Nejníže</t>
+  </si>
+  <si>
+    <t>lab.build.coilOffset.-1</t>
+  </si>
+  <si>
+    <t>Níže</t>
+  </si>
+  <si>
+    <t>lab.build.coilOffset.0</t>
+  </si>
+  <si>
+    <t>Střed</t>
+  </si>
+  <si>
+    <t>lab.build.coilOffset.1</t>
+  </si>
+  <si>
+    <t>Výše</t>
+  </si>
+  <si>
+    <t>lab.build.coilOffset.2</t>
+  </si>
+  <si>
+    <t>Nejvýše</t>
+  </si>
+  <si>
+    <t>lab.build.cottonOffset.-2</t>
+  </si>
+  <si>
+    <t>Méně</t>
+  </si>
+  <si>
+    <t>lab.build.cottonOffset.-1</t>
+  </si>
+  <si>
+    <t>Nejméně</t>
+  </si>
+  <si>
+    <t>lab.build.cottonOffset.0</t>
+  </si>
+  <si>
+    <t>Akorát</t>
+  </si>
+  <si>
+    <t>lab.build.cottonOffset.1</t>
+  </si>
+  <si>
+    <t>Více</t>
+  </si>
+  <si>
+    <t>lab.build.cottonOffset.2</t>
+  </si>
+  <si>
+    <t>Nejvíce</t>
+  </si>
+  <si>
+    <t>lab.build.glow.1</t>
+  </si>
+  <si>
+    <t>Pomalé</t>
+  </si>
+  <si>
+    <t>lab.build.glow.2</t>
+  </si>
+  <si>
+    <t>Střední</t>
+  </si>
+  <si>
+    <t>lab.build.glow.3</t>
+  </si>
+  <si>
+    <t>Běžné</t>
+  </si>
+  <si>
+    <t>lab.build.glow.4</t>
+  </si>
+  <si>
+    <t>Rychlé</t>
+  </si>
+  <si>
+    <t>lab.build.glow.5</t>
+  </si>
+  <si>
+    <t>Velmi rychlé</t>
+  </si>
+  <si>
+    <t>lab.build.preview.glow</t>
+  </si>
+  <si>
+    <t>Rychlost žhavení</t>
   </si>
 </sst>
 </file>
@@ -4506,10 +4602,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C856"/>
+  <dimension ref="A1:C872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A838" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C856" sqref="C856"/>
+    <sheetView tabSelected="1" topLeftCell="A853" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B863" sqref="B863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13933,6 +14029,182 @@
       </c>
       <c r="C856" s="1" t="s">
         <v>1343</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A857" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B857" s="1" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C857" s="1" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A858" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B858" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C858" s="1" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A859" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B859" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C859" s="1" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A860" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B860" s="1" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C860" s="1" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A861" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B861" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C861" s="1" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A862" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B862" s="1" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C862" s="1" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A863" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B863" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C863" s="1" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A864" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B864" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C864" s="1" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A865" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B865" s="1" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C865" s="1" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A866" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B866" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C866" s="1" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A867" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B867" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C867" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A868" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B868" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C868" s="1" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A869" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B869" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C869" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A870" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B870" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C870" s="1" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A871" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B871" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C871" s="1" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A872" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B872" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C872" s="1" t="s">
+        <v>1402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So improved build section
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CAEC4-7CB3-4147-B46F-E26E493DE828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F469285A-7303-46C0-9D1A-4D6CAFA9CDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1411">
   <si>
     <t>cs</t>
   </si>
@@ -4239,6 +4239,30 @@
   </si>
   <si>
     <t>Rychlost žhavení</t>
+  </si>
+  <si>
+    <t>lab.build.coilCount.1</t>
+  </si>
+  <si>
+    <t>Jedna</t>
+  </si>
+  <si>
+    <t>Dvě</t>
+  </si>
+  <si>
+    <t>Tři</t>
+  </si>
+  <si>
+    <t>Čtyři</t>
+  </si>
+  <si>
+    <t>lab.build.coilCount.4</t>
+  </si>
+  <si>
+    <t>lab.build.coilCount.3</t>
+  </si>
+  <si>
+    <t>lab.build.coilCount.2</t>
   </si>
 </sst>
 </file>
@@ -4602,10 +4626,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C872"/>
+  <dimension ref="A1:C876"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A853" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B863" sqref="B863"/>
+      <selection activeCell="B866" sqref="B866"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14205,6 +14229,50 @@
       </c>
       <c r="C872" s="1" t="s">
         <v>1402</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A873" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B873" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C873" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A874" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B874" s="1" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C874" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="875" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A875" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B875" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C875" s="1" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="876" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A876" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B876" s="1" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C876" s="1" t="s">
+        <v>1407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Still improving form stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F469285A-7303-46C0-9D1A-4D6CAFA9CDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CF964-310F-498E-854C-0229D2540FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="1438">
   <si>
     <t>cs</t>
   </si>
@@ -4263,6 +4263,87 @@
   </si>
   <si>
     <t>lab.build.coilCount.2</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.0</t>
+  </si>
+  <si>
+    <t>Žádné</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.1</t>
+  </si>
+  <si>
+    <t>Drobné</t>
+  </si>
+  <si>
+    <t>Větší</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.2</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.3</t>
+  </si>
+  <si>
+    <t>Totální</t>
+  </si>
+  <si>
+    <t>lab.vape.leaks.4</t>
+  </si>
+  <si>
+    <t>Občasné</t>
+  </si>
+  <si>
+    <t>lab.vape.dryhit.0</t>
+  </si>
+  <si>
+    <t>lab.vape.dryhit.1</t>
+  </si>
+  <si>
+    <t>Občas</t>
+  </si>
+  <si>
+    <t>lab.vape.dryhit.2</t>
+  </si>
+  <si>
+    <t>Velmi často</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.0</t>
+  </si>
+  <si>
+    <t>Utažený</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.1</t>
+  </si>
+  <si>
+    <t>Mírně utažený</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.2</t>
+  </si>
+  <si>
+    <t>Volný</t>
+  </si>
+  <si>
+    <t>lab.vape.airflow.3</t>
+  </si>
+  <si>
+    <t>Zcela otevřený</t>
+  </si>
+  <si>
+    <t>lab.vape.juice.0</t>
+  </si>
+  <si>
+    <t>lab.vape.juice.1</t>
+  </si>
+  <si>
+    <t>Mírně otevřený</t>
+  </si>
+  <si>
+    <t>lab.vape.juice.2</t>
   </si>
 </sst>
 </file>
@@ -4626,10 +4707,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C876"/>
+  <dimension ref="A1:C891"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A853" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B866" sqref="B866"/>
+    <sheetView tabSelected="1" topLeftCell="A874" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B889" sqref="B889"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14273,6 +14354,171 @@
       </c>
       <c r="C876" s="1" t="s">
         <v>1407</v>
+      </c>
+    </row>
+    <row r="877" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A877" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B877" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C877" s="1" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="878" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A878" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B878" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C878" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A879" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B879" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C879" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="880" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A880" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B880" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C880" s="1" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A881" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B881" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C881" s="1" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A882" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B882" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C882" s="1" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A883" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B883" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C883" s="1" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A884" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B884" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C884" s="1" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A885" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B885" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C885" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A886" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B886" s="1" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C886" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A887" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B887" s="1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C887" s="1" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A888" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B888" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C888" s="1" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A889" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B889" s="1" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C889" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A890" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B890" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C890" s="1" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A891" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B891" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C891" s="1" t="s">
+        <v>1433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved vape stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CF964-310F-498E-854C-0229D2540FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB61119-4B98-420A-A507-851D5E4AEA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="1467">
   <si>
     <t>cs</t>
   </si>
@@ -4298,6 +4307,9 @@
     <t>lab.vape.dryhit.0</t>
   </si>
   <si>
+    <t>Žádný</t>
+  </si>
+  <si>
     <t>lab.vape.dryhit.1</t>
   </si>
   <si>
@@ -4344,6 +4356,90 @@
   </si>
   <si>
     <t>lab.vape.juice.2</t>
+  </si>
+  <si>
+    <t>common.rate.1</t>
+  </si>
+  <si>
+    <t>Velmí špatné</t>
+  </si>
+  <si>
+    <t>common.rate.2</t>
+  </si>
+  <si>
+    <t>Ucházející</t>
+  </si>
+  <si>
+    <t>common.rate.3</t>
+  </si>
+  <si>
+    <t>common.rate.4</t>
+  </si>
+  <si>
+    <t>Výborné</t>
+  </si>
+  <si>
+    <t>common.rate.5</t>
+  </si>
+  <si>
+    <t>Excelentní</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.0</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.1</t>
+  </si>
+  <si>
+    <t>Menší</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.2</t>
+  </si>
+  <si>
+    <t>lab.vape.clouds.3</t>
+  </si>
+  <si>
+    <t>Extrémní</t>
+  </si>
+  <si>
+    <t>Nepatrná</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.0</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.1</t>
+  </si>
+  <si>
+    <t>Nepatrný</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.2</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.3</t>
+  </si>
+  <si>
+    <t>lab.vape.throathit.4</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.0</t>
+  </si>
+  <si>
+    <t>Žádná</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.1</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.2</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.3</t>
+  </si>
+  <si>
+    <t>lab.vape.fresh.4</t>
   </si>
 </sst>
 </file>
@@ -4707,10 +4803,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C891"/>
+  <dimension ref="A1:C910"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A874" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B889" sqref="B889"/>
+    <sheetView tabSelected="1" topLeftCell="A892" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B908" sqref="B908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14427,10 +14523,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
@@ -14438,10 +14534,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -14449,10 +14545,10 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.25">
@@ -14460,10 +14556,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.25">
@@ -14471,10 +14567,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.25">
@@ -14482,10 +14578,10 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.25">
@@ -14493,10 +14589,10 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.25">
@@ -14504,10 +14600,10 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.25">
@@ -14515,10 +14611,219 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A892" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B892" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C892" s="1" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A893" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B893" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C893" s="1" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A894" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B894" s="1" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C894" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A895" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B895" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C895" s="1" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A896" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B896" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C896" s="1" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A897" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B897" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C897" s="1" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A898" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B898" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C898" s="1" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A899" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B899" s="1" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C899" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A900" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B900" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C900" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A901" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B901" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C901" s="1" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A902" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B902" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C902" s="1" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A903" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B903" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C903" s="1" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A904" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B904" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C904" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A905" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B905" s="1" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C905" s="1" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A906" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B906" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C906" s="1" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A907" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B907" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C907" s="1" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A908" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B908" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C908" s="1" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A909" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B909" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C909" s="1" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="910" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A910" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B910" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C910" s="1" t="s">
+        <v>1453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved a little things
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9730AD-0DFC-476F-95A6-74018CA38983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B566CC3-4332-495A-AD5B-F8E2DAB8D34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="1481">
   <si>
     <t>cs</t>
   </si>
@@ -4476,6 +4476,12 @@
   </si>
   <si>
     <t>Vymazat</t>
+  </si>
+  <si>
+    <t>lab.coil.table.size</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.size</t>
   </si>
 </sst>
 </file>
@@ -4839,10 +4845,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C916"/>
+  <dimension ref="A1:C918"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A898" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B913" sqref="B913"/>
+      <selection activeCell="B908" sqref="B908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14926,6 +14932,28 @@
       </c>
       <c r="C916" s="1" t="s">
         <v>1478</v>
+      </c>
+    </row>
+    <row r="917" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A917" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B917" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C917" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="918" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A918" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B918" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C918" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added empty comment
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D35F4-DF55-4453-88AD-5F87BF9A964E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95995672-AFF7-4AD5-AE11-54AFFAFD786F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="1487">
   <si>
     <t>cs</t>
   </si>
@@ -4488,6 +4488,18 @@
   </si>
   <si>
     <t>lab.vape.preview.stamp</t>
+  </si>
+  <si>
+    <t>lab.comment.no-comments.title</t>
+  </si>
+  <si>
+    <t>Nejsou dostupné žádné komentáře.</t>
+  </si>
+  <si>
+    <t>lab.comment.no-comments.subtitle</t>
+  </si>
+  <si>
+    <t>Tady zatím nebylo nic okomentováno.</t>
   </si>
 </sst>
 </file>
@@ -4851,10 +4863,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C920"/>
+  <dimension ref="A1:C922"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A898" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B918" sqref="B918"/>
+      <selection activeCell="B912" sqref="B912"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14982,6 +14994,28 @@
       </c>
       <c r="C920" s="1" t="s">
         <v>938</v>
+      </c>
+    </row>
+    <row r="921" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A921" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B921" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C921" s="1" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="922" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A922" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B922" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C922" s="1" t="s">
+        <v>1486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing improved menu stuff in mobile
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B481CAAC-E0EC-48C3-87C1-750DCE36844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A49F998-F598-497B-9310-616380DF5F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="1497">
   <si>
     <t>cs</t>
   </si>
@@ -4527,6 +4527,9 @@
   </si>
   <si>
     <t>lab.mod.preview.name</t>
+  </si>
+  <si>
+    <t>lab.drawer.menu</t>
   </si>
 </sst>
 </file>
@@ -4890,10 +4893,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C929"/>
+  <dimension ref="A1:C930"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A912" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B925" sqref="B925"/>
+      <selection activeCell="B926" sqref="B926"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15120,6 +15123,17 @@
       </c>
       <c r="C929" s="1" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="930" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A930" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B930" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C930" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improving UI a lot
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF41BBA5-31D2-4C93-884A-C123138D1C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29C3820-D7C8-4986-9DC1-8D8662940755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2805" uniqueCount="1498">
   <si>
     <t>cs</t>
   </si>
@@ -4527,6 +4527,12 @@
   </si>
   <si>
     <t>lab.drawer.menu</t>
+  </si>
+  <si>
+    <t>lab.build.context.menu</t>
+  </si>
+  <si>
+    <t>Build [{{data.atomizer.name}}]</t>
   </si>
 </sst>
 </file>
@@ -4890,10 +4896,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C930"/>
+  <dimension ref="A1:C931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C310" sqref="C310"/>
+    <sheetView tabSelected="1" topLeftCell="A919" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B927" sqref="B927"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15131,6 +15137,17 @@
       </c>
       <c r="C930" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="931" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A931" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B931" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C931" s="1" t="s">
+        <v>1497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Liquid stuff updated
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94455DA-3ACC-47BB-BD30-AC915C2BE5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76354BA4-F5E3-4A0E-A82E-02F42ACB142E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2811" uniqueCount="1502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="1504">
   <si>
     <t>cs</t>
   </si>
@@ -4545,6 +4545,12 @@
   </si>
   <si>
     <t>Mix [{{data.liquid.name}}]</t>
+  </si>
+  <si>
+    <t>lab.liquid.context.menu</t>
+  </si>
+  <si>
+    <t>Liquid [{{data.name}}]</t>
   </si>
 </sst>
 </file>
@@ -4908,10 +4914,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C933"/>
+  <dimension ref="A1:C934"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A919" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B932" sqref="B932"/>
+      <selection activeCell="B928" sqref="B928"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15182,6 +15188,17 @@
       </c>
       <c r="C933" s="1" t="s">
         <v>1501</v>
+      </c>
+    </row>
+    <row r="934" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A934" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B934" s="1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C934" s="1" t="s">
+        <v>1503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial comments for atomizers
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBE0AA6-115C-7345-863C-0FDE8DC38142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BC77D-C5E1-9A40-A74E-8056D600A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1544">
   <si>
     <t>cs</t>
   </si>
@@ -4653,6 +4653,24 @@
   </si>
   <si>
     <t>lab.atomizer.list.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.common.tab</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.build.tab</t>
+  </si>
+  <si>
+    <t>Komentáře buildů</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.atomizer.tab</t>
+  </si>
+  <si>
+    <t>Komentáře atomizéru</t>
   </si>
 </sst>
 </file>
@@ -5016,10 +5034,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C958"/>
+  <dimension ref="A1:C962"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A935" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B949" sqref="B949"/>
+    <sheetView tabSelected="1" topLeftCell="A945" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B953" sqref="B953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15565,6 +15583,50 @@
       </c>
       <c r="C958" s="1" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A959" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B959" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C959" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A960" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B960" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C960" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="961" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A961" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B961" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C961" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A962" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B962" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C962" s="1" t="s">
+        <v>1543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared vape & atomizer comments
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BC77D-C5E1-9A40-A74E-8056D600A64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC799B0-120A-7E45-A930-8559414CE9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="1546">
   <si>
     <t>cs</t>
   </si>
@@ -4671,6 +4671,12 @@
   </si>
   <si>
     <t>Komentáře atomizéru</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.vape.tab</t>
+  </si>
+  <si>
+    <t>Komentáře vapů</t>
   </si>
 </sst>
 </file>
@@ -5034,10 +5040,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C962"/>
+  <dimension ref="A1:C963"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A945" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B953" sqref="B953"/>
+      <selection activeCell="B957" sqref="B957"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15627,6 +15633,17 @@
       </c>
       <c r="C962" s="1" t="s">
         <v>1543</v>
+      </c>
+    </row>
+    <row r="963" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A963" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B963" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C963" s="1" t="s">
+        <v>1545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So, atomizer stuff looks good now
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC799B0-120A-7E45-A930-8559414CE9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F3DC87-CA10-CC4C-B9DB-2A664A807310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="1546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2913" uniqueCount="1550">
   <si>
     <t>cs</t>
   </si>
@@ -4677,6 +4677,18 @@
   </si>
   <si>
     <t>Komentáře vapů</t>
+  </si>
+  <si>
+    <t>lab.atomizer.vape.plot.tab</t>
+  </si>
+  <si>
+    <t>lab.atomizer.plot.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.plot.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.button.plot</t>
   </si>
 </sst>
 </file>
@@ -5040,10 +5052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C963"/>
+  <dimension ref="A1:C967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A945" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B957" sqref="B957"/>
+      <selection activeCell="C966" sqref="C966"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15533,7 +15545,7 @@
         <v>1532</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>1513</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="954" spans="1:3" x14ac:dyDescent="0.2">
@@ -15644,6 +15656,50 @@
       </c>
       <c r="C963" s="1" t="s">
         <v>1545</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A964" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B964" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C964" s="1" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="965" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A965" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B965" s="1" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C965" s="1" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="966" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A966" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B966" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C966" s="1" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="967" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A967" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B967" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C967" s="1" t="s">
+        <v>1334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Massive refactor of comments
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F3DC87-CA10-CC4C-B9DB-2A664A807310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A487E0F3-8BF6-1449-8DD0-3AC4ABDF2FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="3440" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2913" uniqueCount="1550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="1552">
   <si>
     <t>cs</t>
   </si>
@@ -4689,6 +4689,12 @@
   </si>
   <si>
     <t>lab.atomizer.button.plot</t>
+  </si>
+  <si>
+    <t>lab.vape.comments.build.tab</t>
+  </si>
+  <si>
+    <t>lab.vape.comments.vape.tab</t>
   </si>
 </sst>
 </file>
@@ -5052,10 +5058,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C967"/>
+  <dimension ref="A1:C969"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A945" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C966" sqref="C966"/>
+      <selection activeCell="B961" sqref="B961"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15700,6 +15706,28 @@
       </c>
       <c r="C967" s="1" t="s">
         <v>1334</v>
+      </c>
+    </row>
+    <row r="968" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A968" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B968" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C968" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="969" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A969" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B969" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C969" s="1" t="s">
+        <v>1545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added cross-comment to mixtures
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A487E0F3-8BF6-1449-8DD0-3AC4ABDF2FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86275899-D9FB-8C45-B867-5E46FECFD9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="3440" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="1552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="1555">
   <si>
     <t>cs</t>
   </si>
@@ -4695,6 +4695,15 @@
   </si>
   <si>
     <t>lab.vape.comments.vape.tab</t>
+  </si>
+  <si>
+    <t>lab.mixture.comments.mixture.tab</t>
+  </si>
+  <si>
+    <t>Komentáře mixu</t>
+  </si>
+  <si>
+    <t>Komentáře liquidu</t>
   </si>
 </sst>
 </file>
@@ -5058,10 +5067,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C969"/>
+  <dimension ref="A1:C971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A945" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B961" sqref="B961"/>
+    <sheetView tabSelected="1" topLeftCell="A953" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B965" sqref="B965"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15728,6 +15737,28 @@
       </c>
       <c r="C969" s="1" t="s">
         <v>1545</v>
+      </c>
+    </row>
+    <row r="970" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A970" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B970" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C970" s="1" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="971" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A971" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B971" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C971" s="1" t="s">
+        <v>1554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Even more improved comment stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86275899-D9FB-8C45-B867-5E46FECFD9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373D406A-5504-D643-B58C-EEAA5CAD1121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="3440" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="1555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2937" uniqueCount="1561">
   <si>
     <t>cs</t>
   </si>
@@ -4136,15 +4136,9 @@
     <t>lab.build.comments.build.tab</t>
   </si>
   <si>
-    <t>Komentáře k buildu</t>
-  </si>
-  <si>
     <t>lab.build.comments.vape.tab</t>
   </si>
   <si>
-    <t>Komentáře k vapování</t>
-  </si>
-  <si>
     <t>lab.vape.button.plot</t>
   </si>
   <si>
@@ -4704,6 +4698,30 @@
   </si>
   <si>
     <t>Komentáře liquidu</t>
+  </si>
+  <si>
+    <t>lab.build.comments.atomizer.tab</t>
+  </si>
+  <si>
+    <t>Komentáře buildu</t>
+  </si>
+  <si>
+    <t>lab.vape.comments.atomizer.tab</t>
+  </si>
+  <si>
+    <t>Komentáře vapování</t>
+  </si>
+  <si>
+    <t>lab.mixture.comments.liquid.tab</t>
+  </si>
+  <si>
+    <t>lab.liquid.comments.liquid.tab</t>
+  </si>
+  <si>
+    <t>lab.liquid.comments.mixture.tab</t>
+  </si>
+  <si>
+    <t>Komentáře mixů</t>
   </si>
 </sst>
 </file>
@@ -5067,10 +5085,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C971"/>
+  <dimension ref="A1:C975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A953" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B965" sqref="B965"/>
+    <sheetView tabSelected="1" topLeftCell="A960" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B970" sqref="B970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14460,7 +14478,7 @@
         <v>1364</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>1365</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.2">
@@ -14468,10 +14486,10 @@
         <v>0</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>1367</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.2">
@@ -14479,7 +14497,7 @@
         <v>0</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C855" s="1" t="s">
         <v>1334</v>
@@ -14490,7 +14508,7 @@
         <v>0</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C856" s="1" t="s">
         <v>1342</v>
@@ -14501,10 +14519,10 @@
         <v>0</v>
       </c>
       <c r="B857" s="1" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="C857" s="1" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.2">
@@ -14512,10 +14530,10 @@
         <v>0</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.2">
@@ -14523,10 +14541,10 @@
         <v>0</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.2">
@@ -14534,10 +14552,10 @@
         <v>0</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.2">
@@ -14545,10 +14563,10 @@
         <v>0</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.2">
@@ -14556,10 +14574,10 @@
         <v>0</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.2">
@@ -14567,10 +14585,10 @@
         <v>0</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.2">
@@ -14578,10 +14596,10 @@
         <v>0</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.2">
@@ -14589,10 +14607,10 @@
         <v>0</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.2">
@@ -14600,10 +14618,10 @@
         <v>0</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.2">
@@ -14611,10 +14629,10 @@
         <v>0</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.2">
@@ -14622,10 +14640,10 @@
         <v>0</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.2">
@@ -14633,10 +14651,10 @@
         <v>0</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="C869" s="1" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.2">
@@ -14644,10 +14662,10 @@
         <v>0</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="C870" s="1" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.2">
@@ -14655,10 +14673,10 @@
         <v>0</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="C871" s="1" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.2">
@@ -14666,10 +14684,10 @@
         <v>0</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="C872" s="1" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.2">
@@ -14677,10 +14695,10 @@
         <v>0</v>
       </c>
       <c r="B873" s="1" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="C873" s="1" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.2">
@@ -14688,10 +14706,10 @@
         <v>0</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.2">
@@ -14699,10 +14717,10 @@
         <v>0</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.2">
@@ -14710,10 +14728,10 @@
         <v>0</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.2">
@@ -14721,10 +14739,10 @@
         <v>0</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="C877" s="1" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.2">
@@ -14732,10 +14750,10 @@
         <v>0</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.2">
@@ -14743,10 +14761,10 @@
         <v>0</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.2">
@@ -14754,10 +14772,10 @@
         <v>0</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.2">
@@ -14765,10 +14783,10 @@
         <v>0</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.2">
@@ -14776,10 +14794,10 @@
         <v>0</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.2">
@@ -14787,10 +14805,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.2">
@@ -14798,10 +14816,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.2">
@@ -14809,10 +14827,10 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.2">
@@ -14820,10 +14838,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.2">
@@ -14831,10 +14849,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.2">
@@ -14842,10 +14860,10 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.2">
@@ -14853,10 +14871,10 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.2">
@@ -14864,10 +14882,10 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.2">
@@ -14875,10 +14893,10 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.2">
@@ -14886,10 +14904,10 @@
         <v>0</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.2">
@@ -14897,10 +14915,10 @@
         <v>0</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.2">
@@ -14908,7 +14926,7 @@
         <v>0</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="C894" s="1" t="s">
         <v>1311</v>
@@ -14919,10 +14937,10 @@
         <v>0</v>
       </c>
       <c r="B895" s="1" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.2">
@@ -14930,10 +14948,10 @@
         <v>0</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.2">
@@ -14941,10 +14959,10 @@
         <v>0</v>
       </c>
       <c r="B897" s="1" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.2">
@@ -14952,10 +14970,10 @@
         <v>0</v>
       </c>
       <c r="B898" s="1" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.2">
@@ -14963,10 +14981,10 @@
         <v>0</v>
       </c>
       <c r="B899" s="1" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.2">
@@ -14974,10 +14992,10 @@
         <v>0</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.2">
@@ -14985,10 +15003,10 @@
         <v>0</v>
       </c>
       <c r="B901" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.2">
@@ -14996,10 +15014,10 @@
         <v>0</v>
       </c>
       <c r="B902" s="1" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.2">
@@ -15007,10 +15025,10 @@
         <v>0</v>
       </c>
       <c r="B903" s="1" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.2">
@@ -15018,10 +15036,10 @@
         <v>0</v>
       </c>
       <c r="B904" s="1" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.2">
@@ -15029,10 +15047,10 @@
         <v>0</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.2">
@@ -15040,10 +15058,10 @@
         <v>0</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.2">
@@ -15051,10 +15069,10 @@
         <v>0</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.2">
@@ -15062,10 +15080,10 @@
         <v>0</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.2">
@@ -15073,10 +15091,10 @@
         <v>0</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.2">
@@ -15084,10 +15102,10 @@
         <v>0</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.2">
@@ -15095,10 +15113,10 @@
         <v>0</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.2">
@@ -15106,10 +15124,10 @@
         <v>0</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.2">
@@ -15117,10 +15135,10 @@
         <v>0</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.2">
@@ -15128,10 +15146,10 @@
         <v>0</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="C914" s="1" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.2">
@@ -15139,10 +15157,10 @@
         <v>0</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="C915" s="1" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="916" spans="1:3" x14ac:dyDescent="0.2">
@@ -15150,10 +15168,10 @@
         <v>0</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.2">
@@ -15161,7 +15179,7 @@
         <v>0</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>204</v>
@@ -15172,7 +15190,7 @@
         <v>0</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>204</v>
@@ -15183,7 +15201,7 @@
         <v>0</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="C919" s="1" t="s">
         <v>937</v>
@@ -15194,7 +15212,7 @@
         <v>0</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>937</v>
@@ -15205,10 +15223,10 @@
         <v>0</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.2">
@@ -15216,10 +15234,10 @@
         <v>0</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.2">
@@ -15227,7 +15245,7 @@
         <v>0</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="C923" s="1" t="s">
         <v>890</v>
@@ -15238,7 +15256,7 @@
         <v>0</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>890</v>
@@ -15249,10 +15267,10 @@
         <v>0</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="C925" s="1" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.2">
@@ -15260,7 +15278,7 @@
         <v>0</v>
       </c>
       <c r="B926" s="1" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C926" s="1" t="s">
         <v>381</v>
@@ -15271,7 +15289,7 @@
         <v>0</v>
       </c>
       <c r="B927" s="1" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="C927" s="1" t="s">
         <v>381</v>
@@ -15282,10 +15300,10 @@
         <v>0</v>
       </c>
       <c r="B928" s="1" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.2">
@@ -15293,7 +15311,7 @@
         <v>0</v>
       </c>
       <c r="B929" s="1" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C929" s="1" t="s">
         <v>381</v>
@@ -15304,7 +15322,7 @@
         <v>0</v>
       </c>
       <c r="B930" s="1" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="C930" s="1" t="s">
         <v>15</v>
@@ -15315,10 +15333,10 @@
         <v>0</v>
       </c>
       <c r="B931" s="1" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.2">
@@ -15326,10 +15344,10 @@
         <v>0</v>
       </c>
       <c r="B932" s="1" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.2">
@@ -15337,10 +15355,10 @@
         <v>0</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="C933" s="1" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.2">
@@ -15348,10 +15366,10 @@
         <v>0</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C934" s="1" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.2">
@@ -15359,10 +15377,10 @@
         <v>0</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.2">
@@ -15370,7 +15388,7 @@
         <v>0</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="C936" s="1" t="s">
         <v>491</v>
@@ -15381,7 +15399,7 @@
         <v>0</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="C937" s="1" t="s">
         <v>491</v>
@@ -15392,10 +15410,10 @@
         <v>0</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.2">
@@ -15403,7 +15421,7 @@
         <v>0</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C939" s="1" t="s">
         <v>298</v>
@@ -15414,7 +15432,7 @@
         <v>0</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="C940" s="1" t="s">
         <v>393</v>
@@ -15425,10 +15443,10 @@
         <v>0</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.2">
@@ -15436,10 +15454,10 @@
         <v>0</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.2">
@@ -15447,10 +15465,10 @@
         <v>0</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.2">
@@ -15458,10 +15476,10 @@
         <v>0</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.2">
@@ -15469,10 +15487,10 @@
         <v>0</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.2">
@@ -15480,10 +15498,10 @@
         <v>0</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="947" spans="1:3" x14ac:dyDescent="0.2">
@@ -15491,10 +15509,10 @@
         <v>0</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="948" spans="1:3" x14ac:dyDescent="0.2">
@@ -15502,10 +15520,10 @@
         <v>0</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="949" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -15513,10 +15531,10 @@
         <v>0</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.2">
@@ -15524,10 +15542,10 @@
         <v>0</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="951" spans="1:3" x14ac:dyDescent="0.2">
@@ -15535,7 +15553,7 @@
         <v>0</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C951" s="1" t="s">
         <v>358</v>
@@ -15546,10 +15564,10 @@
         <v>0</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="953" spans="1:3" x14ac:dyDescent="0.2">
@@ -15557,7 +15575,7 @@
         <v>0</v>
       </c>
       <c r="B953" s="1" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="C953" s="1" t="s">
         <v>1260</v>
@@ -15568,10 +15586,10 @@
         <v>0</v>
       </c>
       <c r="B954" s="1" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="955" spans="1:3" x14ac:dyDescent="0.2">
@@ -15579,7 +15597,7 @@
         <v>0</v>
       </c>
       <c r="B955" s="1" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="C955" s="1" t="s">
         <v>1258</v>
@@ -15590,7 +15608,7 @@
         <v>0</v>
       </c>
       <c r="B956" s="1" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="C956" s="1" t="s">
         <v>289</v>
@@ -15601,10 +15619,10 @@
         <v>0</v>
       </c>
       <c r="B957" s="1" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="958" spans="1:3" x14ac:dyDescent="0.2">
@@ -15623,7 +15641,7 @@
         <v>0</v>
       </c>
       <c r="B959" s="1" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="C959" s="1" t="s">
         <v>119</v>
@@ -15634,7 +15652,7 @@
         <v>0</v>
       </c>
       <c r="B960" s="1" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="C960" s="1" t="s">
         <v>1128</v>
@@ -15645,10 +15663,10 @@
         <v>0</v>
       </c>
       <c r="B961" s="1" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="962" spans="1:3" x14ac:dyDescent="0.2">
@@ -15656,10 +15674,10 @@
         <v>0</v>
       </c>
       <c r="B962" s="1" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="963" spans="1:3" x14ac:dyDescent="0.2">
@@ -15667,10 +15685,10 @@
         <v>0</v>
       </c>
       <c r="B963" s="1" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="964" spans="1:3" x14ac:dyDescent="0.2">
@@ -15678,7 +15696,7 @@
         <v>0</v>
       </c>
       <c r="B964" s="1" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C964" s="1" t="s">
         <v>1334</v>
@@ -15689,7 +15707,7 @@
         <v>0</v>
       </c>
       <c r="B965" s="1" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="C965" s="1" t="s">
         <v>1342</v>
@@ -15700,7 +15718,7 @@
         <v>0</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="C966" s="1" t="s">
         <v>1334</v>
@@ -15711,7 +15729,7 @@
         <v>0</v>
       </c>
       <c r="B967" s="1" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="C967" s="1" t="s">
         <v>1334</v>
@@ -15722,10 +15740,10 @@
         <v>0</v>
       </c>
       <c r="B968" s="1" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>1541</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="969" spans="1:3" x14ac:dyDescent="0.2">
@@ -15733,10 +15751,10 @@
         <v>0</v>
       </c>
       <c r="B969" s="1" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="970" spans="1:3" x14ac:dyDescent="0.2">
@@ -15744,10 +15762,10 @@
         <v>0</v>
       </c>
       <c r="B970" s="1" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="971" spans="1:3" x14ac:dyDescent="0.2">
@@ -15755,10 +15773,54 @@
         <v>0</v>
       </c>
       <c r="B971" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C971" s="1" t="s">
         <v>1552</v>
       </c>
-      <c r="C971" s="1" t="s">
-        <v>1554</v>
+    </row>
+    <row r="972" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A972" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B972" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C972" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="973" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A973" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B973" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C973" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="974" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A974" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B974" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C974" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="975" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A975" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B975" s="1" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C975" s="1" t="s">
+        <v>1560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved menu structures
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2C0FA5-6C28-43BB-9605-A31F59AFF58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3357443-FD42-4A67-8131-607837CEACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2949" uniqueCount="1569">
   <si>
     <t>cs</t>
   </si>
@@ -4728,6 +4728,24 @@
   </si>
   <si>
     <t>Náhled vaty</t>
+  </si>
+  <si>
+    <t>lab.coil.table.wire.ga</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>lab.coil.table.wire.description</t>
+  </si>
+  <si>
+    <t>Popis drátu</t>
+  </si>
+  <si>
+    <t>lab.coil.created.message</t>
+  </si>
+  <si>
+    <t>Spirálka vytvořena.</t>
   </si>
 </sst>
 </file>
@@ -5091,10 +5109,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C976"/>
+  <dimension ref="A1:C979"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A960" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B969" sqref="B969"/>
+      <selection activeCell="B972" sqref="B972"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15838,6 +15856,39 @@
       </c>
       <c r="C976" s="1" t="s">
         <v>1562</v>
+      </c>
+    </row>
+    <row r="977" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A977" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B977" s="1" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C977" s="1" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="978" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A978" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B978" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C978" s="1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="979" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A979" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B979" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C979" s="1" t="s">
+        <v>1568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Experimentally added vape plot to build
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED5819-7D83-4416-B8AC-158EB8F6774B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A04B5-240B-469C-B61E-2641B4A68FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2952" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="1574">
   <si>
     <t>cs</t>
   </si>
@@ -4749,6 +4749,18 @@
   </si>
   <si>
     <t>lab.atomizer.create.label</t>
+  </si>
+  <si>
+    <t>lab.vape.wireId.label</t>
+  </si>
+  <si>
+    <t>lab.vape.coilSize.label</t>
+  </si>
+  <si>
+    <t>Velikost spirálky</t>
+  </si>
+  <si>
+    <t>lab.vape.cottonId.label</t>
   </si>
 </sst>
 </file>
@@ -5112,7 +5124,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C980"/>
+  <dimension ref="A1:C983"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A960" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B976" sqref="B976"/>
@@ -15903,6 +15915,39 @@
       </c>
       <c r="C980" s="1" t="s">
         <v>1261</v>
+      </c>
+    </row>
+    <row r="981" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A981" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B981" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C981" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="982" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A982" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B982" s="1" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C982" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="983" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A983" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B983" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C983" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Build on mobile somehow works
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A04B5-240B-469C-B61E-2641B4A68FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876AA237-7F20-469B-A14A-BE1FD51AD43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="1574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="1575">
   <si>
     <t>cs</t>
   </si>
@@ -4761,6 +4761,9 @@
   </si>
   <si>
     <t>lab.vape.cottonId.label</t>
+  </si>
+  <si>
+    <t>lab.build.create.preview.button</t>
   </si>
 </sst>
 </file>
@@ -5124,7 +5127,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C983"/>
+  <dimension ref="A1:C984"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A960" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B976" sqref="B976"/>
@@ -15948,6 +15951,17 @@
       </c>
       <c r="C983" s="1" t="s">
         <v>362</v>
+      </c>
+    </row>
+    <row r="984" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A984" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B984" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C984" s="1" t="s">
+        <v>893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fuck that! Added comments to build creation, whoat!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFBFDF8-7C62-41F7-AB2C-78803039C2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C3723E-194D-49C7-93E1-18A4EB11D2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="4470" windowWidth="23955" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="1579">
   <si>
     <t>cs</t>
   </si>
@@ -4764,6 +4764,18 @@
   </si>
   <si>
     <t>lab.build.create.preview.button</t>
+  </si>
+  <si>
+    <t>lab.build.create.atomizer.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.build.create.vape.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.build.create.plot.tab</t>
+  </si>
+  <si>
+    <t>Náhled hodnocení</t>
   </si>
 </sst>
 </file>
@@ -5127,10 +5139,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C984"/>
+  <dimension ref="A1:C987"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A960" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C984" sqref="C984"/>
+      <selection activeCell="B983" sqref="B983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15962,6 +15974,39 @@
       </c>
       <c r="C984" s="1" t="s">
         <v>803</v>
+      </c>
+    </row>
+    <row r="985" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A985" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B985" s="1" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C985" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="986" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A986" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B986" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C986" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="987" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A987" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B987" s="1" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C987" s="1" t="s">
+        <v>1578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing image gallery for builds
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF1B375-56F9-A341-A098-27C26BDF1636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2256A6C0-47A0-CA4D-9E07-93A7811DC0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2976" uniqueCount="1580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="1582">
   <si>
     <t>cs</t>
   </si>
@@ -4779,6 +4779,12 @@
   </si>
   <si>
     <t>lab.build.create.build.comments.tab</t>
+  </si>
+  <si>
+    <t>lab.build.create.vape.images.tab</t>
+  </si>
+  <si>
+    <t>Obrázky buildů</t>
   </si>
 </sst>
 </file>
@@ -5142,10 +5148,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C988"/>
+  <dimension ref="A1:C989"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A975" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B982" sqref="B982"/>
+      <selection activeCell="B986" sqref="B986"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16021,6 +16027,17 @@
       </c>
       <c r="C988" s="1" t="s">
         <v>1539</v>
+      </c>
+    </row>
+    <row r="989" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A989" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B989" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C989" s="1" t="s">
+        <v>1581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added spaced coil
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2256A6C0-47A0-CA4D-9E07-93A7811DC0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1912CE74-8933-0643-8231-BA1C9615A104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3460" windowWidth="23960" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="1587">
   <si>
     <t>cs</t>
   </si>
@@ -4785,6 +4785,21 @@
   </si>
   <si>
     <t>Obrázky buildů</t>
+  </si>
+  <si>
+    <t>lab.coil.spaced.label</t>
+  </si>
+  <si>
+    <t>Spaced coil</t>
+  </si>
+  <si>
+    <t>lab.coil.table.spaced</t>
+  </si>
+  <si>
+    <t>Spaced</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.spaced</t>
   </si>
 </sst>
 </file>
@@ -5148,9 +5163,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C989"/>
+  <dimension ref="A1:C992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A975" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A978" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B986" sqref="B986"/>
     </sheetView>
   </sheetViews>
@@ -16038,6 +16053,39 @@
       </c>
       <c r="C989" s="1" t="s">
         <v>1581</v>
+      </c>
+    </row>
+    <row r="990" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A990" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B990" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C990" s="1" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="991" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A991" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B991" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C991" s="1" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="992" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A992" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B992" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C992" s="1" t="s">
+        <v>1585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Preparing new image gallery
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FC3AB8-0A52-4F3D-8D3C-896CF87393A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB960967-B57A-48C0-9A2A-3E6F52F35A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="3030" windowWidth="25245" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2994" uniqueCount="1591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="1593">
   <si>
     <t>cs</t>
   </si>
@@ -4812,6 +4812,12 @@
   </si>
   <si>
     <t>Čištění souborů</t>
+  </si>
+  <si>
+    <t>job-service.Edde\Image\ImageJobService</t>
+  </si>
+  <si>
+    <t>Aktualizace obrázků</t>
   </si>
 </sst>
 </file>
@@ -5175,10 +5181,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C994"/>
+  <dimension ref="A1:C995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A978" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B987" sqref="B987"/>
+      <selection activeCell="B991" sqref="B991"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16120,6 +16126,17 @@
       </c>
       <c r="C994" s="1" t="s">
         <v>1590</v>
+      </c>
+    </row>
+    <row r="995" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A995" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B995" s="1" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C995" s="1" t="s">
+        <v>1592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Simplification in progress
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB960967-B57A-48C0-9A2A-3E6F52F35A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AABBCD-9E10-46AC-93D4-2CB0B997CF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="3030" windowWidth="25245" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="1593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="1592">
   <si>
     <t>cs</t>
   </si>
@@ -3816,9 +3816,6 @@
   </si>
   <si>
     <t>Editace</t>
-  </si>
-  <si>
-    <t>Detail</t>
   </si>
   <si>
     <t>Seznam</t>
@@ -5183,8 +5180,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A978" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B991" sqref="B991"/>
+    <sheetView tabSelected="1" topLeftCell="A971" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A993" sqref="A993"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9723,7 +9720,7 @@
         <v>709</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -10889,7 +10886,7 @@
         <v>873</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -11857,7 +11854,7 @@
         <v>997</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.25">
@@ -11868,7 +11865,7 @@
         <v>998</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
@@ -13771,7 +13768,7 @@
         <v>1254</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
@@ -13782,7 +13779,7 @@
         <v>1255</v>
       </c>
       <c r="C781" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
@@ -13804,7 +13801,7 @@
         <v>1257</v>
       </c>
       <c r="C783" s="1" t="s">
-        <v>1259</v>
+        <v>532</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
@@ -13812,7 +13809,7 @@
         <v>0</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C784" s="1" t="s">
         <v>241</v>
@@ -13823,10 +13820,10 @@
         <v>0</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C785" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.25">
@@ -13834,10 +13831,10 @@
         <v>0</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C786" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
@@ -13845,10 +13842,10 @@
         <v>0</v>
       </c>
       <c r="B787" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C787" s="1" t="s">
         <v>1265</v>
-      </c>
-      <c r="C787" s="1" t="s">
-        <v>1266</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
@@ -13856,7 +13853,7 @@
         <v>0</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C788" s="1" t="s">
         <v>366</v>
@@ -13867,7 +13864,7 @@
         <v>0</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C789" s="1" t="s">
         <v>1258</v>
@@ -13878,10 +13875,10 @@
         <v>0</v>
       </c>
       <c r="B790" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C790" s="1" t="s">
         <v>1269</v>
-      </c>
-      <c r="C790" s="1" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.25">
@@ -13889,10 +13886,10 @@
         <v>0</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C791" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
@@ -13900,10 +13897,10 @@
         <v>0</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C792" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
@@ -13911,7 +13908,7 @@
         <v>0</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C793" s="1" t="s">
         <v>528</v>
@@ -13922,10 +13919,10 @@
         <v>0</v>
       </c>
       <c r="B794" s="1" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C794" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
@@ -13933,7 +13930,7 @@
         <v>0</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>1258</v>
@@ -13944,7 +13941,7 @@
         <v>0</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>489</v>
@@ -13955,10 +13952,10 @@
         <v>0</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.25">
@@ -13966,10 +13963,10 @@
         <v>0</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
@@ -13977,7 +13974,7 @@
         <v>0</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>579</v>
@@ -13988,7 +13985,7 @@
         <v>0</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>1258</v>
@@ -13999,7 +13996,7 @@
         <v>0</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>503</v>
@@ -14010,10 +14007,10 @@
         <v>0</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.25">
@@ -14021,10 +14018,10 @@
         <v>0</v>
       </c>
       <c r="B803" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C803" s="1" t="s">
         <v>1283</v>
-      </c>
-      <c r="C803" s="1" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
@@ -14032,7 +14029,7 @@
         <v>0</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>354</v>
@@ -14043,7 +14040,7 @@
         <v>0</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>1258</v>
@@ -14054,10 +14051,10 @@
         <v>0</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.25">
@@ -14065,10 +14062,10 @@
         <v>0</v>
       </c>
       <c r="B807" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C807" s="1" t="s">
         <v>1288</v>
-      </c>
-      <c r="C807" s="1" t="s">
-        <v>1289</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">
@@ -14076,10 +14073,10 @@
         <v>0</v>
       </c>
       <c r="B808" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C808" s="1" t="s">
         <v>1290</v>
-      </c>
-      <c r="C808" s="1" t="s">
-        <v>1291</v>
       </c>
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.25">
@@ -14087,10 +14084,10 @@
         <v>0</v>
       </c>
       <c r="B809" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C809" s="1" t="s">
         <v>1292</v>
-      </c>
-      <c r="C809" s="1" t="s">
-        <v>1293</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.25">
@@ -14098,7 +14095,7 @@
         <v>0</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C810" s="1" t="s">
         <v>803</v>
@@ -14109,10 +14106,10 @@
         <v>0</v>
       </c>
       <c r="B811" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C811" s="1" t="s">
         <v>1299</v>
-      </c>
-      <c r="C811" s="1" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.25">
@@ -14120,10 +14117,10 @@
         <v>0</v>
       </c>
       <c r="B812" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C812" s="1" t="s">
         <v>1301</v>
-      </c>
-      <c r="C812" s="1" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.25">
@@ -14131,10 +14128,10 @@
         <v>0</v>
       </c>
       <c r="B813" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C813" s="1" t="s">
         <v>1303</v>
-      </c>
-      <c r="C813" s="1" t="s">
-        <v>1304</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.25">
@@ -14142,10 +14139,10 @@
         <v>0</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.25">
@@ -14153,10 +14150,10 @@
         <v>0</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.25">
@@ -14164,10 +14161,10 @@
         <v>0</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.25">
@@ -14175,10 +14172,10 @@
         <v>0</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.25">
@@ -14186,10 +14183,10 @@
         <v>0</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.25">
@@ -14197,10 +14194,10 @@
         <v>0</v>
       </c>
       <c r="B819" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C819" s="1" t="s">
         <v>1313</v>
-      </c>
-      <c r="C819" s="1" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.25">
@@ -14208,7 +14205,7 @@
         <v>0</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C820" s="1" t="s">
         <v>729</v>
@@ -14219,7 +14216,7 @@
         <v>0</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C821" s="1" t="s">
         <v>805</v>
@@ -14230,7 +14227,7 @@
         <v>0</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="C822" s="1" t="s">
         <v>740</v>
@@ -14241,7 +14238,7 @@
         <v>0</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>752</v>
@@ -14252,7 +14249,7 @@
         <v>0</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>744</v>
@@ -14263,7 +14260,7 @@
         <v>0</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="C825" s="1" t="s">
         <v>756</v>
@@ -14274,7 +14271,7 @@
         <v>0</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>834</v>
@@ -14285,7 +14282,7 @@
         <v>0</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="C827" s="1" t="s">
         <v>835</v>
@@ -14296,7 +14293,7 @@
         <v>0</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C828" s="1" t="s">
         <v>942</v>
@@ -14307,7 +14304,7 @@
         <v>0</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C829" s="1" t="s">
         <v>748</v>
@@ -14318,10 +14315,10 @@
         <v>0</v>
       </c>
       <c r="B830" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C830" s="1" t="s">
         <v>1325</v>
-      </c>
-      <c r="C830" s="1" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.25">
@@ -14329,10 +14326,10 @@
         <v>0</v>
       </c>
       <c r="B831" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C831" s="1" t="s">
         <v>1327</v>
-      </c>
-      <c r="C831" s="1" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.25">
@@ -14340,10 +14337,10 @@
         <v>0</v>
       </c>
       <c r="B832" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C832" s="1" t="s">
         <v>1330</v>
-      </c>
-      <c r="C832" s="1" t="s">
-        <v>1331</v>
       </c>
     </row>
     <row r="833" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -14351,10 +14348,10 @@
         <v>0</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.25">
@@ -14362,10 +14359,10 @@
         <v>0</v>
       </c>
       <c r="B834" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C834" s="1" t="s">
         <v>1333</v>
-      </c>
-      <c r="C834" s="1" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.25">
@@ -14373,10 +14370,10 @@
         <v>0</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.25">
@@ -14384,10 +14381,10 @@
         <v>0</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.25">
@@ -14395,10 +14392,10 @@
         <v>0</v>
       </c>
       <c r="B837" s="1" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C837" s="1" t="s">
         <v>1337</v>
-      </c>
-      <c r="C837" s="1" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.25">
@@ -14406,10 +14403,10 @@
         <v>0</v>
       </c>
       <c r="B838" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C838" s="1" t="s">
         <v>1339</v>
-      </c>
-      <c r="C838" s="1" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.25">
@@ -14417,10 +14414,10 @@
         <v>0</v>
       </c>
       <c r="B839" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C839" s="1" t="s">
         <v>1341</v>
-      </c>
-      <c r="C839" s="1" t="s">
-        <v>1342</v>
       </c>
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.25">
@@ -14428,10 +14425,10 @@
         <v>0</v>
       </c>
       <c r="B840" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C840" s="1" t="s">
         <v>1343</v>
-      </c>
-      <c r="C840" s="1" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.25">
@@ -14439,10 +14436,10 @@
         <v>0</v>
       </c>
       <c r="B841" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C841" s="1" t="s">
         <v>1345</v>
-      </c>
-      <c r="C841" s="1" t="s">
-        <v>1346</v>
       </c>
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.25">
@@ -14450,10 +14447,10 @@
         <v>0</v>
       </c>
       <c r="B842" s="1" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C842" s="1" t="s">
         <v>1347</v>
-      </c>
-      <c r="C842" s="1" t="s">
-        <v>1348</v>
       </c>
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.25">
@@ -14461,10 +14458,10 @@
         <v>0</v>
       </c>
       <c r="B843" s="1" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C843" s="1" t="s">
         <v>1349</v>
-      </c>
-      <c r="C843" s="1" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.25">
@@ -14472,10 +14469,10 @@
         <v>0</v>
       </c>
       <c r="B844" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C844" s="1" t="s">
         <v>1351</v>
-      </c>
-      <c r="C844" s="1" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.25">
@@ -14483,10 +14480,10 @@
         <v>0</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.25">
@@ -14494,10 +14491,10 @@
         <v>0</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.25">
@@ -14505,10 +14502,10 @@
         <v>0</v>
       </c>
       <c r="B847" s="1" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C847" s="1" t="s">
         <v>1355</v>
-      </c>
-      <c r="C847" s="1" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.25">
@@ -14516,10 +14513,10 @@
         <v>0</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.25">
@@ -14527,10 +14524,10 @@
         <v>0</v>
       </c>
       <c r="B849" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C849" s="1" t="s">
         <v>1359</v>
-      </c>
-      <c r="C849" s="1" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.25">
@@ -14538,10 +14535,10 @@
         <v>0</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.25">
@@ -14549,10 +14546,10 @@
         <v>0</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.25">
@@ -14560,10 +14557,10 @@
         <v>0</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.25">
@@ -14571,10 +14568,10 @@
         <v>0</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.25">
@@ -14582,10 +14579,10 @@
         <v>0</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.25">
@@ -14593,10 +14590,10 @@
         <v>0</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.25">
@@ -14604,10 +14601,10 @@
         <v>0</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="C856" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.25">
@@ -14615,10 +14612,10 @@
         <v>0</v>
       </c>
       <c r="B857" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C857" s="1" t="s">
         <v>1368</v>
-      </c>
-      <c r="C857" s="1" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">
@@ -14626,10 +14623,10 @@
         <v>0</v>
       </c>
       <c r="B858" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C858" s="1" t="s">
         <v>1370</v>
-      </c>
-      <c r="C858" s="1" t="s">
-        <v>1371</v>
       </c>
     </row>
     <row r="859" spans="1:3" x14ac:dyDescent="0.25">
@@ -14637,10 +14634,10 @@
         <v>0</v>
       </c>
       <c r="B859" s="1" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C859" s="1" t="s">
         <v>1372</v>
-      </c>
-      <c r="C859" s="1" t="s">
-        <v>1373</v>
       </c>
     </row>
     <row r="860" spans="1:3" x14ac:dyDescent="0.25">
@@ -14648,10 +14645,10 @@
         <v>0</v>
       </c>
       <c r="B860" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C860" s="1" t="s">
         <v>1374</v>
-      </c>
-      <c r="C860" s="1" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -14659,10 +14656,10 @@
         <v>0</v>
       </c>
       <c r="B861" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C861" s="1" t="s">
         <v>1376</v>
-      </c>
-      <c r="C861" s="1" t="s">
-        <v>1377</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
@@ -14670,10 +14667,10 @@
         <v>0</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
@@ -14681,10 +14678,10 @@
         <v>0</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
@@ -14692,10 +14689,10 @@
         <v>0</v>
       </c>
       <c r="B864" s="1" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C864" s="1" t="s">
         <v>1382</v>
-      </c>
-      <c r="C864" s="1" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
@@ -14703,10 +14700,10 @@
         <v>0</v>
       </c>
       <c r="B865" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C865" s="1" t="s">
         <v>1384</v>
-      </c>
-      <c r="C865" s="1" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
@@ -14714,10 +14711,10 @@
         <v>0</v>
       </c>
       <c r="B866" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C866" s="1" t="s">
         <v>1386</v>
-      </c>
-      <c r="C866" s="1" t="s">
-        <v>1387</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
@@ -14725,10 +14722,10 @@
         <v>0</v>
       </c>
       <c r="B867" s="1" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C867" s="1" t="s">
         <v>1388</v>
-      </c>
-      <c r="C867" s="1" t="s">
-        <v>1389</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
@@ -14736,10 +14733,10 @@
         <v>0</v>
       </c>
       <c r="B868" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C868" s="1" t="s">
         <v>1390</v>
-      </c>
-      <c r="C868" s="1" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.25">
@@ -14747,10 +14744,10 @@
         <v>0</v>
       </c>
       <c r="B869" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C869" s="1" t="s">
         <v>1392</v>
-      </c>
-      <c r="C869" s="1" t="s">
-        <v>1393</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.25">
@@ -14758,10 +14755,10 @@
         <v>0</v>
       </c>
       <c r="B870" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C870" s="1" t="s">
         <v>1394</v>
-      </c>
-      <c r="C870" s="1" t="s">
-        <v>1395</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.25">
@@ -14769,10 +14766,10 @@
         <v>0</v>
       </c>
       <c r="B871" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C871" s="1" t="s">
         <v>1396</v>
-      </c>
-      <c r="C871" s="1" t="s">
-        <v>1397</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.25">
@@ -14780,10 +14777,10 @@
         <v>0</v>
       </c>
       <c r="B872" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C872" s="1" t="s">
         <v>1398</v>
-      </c>
-      <c r="C872" s="1" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.25">
@@ -14791,10 +14788,10 @@
         <v>0</v>
       </c>
       <c r="B873" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C873" s="1" t="s">
         <v>1400</v>
-      </c>
-      <c r="C873" s="1" t="s">
-        <v>1401</v>
       </c>
     </row>
     <row r="874" spans="1:3" x14ac:dyDescent="0.25">
@@ -14802,10 +14799,10 @@
         <v>0</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.25">
@@ -14813,10 +14810,10 @@
         <v>0</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.25">
@@ -14824,10 +14821,10 @@
         <v>0</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.25">
@@ -14835,10 +14832,10 @@
         <v>0</v>
       </c>
       <c r="B877" s="1" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C877" s="1" t="s">
         <v>1408</v>
-      </c>
-      <c r="C877" s="1" t="s">
-        <v>1409</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.25">
@@ -14846,10 +14843,10 @@
         <v>0</v>
       </c>
       <c r="B878" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C878" s="1" t="s">
         <v>1410</v>
-      </c>
-      <c r="C878" s="1" t="s">
-        <v>1411</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.25">
@@ -14857,10 +14854,10 @@
         <v>0</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.25">
@@ -14868,10 +14865,10 @@
         <v>0</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.25">
@@ -14879,10 +14876,10 @@
         <v>0</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.25">
@@ -14890,10 +14887,10 @@
         <v>0</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.25">
@@ -14901,10 +14898,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C883" s="1" t="s">
         <v>1420</v>
-      </c>
-      <c r="C883" s="1" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
@@ -14912,10 +14909,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C884" s="1" t="s">
         <v>1422</v>
-      </c>
-      <c r="C884" s="1" t="s">
-        <v>1423</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -14923,10 +14920,10 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C885" s="1" t="s">
         <v>1424</v>
-      </c>
-      <c r="C885" s="1" t="s">
-        <v>1425</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.25">
@@ -14934,10 +14931,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C886" s="1" t="s">
         <v>1426</v>
-      </c>
-      <c r="C886" s="1" t="s">
-        <v>1427</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.25">
@@ -14945,10 +14942,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C887" s="1" t="s">
         <v>1428</v>
-      </c>
-      <c r="C887" s="1" t="s">
-        <v>1429</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.25">
@@ -14956,10 +14953,10 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C888" s="1" t="s">
         <v>1430</v>
-      </c>
-      <c r="C888" s="1" t="s">
-        <v>1431</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.25">
@@ -14967,10 +14964,10 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.25">
@@ -14978,10 +14975,10 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C890" s="1" t="s">
         <v>1433</v>
-      </c>
-      <c r="C890" s="1" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.25">
@@ -14989,10 +14986,10 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.25">
@@ -15000,10 +14997,10 @@
         <v>0</v>
       </c>
       <c r="B892" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C892" s="1" t="s">
         <v>1436</v>
-      </c>
-      <c r="C892" s="1" t="s">
-        <v>1437</v>
       </c>
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.25">
@@ -15011,10 +15008,10 @@
         <v>0</v>
       </c>
       <c r="B893" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C893" s="1" t="s">
         <v>1438</v>
-      </c>
-      <c r="C893" s="1" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.25">
@@ -15022,10 +15019,10 @@
         <v>0</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="895" spans="1:3" x14ac:dyDescent="0.25">
@@ -15033,10 +15030,10 @@
         <v>0</v>
       </c>
       <c r="B895" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C895" s="1" t="s">
         <v>1441</v>
-      </c>
-      <c r="C895" s="1" t="s">
-        <v>1442</v>
       </c>
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.25">
@@ -15044,10 +15041,10 @@
         <v>0</v>
       </c>
       <c r="B896" s="1" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C896" s="1" t="s">
         <v>1443</v>
-      </c>
-      <c r="C896" s="1" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.25">
@@ -15055,10 +15052,10 @@
         <v>0</v>
       </c>
       <c r="B897" s="1" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.25">
@@ -15066,10 +15063,10 @@
         <v>0</v>
       </c>
       <c r="B898" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C898" s="1" t="s">
         <v>1446</v>
-      </c>
-      <c r="C898" s="1" t="s">
-        <v>1447</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.25">
@@ -15077,10 +15074,10 @@
         <v>0</v>
       </c>
       <c r="B899" s="1" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.25">
@@ -15088,10 +15085,10 @@
         <v>0</v>
       </c>
       <c r="B900" s="1" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C900" s="1" t="s">
         <v>1449</v>
-      </c>
-      <c r="C900" s="1" t="s">
-        <v>1450</v>
       </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.25">
@@ -15099,10 +15096,10 @@
         <v>0</v>
       </c>
       <c r="B901" s="1" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.25">
@@ -15110,10 +15107,10 @@
         <v>0</v>
       </c>
       <c r="B902" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C902" s="1" t="s">
         <v>1453</v>
-      </c>
-      <c r="C902" s="1" t="s">
-        <v>1454</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.25">
@@ -15121,10 +15118,10 @@
         <v>0</v>
       </c>
       <c r="B903" s="1" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.25">
@@ -15132,10 +15129,10 @@
         <v>0</v>
       </c>
       <c r="B904" s="1" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.25">
@@ -15143,10 +15140,10 @@
         <v>0</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.25">
@@ -15154,10 +15151,10 @@
         <v>0</v>
       </c>
       <c r="B906" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C906" s="1" t="s">
         <v>1458</v>
-      </c>
-      <c r="C906" s="1" t="s">
-        <v>1459</v>
       </c>
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.25">
@@ -15165,10 +15162,10 @@
         <v>0</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.25">
@@ -15176,10 +15173,10 @@
         <v>0</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.25">
@@ -15187,10 +15184,10 @@
         <v>0</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.25">
@@ -15198,10 +15195,10 @@
         <v>0</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.25">
@@ -15209,10 +15206,10 @@
         <v>0</v>
       </c>
       <c r="B911" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C911" s="1" t="s">
         <v>1464</v>
-      </c>
-      <c r="C911" s="1" t="s">
-        <v>1465</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.25">
@@ -15220,10 +15217,10 @@
         <v>0</v>
       </c>
       <c r="B912" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C912" s="1" t="s">
         <v>1466</v>
-      </c>
-      <c r="C912" s="1" t="s">
-        <v>1467</v>
       </c>
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.25">
@@ -15231,10 +15228,10 @@
         <v>0</v>
       </c>
       <c r="B913" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C913" s="1" t="s">
         <v>1468</v>
-      </c>
-      <c r="C913" s="1" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.25">
@@ -15242,10 +15239,10 @@
         <v>0</v>
       </c>
       <c r="B914" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C914" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="C914" s="1" t="s">
-        <v>1471</v>
       </c>
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.25">
@@ -15253,10 +15250,10 @@
         <v>0</v>
       </c>
       <c r="B915" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C915" s="1" t="s">
         <v>1472</v>
-      </c>
-      <c r="C915" s="1" t="s">
-        <v>1473</v>
       </c>
     </row>
     <row r="916" spans="1:3" x14ac:dyDescent="0.25">
@@ -15264,10 +15261,10 @@
         <v>0</v>
       </c>
       <c r="B916" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C916" s="1" t="s">
         <v>1474</v>
-      </c>
-      <c r="C916" s="1" t="s">
-        <v>1475</v>
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.25">
@@ -15275,7 +15272,7 @@
         <v>0</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>204</v>
@@ -15286,7 +15283,7 @@
         <v>0</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>204</v>
@@ -15297,7 +15294,7 @@
         <v>0</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="C919" s="1" t="s">
         <v>937</v>
@@ -15308,7 +15305,7 @@
         <v>0</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>937</v>
@@ -15319,10 +15316,10 @@
         <v>0</v>
       </c>
       <c r="B921" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C921" s="1" t="s">
         <v>1480</v>
-      </c>
-      <c r="C921" s="1" t="s">
-        <v>1481</v>
       </c>
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.25">
@@ -15330,10 +15327,10 @@
         <v>0</v>
       </c>
       <c r="B922" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C922" s="1" t="s">
         <v>1482</v>
-      </c>
-      <c r="C922" s="1" t="s">
-        <v>1483</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.25">
@@ -15341,7 +15338,7 @@
         <v>0</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="C923" s="1" t="s">
         <v>890</v>
@@ -15352,7 +15349,7 @@
         <v>0</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>890</v>
@@ -15363,10 +15360,10 @@
         <v>0</v>
       </c>
       <c r="B925" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C925" s="1" t="s">
         <v>1486</v>
-      </c>
-      <c r="C925" s="1" t="s">
-        <v>1487</v>
       </c>
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.25">
@@ -15374,7 +15371,7 @@
         <v>0</v>
       </c>
       <c r="B926" s="1" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C926" s="1" t="s">
         <v>381</v>
@@ -15385,7 +15382,7 @@
         <v>0</v>
       </c>
       <c r="B927" s="1" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C927" s="1" t="s">
         <v>381</v>
@@ -15396,10 +15393,10 @@
         <v>0</v>
       </c>
       <c r="B928" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C928" s="1" t="s">
         <v>1490</v>
-      </c>
-      <c r="C928" s="1" t="s">
-        <v>1491</v>
       </c>
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.25">
@@ -15407,7 +15404,7 @@
         <v>0</v>
       </c>
       <c r="B929" s="1" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="C929" s="1" t="s">
         <v>381</v>
@@ -15418,7 +15415,7 @@
         <v>0</v>
       </c>
       <c r="B930" s="1" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="C930" s="1" t="s">
         <v>15</v>
@@ -15429,10 +15426,10 @@
         <v>0</v>
       </c>
       <c r="B931" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C931" s="1" t="s">
         <v>1494</v>
-      </c>
-      <c r="C931" s="1" t="s">
-        <v>1495</v>
       </c>
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.25">
@@ -15440,10 +15437,10 @@
         <v>0</v>
       </c>
       <c r="B932" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C932" s="1" t="s">
         <v>1496</v>
-      </c>
-      <c r="C932" s="1" t="s">
-        <v>1497</v>
       </c>
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.25">
@@ -15451,10 +15448,10 @@
         <v>0</v>
       </c>
       <c r="B933" s="1" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C933" s="1" t="s">
         <v>1498</v>
-      </c>
-      <c r="C933" s="1" t="s">
-        <v>1499</v>
       </c>
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.25">
@@ -15462,10 +15459,10 @@
         <v>0</v>
       </c>
       <c r="B934" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C934" s="1" t="s">
         <v>1500</v>
-      </c>
-      <c r="C934" s="1" t="s">
-        <v>1501</v>
       </c>
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.25">
@@ -15473,10 +15470,10 @@
         <v>0</v>
       </c>
       <c r="B935" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C935" s="1" t="s">
         <v>1502</v>
-      </c>
-      <c r="C935" s="1" t="s">
-        <v>1503</v>
       </c>
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.25">
@@ -15484,7 +15481,7 @@
         <v>0</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C936" s="1" t="s">
         <v>491</v>
@@ -15495,7 +15492,7 @@
         <v>0</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C937" s="1" t="s">
         <v>491</v>
@@ -15506,10 +15503,10 @@
         <v>0</v>
       </c>
       <c r="B938" s="1" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C938" s="1" t="s">
         <v>1506</v>
-      </c>
-      <c r="C938" s="1" t="s">
-        <v>1507</v>
       </c>
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.25">
@@ -15517,7 +15514,7 @@
         <v>0</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C939" s="1" t="s">
         <v>298</v>
@@ -15528,7 +15525,7 @@
         <v>0</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C940" s="1" t="s">
         <v>393</v>
@@ -15539,10 +15536,10 @@
         <v>0</v>
       </c>
       <c r="B941" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C941" s="1" t="s">
         <v>1510</v>
-      </c>
-      <c r="C941" s="1" t="s">
-        <v>1511</v>
       </c>
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.25">
@@ -15550,10 +15547,10 @@
         <v>0</v>
       </c>
       <c r="B942" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C942" s="1" t="s">
         <v>1512</v>
-      </c>
-      <c r="C942" s="1" t="s">
-        <v>1513</v>
       </c>
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.25">
@@ -15561,10 +15558,10 @@
         <v>0</v>
       </c>
       <c r="B943" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C943" s="1" t="s">
         <v>1514</v>
-      </c>
-      <c r="C943" s="1" t="s">
-        <v>1515</v>
       </c>
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.25">
@@ -15572,10 +15569,10 @@
         <v>0</v>
       </c>
       <c r="B944" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C944" s="1" t="s">
         <v>1516</v>
-      </c>
-      <c r="C944" s="1" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.25">
@@ -15583,10 +15580,10 @@
         <v>0</v>
       </c>
       <c r="B945" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C945" s="1" t="s">
         <v>1518</v>
-      </c>
-      <c r="C945" s="1" t="s">
-        <v>1519</v>
       </c>
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.25">
@@ -15594,10 +15591,10 @@
         <v>0</v>
       </c>
       <c r="B946" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C946" s="1" t="s">
         <v>1520</v>
-      </c>
-      <c r="C946" s="1" t="s">
-        <v>1521</v>
       </c>
     </row>
     <row r="947" spans="1:3" x14ac:dyDescent="0.25">
@@ -15605,10 +15602,10 @@
         <v>0</v>
       </c>
       <c r="B947" s="1" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C947" s="1" t="s">
         <v>1522</v>
-      </c>
-      <c r="C947" s="1" t="s">
-        <v>1523</v>
       </c>
     </row>
     <row r="948" spans="1:3" x14ac:dyDescent="0.25">
@@ -15616,10 +15613,10 @@
         <v>0</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="949" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -15627,10 +15624,10 @@
         <v>0</v>
       </c>
       <c r="B949" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C949" s="1" t="s">
         <v>1525</v>
-      </c>
-      <c r="C949" s="1" t="s">
-        <v>1526</v>
       </c>
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.25">
@@ -15638,10 +15635,10 @@
         <v>0</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="951" spans="1:3" x14ac:dyDescent="0.25">
@@ -15649,7 +15646,7 @@
         <v>0</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="C951" s="1" t="s">
         <v>358</v>
@@ -15660,10 +15657,10 @@
         <v>0</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="953" spans="1:3" x14ac:dyDescent="0.25">
@@ -15671,10 +15668,10 @@
         <v>0</v>
       </c>
       <c r="B953" s="1" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="954" spans="1:3" x14ac:dyDescent="0.25">
@@ -15682,10 +15679,10 @@
         <v>0</v>
       </c>
       <c r="B954" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C954" s="1" t="s">
         <v>1531</v>
-      </c>
-      <c r="C954" s="1" t="s">
-        <v>1532</v>
       </c>
     </row>
     <row r="955" spans="1:3" x14ac:dyDescent="0.25">
@@ -15693,7 +15690,7 @@
         <v>0</v>
       </c>
       <c r="B955" s="1" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="C955" s="1" t="s">
         <v>1258</v>
@@ -15704,7 +15701,7 @@
         <v>0</v>
       </c>
       <c r="B956" s="1" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="C956" s="1" t="s">
         <v>289</v>
@@ -15715,10 +15712,10 @@
         <v>0</v>
       </c>
       <c r="B957" s="1" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="958" spans="1:3" x14ac:dyDescent="0.25">
@@ -15737,7 +15734,7 @@
         <v>0</v>
       </c>
       <c r="B959" s="1" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="C959" s="1" t="s">
         <v>119</v>
@@ -15748,7 +15745,7 @@
         <v>0</v>
       </c>
       <c r="B960" s="1" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C960" s="1" t="s">
         <v>1128</v>
@@ -15759,10 +15756,10 @@
         <v>0</v>
       </c>
       <c r="B961" s="1" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C961" s="1" t="s">
         <v>1538</v>
-      </c>
-      <c r="C961" s="1" t="s">
-        <v>1539</v>
       </c>
     </row>
     <row r="962" spans="1:3" x14ac:dyDescent="0.25">
@@ -15770,10 +15767,10 @@
         <v>0</v>
       </c>
       <c r="B962" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C962" s="1" t="s">
         <v>1540</v>
-      </c>
-      <c r="C962" s="1" t="s">
-        <v>1541</v>
       </c>
     </row>
     <row r="963" spans="1:3" x14ac:dyDescent="0.25">
@@ -15781,10 +15778,10 @@
         <v>0</v>
       </c>
       <c r="B963" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C963" s="1" t="s">
         <v>1542</v>
-      </c>
-      <c r="C963" s="1" t="s">
-        <v>1543</v>
       </c>
     </row>
     <row r="964" spans="1:3" x14ac:dyDescent="0.25">
@@ -15792,10 +15789,10 @@
         <v>0</v>
       </c>
       <c r="B964" s="1" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="965" spans="1:3" x14ac:dyDescent="0.25">
@@ -15803,10 +15800,10 @@
         <v>0</v>
       </c>
       <c r="B965" s="1" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="966" spans="1:3" x14ac:dyDescent="0.25">
@@ -15814,10 +15811,10 @@
         <v>0</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="967" spans="1:3" x14ac:dyDescent="0.25">
@@ -15825,10 +15822,10 @@
         <v>0</v>
       </c>
       <c r="B967" s="1" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="968" spans="1:3" x14ac:dyDescent="0.25">
@@ -15836,10 +15833,10 @@
         <v>0</v>
       </c>
       <c r="B968" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="969" spans="1:3" x14ac:dyDescent="0.25">
@@ -15847,10 +15844,10 @@
         <v>0</v>
       </c>
       <c r="B969" s="1" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="970" spans="1:3" x14ac:dyDescent="0.25">
@@ -15858,10 +15855,10 @@
         <v>0</v>
       </c>
       <c r="B970" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C970" s="1" t="s">
         <v>1550</v>
-      </c>
-      <c r="C970" s="1" t="s">
-        <v>1551</v>
       </c>
     </row>
     <row r="971" spans="1:3" x14ac:dyDescent="0.25">
@@ -15869,10 +15866,10 @@
         <v>0</v>
       </c>
       <c r="B971" s="1" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="972" spans="1:3" x14ac:dyDescent="0.25">
@@ -15880,10 +15877,10 @@
         <v>0</v>
       </c>
       <c r="B972" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="973" spans="1:3" x14ac:dyDescent="0.25">
@@ -15891,10 +15888,10 @@
         <v>0</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C973" s="1" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="974" spans="1:3" x14ac:dyDescent="0.25">
@@ -15902,10 +15899,10 @@
         <v>0</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C974" s="1" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="975" spans="1:3" x14ac:dyDescent="0.25">
@@ -15913,10 +15910,10 @@
         <v>0</v>
       </c>
       <c r="B975" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C975" s="1" t="s">
         <v>1559</v>
-      </c>
-      <c r="C975" s="1" t="s">
-        <v>1560</v>
       </c>
     </row>
     <row r="976" spans="1:3" x14ac:dyDescent="0.25">
@@ -15924,10 +15921,10 @@
         <v>0</v>
       </c>
       <c r="B976" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C976" s="1" t="s">
         <v>1561</v>
-      </c>
-      <c r="C976" s="1" t="s">
-        <v>1562</v>
       </c>
     </row>
     <row r="977" spans="1:3" x14ac:dyDescent="0.25">
@@ -15935,10 +15932,10 @@
         <v>0</v>
       </c>
       <c r="B977" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C977" s="1" t="s">
         <v>1563</v>
-      </c>
-      <c r="C977" s="1" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="978" spans="1:3" x14ac:dyDescent="0.25">
@@ -15946,10 +15943,10 @@
         <v>0</v>
       </c>
       <c r="B978" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C978" s="1" t="s">
         <v>1565</v>
-      </c>
-      <c r="C978" s="1" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="979" spans="1:3" x14ac:dyDescent="0.25">
@@ -15957,10 +15954,10 @@
         <v>0</v>
       </c>
       <c r="B979" s="1" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C979" s="1" t="s">
         <v>1567</v>
-      </c>
-      <c r="C979" s="1" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="980" spans="1:3" x14ac:dyDescent="0.25">
@@ -15968,10 +15965,10 @@
         <v>0</v>
       </c>
       <c r="B980" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="981" spans="1:3" x14ac:dyDescent="0.25">
@@ -15979,7 +15976,7 @@
         <v>0</v>
       </c>
       <c r="B981" s="1" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C981" s="1" t="s">
         <v>1052</v>
@@ -15990,10 +15987,10 @@
         <v>0</v>
       </c>
       <c r="B982" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C982" s="1" t="s">
         <v>1571</v>
-      </c>
-      <c r="C982" s="1" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="983" spans="1:3" x14ac:dyDescent="0.25">
@@ -16001,7 +15998,7 @@
         <v>0</v>
       </c>
       <c r="B983" s="1" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C983" s="1" t="s">
         <v>362</v>
@@ -16012,7 +16009,7 @@
         <v>0</v>
       </c>
       <c r="B984" s="1" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C984" s="1" t="s">
         <v>803</v>
@@ -16023,10 +16020,10 @@
         <v>0</v>
       </c>
       <c r="B985" s="1" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="986" spans="1:3" x14ac:dyDescent="0.25">
@@ -16034,10 +16031,10 @@
         <v>0</v>
       </c>
       <c r="B986" s="1" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="987" spans="1:3" x14ac:dyDescent="0.25">
@@ -16045,10 +16042,10 @@
         <v>0</v>
       </c>
       <c r="B987" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C987" s="1" t="s">
         <v>1577</v>
-      </c>
-      <c r="C987" s="1" t="s">
-        <v>1578</v>
       </c>
     </row>
     <row r="988" spans="1:3" x14ac:dyDescent="0.25">
@@ -16056,10 +16053,10 @@
         <v>0</v>
       </c>
       <c r="B988" s="1" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="989" spans="1:3" x14ac:dyDescent="0.25">
@@ -16067,10 +16064,10 @@
         <v>0</v>
       </c>
       <c r="B989" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C989" s="1" t="s">
         <v>1580</v>
-      </c>
-      <c r="C989" s="1" t="s">
-        <v>1581</v>
       </c>
     </row>
     <row r="990" spans="1:3" x14ac:dyDescent="0.25">
@@ -16078,10 +16075,10 @@
         <v>0</v>
       </c>
       <c r="B990" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C990" s="1" t="s">
         <v>1582</v>
-      </c>
-      <c r="C990" s="1" t="s">
-        <v>1583</v>
       </c>
     </row>
     <row r="991" spans="1:3" x14ac:dyDescent="0.25">
@@ -16089,10 +16086,10 @@
         <v>0</v>
       </c>
       <c r="B991" s="1" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C991" s="1" t="s">
         <v>1584</v>
-      </c>
-      <c r="C991" s="1" t="s">
-        <v>1585</v>
       </c>
     </row>
     <row r="992" spans="1:3" x14ac:dyDescent="0.25">
@@ -16100,10 +16097,10 @@
         <v>0</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C992" s="1" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="993" spans="1:3" x14ac:dyDescent="0.25">
@@ -16111,10 +16108,10 @@
         <v>0</v>
       </c>
       <c r="B993" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C993" s="1" t="s">
         <v>1587</v>
-      </c>
-      <c r="C993" s="1" t="s">
-        <v>1588</v>
       </c>
     </row>
     <row r="994" spans="1:3" x14ac:dyDescent="0.25">
@@ -16122,10 +16119,10 @@
         <v>0</v>
       </c>
       <c r="B994" s="1" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C994" s="1" t="s">
         <v>1589</v>
-      </c>
-      <c r="C994" s="1" t="s">
-        <v>1590</v>
       </c>
     </row>
     <row r="995" spans="1:3" x14ac:dyDescent="0.25">
@@ -16133,10 +16130,10 @@
         <v>0</v>
       </c>
       <c r="B995" s="1" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C995" s="1" t="s">
         <v>1591</v>
-      </c>
-      <c r="C995" s="1" t="s">
-        <v>1592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A lot things simplified
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AABBCD-9E10-46AC-93D4-2CB0B997CF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375ED437-9AF9-4D32-97D7-D9FBE1DD2A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="3030" windowWidth="25245" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="1592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="1594">
   <si>
     <t>cs</t>
   </si>
@@ -4815,6 +4815,12 @@
   </si>
   <si>
     <t>Aktualizace obrázků</t>
+  </si>
+  <si>
+    <t>lab.atomizer.update.message</t>
+  </si>
+  <si>
+    <t>Atomizér [{{data.name}}] byl aktualizován.</t>
   </si>
 </sst>
 </file>
@@ -5178,10 +5184,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C995"/>
+  <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A971" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A993" sqref="A993"/>
+      <selection activeCell="B984" sqref="B984"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16134,6 +16140,17 @@
       </c>
       <c r="C995" s="1" t="s">
         <v>1591</v>
+      </c>
+    </row>
+    <row r="996" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A996" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B996" s="1" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C996" s="1" t="s">
+        <v>1593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Updated mixture stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDC5DE1-1469-4394-BB7D-C4A5460841A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E313237-D0B2-4CF5-B985-749643390295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="3030" windowWidth="25245" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="1597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1598">
   <si>
     <t>cs</t>
   </si>
@@ -4830,6 +4830,9 @@
   </si>
   <si>
     <t>Liquid [{{data.name}}] byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.mixture.table.vendor</t>
   </si>
 </sst>
 </file>
@@ -5193,7 +5196,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C998"/>
+  <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A975" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B990" sqref="B990"/>
@@ -16182,6 +16185,17 @@
       </c>
       <c r="C998" s="1" t="s">
         <v>1596</v>
+      </c>
+    </row>
+    <row r="999" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A999" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B999" s="1" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C999" s="1" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added default driptip support
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E313237-D0B2-4CF5-B985-749643390295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0674AB85-3D61-435A-A8DB-1E16BFBCFC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="3030" windowWidth="25245" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1602">
   <si>
     <t>cs</t>
   </si>
@@ -4833,6 +4833,18 @@
   </si>
   <si>
     <t>lab.mixture.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.build.driptipId.label</t>
+  </si>
+  <si>
+    <t>Driptip</t>
+  </si>
+  <si>
+    <t>lab.build.driptipId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Zde se předpokládá, že na atomizéru je použitý výchozí nebo oblíbený náústek, tudíž není žádoucí při každém zadávání vapu tento měnit; pokud ovšem bude použitý jiný, lze jej nastavit.</t>
   </si>
 </sst>
 </file>
@@ -5196,10 +5208,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C999"/>
+  <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A975" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B990" sqref="B990"/>
+    <sheetView tabSelected="1" topLeftCell="A969" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B994" sqref="B994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16196,6 +16208,28 @@
       </c>
       <c r="C999" s="1" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1000" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1000" s="1" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C1000" s="1" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1001" s="1" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C1001" s="1" t="s">
+        <v>1601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved build preview; query is not refetching for some reason
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EF20BC-FCED-944D-B7A7-963EF945C559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486ED532-0EE0-1B43-A07D-4ADCA3F0049A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3021" uniqueCount="1606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1607">
   <si>
     <t>cs</t>
   </si>
@@ -4857,6 +4857,9 @@
   </si>
   <si>
     <t>Je to smutné, ale žádný z buildů vybraného atomizéru nemá žádné obrázky.</t>
+  </si>
+  <si>
+    <t>lab.build.preview.driptip</t>
   </si>
 </sst>
 </file>
@@ -5220,10 +5223,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1003"/>
+  <dimension ref="A1:C1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A981" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B990" sqref="B990"/>
+      <selection activeCell="B994" sqref="B994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16264,6 +16267,17 @@
       </c>
       <c r="C1003" s="1" t="s">
         <v>1605</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1004" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1004" s="1" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C1004" s="1" t="s">
+        <v>1599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added shortcut for builds from atomizers
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486ED532-0EE0-1B43-A07D-4ADCA3F0049A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1A917D-76A8-D446-A87C-492FC5C232A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3027" uniqueCount="1608">
   <si>
     <t>cs</t>
   </si>
@@ -4860,6 +4860,9 @@
   </si>
   <si>
     <t>lab.build.preview.driptip</t>
+  </si>
+  <si>
+    <t>lab.atomizer.build.create</t>
   </si>
 </sst>
 </file>
@@ -5223,10 +5226,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1004"/>
+  <dimension ref="A1:C1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A981" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B994" sqref="B994"/>
+      <selection activeCell="B997" sqref="B997"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16278,6 +16281,17 @@
       </c>
       <c r="C1004" s="1" t="s">
         <v>1599</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1005" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1005" s="1" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C1005" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial mod section is done
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1A917D-76A8-D446-A87C-492FC5C232A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB0EDC6-F2C7-5A48-B602-8A3FA575DB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3027" uniqueCount="1608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="1637">
   <si>
     <t>cs</t>
   </si>
@@ -4863,6 +4863,93 @@
   </si>
   <si>
     <t>lab.atomizer.build.create</t>
+  </si>
+  <si>
+    <t>lab.mod.label</t>
+  </si>
+  <si>
+    <t>lab.mod.title</t>
+  </si>
+  <si>
+    <t>lab.mod.filter.title</t>
+  </si>
+  <si>
+    <t>Filtr modů</t>
+  </si>
+  <si>
+    <t>lab.mod.button.create</t>
+  </si>
+  <si>
+    <t>lab.mod.table.name</t>
+  </si>
+  <si>
+    <t>lab.mod.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.mod.table.footer.label</t>
+  </si>
+  <si>
+    <t>Počet modů [{{data.total}}]</t>
+  </si>
+  <si>
+    <t>lab.mod.context.menu</t>
+  </si>
+  <si>
+    <t>Mod [{{data.name}}]</t>
+  </si>
+  <si>
+    <t>lab.mod.preview</t>
+  </si>
+  <si>
+    <t>Náhled modu</t>
+  </si>
+  <si>
+    <t>lab.mod.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit mod</t>
+  </si>
+  <si>
+    <t>lab.mod.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit mod</t>
+  </si>
+  <si>
+    <t>lab.mod.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.mod.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný mod? Bude smazána velké množství dat, která jsou spojená s jeho využitím ve vapování (případně jinde). Použijte s rozvahou, poněvadž není cesty zpět.</t>
+  </si>
+  <si>
+    <t>lab.mod.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.mod.deleted.success</t>
+  </si>
+  <si>
+    <t>Mod [{{data.name}}] byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.mod.index.label</t>
+  </si>
+  <si>
+    <t>lab.mod.index.title</t>
+  </si>
+  <si>
+    <t>Detail modu</t>
+  </si>
+  <si>
+    <t>lab.mod.update.submit</t>
+  </si>
+  <si>
+    <t>lab.mod.updated.message</t>
+  </si>
+  <si>
+    <t>Mod [{{data.name}}] byl úspěšně aktualizován.</t>
   </si>
 </sst>
 </file>
@@ -5226,10 +5313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1005"/>
+  <dimension ref="A1:C1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A981" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B997" sqref="B997"/>
+    <sheetView tabSelected="1" topLeftCell="A1005" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1016" sqref="B1016"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16292,6 +16379,215 @@
       </c>
       <c r="C1005" s="1" t="s">
         <v>374</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1006" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1006" s="1" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C1006" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1007" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1007" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C1007" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1008" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1008" s="1" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C1008" s="1" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1009" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1009" s="1" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C1009" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1010" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1010" s="1" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C1010" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1011" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1011" s="1" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C1011" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1012" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1012" s="1" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C1012" s="1" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1013" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1013" s="1" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C1013" s="1" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1014" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1014" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C1014" s="1" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1015" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1015" s="1" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C1015" s="1" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1016" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1016" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C1016" s="1" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1017" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1017" s="1" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C1017" s="1" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1018" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1018" s="1" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C1018" s="1" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1019" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1019" s="1" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C1019" s="1" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1020" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1020" s="1" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C1020" s="1" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1021" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1021" s="1" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C1021" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1022" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1022" s="1" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C1022" s="1" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1023" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1023" s="1" t="s">
+        <v>1634</v>
+      </c>
+      <c r="C1023" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1024" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1024" s="1" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C1024" s="1" t="s">
+        <v>1636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some more cotton stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB0EDC6-F2C7-5A48-B602-8A3FA575DB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128289C-F7DB-4F44-B2F0-1C52B2DB4073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="1637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="1663">
   <si>
     <t>cs</t>
   </si>
@@ -4950,6 +4950,84 @@
   </si>
   <si>
     <t>Mod [{{data.name}}] byl úspěšně aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.cotton.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.title</t>
+  </si>
+  <si>
+    <t>lab.cotton.filter.title</t>
+  </si>
+  <si>
+    <t>Filtr vat</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.create</t>
+  </si>
+  <si>
+    <t>Nová vata</t>
+  </si>
+  <si>
+    <t>lab.cotton.table.name</t>
+  </si>
+  <si>
+    <t>lab.cotton.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.cotton.context.menu</t>
+  </si>
+  <si>
+    <t>Vata [{{data.name}}]</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit vatu</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit vatu</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybranou vatu? Tato akce pravděpodobně smaže velké množství jiných dat, hlavně pak záznamy o vapování. Není cesty zpět, postupujte tedy prosím obezřetně.</t>
+  </si>
+  <si>
+    <t>lab.cotton.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.cotton.table.description</t>
+  </si>
+  <si>
+    <t>lab.cotton.index.label</t>
+  </si>
+  <si>
+    <t>lab.cotton.index.title</t>
+  </si>
+  <si>
+    <t>Detail vaty</t>
+  </si>
+  <si>
+    <t>lab.cotton.update.submit</t>
+  </si>
+  <si>
+    <t>Aktulizovat vatu</t>
+  </si>
+  <si>
+    <t>lab.cotton.updated.message</t>
+  </si>
+  <si>
+    <t>Vata [{{data.name}}] byla aktualizována.</t>
   </si>
 </sst>
 </file>
@@ -5313,10 +5391,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1024"/>
+  <dimension ref="A1:C1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1005" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1016" sqref="B1016"/>
+    <sheetView tabSelected="1" topLeftCell="A1018" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1030" sqref="B1030"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16588,6 +16666,204 @@
       </c>
       <c r="C1024" s="1" t="s">
         <v>1636</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1025" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1025" s="1" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C1025" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1026" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1026" s="1" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C1026" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1027" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C1027" s="1" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1028" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C1028" s="1" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1029" s="1" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C1029" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1030" s="1" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C1030" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1031" s="1" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C1031" s="1" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1032" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1032" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C1032" s="1" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1033" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1033" s="1" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C1033" s="1" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1034" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1034" s="1" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C1034" s="1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1035" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1035" s="1" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C1035" s="1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1036" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1036" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C1036" s="1" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1037" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1037" s="1" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C1037" s="1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1038" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1038" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C1038" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1039" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1039" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C1039" s="1" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1040" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1040" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C1040" s="1" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1041" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1041" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C1041" s="1" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1042" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1042" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C1042" s="1" t="s">
+        <v>1662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial wire stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128289C-F7DB-4F44-B2F0-1C52B2DB4073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F68B58-D12B-FB41-BC83-CD836DFFDB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="1663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="1672">
   <si>
     <t>cs</t>
   </si>
@@ -5028,6 +5028,33 @@
   </si>
   <si>
     <t>Vata [{{data.name}}] byla aktualizována.</t>
+  </si>
+  <si>
+    <t>lab.wire.label</t>
+  </si>
+  <si>
+    <t>lab.wire.title</t>
+  </si>
+  <si>
+    <t>lab.wire.button.create</t>
+  </si>
+  <si>
+    <t>lab.wire.filter.title</t>
+  </si>
+  <si>
+    <t>Filtr drátů</t>
+  </si>
+  <si>
+    <t>lab.wire.table.name</t>
+  </si>
+  <si>
+    <t>lab.wire.table.ga</t>
+  </si>
+  <si>
+    <t>lab.wire.table.description</t>
+  </si>
+  <si>
+    <t>lab.wire.table.vendor</t>
   </si>
 </sst>
 </file>
@@ -5391,10 +5418,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1042"/>
+  <dimension ref="A1:C1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1018" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1030" sqref="B1030"/>
+    <sheetView tabSelected="1" topLeftCell="A1027" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1049" sqref="B1049"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16864,6 +16891,94 @@
       </c>
       <c r="C1042" s="1" t="s">
         <v>1662</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1043" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1043" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C1043" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1044" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1044" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C1044" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1045" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1045" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C1045" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1046" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1046" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C1046" s="1" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1047" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1047" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C1047" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1048" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1048" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C1048" s="1" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1049" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1049" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C1049" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1050" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1050" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C1050" s="1" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Updated wire stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F68B58-D12B-FB41-BC83-CD836DFFDB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B28DA59-69FB-B740-AFC3-6229C57500A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="1672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="1688">
   <si>
     <t>cs</t>
   </si>
@@ -5055,6 +5055,54 @@
   </si>
   <si>
     <t>lab.wire.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.wire.context.menu</t>
+  </si>
+  <si>
+    <t>Drát [{{data.name}}]</t>
+  </si>
+  <si>
+    <t>lab.wire.preview</t>
+  </si>
+  <si>
+    <t>Náhled drátu</t>
+  </si>
+  <si>
+    <t>lab.wire.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit drát</t>
+  </si>
+  <si>
+    <t>lab.wire.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit drát</t>
+  </si>
+  <si>
+    <t>lab.wire.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.wire.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný drát? Můžete tím smazst velké množství dat, hlavně pak záznamy o vapování. Není cesty zpět, dbejte prosím zvýšené opatrnosti.</t>
+  </si>
+  <si>
+    <t>lab.wire.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.wire.deleted.success</t>
+  </si>
+  <si>
+    <t>Drát [{{data.name}}] byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.wire.table.footer.label</t>
+  </si>
+  <si>
+    <t>Počet drátů [{{data.total}}]</t>
   </si>
 </sst>
 </file>
@@ -5418,10 +5466,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1050"/>
+  <dimension ref="A1:C1059"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1027" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1049" sqref="B1049"/>
+    <sheetView tabSelected="1" topLeftCell="A1031" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1054" sqref="B1054"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16979,6 +17027,105 @@
       </c>
       <c r="C1050" s="1" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1051" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1051" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C1051" s="1" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1052" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1052" s="1" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C1052" s="1" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1053" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1053" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C1053" s="1" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1054" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1054" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="C1054" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1055" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1055" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C1055" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1056" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1056" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C1056" s="1" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1057" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1057" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C1057" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1058" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1058" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C1058" s="1" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1059" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1059" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C1059" s="1" t="s">
+        <v>1687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite nice vendor stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B28DA59-69FB-B740-AFC3-6229C57500A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1D2DB7-1EAD-A641-8C48-766AE922EC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="1717">
   <si>
     <t>cs</t>
   </si>
@@ -5103,6 +5103,93 @@
   </si>
   <si>
     <t>Počet drátů [{{data.total}}]</t>
+  </si>
+  <si>
+    <t>lab.vendor.label</t>
+  </si>
+  <si>
+    <t>lab.vendor.title</t>
+  </si>
+  <si>
+    <t>lab.vendor.table.name</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.create</t>
+  </si>
+  <si>
+    <t>Nový výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.filter.title</t>
+  </si>
+  <si>
+    <t>Filtrovat výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.context.menu</t>
+  </si>
+  <si>
+    <t>Výrobce [{{data.name}}]</t>
+  </si>
+  <si>
+    <t>lab.vendor.preview</t>
+  </si>
+  <si>
+    <t>Náhled výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit výrobce</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.vendor.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraného výrobce? Tento krok s sebou efektivně může vzít opravdu velké množství dat ze systému, jelikož výrobci jsou použiti u atomizérů, modů, drátů, zkrátka všude. Díky tomu může dojít k brutálnímu promazání dat. Před tím, než budete pokračovat, se hezky pomodlete ke svému oblíbenému božstvu.</t>
+  </si>
+  <si>
+    <t>lab.vendor.table.footer.label</t>
+  </si>
+  <si>
+    <t>Počet výrobců [{{data.total}}]</t>
+  </si>
+  <si>
+    <t>lab.vendor.preview.name</t>
+  </si>
+  <si>
+    <t>lab.vendor.common.tab</t>
+  </si>
+  <si>
+    <t>lab.vendor.atomizers.tab</t>
+  </si>
+  <si>
+    <t>lab.vendor.mods.tab</t>
+  </si>
+  <si>
+    <t>lab.vendor.liquid.tab</t>
+  </si>
+  <si>
+    <t>lab.vendor.index.label</t>
+  </si>
+  <si>
+    <t>lab.vendor.index.title</t>
+  </si>
+  <si>
+    <t>Detail výrobce</t>
   </si>
 </sst>
 </file>
@@ -5466,10 +5553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1059"/>
+  <dimension ref="A1:C1080"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1031" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1054" sqref="B1054"/>
+    <sheetView tabSelected="1" topLeftCell="A1053" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1071" sqref="B1071"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17126,6 +17213,237 @@
       </c>
       <c r="C1059" s="1" t="s">
         <v>1687</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1060" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1060" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C1060" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1061" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1061" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C1061" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1062" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1062" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C1062" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1063" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1063" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C1063" s="1" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1064" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1064" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C1064" s="1" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1065" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1065" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C1065" s="1" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1066" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1066" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C1066" s="1" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1067" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1067" s="1" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C1067" s="1" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1068" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1068" s="1" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C1068" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1069" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1069" s="1" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C1069" s="1" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1070" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1070" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C1070" s="1" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1071" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1071" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C1071" s="1" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A1072" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1072" s="1" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C1072" s="1" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1073" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1073" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C1073" s="1" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1074" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1074" s="1" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C1074" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1075" s="1" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C1075" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1076" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1076" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C1076" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1077" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1077" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1077" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1078" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1078" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C1078" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1079" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1079" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C1079" s="1" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1080" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1080" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C1080" s="1" t="s">
+        <v>1716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Prepared cell stuff, improved some little pieces on the other places
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1D2DB7-1EAD-A641-8C48-766AE922EC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F908D6B-D4F0-F442-8881-6231EB62C115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="2560" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1784">
   <si>
     <t>cs</t>
   </si>
@@ -5190,6 +5190,207 @@
   </si>
   <si>
     <t>Detail výrobce</t>
+  </si>
+  <si>
+    <t>lab.cell.label</t>
+  </si>
+  <si>
+    <t>lab.cell.title</t>
+  </si>
+  <si>
+    <t>lab.cell.button.create</t>
+  </si>
+  <si>
+    <t>Nový článek</t>
+  </si>
+  <si>
+    <t>lab.cell.filter.title</t>
+  </si>
+  <si>
+    <t>Filtrování článků</t>
+  </si>
+  <si>
+    <t>lab.cell.table.name</t>
+  </si>
+  <si>
+    <t>lab.cell.table.size</t>
+  </si>
+  <si>
+    <t>lab.cell.table.drain</t>
+  </si>
+  <si>
+    <t>Vybíjecí proud</t>
+  </si>
+  <si>
+    <t>lab.cell.table.voltage</t>
+  </si>
+  <si>
+    <t>Napětí</t>
+  </si>
+  <si>
+    <t>lab.cell.table.ohm</t>
+  </si>
+  <si>
+    <t>Bezpečný odpor</t>
+  </si>
+  <si>
+    <t>lab.cell.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.cell.table.footer.label</t>
+  </si>
+  <si>
+    <t>Počet článků [{{data.total}}]</t>
+  </si>
+  <si>
+    <t>lab.cell.name.label</t>
+  </si>
+  <si>
+    <t>lab.cell.name.label.tooltip</t>
+  </si>
+  <si>
+    <t>Použijte prosím obchodní označení článku tak, aby ostatní mohli tento článek snadno najít. </t>
+  </si>
+  <si>
+    <t>lab.cell.drain.label</t>
+  </si>
+  <si>
+    <t>lab.cell.drain.label.tooltip</t>
+  </si>
+  <si>
+    <t>Bezpečný vybíjecí proud článku; uveďte prosím reálnou hodnotu, poněvadž aplikace s ní pak bude počítat pro různé kontroly a pokud by tato hodnota neodpovádala realitě, může vás to pak ohrozit. Tak či tak, pro výpočet bezpečného odporu na tomto článkui je použito pouze 75% vybíjecího proudu, poněvadž se očekává, že výrobci budou optimisti a nám to za to nestojí.</t>
+  </si>
+  <si>
+    <t>lab.cell.vendorId.label</t>
+  </si>
+  <si>
+    <t>lab.cell.voltage.label</t>
+  </si>
+  <si>
+    <t>lab.cell.voltage.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tuto hodnotu standardně není třeba měnit, pokud ovšem nemáte nějaký ultra zvláštní článek.</t>
+  </si>
+  <si>
+    <t>lab.cell.create.submit</t>
+  </si>
+  <si>
+    <t>lab.cell.size.label</t>
+  </si>
+  <si>
+    <t>Velikost článku</t>
+  </si>
+  <si>
+    <t>lab.cell.size.label.tooltip</t>
+  </si>
+  <si>
+    <t>Použijte prosím standardní rozměr udaný výrobcem (např. 21700) .</t>
+  </si>
+  <si>
+    <t>lab.cell.size.label.required</t>
+  </si>
+  <si>
+    <t>Prosím udejte velikost článku.</t>
+  </si>
+  <si>
+    <t>lab.cell.create.success</t>
+  </si>
+  <si>
+    <t>Článek [{{data.vendor.name}} {{data.name}}] byl úspěšně uložen.</t>
+  </si>
+  <si>
+    <t>lab.cell.preview.name</t>
+  </si>
+  <si>
+    <t>lab.cell.context.menu</t>
+  </si>
+  <si>
+    <t>Článek [{{data.vendor.name}} {{data.name}}]</t>
+  </si>
+  <si>
+    <t>lab.cell.preview</t>
+  </si>
+  <si>
+    <t>Náhled článku</t>
+  </si>
+  <si>
+    <t>lab.cell.button.edit</t>
+  </si>
+  <si>
+    <t>Upravit článek</t>
+  </si>
+  <si>
+    <t>lab.cell.button.delete</t>
+  </si>
+  <si>
+    <t>Odstranit článek</t>
+  </si>
+  <si>
+    <t>lab.cell.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.cell.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.cell.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný článek? Tato skce je nezvratná a může být smazáno větší množství dat.</t>
+  </si>
+  <si>
+    <t>lab.cell.deleted.success</t>
+  </si>
+  <si>
+    <t>Článek [{{data.vendor.name}} {{data.name}}] byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.cell.index.label</t>
+  </si>
+  <si>
+    <t>lab.cell.index.title</t>
+  </si>
+  <si>
+    <t>Detail článku</t>
+  </si>
+  <si>
+    <t>lab.cell.preview.size</t>
+  </si>
+  <si>
+    <t>lab.cell.preview.drain</t>
+  </si>
+  <si>
+    <t>lab.cell.preview.ohm</t>
+  </si>
+  <si>
+    <t>Minimální bezpečný odpor</t>
+  </si>
+  <si>
+    <t>lab.cell.preview.voltage</t>
+  </si>
+  <si>
+    <t>Pracovní napětí</t>
+  </si>
+  <si>
+    <t>lab.cell.update.submit</t>
+  </si>
+  <si>
+    <t>lab.cell.updated.message</t>
+  </si>
+  <si>
+    <t>Článek [{{data.vendor.name}} {{data.name}}] byl úspěšně aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.mod.table.power</t>
+  </si>
+  <si>
+    <t>lab.mod.preview.power</t>
+  </si>
+  <si>
+    <t>Maximální výkon</t>
+  </si>
+  <si>
+    <t>lab.liquid.table.vendor</t>
   </si>
 </sst>
 </file>
@@ -5553,10 +5754,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1080"/>
+  <dimension ref="A1:C1123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1053" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1071" sqref="B1071"/>
+    <sheetView tabSelected="1" topLeftCell="A1098" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1112" sqref="B1112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17444,6 +17645,479 @@
       </c>
       <c r="C1080" s="1" t="s">
         <v>1716</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1081" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1081" s="1" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C1081" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1082" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1082" s="1" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C1082" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1083" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1083" s="1" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C1083" s="1" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1084" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1084" s="1" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C1084" s="1" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1085" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1085" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C1085" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1086" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1086" s="1" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C1086" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1087" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1087" s="1" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1087" s="1" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1088" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1088" s="1" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C1088" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1089" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1089" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C1089" s="1" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1090" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1090" s="1" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C1090" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1091" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1091" s="1" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C1091" s="1" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1092" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1092" s="1" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C1092" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1093" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1093" s="1" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C1093" s="1" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1094" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1094" s="1" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C1094" s="1" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A1095" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1095" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C1095" s="1" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1096" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1096" s="1" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C1096" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1097" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1097" s="1" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C1097" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1098" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C1098" s="1" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1099" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C1099" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1100" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C1100" s="1" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1101" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C1101" s="1" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1102" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C1102" s="1" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1103" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C1103" s="1" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1104" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C1104" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1105" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C1105" s="1" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1106" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C1106" s="1" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1107" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C1107" s="1" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1108" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C1108" s="1" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1109" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C1109" s="1" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1110" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1110" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C1110" s="1" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1111" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C1111" s="1" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1112" s="1" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C1112" s="1" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1113" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C1113" s="1" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1114" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C1114" s="1" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1115" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C1115" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1116" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C1116" s="1" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1117" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="C1117" s="1" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1118" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1118" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C1118" s="1" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1119" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C1119" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1120" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C1120" s="1" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1121" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C1121" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1122" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="C1122" s="1" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1123" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="C1123" s="1" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A little build tuning
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F908D6B-D4F0-F442-8881-6231EB62C115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A90B83-5C9E-CC46-9519-F05CA1749B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2560" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3390" uniqueCount="1788">
   <si>
     <t>cs</t>
   </si>
@@ -5391,6 +5391,18 @@
   </si>
   <si>
     <t>lab.liquid.table.vendor</t>
+  </si>
+  <si>
+    <t>lab.cotton.preview.description</t>
+  </si>
+  <si>
+    <t>lab.build.create.other.tab</t>
+  </si>
+  <si>
+    <t>lab.build.other.no-builds</t>
+  </si>
+  <si>
+    <t>Tento atomizér nemá zatím žádné buildy.</t>
   </si>
 </sst>
 </file>
@@ -5754,10 +5766,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1123"/>
+  <dimension ref="A1:C1126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1098" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1112" sqref="B1112"/>
+      <selection activeCell="B1120" sqref="B1120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18118,6 +18130,39 @@
       </c>
       <c r="C1123" s="1" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1124" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="C1124" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1125" s="1" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C1125" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1126" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C1126" s="1" t="s">
+        <v>1787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial idea of quick puff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A6D07-4B59-E142-BBC3-5C3873CF5014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635C754B-0E35-834D-97B8-B7CAE7A306B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3399" uniqueCount="1794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1800">
   <si>
     <t>cs</t>
   </si>
@@ -5421,6 +5421,24 @@
   </si>
   <si>
     <t>Atomizér [{{data.name}}] byl odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.quick-puff.builds.title</t>
+  </si>
+  <si>
+    <t>lab.quick-puff.builds.subtitle</t>
+  </si>
+  <si>
+    <t>Nejnovější aktivní buildy</t>
+  </si>
+  <si>
+    <t>lab.quick-puff.vapes.title</t>
+  </si>
+  <si>
+    <t>lab.quick-puff.vapes.subtitle</t>
+  </si>
+  <si>
+    <t>Nejnovější vape</t>
   </si>
 </sst>
 </file>
@@ -5784,7 +5802,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1129"/>
+  <dimension ref="A1:C1133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1123" sqref="B1123"/>
@@ -18214,6 +18232,50 @@
       </c>
       <c r="C1129" s="1" t="s">
         <v>1793</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1130" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1130" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C1130" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1131" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C1131" s="1" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1132" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C1132" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1133" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C1133" s="1" t="s">
+        <v>1799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A little improvements
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635C754B-0E35-834D-97B8-B7CAE7A306B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4234926-FCBD-E34B-9AF3-349E0FBDB3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="1803">
   <si>
     <t>cs</t>
   </si>
@@ -5439,6 +5439,15 @@
   </si>
   <si>
     <t>Nejnovější vape</t>
+  </si>
+  <si>
+    <t>lab.build.age.tooltip</t>
+  </si>
+  <si>
+    <t>lab.vape.age.tooltip</t>
+  </si>
+  <si>
+    <t>Stáří vapu</t>
   </si>
 </sst>
 </file>
@@ -5802,10 +5811,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1133"/>
+  <dimension ref="A1:C1135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1123" sqref="B1123"/>
+      <selection activeCell="B1127" sqref="B1127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18276,6 +18285,28 @@
       </c>
       <c r="C1133" s="1" t="s">
         <v>1799</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1134" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1134" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C1134" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1135" s="1" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C1135" s="1" t="s">
+        <v>1802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Experimenta plot on home screen
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4234926-FCBD-E34B-9AF3-349E0FBDB3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED625EF-1E03-854C-8013-9E598A30563C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="1803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="1804">
   <si>
     <t>cs</t>
   </si>
@@ -5448,6 +5448,9 @@
   </si>
   <si>
     <t>Stáří vapu</t>
+  </si>
+  <si>
+    <t>lab.quick-puff.plot.title</t>
   </si>
 </sst>
 </file>
@@ -5811,10 +5814,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1135"/>
+  <dimension ref="A1:C1136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1127" sqref="B1127"/>
+    <sheetView tabSelected="1" topLeftCell="A1111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1129" sqref="B1129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18307,6 +18310,17 @@
       </c>
       <c r="C1135" s="1" t="s">
         <v>1802</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1136" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1136" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C1136" s="1" t="s">
+        <v>728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added leaks, fied vape
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED625EF-1E03-854C-8013-9E598A30563C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B798DAC-4E66-A64C-89A5-95D490AC7C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="500" windowWidth="25240" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="1804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3423" uniqueCount="1805">
   <si>
     <t>cs</t>
   </si>
@@ -5451,6 +5451,9 @@
   </si>
   <si>
     <t>lab.quick-puff.plot.title</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.leask.column</t>
   </si>
 </sst>
 </file>
@@ -5814,10 +5817,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1136"/>
+  <dimension ref="A1:C1137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1129" sqref="B1129"/>
+      <selection activeCell="B1135" sqref="B1135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18321,6 +18324,17 @@
       </c>
       <c r="C1136" s="1" t="s">
         <v>728</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1137" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C1137" s="1" t="s">
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Sooo, atomizer purchasing as a prototype somehow works!
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669984A8-0F49-4691-8441-3DD006FBB491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23813657-95B3-4EBC-B7BE-705A5B8D2BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="1050" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3453" uniqueCount="1824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3495" uniqueCount="1845">
   <si>
     <t>cs</t>
   </si>
@@ -5511,6 +5511,69 @@
   </si>
   <si>
     <t>lab.build.image.upload.failed</t>
+  </si>
+  <si>
+    <t>lab.atomizer.purchase.button</t>
+  </si>
+  <si>
+    <t>Pořídit atomizér</t>
+  </si>
+  <si>
+    <t>lab.atomizer.purchase.submit</t>
+  </si>
+  <si>
+    <t>Pořídit</t>
+  </si>
+  <si>
+    <t>lab.atomizer.purchase.driptipId.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.purchase.driptipId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Můžete si vybrat náústek k atomizéru, který se pak bude nabízet jako výchozí ve zbytku aplikace (např. můžete vytvořit a přiřadit výchozí náústek výrobce - něco jako Taifun GT IV Native nebo tak).</t>
+  </si>
+  <si>
+    <t>lab.atomizer.purchase.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste si pořídili atomizér [{{data.atomizer.name}}].</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.button.delete</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.button.delete.confirm.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.button.delete.confirm.ok</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.button.delete.confirm</t>
+  </si>
+  <si>
+    <t>Opravdu si přejete odstranit vybraný atomizér? Tato akce pouze odstraní záznam o jeho vlastnictví a přidružená data (např. výchozí náústek). Dále se přestane nabízet v různých seznamech. Tato akce je nezvratná, nikoli však destruktivní.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.deleted.success</t>
+  </si>
+  <si>
+    <t>Atomizér [{{data.atomizer.name}}] byl úspěšně odstraněn.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.edit.button</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.driptipId.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.update</t>
+  </si>
+  <si>
+    <t>lab.atomizer.user.update.success</t>
+  </si>
+  <si>
+    <t>Atomizér byl úspěšně uložen.</t>
   </si>
 </sst>
 </file>
@@ -5874,10 +5937,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1147"/>
+  <dimension ref="A1:C1161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1137" sqref="B1137"/>
+    <sheetView tabSelected="1" topLeftCell="A1129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1154" sqref="B1154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18502,6 +18565,160 @@
       </c>
       <c r="C1147" s="1" t="s">
         <v>1818</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1148" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1148" s="1" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1149" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C1149" s="1" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1150" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1150" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C1150" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1151" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C1151" s="1" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1152" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C1152" s="1" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1153" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C1153" s="1" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1154" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C1154" s="1" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1155" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C1155" s="1" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1156" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C1156" s="1" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1157" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1157" s="1" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1158" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1158" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C1158" s="1" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1159" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C1159" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1160" s="1" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C1160" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1161" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C1161" s="1" t="s">
+        <v>1844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some experiment with tags on atomizer and wires
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3F79C9-6F69-43AA-B394-F4B513A75C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51366B-45AE-423D-8499-DE7CE24CD8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1965" yWindow="2685" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="1860">
   <si>
     <t>cs</t>
   </si>
@@ -5601,6 +5601,24 @@
   </si>
   <si>
     <t>lab.atomizer.table.draw</t>
+  </si>
+  <si>
+    <t>lab.wire.table.draw</t>
+  </si>
+  <si>
+    <t>Vhodný pro</t>
+  </si>
+  <si>
+    <t>lab.wire.drawIds.label</t>
+  </si>
+  <si>
+    <t>lab.wire.update.submit</t>
+  </si>
+  <si>
+    <t>lab.wire.updated.message</t>
+  </si>
+  <si>
+    <t>Drát [{{data.name}}] byl úspěšně aktualizován.</t>
   </si>
 </sst>
 </file>
@@ -5964,10 +5982,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1168"/>
+  <dimension ref="A1:C1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1157" sqref="B1157"/>
+      <selection activeCell="B1162" sqref="B1162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18823,6 +18841,61 @@
       </c>
       <c r="C1168" s="1" t="s">
         <v>1845</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1169" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C1169" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1170" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C1170" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1171" s="1" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C1171" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1172" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1172" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C1172" s="1" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1173" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C1173" s="1" t="s">
+        <v>1855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added tag support for builds (mark draw type with tags)
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51366B-45AE-423D-8499-DE7CE24CD8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A428845B-A6A6-4E01-AD31-B91AC1E42147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="2685" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="2340" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="1860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="1863">
   <si>
     <t>cs</t>
   </si>
@@ -5619,6 +5619,15 @@
   </si>
   <si>
     <t>Drát [{{data.name}}] byl úspěšně aktualizován.</t>
+  </si>
+  <si>
+    <t>lab.build.drawIds.label</t>
+  </si>
+  <si>
+    <t>lab.build.preview.draw</t>
+  </si>
+  <si>
+    <t>lab.build.table.draw</t>
   </si>
 </sst>
 </file>
@@ -5982,10 +5991,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1173"/>
+  <dimension ref="A1:C1176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1162" sqref="B1162"/>
+      <selection activeCell="B1171" sqref="B1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18896,6 +18905,39 @@
       </c>
       <c r="C1173" s="1" t="s">
         <v>1855</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1174" s="1" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C1174" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1175" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C1175" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1176" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C1176" s="1" t="s">
+        <v>1845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added draw type filter to vapes
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A428845B-A6A6-4E01-AD31-B91AC1E42147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0F0405-6DDB-4416-854A-3B8306C91F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="2340" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="1863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="1864">
   <si>
     <t>cs</t>
   </si>
@@ -5628,6 +5628,9 @@
   </si>
   <si>
     <t>lab.build.table.draw</t>
+  </si>
+  <si>
+    <t>lab.vape.drawIds.label</t>
   </si>
 </sst>
 </file>
@@ -5991,10 +5994,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1176"/>
+  <dimension ref="A1:C1177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1171" sqref="B1171"/>
+      <selection activeCell="B1164" sqref="B1164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18937,6 +18940,17 @@
         <v>1862</v>
       </c>
       <c r="C1176" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1177" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C1177" s="1" t="s">
         <v>1845</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Draw type on atomizer
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0F0405-6DDB-4416-854A-3B8306C91F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A795F9-66D2-4A35-A3C0-DBA1257D4E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="2340" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="1864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="1865">
   <si>
     <t>cs</t>
   </si>
@@ -5631,6 +5631,9 @@
   </si>
   <si>
     <t>lab.vape.drawIds.label</t>
+  </si>
+  <si>
+    <t>lab.atomizer.preview.draw</t>
   </si>
 </sst>
 </file>
@@ -5994,10 +5997,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1177"/>
+  <dimension ref="A1:C1178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1164" sqref="B1164"/>
+      <selection activeCell="B1163" sqref="B1163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18951,6 +18954,17 @@
         <v>1863</v>
       </c>
       <c r="C1177" s="1" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1178" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C1178" s="1" t="s">
         <v>1845</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Common: Added an experimental feature with displaying comments in index
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A795F9-66D2-4A35-A3C0-DBA1257D4E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E73E0D-38AB-457F-8EC8-33F19FA15712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="2340" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9285" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="1865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1871">
   <si>
     <t>cs</t>
   </si>
@@ -5634,6 +5634,24 @@
   </si>
   <si>
     <t>lab.atomizer.preview.draw</t>
+  </si>
+  <si>
+    <t>lab.vape.comments.drawer.button</t>
+  </si>
+  <si>
+    <t>Komentáře k vapům</t>
+  </si>
+  <si>
+    <t>lab.build.comments.drawer.button</t>
+  </si>
+  <si>
+    <t>Komentáře k buildům</t>
+  </si>
+  <si>
+    <t>lab.vape.comments.drawer.title</t>
+  </si>
+  <si>
+    <t>lab.build.comments.drawer.title</t>
   </si>
 </sst>
 </file>
@@ -5997,10 +6015,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1178"/>
+  <dimension ref="A1:C1182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1163" sqref="B1163"/>
+    <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1171" sqref="B1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18966,6 +18984,50 @@
       </c>
       <c r="C1178" s="1" t="s">
         <v>1845</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1179" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C1179" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1180" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C1180" s="1" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1181" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="C1181" s="1" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1182" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C1182" s="1" t="s">
+        <v>1868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added atomizer comments
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E73E0D-38AB-457F-8EC8-33F19FA15712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7327E52B-702A-4B40-93C7-7DF7C36CC36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9285" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="1874">
   <si>
     <t>cs</t>
   </si>
@@ -5652,6 +5652,15 @@
   </si>
   <si>
     <t>lab.build.comments.drawer.title</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.drawer.button</t>
+  </si>
+  <si>
+    <t>Komentáře k atomizérům</t>
+  </si>
+  <si>
+    <t>lab.atomizer.comments.drawer.title</t>
   </si>
 </sst>
 </file>
@@ -6015,10 +6024,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1182"/>
+  <dimension ref="A1:C1184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1171" sqref="B1171"/>
+      <selection activeCell="B1177" sqref="B1177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19028,6 +19037,28 @@
       </c>
       <c r="C1182" s="1" t="s">
         <v>1868</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1183" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C1183" s="1" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1184" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C1184" s="1" t="s">
+        <v>1872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Filtered user's comments
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE83A70-EEE0-4C64-971F-1D73AB038E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C69AEA4-96BF-4FC1-851E-F2B8465F8A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7905" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="1875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="1877">
   <si>
     <t>cs</t>
   </si>
@@ -5664,6 +5664,12 @@
   </si>
   <si>
     <t>Volné MTL</t>
+  </si>
+  <si>
+    <t>lab.mixture.comments.drawer.button</t>
+  </si>
+  <si>
+    <t>lab.mixture.comments.drawer.title</t>
   </si>
 </sst>
 </file>
@@ -6027,10 +6033,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1187"/>
+  <dimension ref="A1:C1189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1187" sqref="C1187"/>
+      <selection activeCell="B1171" sqref="B1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19095,6 +19101,28 @@
       </c>
       <c r="C1187" s="1" t="s">
         <v>1874</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1188" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1188" s="1" t="s">
+        <v>1875</v>
+      </c>
+      <c r="C1188" s="1" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1189" s="1" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C1189" s="1" t="s">
+        <v>1127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added possibility to add default mod to a build
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3673FF-3893-4B92-A452-9B014871DB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BD5F96-98D2-4552-AFA2-43F013D4F09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7905" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3618" uniqueCount="1894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="1898">
   <si>
     <t>cs</t>
   </si>
@@ -5721,6 +5721,18 @@
   </si>
   <si>
     <t>lab.atomizer.table.type</t>
+  </si>
+  <si>
+    <t>lab.build.modId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Výchozí mod pro tento build; je použitý pouze pro předvyplnění dat o vapování.</t>
+  </si>
+  <si>
+    <t>lab.build.preview.mod</t>
+  </si>
+  <si>
+    <t>lab.build.table.mod</t>
   </si>
 </sst>
 </file>
@@ -6084,10 +6096,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1202"/>
+  <dimension ref="A1:C1205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1193" sqref="B1193"/>
+    <sheetView tabSelected="1" topLeftCell="A1168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1198" sqref="B1198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19317,6 +19329,39 @@
       </c>
       <c r="C1202" s="1" t="s">
         <v>1892</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1203" s="1" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C1203" s="1" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1204" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1204" s="1" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C1204" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1205" s="1" t="s">
+        <v>1897</v>
+      </c>
+      <c r="C1205" s="1" t="s">
+        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Experimental upgrade of build creation
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BD5F96-98D2-4552-AFA2-43F013D4F09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0DE6FE-D0BD-4C5A-9F6D-244F6F71A081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7905" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="1898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1899">
   <si>
     <t>cs</t>
   </si>
@@ -5733,6 +5733,9 @@
   </si>
   <si>
     <t>lab.build.table.mod</t>
+  </si>
+  <si>
+    <t>lab.build.create.form.tab</t>
   </si>
 </sst>
 </file>
@@ -6096,10 +6099,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1205"/>
+  <dimension ref="A1:C1206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1198" sqref="B1198"/>
+      <selection activeCell="B1204" sqref="B1204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19362,6 +19365,17 @@
       </c>
       <c r="C1205" s="1" t="s">
         <v>672</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1206" s="1" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C1206" s="1" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved plot and much improved vape preview
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0DE6FE-D0BD-4C5A-9F6D-244F6F71A081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB427A-46FB-4183-902F-5C0A3C3B77AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="2805" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="2145" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="1809">
   <si>
     <t>cs</t>
   </si>
@@ -4139,294 +4139,6 @@
     <t>lab.vape.plot.label</t>
   </si>
   <si>
-    <t>lab.build.coilOffset.-2</t>
-  </si>
-  <si>
-    <t>Nejníže</t>
-  </si>
-  <si>
-    <t>lab.build.coilOffset.-1</t>
-  </si>
-  <si>
-    <t>Níže</t>
-  </si>
-  <si>
-    <t>lab.build.coilOffset.0</t>
-  </si>
-  <si>
-    <t>Střed</t>
-  </si>
-  <si>
-    <t>lab.build.coilOffset.1</t>
-  </si>
-  <si>
-    <t>Výše</t>
-  </si>
-  <si>
-    <t>lab.build.coilOffset.2</t>
-  </si>
-  <si>
-    <t>Nejvýše</t>
-  </si>
-  <si>
-    <t>lab.build.cottonOffset.-2</t>
-  </si>
-  <si>
-    <t>Méně</t>
-  </si>
-  <si>
-    <t>lab.build.cottonOffset.-1</t>
-  </si>
-  <si>
-    <t>Nejméně</t>
-  </si>
-  <si>
-    <t>lab.build.cottonOffset.0</t>
-  </si>
-  <si>
-    <t>Akorát</t>
-  </si>
-  <si>
-    <t>lab.build.cottonOffset.1</t>
-  </si>
-  <si>
-    <t>Více</t>
-  </si>
-  <si>
-    <t>lab.build.cottonOffset.2</t>
-  </si>
-  <si>
-    <t>Nejvíce</t>
-  </si>
-  <si>
-    <t>lab.build.glow.1</t>
-  </si>
-  <si>
-    <t>Pomalé</t>
-  </si>
-  <si>
-    <t>lab.build.glow.2</t>
-  </si>
-  <si>
-    <t>Střední</t>
-  </si>
-  <si>
-    <t>lab.build.glow.3</t>
-  </si>
-  <si>
-    <t>Běžné</t>
-  </si>
-  <si>
-    <t>lab.build.glow.4</t>
-  </si>
-  <si>
-    <t>Rychlé</t>
-  </si>
-  <si>
-    <t>lab.build.glow.5</t>
-  </si>
-  <si>
-    <t>Velmi rychlé</t>
-  </si>
-  <si>
-    <t>lab.build.preview.glow</t>
-  </si>
-  <si>
-    <t>Rychlost žhavení</t>
-  </si>
-  <si>
-    <t>lab.build.coilCount.1</t>
-  </si>
-  <si>
-    <t>Jedna</t>
-  </si>
-  <si>
-    <t>Dvě</t>
-  </si>
-  <si>
-    <t>Tři</t>
-  </si>
-  <si>
-    <t>Čtyři</t>
-  </si>
-  <si>
-    <t>lab.build.coilCount.4</t>
-  </si>
-  <si>
-    <t>lab.build.coilCount.3</t>
-  </si>
-  <si>
-    <t>lab.build.coilCount.2</t>
-  </si>
-  <si>
-    <t>lab.vape.leaks.0</t>
-  </si>
-  <si>
-    <t>Žádné</t>
-  </si>
-  <si>
-    <t>lab.vape.leaks.1</t>
-  </si>
-  <si>
-    <t>Drobné</t>
-  </si>
-  <si>
-    <t>Větší</t>
-  </si>
-  <si>
-    <t>lab.vape.leaks.2</t>
-  </si>
-  <si>
-    <t>lab.vape.leaks.3</t>
-  </si>
-  <si>
-    <t>Totální</t>
-  </si>
-  <si>
-    <t>lab.vape.leaks.4</t>
-  </si>
-  <si>
-    <t>Občasné</t>
-  </si>
-  <si>
-    <t>lab.vape.dryhit.0</t>
-  </si>
-  <si>
-    <t>Žádný</t>
-  </si>
-  <si>
-    <t>lab.vape.dryhit.1</t>
-  </si>
-  <si>
-    <t>Občas</t>
-  </si>
-  <si>
-    <t>lab.vape.dryhit.2</t>
-  </si>
-  <si>
-    <t>Velmi často</t>
-  </si>
-  <si>
-    <t>lab.vape.airflow.0</t>
-  </si>
-  <si>
-    <t>Utažený</t>
-  </si>
-  <si>
-    <t>lab.vape.airflow.1</t>
-  </si>
-  <si>
-    <t>Mírně utažený</t>
-  </si>
-  <si>
-    <t>lab.vape.airflow.2</t>
-  </si>
-  <si>
-    <t>Volný</t>
-  </si>
-  <si>
-    <t>lab.vape.airflow.3</t>
-  </si>
-  <si>
-    <t>Zcela otevřený</t>
-  </si>
-  <si>
-    <t>lab.vape.juice.0</t>
-  </si>
-  <si>
-    <t>lab.vape.juice.1</t>
-  </si>
-  <si>
-    <t>Mírně otevřený</t>
-  </si>
-  <si>
-    <t>lab.vape.juice.2</t>
-  </si>
-  <si>
-    <t>common.rate.1</t>
-  </si>
-  <si>
-    <t>Velmí špatné</t>
-  </si>
-  <si>
-    <t>common.rate.2</t>
-  </si>
-  <si>
-    <t>Ucházející</t>
-  </si>
-  <si>
-    <t>common.rate.3</t>
-  </si>
-  <si>
-    <t>common.rate.4</t>
-  </si>
-  <si>
-    <t>Výborné</t>
-  </si>
-  <si>
-    <t>common.rate.5</t>
-  </si>
-  <si>
-    <t>Excelentní</t>
-  </si>
-  <si>
-    <t>lab.vape.clouds.0</t>
-  </si>
-  <si>
-    <t>lab.vape.clouds.1</t>
-  </si>
-  <si>
-    <t>Menší</t>
-  </si>
-  <si>
-    <t>lab.vape.clouds.2</t>
-  </si>
-  <si>
-    <t>lab.vape.clouds.3</t>
-  </si>
-  <si>
-    <t>Extrémní</t>
-  </si>
-  <si>
-    <t>Nepatrná</t>
-  </si>
-  <si>
-    <t>lab.vape.throathit.0</t>
-  </si>
-  <si>
-    <t>lab.vape.throathit.1</t>
-  </si>
-  <si>
-    <t>Nepatrný</t>
-  </si>
-  <si>
-    <t>lab.vape.throathit.2</t>
-  </si>
-  <si>
-    <t>lab.vape.throathit.3</t>
-  </si>
-  <si>
-    <t>lab.vape.throathit.4</t>
-  </si>
-  <si>
-    <t>lab.vape.fresh.0</t>
-  </si>
-  <si>
-    <t>Žádná</t>
-  </si>
-  <si>
-    <t>lab.vape.fresh.1</t>
-  </si>
-  <si>
-    <t>lab.vape.fresh.2</t>
-  </si>
-  <si>
-    <t>lab.vape.fresh.3</t>
-  </si>
-  <si>
-    <t>lab.vape.fresh.4</t>
-  </si>
-  <si>
     <t>lab.vape.airflow.label.required</t>
   </si>
   <si>
@@ -5736,6 +5448,24 @@
   </si>
   <si>
     <t>lab.build.create.form.tab</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.leaks.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.dryhit.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.juice.column</t>
+  </si>
+  <si>
+    <t>Juiceflow</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.airflow.column</t>
+  </si>
+  <si>
+    <t>lab.vape.plot.rating.label</t>
   </si>
 </sst>
 </file>
@@ -6099,10 +5829,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1206"/>
+  <dimension ref="A1:C1157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1204" sqref="B1204"/>
+    <sheetView tabSelected="1" topLeftCell="A1133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1153" sqref="B1153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15492,7 +15222,7 @@
         <v>1362</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>1552</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.25">
@@ -15503,7 +15233,7 @@
         <v>1363</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>1554</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.25">
@@ -15591,7 +15321,7 @@
         <v>1376</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
@@ -15602,7 +15332,7 @@
         <v>1378</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>1377</v>
+        <v>204</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
@@ -15610,10 +15340,10 @@
         <v>0</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>1381</v>
+        <v>204</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
@@ -15621,10 +15351,10 @@
         <v>0</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>1383</v>
+        <v>936</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
@@ -15632,10 +15362,10 @@
         <v>0</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>1385</v>
+        <v>936</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
@@ -15643,10 +15373,10 @@
         <v>0</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
@@ -15654,10 +15384,10 @@
         <v>0</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="869" spans="1:3" x14ac:dyDescent="0.25">
@@ -15665,10 +15395,10 @@
         <v>0</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="C869" s="1" t="s">
-        <v>1391</v>
+        <v>889</v>
       </c>
     </row>
     <row r="870" spans="1:3" x14ac:dyDescent="0.25">
@@ -15676,10 +15406,10 @@
         <v>0</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>1392</v>
+        <v>1387</v>
       </c>
       <c r="C870" s="1" t="s">
-        <v>1393</v>
+        <v>889</v>
       </c>
     </row>
     <row r="871" spans="1:3" x14ac:dyDescent="0.25">
@@ -15687,10 +15417,10 @@
         <v>0</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="C871" s="1" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="872" spans="1:3" x14ac:dyDescent="0.25">
@@ -15698,10 +15428,10 @@
         <v>0</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="C872" s="1" t="s">
-        <v>1397</v>
+        <v>381</v>
       </c>
     </row>
     <row r="873" spans="1:3" x14ac:dyDescent="0.25">
@@ -15709,21 +15439,21 @@
         <v>0</v>
       </c>
       <c r="B873" s="1" t="s">
-        <v>1398</v>
+        <v>1391</v>
       </c>
       <c r="C873" s="1" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="874" spans="1:3" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>1405</v>
+        <v>1392</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>1400</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="875" spans="1:3" x14ac:dyDescent="0.25">
@@ -15731,10 +15461,10 @@
         <v>0</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>1404</v>
+        <v>1394</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>1401</v>
+        <v>381</v>
       </c>
     </row>
     <row r="876" spans="1:3" x14ac:dyDescent="0.25">
@@ -15742,10 +15472,10 @@
         <v>0</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>1403</v>
+        <v>1395</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>1402</v>
+        <v>15</v>
       </c>
     </row>
     <row r="877" spans="1:3" x14ac:dyDescent="0.25">
@@ -15753,10 +15483,10 @@
         <v>0</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>1406</v>
+        <v>1396</v>
       </c>
       <c r="C877" s="1" t="s">
-        <v>1407</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="878" spans="1:3" x14ac:dyDescent="0.25">
@@ -15764,10 +15494,10 @@
         <v>0</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>1408</v>
+        <v>1398</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>1409</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="879" spans="1:3" x14ac:dyDescent="0.25">
@@ -15775,10 +15505,10 @@
         <v>0</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>1412</v>
+        <v>1400</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>1410</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="880" spans="1:3" x14ac:dyDescent="0.25">
@@ -15786,10 +15516,10 @@
         <v>0</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>1414</v>
+        <v>1402</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>1413</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="881" spans="1:3" x14ac:dyDescent="0.25">
@@ -15797,10 +15527,10 @@
         <v>0</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>1411</v>
+        <v>1404</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>1415</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.25">
@@ -15808,10 +15538,10 @@
         <v>0</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>1416</v>
+        <v>1406</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>1407</v>
+        <v>491</v>
       </c>
     </row>
     <row r="883" spans="1:3" x14ac:dyDescent="0.25">
@@ -15819,10 +15549,10 @@
         <v>0</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>1418</v>
+        <v>1407</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>1419</v>
+        <v>491</v>
       </c>
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.25">
@@ -15830,10 +15560,10 @@
         <v>0</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>1420</v>
+        <v>1408</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>1421</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="885" spans="1:3" x14ac:dyDescent="0.25">
@@ -15841,10 +15571,10 @@
         <v>0</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>1422</v>
+        <v>1410</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>1423</v>
+        <v>298</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.25">
@@ -15852,10 +15582,10 @@
         <v>0</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>1424</v>
+        <v>1411</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>1425</v>
+        <v>393</v>
       </c>
     </row>
     <row r="887" spans="1:3" x14ac:dyDescent="0.25">
@@ -15863,10 +15593,10 @@
         <v>0</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>1426</v>
+        <v>1412</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>1427</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="888" spans="1:3" x14ac:dyDescent="0.25">
@@ -15874,10 +15604,10 @@
         <v>0</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>1428</v>
+        <v>1414</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>1429</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.25">
@@ -15885,10 +15615,10 @@
         <v>0</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>1430</v>
+        <v>1416</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="890" spans="1:3" x14ac:dyDescent="0.25">
@@ -15896,10 +15626,10 @@
         <v>0</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>1431</v>
+        <v>1418</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>1432</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="891" spans="1:3" x14ac:dyDescent="0.25">
@@ -15907,10 +15637,10 @@
         <v>0</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>1433</v>
+        <v>1420</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>1429</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="892" spans="1:3" x14ac:dyDescent="0.25">
@@ -15918,10 +15648,10 @@
         <v>0</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>1434</v>
+        <v>1422</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>1435</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="893" spans="1:3" x14ac:dyDescent="0.25">
@@ -15929,10 +15659,10 @@
         <v>0</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>1436</v>
+        <v>1424</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>1437</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.25">
@@ -15940,21 +15670,21 @@
         <v>0</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1438</v>
+        <v>1426</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="895" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B895" s="1" t="s">
-        <v>1439</v>
+        <v>1427</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>1440</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="896" spans="1:3" x14ac:dyDescent="0.25">
@@ -15962,10 +15692,10 @@
         <v>0</v>
       </c>
       <c r="B896" s="1" t="s">
-        <v>1441</v>
+        <v>1429</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>1442</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="897" spans="1:3" x14ac:dyDescent="0.25">
@@ -15973,10 +15703,10 @@
         <v>0</v>
       </c>
       <c r="B897" s="1" t="s">
-        <v>1443</v>
+        <v>1430</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>1449</v>
+        <v>358</v>
       </c>
     </row>
     <row r="898" spans="1:3" x14ac:dyDescent="0.25">
@@ -15984,10 +15714,10 @@
         <v>0</v>
       </c>
       <c r="B898" s="1" t="s">
-        <v>1444</v>
+        <v>1431</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>1445</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="899" spans="1:3" x14ac:dyDescent="0.25">
@@ -15995,10 +15725,10 @@
         <v>0</v>
       </c>
       <c r="B899" s="1" t="s">
-        <v>1446</v>
+        <v>1432</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>1410</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="900" spans="1:3" x14ac:dyDescent="0.25">
@@ -16006,10 +15736,10 @@
         <v>0</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>1447</v>
+        <v>1433</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>1448</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="901" spans="1:3" x14ac:dyDescent="0.25">
@@ -16017,10 +15747,10 @@
         <v>0</v>
       </c>
       <c r="B901" s="1" t="s">
-        <v>1450</v>
+        <v>1435</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>1417</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="902" spans="1:3" x14ac:dyDescent="0.25">
@@ -16028,10 +15758,10 @@
         <v>0</v>
       </c>
       <c r="B902" s="1" t="s">
-        <v>1451</v>
+        <v>1436</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>1452</v>
+        <v>289</v>
       </c>
     </row>
     <row r="903" spans="1:3" x14ac:dyDescent="0.25">
@@ -16039,10 +15769,10 @@
         <v>0</v>
       </c>
       <c r="B903" s="1" t="s">
-        <v>1453</v>
+        <v>1437</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>1381</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="904" spans="1:3" x14ac:dyDescent="0.25">
@@ -16050,10 +15780,10 @@
         <v>0</v>
       </c>
       <c r="B904" s="1" t="s">
-        <v>1454</v>
+        <v>392</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>1410</v>
+        <v>393</v>
       </c>
     </row>
     <row r="905" spans="1:3" x14ac:dyDescent="0.25">
@@ -16061,10 +15791,10 @@
         <v>0</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>1455</v>
+        <v>1438</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>1448</v>
+        <v>119</v>
       </c>
     </row>
     <row r="906" spans="1:3" x14ac:dyDescent="0.25">
@@ -16072,10 +15802,10 @@
         <v>0</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>1456</v>
+        <v>1439</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>1457</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="907" spans="1:3" x14ac:dyDescent="0.25">
@@ -16083,10 +15813,10 @@
         <v>0</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>1458</v>
+        <v>1440</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>1449</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="908" spans="1:3" x14ac:dyDescent="0.25">
@@ -16094,10 +15824,10 @@
         <v>0</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>1459</v>
+        <v>1442</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>1381</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="909" spans="1:3" x14ac:dyDescent="0.25">
@@ -16105,10 +15835,10 @@
         <v>0</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>1460</v>
+        <v>1444</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>1410</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="910" spans="1:3" x14ac:dyDescent="0.25">
@@ -16116,10 +15846,10 @@
         <v>0</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>1461</v>
+        <v>1446</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>1448</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="911" spans="1:3" x14ac:dyDescent="0.25">
@@ -16127,10 +15857,10 @@
         <v>0</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>1462</v>
+        <v>1447</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>1463</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="912" spans="1:3" x14ac:dyDescent="0.25">
@@ -16138,10 +15868,10 @@
         <v>0</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>1464</v>
+        <v>1448</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>1465</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="913" spans="1:3" x14ac:dyDescent="0.25">
@@ -16149,10 +15879,10 @@
         <v>0</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>1466</v>
+        <v>1449</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>1467</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="914" spans="1:3" x14ac:dyDescent="0.25">
@@ -16160,10 +15890,10 @@
         <v>0</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>1468</v>
+        <v>1450</v>
       </c>
       <c r="C914" s="1" t="s">
-        <v>1469</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="915" spans="1:3" x14ac:dyDescent="0.25">
@@ -16171,10 +15901,10 @@
         <v>0</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>1470</v>
+        <v>1451</v>
       </c>
       <c r="C915" s="1" t="s">
-        <v>1471</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="916" spans="1:3" x14ac:dyDescent="0.25">
@@ -16182,10 +15912,10 @@
         <v>0</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>1472</v>
+        <v>1452</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>1473</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="917" spans="1:3" x14ac:dyDescent="0.25">
@@ -16193,10 +15923,10 @@
         <v>0</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>1474</v>
+        <v>1459</v>
       </c>
       <c r="C917" s="1" t="s">
-        <v>204</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="918" spans="1:3" x14ac:dyDescent="0.25">
@@ -16204,10 +15934,10 @@
         <v>0</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>1475</v>
+        <v>1455</v>
       </c>
       <c r="C918" s="1" t="s">
-        <v>204</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="919" spans="1:3" x14ac:dyDescent="0.25">
@@ -16215,10 +15945,10 @@
         <v>0</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>1476</v>
+        <v>1457</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>936</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="920" spans="1:3" x14ac:dyDescent="0.25">
@@ -16226,10 +15956,10 @@
         <v>0</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>1477</v>
+        <v>1460</v>
       </c>
       <c r="C920" s="1" t="s">
-        <v>936</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="921" spans="1:3" x14ac:dyDescent="0.25">
@@ -16237,10 +15967,10 @@
         <v>0</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>1478</v>
+        <v>1461</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>1479</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="922" spans="1:3" x14ac:dyDescent="0.25">
@@ -16248,10 +15978,10 @@
         <v>0</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>1480</v>
+        <v>1463</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>1481</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.25">
@@ -16259,10 +15989,10 @@
         <v>0</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>1482</v>
+        <v>1465</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>889</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="924" spans="1:3" x14ac:dyDescent="0.25">
@@ -16270,10 +16000,10 @@
         <v>0</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>1483</v>
+        <v>1467</v>
       </c>
       <c r="C924" s="1" t="s">
-        <v>889</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.25">
@@ -16281,10 +16011,10 @@
         <v>0</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>1484</v>
+        <v>1469</v>
       </c>
       <c r="C925" s="1" t="s">
-        <v>1485</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="926" spans="1:3" x14ac:dyDescent="0.25">
@@ -16292,10 +16022,10 @@
         <v>0</v>
       </c>
       <c r="B926" s="1" t="s">
-        <v>1486</v>
+        <v>1471</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>381</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="927" spans="1:3" x14ac:dyDescent="0.25">
@@ -16303,21 +16033,21 @@
         <v>0</v>
       </c>
       <c r="B927" s="1" t="s">
-        <v>1487</v>
+        <v>1472</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="928" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="928" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B928" s="1" t="s">
-        <v>1488</v>
+        <v>1473</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>1489</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="929" spans="1:3" x14ac:dyDescent="0.25">
@@ -16325,10 +16055,10 @@
         <v>0</v>
       </c>
       <c r="B929" s="1" t="s">
-        <v>1490</v>
+        <v>1475</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
     </row>
     <row r="930" spans="1:3" x14ac:dyDescent="0.25">
@@ -16336,10 +16066,10 @@
         <v>0</v>
       </c>
       <c r="B930" s="1" t="s">
-        <v>1491</v>
+        <v>1476</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>15</v>
+        <v>802</v>
       </c>
     </row>
     <row r="931" spans="1:3" x14ac:dyDescent="0.25">
@@ -16347,10 +16077,10 @@
         <v>0</v>
       </c>
       <c r="B931" s="1" t="s">
-        <v>1492</v>
+        <v>1477</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>1493</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="932" spans="1:3" x14ac:dyDescent="0.25">
@@ -16358,10 +16088,10 @@
         <v>0</v>
       </c>
       <c r="B932" s="1" t="s">
-        <v>1494</v>
+        <v>1478</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>1495</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="933" spans="1:3" x14ac:dyDescent="0.25">
@@ -16369,10 +16099,10 @@
         <v>0</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>1496</v>
+        <v>1479</v>
       </c>
       <c r="C933" s="1" t="s">
-        <v>1497</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="934" spans="1:3" x14ac:dyDescent="0.25">
@@ -16380,10 +16110,10 @@
         <v>0</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>1498</v>
+        <v>1481</v>
       </c>
       <c r="C934" s="1" t="s">
-        <v>1499</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.25">
@@ -16391,10 +16121,10 @@
         <v>0</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>1500</v>
+        <v>1482</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>1501</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="936" spans="1:3" x14ac:dyDescent="0.25">
@@ -16402,10 +16132,10 @@
         <v>0</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>1502</v>
+        <v>1484</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>491</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="937" spans="1:3" x14ac:dyDescent="0.25">
@@ -16413,10 +16143,10 @@
         <v>0</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>1503</v>
+        <v>1486</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>491</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="938" spans="1:3" x14ac:dyDescent="0.25">
@@ -16424,10 +16154,10 @@
         <v>0</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>1504</v>
+        <v>1488</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>1505</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="939" spans="1:3" x14ac:dyDescent="0.25">
@@ -16435,10 +16165,10 @@
         <v>0</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>1506</v>
+        <v>1489</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>298</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="940" spans="1:3" x14ac:dyDescent="0.25">
@@ -16446,10 +16176,10 @@
         <v>0</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>1507</v>
+        <v>1491</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>393</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="941" spans="1:3" x14ac:dyDescent="0.25">
@@ -16457,10 +16187,10 @@
         <v>0</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>1508</v>
+        <v>1493</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>1509</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.25">
@@ -16468,10 +16198,10 @@
         <v>0</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>1510</v>
+        <v>1495</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>1511</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="943" spans="1:3" x14ac:dyDescent="0.25">
@@ -16479,10 +16209,10 @@
         <v>0</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>1512</v>
+        <v>1497</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>1513</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.25">
@@ -16490,10 +16220,10 @@
         <v>0</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>1514</v>
+        <v>1499</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>1515</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="945" spans="1:3" x14ac:dyDescent="0.25">
@@ -16501,10 +16231,10 @@
         <v>0</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>1516</v>
+        <v>1501</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>1517</v>
+        <v>393</v>
       </c>
     </row>
     <row r="946" spans="1:3" x14ac:dyDescent="0.25">
@@ -16512,21 +16242,21 @@
         <v>0</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>1518</v>
+        <v>1502</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="947" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="947" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>1520</v>
+        <v>1504</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>1521</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="948" spans="1:3" x14ac:dyDescent="0.25">
@@ -16534,21 +16264,21 @@
         <v>0</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>1522</v>
+        <v>1506</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="949" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="949" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>1523</v>
+        <v>1508</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>1524</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.25">
@@ -16556,10 +16286,10 @@
         <v>0</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>1525</v>
+        <v>1510</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>1521</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="951" spans="1:3" x14ac:dyDescent="0.25">
@@ -16567,10 +16297,10 @@
         <v>0</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>1526</v>
+        <v>1511</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>358</v>
+        <v>374</v>
       </c>
     </row>
     <row r="952" spans="1:3" x14ac:dyDescent="0.25">
@@ -16578,10 +16308,10 @@
         <v>0</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>1527</v>
+        <v>1512</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>1517</v>
+        <v>493</v>
       </c>
     </row>
     <row r="953" spans="1:3" x14ac:dyDescent="0.25">
@@ -16589,10 +16319,10 @@
         <v>0</v>
       </c>
       <c r="B953" s="1" t="s">
-        <v>1528</v>
+        <v>1513</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>1258</v>
+        <v>493</v>
       </c>
     </row>
     <row r="954" spans="1:3" x14ac:dyDescent="0.25">
@@ -16600,10 +16330,10 @@
         <v>0</v>
       </c>
       <c r="B954" s="1" t="s">
-        <v>1529</v>
+        <v>1514</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>1530</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="955" spans="1:3" x14ac:dyDescent="0.25">
@@ -16611,10 +16341,10 @@
         <v>0</v>
       </c>
       <c r="B955" s="1" t="s">
-        <v>1531</v>
+        <v>1516</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>1257</v>
+        <v>688</v>
       </c>
     </row>
     <row r="956" spans="1:3" x14ac:dyDescent="0.25">
@@ -16622,10 +16352,10 @@
         <v>0</v>
       </c>
       <c r="B956" s="1" t="s">
-        <v>1532</v>
+        <v>1517</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="957" spans="1:3" x14ac:dyDescent="0.25">
@@ -16633,10 +16363,10 @@
         <v>0</v>
       </c>
       <c r="B957" s="1" t="s">
-        <v>1533</v>
+        <v>1518</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>1509</v>
+        <v>393</v>
       </c>
     </row>
     <row r="958" spans="1:3" x14ac:dyDescent="0.25">
@@ -16644,10 +16374,10 @@
         <v>0</v>
       </c>
       <c r="B958" s="1" t="s">
-        <v>392</v>
+        <v>1519</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>393</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="959" spans="1:3" x14ac:dyDescent="0.25">
@@ -16655,10 +16385,10 @@
         <v>0</v>
       </c>
       <c r="B959" s="1" t="s">
-        <v>1534</v>
+        <v>1521</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>119</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="960" spans="1:3" x14ac:dyDescent="0.25">
@@ -16666,10 +16396,10 @@
         <v>0</v>
       </c>
       <c r="B960" s="1" t="s">
-        <v>1535</v>
+        <v>1523</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>1127</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="961" spans="1:3" x14ac:dyDescent="0.25">
@@ -16677,10 +16407,10 @@
         <v>0</v>
       </c>
       <c r="B961" s="1" t="s">
-        <v>1536</v>
+        <v>1525</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>1537</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="962" spans="1:3" x14ac:dyDescent="0.25">
@@ -16688,10 +16418,10 @@
         <v>0</v>
       </c>
       <c r="B962" s="1" t="s">
-        <v>1538</v>
+        <v>1527</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>1539</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="963" spans="1:3" x14ac:dyDescent="0.25">
@@ -16699,21 +16429,21 @@
         <v>0</v>
       </c>
       <c r="B963" s="1" t="s">
-        <v>1540</v>
+        <v>1529</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="964" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B964" s="1" t="s">
-        <v>1542</v>
+        <v>1530</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>1332</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="965" spans="1:3" x14ac:dyDescent="0.25">
@@ -16721,10 +16451,10 @@
         <v>0</v>
       </c>
       <c r="B965" s="1" t="s">
-        <v>1543</v>
+        <v>1532</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>1340</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="966" spans="1:3" x14ac:dyDescent="0.25">
@@ -16732,10 +16462,10 @@
         <v>0</v>
       </c>
       <c r="B966" s="1" t="s">
-        <v>1544</v>
+        <v>1533</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>1332</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="967" spans="1:3" x14ac:dyDescent="0.25">
@@ -16743,10 +16473,10 @@
         <v>0</v>
       </c>
       <c r="B967" s="1" t="s">
-        <v>1545</v>
+        <v>1535</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>1332</v>
+        <v>672</v>
       </c>
     </row>
     <row r="968" spans="1:3" x14ac:dyDescent="0.25">
@@ -16754,10 +16484,10 @@
         <v>0</v>
       </c>
       <c r="B968" s="1" t="s">
-        <v>1546</v>
+        <v>1536</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>1552</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="969" spans="1:3" x14ac:dyDescent="0.25">
@@ -16765,10 +16495,10 @@
         <v>0</v>
       </c>
       <c r="B969" s="1" t="s">
-        <v>1547</v>
+        <v>1538</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>1541</v>
+        <v>289</v>
       </c>
     </row>
     <row r="970" spans="1:3" x14ac:dyDescent="0.25">
@@ -16776,10 +16506,10 @@
         <v>0</v>
       </c>
       <c r="B970" s="1" t="s">
-        <v>1548</v>
+        <v>1539</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>1549</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="971" spans="1:3" x14ac:dyDescent="0.25">
@@ -16787,10 +16517,10 @@
         <v>0</v>
       </c>
       <c r="B971" s="1" t="s">
-        <v>1555</v>
+        <v>1541</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>1550</v>
+        <v>499</v>
       </c>
     </row>
     <row r="972" spans="1:3" x14ac:dyDescent="0.25">
@@ -16798,10 +16528,10 @@
         <v>0</v>
       </c>
       <c r="B972" s="1" t="s">
-        <v>1551</v>
+        <v>1542</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>1539</v>
+        <v>499</v>
       </c>
     </row>
     <row r="973" spans="1:3" x14ac:dyDescent="0.25">
@@ -16809,10 +16539,10 @@
         <v>0</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>1553</v>
+        <v>1543</v>
       </c>
       <c r="C973" s="1" t="s">
-        <v>1539</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="974" spans="1:3" x14ac:dyDescent="0.25">
@@ -16820,10 +16550,10 @@
         <v>0</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>1556</v>
+        <v>1545</v>
       </c>
       <c r="C974" s="1" t="s">
-        <v>1550</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="975" spans="1:3" x14ac:dyDescent="0.25">
@@ -16831,10 +16561,10 @@
         <v>0</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>1557</v>
+        <v>1547</v>
       </c>
       <c r="C975" s="1" t="s">
-        <v>1558</v>
+        <v>298</v>
       </c>
     </row>
     <row r="976" spans="1:3" x14ac:dyDescent="0.25">
@@ -16842,10 +16572,10 @@
         <v>0</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>1559</v>
+        <v>1548</v>
       </c>
       <c r="C976" s="1" t="s">
-        <v>1560</v>
+        <v>393</v>
       </c>
     </row>
     <row r="977" spans="1:3" x14ac:dyDescent="0.25">
@@ -16853,10 +16583,10 @@
         <v>0</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>1561</v>
+        <v>1545</v>
       </c>
       <c r="C977" s="1" t="s">
-        <v>1562</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="978" spans="1:3" x14ac:dyDescent="0.25">
@@ -16864,10 +16594,10 @@
         <v>0</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>1563</v>
+        <v>1549</v>
       </c>
       <c r="C978" s="1" t="s">
-        <v>1564</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="979" spans="1:3" x14ac:dyDescent="0.25">
@@ -16875,10 +16605,10 @@
         <v>0</v>
       </c>
       <c r="B979" s="1" t="s">
-        <v>1565</v>
+        <v>1551</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>1566</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="980" spans="1:3" x14ac:dyDescent="0.25">
@@ -16886,10 +16616,10 @@
         <v>0</v>
       </c>
       <c r="B980" s="1" t="s">
-        <v>1567</v>
+        <v>1553</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>1259</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="981" spans="1:3" x14ac:dyDescent="0.25">
@@ -16897,21 +16627,21 @@
         <v>0</v>
       </c>
       <c r="B981" s="1" t="s">
-        <v>1568</v>
+        <v>1555</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="982" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="982" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B982" s="1" t="s">
-        <v>1569</v>
+        <v>1556</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>1570</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="983" spans="1:3" x14ac:dyDescent="0.25">
@@ -16919,10 +16649,10 @@
         <v>0</v>
       </c>
       <c r="B983" s="1" t="s">
-        <v>1571</v>
+        <v>1558</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>362</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="984" spans="1:3" x14ac:dyDescent="0.25">
@@ -16930,10 +16660,10 @@
         <v>0</v>
       </c>
       <c r="B984" s="1" t="s">
-        <v>1572</v>
+        <v>1559</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>802</v>
+        <v>448</v>
       </c>
     </row>
     <row r="985" spans="1:3" x14ac:dyDescent="0.25">
@@ -16941,10 +16671,10 @@
         <v>0</v>
       </c>
       <c r="B985" s="1" t="s">
-        <v>1573</v>
+        <v>1560</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>1539</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="986" spans="1:3" x14ac:dyDescent="0.25">
@@ -16952,10 +16682,10 @@
         <v>0</v>
       </c>
       <c r="B986" s="1" t="s">
-        <v>1574</v>
+        <v>1561</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>1554</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="987" spans="1:3" x14ac:dyDescent="0.25">
@@ -16963,10 +16693,10 @@
         <v>0</v>
       </c>
       <c r="B987" s="1" t="s">
-        <v>1575</v>
+        <v>1563</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>1576</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="988" spans="1:3" x14ac:dyDescent="0.25">
@@ -16974,10 +16704,10 @@
         <v>0</v>
       </c>
       <c r="B988" s="1" t="s">
-        <v>1577</v>
+        <v>1565</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>1537</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="989" spans="1:3" x14ac:dyDescent="0.25">
@@ -16985,10 +16715,10 @@
         <v>0</v>
       </c>
       <c r="B989" s="1" t="s">
-        <v>1578</v>
+        <v>1567</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>1579</v>
+        <v>501</v>
       </c>
     </row>
     <row r="990" spans="1:3" x14ac:dyDescent="0.25">
@@ -16996,10 +16726,10 @@
         <v>0</v>
       </c>
       <c r="B990" s="1" t="s">
-        <v>1580</v>
+        <v>1568</v>
       </c>
       <c r="C990" s="1" t="s">
-        <v>1581</v>
+        <v>501</v>
       </c>
     </row>
     <row r="991" spans="1:3" x14ac:dyDescent="0.25">
@@ -17007,10 +16737,10 @@
         <v>0</v>
       </c>
       <c r="B991" s="1" t="s">
-        <v>1582</v>
+        <v>1569</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>1583</v>
+        <v>444</v>
       </c>
     </row>
     <row r="992" spans="1:3" x14ac:dyDescent="0.25">
@@ -17018,10 +16748,10 @@
         <v>0</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>1584</v>
+        <v>1570</v>
       </c>
       <c r="C992" s="1" t="s">
-        <v>1583</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="993" spans="1:3" x14ac:dyDescent="0.25">
@@ -17029,10 +16759,10 @@
         <v>0</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>1585</v>
+        <v>1572</v>
       </c>
       <c r="C993" s="1" t="s">
-        <v>1586</v>
+        <v>381</v>
       </c>
     </row>
     <row r="994" spans="1:3" x14ac:dyDescent="0.25">
@@ -17040,10 +16770,10 @@
         <v>0</v>
       </c>
       <c r="B994" s="1" t="s">
-        <v>1587</v>
+        <v>1573</v>
       </c>
       <c r="C994" s="1" t="s">
-        <v>1588</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="995" spans="1:3" x14ac:dyDescent="0.25">
@@ -17051,10 +16781,10 @@
         <v>0</v>
       </c>
       <c r="B995" s="1" t="s">
-        <v>1589</v>
+        <v>1574</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>1590</v>
+        <v>448</v>
       </c>
     </row>
     <row r="996" spans="1:3" x14ac:dyDescent="0.25">
@@ -17062,10 +16792,10 @@
         <v>0</v>
       </c>
       <c r="B996" s="1" t="s">
-        <v>1591</v>
+        <v>1575</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>1592</v>
+        <v>393</v>
       </c>
     </row>
     <row r="997" spans="1:3" x14ac:dyDescent="0.25">
@@ -17073,10 +16803,10 @@
         <v>0</v>
       </c>
       <c r="B997" s="1" t="s">
-        <v>1593</v>
+        <v>1576</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>1594</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="998" spans="1:3" x14ac:dyDescent="0.25">
@@ -17084,10 +16814,10 @@
         <v>0</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>1595</v>
+        <v>1578</v>
       </c>
       <c r="C998" s="1" t="s">
-        <v>1596</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="999" spans="1:3" x14ac:dyDescent="0.25">
@@ -17095,10 +16825,10 @@
         <v>0</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>1597</v>
+        <v>1580</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>393</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="1000" spans="1:3" x14ac:dyDescent="0.25">
@@ -17106,32 +16836,32 @@
         <v>0</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>1598</v>
+        <v>1582</v>
       </c>
       <c r="C1000" s="1" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="1001" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>1600</v>
+        <v>1584</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="1002" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>1602</v>
+        <v>1585</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>1603</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1003" spans="1:3" x14ac:dyDescent="0.25">
@@ -17139,10 +16869,10 @@
         <v>0</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>1604</v>
+        <v>1587</v>
       </c>
       <c r="C1003" s="1" t="s">
-        <v>1605</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="1004" spans="1:3" x14ac:dyDescent="0.25">
@@ -17150,10 +16880,10 @@
         <v>0</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>1606</v>
+        <v>1588</v>
       </c>
       <c r="C1004" s="1" t="s">
-        <v>1599</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1005" spans="1:3" x14ac:dyDescent="0.25">
@@ -17161,10 +16891,10 @@
         <v>0</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>1607</v>
+        <v>1590</v>
       </c>
       <c r="C1005" s="1" t="s">
-        <v>374</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1006" spans="1:3" x14ac:dyDescent="0.25">
@@ -17172,10 +16902,10 @@
         <v>0</v>
       </c>
       <c r="B1006" s="1" t="s">
-        <v>1608</v>
+        <v>1592</v>
       </c>
       <c r="C1006" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="1007" spans="1:3" x14ac:dyDescent="0.25">
@@ -17183,10 +16913,10 @@
         <v>0</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>1609</v>
+        <v>1593</v>
       </c>
       <c r="C1007" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="1008" spans="1:3" x14ac:dyDescent="0.25">
@@ -17194,10 +16924,10 @@
         <v>0</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>1610</v>
+        <v>1594</v>
       </c>
       <c r="C1008" s="1" t="s">
-        <v>1611</v>
+        <v>381</v>
       </c>
     </row>
     <row r="1009" spans="1:3" x14ac:dyDescent="0.25">
@@ -17205,10 +16935,10 @@
         <v>0</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>1612</v>
+        <v>1595</v>
       </c>
       <c r="C1009" s="1" t="s">
-        <v>688</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1010" spans="1:3" x14ac:dyDescent="0.25">
@@ -17216,10 +16946,10 @@
         <v>0</v>
       </c>
       <c r="B1010" s="1" t="s">
-        <v>1613</v>
+        <v>1597</v>
       </c>
       <c r="C1010" s="1" t="s">
-        <v>298</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1011" spans="1:3" x14ac:dyDescent="0.25">
@@ -17227,10 +16957,10 @@
         <v>0</v>
       </c>
       <c r="B1011" s="1" t="s">
-        <v>1614</v>
+        <v>1595</v>
       </c>
       <c r="C1011" s="1" t="s">
-        <v>393</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1012" spans="1:3" x14ac:dyDescent="0.25">
@@ -17238,10 +16968,10 @@
         <v>0</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>1615</v>
+        <v>1599</v>
       </c>
       <c r="C1012" s="1" t="s">
-        <v>1616</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1013" spans="1:3" x14ac:dyDescent="0.25">
@@ -17249,10 +16979,10 @@
         <v>0</v>
       </c>
       <c r="B1013" s="1" t="s">
-        <v>1617</v>
+        <v>1601</v>
       </c>
       <c r="C1013" s="1" t="s">
-        <v>1618</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1014" spans="1:3" x14ac:dyDescent="0.25">
@@ -17260,10 +16990,10 @@
         <v>0</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>1619</v>
+        <v>1603</v>
       </c>
       <c r="C1014" s="1" t="s">
-        <v>1620</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1015" spans="1:3" x14ac:dyDescent="0.25">
@@ -17271,10 +17001,10 @@
         <v>0</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>1621</v>
+        <v>1605</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>1622</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1016" spans="1:3" x14ac:dyDescent="0.25">
@@ -17282,10 +17012,10 @@
         <v>0</v>
       </c>
       <c r="B1016" s="1" t="s">
-        <v>1623</v>
+        <v>1607</v>
       </c>
       <c r="C1016" s="1" t="s">
-        <v>1624</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1017" spans="1:3" x14ac:dyDescent="0.25">
@@ -17293,21 +17023,21 @@
         <v>0</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>1625</v>
+        <v>1608</v>
       </c>
       <c r="C1017" s="1" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1018" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>1626</v>
+        <v>1609</v>
       </c>
       <c r="C1018" s="1" t="s">
-        <v>1627</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1019" spans="1:3" x14ac:dyDescent="0.25">
@@ -17315,10 +17045,10 @@
         <v>0</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>1628</v>
+        <v>1611</v>
       </c>
       <c r="C1019" s="1" t="s">
-        <v>1624</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1020" spans="1:3" x14ac:dyDescent="0.25">
@@ -17326,10 +17056,10 @@
         <v>0</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>1629</v>
+        <v>1613</v>
       </c>
       <c r="C1020" s="1" t="s">
-        <v>1630</v>
+        <v>381</v>
       </c>
     </row>
     <row r="1021" spans="1:3" x14ac:dyDescent="0.25">
@@ -17337,10 +17067,10 @@
         <v>0</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>1631</v>
+        <v>1614</v>
       </c>
       <c r="C1021" s="1" t="s">
-        <v>672</v>
+        <v>393</v>
       </c>
     </row>
     <row r="1022" spans="1:3" x14ac:dyDescent="0.25">
@@ -17348,10 +17078,10 @@
         <v>0</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>1632</v>
+        <v>1615</v>
       </c>
       <c r="C1022" s="1" t="s">
-        <v>1633</v>
+        <v>491</v>
       </c>
     </row>
     <row r="1023" spans="1:3" x14ac:dyDescent="0.25">
@@ -17359,10 +17089,10 @@
         <v>0</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>1634</v>
+        <v>1616</v>
       </c>
       <c r="C1023" s="1" t="s">
-        <v>289</v>
+        <v>493</v>
       </c>
     </row>
     <row r="1024" spans="1:3" x14ac:dyDescent="0.25">
@@ -17370,10 +17100,10 @@
         <v>0</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>1635</v>
+        <v>1617</v>
       </c>
       <c r="C1024" s="1" t="s">
-        <v>1636</v>
+        <v>489</v>
       </c>
     </row>
     <row r="1025" spans="1:3" x14ac:dyDescent="0.25">
@@ -17381,10 +17111,10 @@
         <v>0</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>1637</v>
+        <v>1618</v>
       </c>
       <c r="C1025" s="1" t="s">
-        <v>499</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1026" spans="1:3" x14ac:dyDescent="0.25">
@@ -17392,10 +17122,10 @@
         <v>0</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>1638</v>
+        <v>1619</v>
       </c>
       <c r="C1026" s="1" t="s">
-        <v>499</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1027" spans="1:3" x14ac:dyDescent="0.25">
@@ -17403,10 +17133,10 @@
         <v>0</v>
       </c>
       <c r="B1027" s="1" t="s">
-        <v>1639</v>
+        <v>1621</v>
       </c>
       <c r="C1027" s="1" t="s">
-        <v>1640</v>
+        <v>495</v>
       </c>
     </row>
     <row r="1028" spans="1:3" x14ac:dyDescent="0.25">
@@ -17414,10 +17144,10 @@
         <v>0</v>
       </c>
       <c r="B1028" s="1" t="s">
-        <v>1641</v>
+        <v>1622</v>
       </c>
       <c r="C1028" s="1" t="s">
-        <v>1642</v>
+        <v>495</v>
       </c>
     </row>
     <row r="1029" spans="1:3" x14ac:dyDescent="0.25">
@@ -17425,10 +17155,10 @@
         <v>0</v>
       </c>
       <c r="B1029" s="1" t="s">
-        <v>1643</v>
+        <v>1623</v>
       </c>
       <c r="C1029" s="1" t="s">
-        <v>298</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="1030" spans="1:3" x14ac:dyDescent="0.25">
@@ -17436,10 +17166,10 @@
         <v>0</v>
       </c>
       <c r="B1030" s="1" t="s">
-        <v>1644</v>
+        <v>1625</v>
       </c>
       <c r="C1030" s="1" t="s">
-        <v>393</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1031" spans="1:3" x14ac:dyDescent="0.25">
@@ -17447,10 +17177,10 @@
         <v>0</v>
       </c>
       <c r="B1031" s="1" t="s">
-        <v>1641</v>
+        <v>1627</v>
       </c>
       <c r="C1031" s="1" t="s">
-        <v>1642</v>
+        <v>381</v>
       </c>
     </row>
     <row r="1032" spans="1:3" x14ac:dyDescent="0.25">
@@ -17458,10 +17188,10 @@
         <v>0</v>
       </c>
       <c r="B1032" s="1" t="s">
-        <v>1645</v>
+        <v>1628</v>
       </c>
       <c r="C1032" s="1" t="s">
-        <v>1646</v>
+        <v>204</v>
       </c>
     </row>
     <row r="1033" spans="1:3" x14ac:dyDescent="0.25">
@@ -17469,10 +17199,10 @@
         <v>0</v>
       </c>
       <c r="B1033" s="1" t="s">
-        <v>1647</v>
+        <v>1629</v>
       </c>
       <c r="C1033" s="1" t="s">
-        <v>1648</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1034" spans="1:3" x14ac:dyDescent="0.25">
@@ -17480,10 +17210,10 @@
         <v>0</v>
       </c>
       <c r="B1034" s="1" t="s">
-        <v>1649</v>
+        <v>1631</v>
       </c>
       <c r="C1034" s="1" t="s">
-        <v>1650</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1035" spans="1:3" x14ac:dyDescent="0.25">
@@ -17491,21 +17221,21 @@
         <v>0</v>
       </c>
       <c r="B1035" s="1" t="s">
-        <v>1651</v>
+        <v>1633</v>
       </c>
       <c r="C1035" s="1" t="s">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1036" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1036" s="1" t="s">
-        <v>1652</v>
+        <v>1635</v>
       </c>
       <c r="C1036" s="1" t="s">
-        <v>1653</v>
+        <v>393</v>
       </c>
     </row>
     <row r="1037" spans="1:3" x14ac:dyDescent="0.25">
@@ -17513,10 +17243,10 @@
         <v>0</v>
       </c>
       <c r="B1037" s="1" t="s">
-        <v>1654</v>
+        <v>1636</v>
       </c>
       <c r="C1037" s="1" t="s">
-        <v>1650</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1038" spans="1:3" x14ac:dyDescent="0.25">
@@ -17524,21 +17254,21 @@
         <v>0</v>
       </c>
       <c r="B1038" s="1" t="s">
-        <v>1655</v>
+        <v>1638</v>
       </c>
       <c r="C1038" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:3" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1039" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1039" s="1" t="s">
-        <v>1656</v>
+        <v>1639</v>
       </c>
       <c r="C1039" s="1" t="s">
-        <v>1646</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1040" spans="1:3" x14ac:dyDescent="0.25">
@@ -17546,21 +17276,21 @@
         <v>0</v>
       </c>
       <c r="B1040" s="1" t="s">
-        <v>1657</v>
+        <v>1641</v>
       </c>
       <c r="C1040" s="1" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1041" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1041" s="1" t="s">
-        <v>1659</v>
+        <v>1642</v>
       </c>
       <c r="C1041" s="1" t="s">
-        <v>1660</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1042" spans="1:3" x14ac:dyDescent="0.25">
@@ -17568,10 +17298,10 @@
         <v>0</v>
       </c>
       <c r="B1042" s="1" t="s">
-        <v>1661</v>
+        <v>1644</v>
       </c>
       <c r="C1042" s="1" t="s">
-        <v>1662</v>
+        <v>393</v>
       </c>
     </row>
     <row r="1043" spans="1:3" x14ac:dyDescent="0.25">
@@ -17579,21 +17309,21 @@
         <v>0</v>
       </c>
       <c r="B1043" s="1" t="s">
-        <v>1663</v>
+        <v>1645</v>
       </c>
       <c r="C1043" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="1044" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1044" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1044" s="1" t="s">
-        <v>1664</v>
+        <v>1646</v>
       </c>
       <c r="C1044" s="1" t="s">
-        <v>501</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1045" spans="1:3" x14ac:dyDescent="0.25">
@@ -17601,10 +17331,10 @@
         <v>0</v>
       </c>
       <c r="B1045" s="1" t="s">
-        <v>1665</v>
+        <v>1648</v>
       </c>
       <c r="C1045" s="1" t="s">
-        <v>444</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1046" spans="1:3" x14ac:dyDescent="0.25">
@@ -17612,10 +17342,10 @@
         <v>0</v>
       </c>
       <c r="B1046" s="1" t="s">
-        <v>1666</v>
+        <v>1649</v>
       </c>
       <c r="C1046" s="1" t="s">
-        <v>1667</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1047" spans="1:3" x14ac:dyDescent="0.25">
@@ -17623,10 +17353,10 @@
         <v>0</v>
       </c>
       <c r="B1047" s="1" t="s">
-        <v>1668</v>
+        <v>1651</v>
       </c>
       <c r="C1047" s="1" t="s">
-        <v>381</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1048" spans="1:3" x14ac:dyDescent="0.25">
@@ -17634,10 +17364,10 @@
         <v>0</v>
       </c>
       <c r="B1048" s="1" t="s">
-        <v>1669</v>
+        <v>1653</v>
       </c>
       <c r="C1048" s="1" t="s">
-        <v>1562</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1049" spans="1:3" x14ac:dyDescent="0.25">
@@ -17645,10 +17375,10 @@
         <v>0</v>
       </c>
       <c r="B1049" s="1" t="s">
-        <v>1670</v>
+        <v>1655</v>
       </c>
       <c r="C1049" s="1" t="s">
-        <v>448</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1050" spans="1:3" x14ac:dyDescent="0.25">
@@ -17656,10 +17386,10 @@
         <v>0</v>
       </c>
       <c r="B1050" s="1" t="s">
-        <v>1671</v>
+        <v>1657</v>
       </c>
       <c r="C1050" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
     </row>
     <row r="1051" spans="1:3" x14ac:dyDescent="0.25">
@@ -17667,10 +17397,10 @@
         <v>0</v>
       </c>
       <c r="B1051" s="1" t="s">
-        <v>1672</v>
+        <v>1658</v>
       </c>
       <c r="C1051" s="1" t="s">
-        <v>1673</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1052" spans="1:3" x14ac:dyDescent="0.25">
@@ -17678,10 +17408,10 @@
         <v>0</v>
       </c>
       <c r="B1052" s="1" t="s">
-        <v>1674</v>
+        <v>1660</v>
       </c>
       <c r="C1052" s="1" t="s">
-        <v>1675</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1053" spans="1:3" x14ac:dyDescent="0.25">
@@ -17689,10 +17419,10 @@
         <v>0</v>
       </c>
       <c r="B1053" s="1" t="s">
-        <v>1676</v>
+        <v>1662</v>
       </c>
       <c r="C1053" s="1" t="s">
-        <v>1677</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1054" spans="1:3" x14ac:dyDescent="0.25">
@@ -17700,10 +17430,10 @@
         <v>0</v>
       </c>
       <c r="B1054" s="1" t="s">
-        <v>1678</v>
+        <v>1664</v>
       </c>
       <c r="C1054" s="1" t="s">
-        <v>1679</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="1055" spans="1:3" x14ac:dyDescent="0.25">
@@ -17711,32 +17441,32 @@
         <v>0</v>
       </c>
       <c r="B1055" s="1" t="s">
-        <v>1680</v>
+        <v>1666</v>
       </c>
       <c r="C1055" s="1" t="s">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="1056" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1056" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1056" s="1" t="s">
-        <v>1681</v>
+        <v>1667</v>
       </c>
       <c r="C1056" s="1" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="1057" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1057" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1057" s="1" t="s">
-        <v>1683</v>
+        <v>1668</v>
       </c>
       <c r="C1057" s="1" t="s">
-        <v>1679</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="1058" spans="1:3" x14ac:dyDescent="0.25">
@@ -17744,10 +17474,10 @@
         <v>0</v>
       </c>
       <c r="B1058" s="1" t="s">
-        <v>1684</v>
+        <v>1670</v>
       </c>
       <c r="C1058" s="1" t="s">
-        <v>1685</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="1059" spans="1:3" x14ac:dyDescent="0.25">
@@ -17755,10 +17485,10 @@
         <v>0</v>
       </c>
       <c r="B1059" s="1" t="s">
-        <v>1686</v>
+        <v>1672</v>
       </c>
       <c r="C1059" s="1" t="s">
-        <v>1687</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1060" spans="1:3" x14ac:dyDescent="0.25">
@@ -17766,10 +17496,10 @@
         <v>0</v>
       </c>
       <c r="B1060" s="1" t="s">
-        <v>1688</v>
+        <v>1673</v>
       </c>
       <c r="C1060" s="1" t="s">
-        <v>497</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="1061" spans="1:3" x14ac:dyDescent="0.25">
@@ -17777,10 +17507,10 @@
         <v>0</v>
       </c>
       <c r="B1061" s="1" t="s">
-        <v>1689</v>
+        <v>1675</v>
       </c>
       <c r="C1061" s="1" t="s">
-        <v>497</v>
+        <v>204</v>
       </c>
     </row>
     <row r="1062" spans="1:3" x14ac:dyDescent="0.25">
@@ -17788,10 +17518,10 @@
         <v>0</v>
       </c>
       <c r="B1062" s="1" t="s">
-        <v>1690</v>
+        <v>1676</v>
       </c>
       <c r="C1062" s="1" t="s">
-        <v>381</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1063" spans="1:3" x14ac:dyDescent="0.25">
@@ -17799,10 +17529,10 @@
         <v>0</v>
       </c>
       <c r="B1063" s="1" t="s">
-        <v>1691</v>
+        <v>1677</v>
       </c>
       <c r="C1063" s="1" t="s">
-        <v>1692</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="1064" spans="1:3" x14ac:dyDescent="0.25">
@@ -17810,10 +17540,10 @@
         <v>0</v>
       </c>
       <c r="B1064" s="1" t="s">
-        <v>1693</v>
+        <v>1679</v>
       </c>
       <c r="C1064" s="1" t="s">
-        <v>1694</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="1065" spans="1:3" x14ac:dyDescent="0.25">
@@ -17821,10 +17551,10 @@
         <v>0</v>
       </c>
       <c r="B1065" s="1" t="s">
-        <v>1691</v>
+        <v>1681</v>
       </c>
       <c r="C1065" s="1" t="s">
-        <v>1692</v>
+        <v>289</v>
       </c>
     </row>
     <row r="1066" spans="1:3" x14ac:dyDescent="0.25">
@@ -17832,10 +17562,10 @@
         <v>0</v>
       </c>
       <c r="B1066" s="1" t="s">
-        <v>1695</v>
+        <v>1682</v>
       </c>
       <c r="C1066" s="1" t="s">
-        <v>1696</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="1067" spans="1:3" x14ac:dyDescent="0.25">
@@ -17843,10 +17573,10 @@
         <v>0</v>
       </c>
       <c r="B1067" s="1" t="s">
-        <v>1697</v>
+        <v>1684</v>
       </c>
       <c r="C1067" s="1" t="s">
-        <v>1698</v>
+        <v>806</v>
       </c>
     </row>
     <row r="1068" spans="1:3" x14ac:dyDescent="0.25">
@@ -17854,10 +17584,10 @@
         <v>0</v>
       </c>
       <c r="B1068" s="1" t="s">
-        <v>1699</v>
+        <v>1685</v>
       </c>
       <c r="C1068" s="1" t="s">
-        <v>1700</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="1069" spans="1:3" x14ac:dyDescent="0.25">
@@ -17865,10 +17595,10 @@
         <v>0</v>
       </c>
       <c r="B1069" s="1" t="s">
-        <v>1701</v>
+        <v>1687</v>
       </c>
       <c r="C1069" s="1" t="s">
-        <v>1702</v>
+        <v>393</v>
       </c>
     </row>
     <row r="1070" spans="1:3" x14ac:dyDescent="0.25">
@@ -17876,10 +17606,10 @@
         <v>0</v>
       </c>
       <c r="B1070" s="1" t="s">
-        <v>1703</v>
+        <v>1688</v>
       </c>
       <c r="C1070" s="1" t="s">
-        <v>1702</v>
+        <v>448</v>
       </c>
     </row>
     <row r="1071" spans="1:3" x14ac:dyDescent="0.25">
@@ -17887,21 +17617,21 @@
         <v>0</v>
       </c>
       <c r="B1071" s="1" t="s">
-        <v>1704</v>
+        <v>1689</v>
       </c>
       <c r="C1071" s="1" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="1072" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1072" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1072" s="1" t="s">
-        <v>1705</v>
+        <v>1693</v>
       </c>
       <c r="C1072" s="1" t="s">
-        <v>1706</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="1073" spans="1:3" x14ac:dyDescent="0.25">
@@ -17909,21 +17639,21 @@
         <v>0</v>
       </c>
       <c r="B1073" s="1" t="s">
-        <v>1707</v>
+        <v>1691</v>
       </c>
       <c r="C1073" s="1" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="1074" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1074" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1074" s="1" t="s">
-        <v>1709</v>
+        <v>1694</v>
       </c>
       <c r="C1074" s="1" t="s">
-        <v>381</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="1075" spans="1:3" x14ac:dyDescent="0.25">
@@ -17931,10 +17661,10 @@
         <v>0</v>
       </c>
       <c r="B1075" s="1" t="s">
-        <v>1710</v>
+        <v>1696</v>
       </c>
       <c r="C1075" s="1" t="s">
-        <v>393</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="1076" spans="1:3" x14ac:dyDescent="0.25">
@@ -17942,10 +17672,10 @@
         <v>0</v>
       </c>
       <c r="B1076" s="1" t="s">
-        <v>1711</v>
+        <v>1698</v>
       </c>
       <c r="C1076" s="1" t="s">
-        <v>491</v>
+        <v>241</v>
       </c>
     </row>
     <row r="1077" spans="1:3" x14ac:dyDescent="0.25">
@@ -17953,10 +17683,10 @@
         <v>0</v>
       </c>
       <c r="B1077" s="1" t="s">
-        <v>1712</v>
+        <v>1699</v>
       </c>
       <c r="C1077" s="1" t="s">
-        <v>493</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="1078" spans="1:3" x14ac:dyDescent="0.25">
@@ -17964,10 +17694,10 @@
         <v>0</v>
       </c>
       <c r="B1078" s="1" t="s">
-        <v>1713</v>
+        <v>1701</v>
       </c>
       <c r="C1078" s="1" t="s">
-        <v>489</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1079" spans="1:3" x14ac:dyDescent="0.25">
@@ -17975,10 +17705,10 @@
         <v>0</v>
       </c>
       <c r="B1079" s="1" t="s">
-        <v>1714</v>
+        <v>1702</v>
       </c>
       <c r="C1079" s="1" t="s">
-        <v>1696</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="1080" spans="1:3" x14ac:dyDescent="0.25">
@@ -17986,10 +17716,10 @@
         <v>0</v>
       </c>
       <c r="B1080" s="1" t="s">
-        <v>1715</v>
+        <v>1704</v>
       </c>
       <c r="C1080" s="1" t="s">
-        <v>1716</v>
+        <v>889</v>
       </c>
     </row>
     <row r="1081" spans="1:3" x14ac:dyDescent="0.25">
@@ -17997,10 +17727,10 @@
         <v>0</v>
       </c>
       <c r="B1081" s="1" t="s">
-        <v>1717</v>
+        <v>1705</v>
       </c>
       <c r="C1081" s="1" t="s">
-        <v>495</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="1082" spans="1:3" x14ac:dyDescent="0.25">
@@ -18008,10 +17738,10 @@
         <v>0</v>
       </c>
       <c r="B1082" s="1" t="s">
-        <v>1718</v>
+        <v>1707</v>
       </c>
       <c r="C1082" s="1" t="s">
-        <v>495</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1083" spans="1:3" x14ac:dyDescent="0.25">
@@ -18019,10 +17749,10 @@
         <v>0</v>
       </c>
       <c r="B1083" s="1" t="s">
-        <v>1719</v>
+        <v>1708</v>
       </c>
       <c r="C1083" s="1" t="s">
-        <v>1720</v>
+        <v>791</v>
       </c>
     </row>
     <row r="1084" spans="1:3" x14ac:dyDescent="0.25">
@@ -18030,10 +17760,10 @@
         <v>0</v>
       </c>
       <c r="B1084" s="1" t="s">
-        <v>1721</v>
+        <v>1709</v>
       </c>
       <c r="C1084" s="1" t="s">
-        <v>1722</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="1085" spans="1:3" x14ac:dyDescent="0.25">
@@ -18041,10 +17771,10 @@
         <v>0</v>
       </c>
       <c r="B1085" s="1" t="s">
-        <v>1723</v>
+        <v>1711</v>
       </c>
       <c r="C1085" s="1" t="s">
-        <v>381</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1086" spans="1:3" x14ac:dyDescent="0.25">
@@ -18052,10 +17782,10 @@
         <v>0</v>
       </c>
       <c r="B1086" s="1" t="s">
-        <v>1724</v>
+        <v>1713</v>
       </c>
       <c r="C1086" s="1" t="s">
-        <v>204</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="1087" spans="1:3" x14ac:dyDescent="0.25">
@@ -18063,10 +17793,10 @@
         <v>0</v>
       </c>
       <c r="B1087" s="1" t="s">
-        <v>1725</v>
+        <v>1715</v>
       </c>
       <c r="C1087" s="1" t="s">
-        <v>1726</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="1088" spans="1:3" x14ac:dyDescent="0.25">
@@ -18074,21 +17804,21 @@
         <v>0</v>
       </c>
       <c r="B1088" s="1" t="s">
-        <v>1727</v>
+        <v>1717</v>
       </c>
       <c r="C1088" s="1" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="1089" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1089" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1089" s="1" t="s">
-        <v>1729</v>
+        <v>1719</v>
       </c>
       <c r="C1089" s="1" t="s">
-        <v>1730</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="1090" spans="1:3" x14ac:dyDescent="0.25">
@@ -18096,10 +17826,10 @@
         <v>0</v>
       </c>
       <c r="B1090" s="1" t="s">
-        <v>1731</v>
+        <v>1721</v>
       </c>
       <c r="C1090" s="1" t="s">
-        <v>393</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1091" spans="1:3" x14ac:dyDescent="0.25">
@@ -18107,10 +17837,10 @@
         <v>0</v>
       </c>
       <c r="B1091" s="1" t="s">
-        <v>1732</v>
+        <v>1723</v>
       </c>
       <c r="C1091" s="1" t="s">
-        <v>1733</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="1092" spans="1:3" x14ac:dyDescent="0.25">
@@ -18118,21 +17848,21 @@
         <v>0</v>
       </c>
       <c r="B1092" s="1" t="s">
-        <v>1734</v>
+        <v>1725</v>
       </c>
       <c r="C1092" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="1093" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1093" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1093" s="1" t="s">
-        <v>1735</v>
+        <v>1727</v>
       </c>
       <c r="C1093" s="1" t="s">
-        <v>1736</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1094" spans="1:3" x14ac:dyDescent="0.25">
@@ -18140,21 +17870,21 @@
         <v>0</v>
       </c>
       <c r="B1094" s="1" t="s">
-        <v>1737</v>
+        <v>1728</v>
       </c>
       <c r="C1094" s="1" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="1095" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1095" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1095" s="1" t="s">
-        <v>1738</v>
+        <v>1730</v>
       </c>
       <c r="C1095" s="1" t="s">
-        <v>1739</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="1096" spans="1:3" x14ac:dyDescent="0.25">
@@ -18162,32 +17892,32 @@
         <v>0</v>
       </c>
       <c r="B1096" s="1" t="s">
-        <v>1740</v>
+        <v>1732</v>
       </c>
       <c r="C1096" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="1097" spans="1:3" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A1097" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1097" s="1" t="s">
-        <v>1741</v>
+        <v>1733</v>
       </c>
       <c r="C1097" s="1" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="1098" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1098" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1098" s="1" t="s">
-        <v>1742</v>
+        <v>1735</v>
       </c>
       <c r="C1098" s="1" t="s">
-        <v>1743</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="1099" spans="1:3" x14ac:dyDescent="0.25">
@@ -18195,10 +17925,10 @@
         <v>0</v>
       </c>
       <c r="B1099" s="1" t="s">
-        <v>1744</v>
+        <v>1737</v>
       </c>
       <c r="C1099" s="1" t="s">
-        <v>1125</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1100" spans="1:3" x14ac:dyDescent="0.25">
@@ -18206,10 +17936,10 @@
         <v>0</v>
       </c>
       <c r="B1100" s="1" t="s">
-        <v>1745</v>
+        <v>1738</v>
       </c>
       <c r="C1100" s="1" t="s">
-        <v>1746</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1101" spans="1:3" x14ac:dyDescent="0.25">
@@ -18217,21 +17947,21 @@
         <v>0</v>
       </c>
       <c r="B1101" s="1" t="s">
-        <v>1747</v>
+        <v>1739</v>
       </c>
       <c r="C1101" s="1" t="s">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="1102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A1102" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1102" s="1" t="s">
-        <v>1749</v>
+        <v>1740</v>
       </c>
       <c r="C1102" s="1" t="s">
-        <v>1750</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="1103" spans="1:3" x14ac:dyDescent="0.25">
@@ -18239,10 +17969,10 @@
         <v>0</v>
       </c>
       <c r="B1103" s="1" t="s">
-        <v>1751</v>
+        <v>1742</v>
       </c>
       <c r="C1103" s="1" t="s">
-        <v>1752</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="1104" spans="1:3" x14ac:dyDescent="0.25">
@@ -18250,10 +17980,10 @@
         <v>0</v>
       </c>
       <c r="B1104" s="1" t="s">
-        <v>1753</v>
+        <v>1744</v>
       </c>
       <c r="C1104" s="1" t="s">
-        <v>381</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1105" spans="1:3" x14ac:dyDescent="0.25">
@@ -18261,10 +17991,10 @@
         <v>0</v>
       </c>
       <c r="B1105" s="1" t="s">
-        <v>1754</v>
+        <v>1745</v>
       </c>
       <c r="C1105" s="1" t="s">
-        <v>1755</v>
+        <v>669</v>
       </c>
     </row>
     <row r="1106" spans="1:3" x14ac:dyDescent="0.25">
@@ -18272,10 +18002,10 @@
         <v>0</v>
       </c>
       <c r="B1106" s="1" t="s">
-        <v>1756</v>
+        <v>1746</v>
       </c>
       <c r="C1106" s="1" t="s">
-        <v>1757</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="1107" spans="1:3" x14ac:dyDescent="0.25">
@@ -18283,10 +18013,10 @@
         <v>0</v>
       </c>
       <c r="B1107" s="1" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
       <c r="C1107" s="1" t="s">
-        <v>1759</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="1108" spans="1:3" x14ac:dyDescent="0.25">
@@ -18294,10 +18024,10 @@
         <v>0</v>
       </c>
       <c r="B1108" s="1" t="s">
-        <v>1760</v>
+        <v>1708</v>
       </c>
       <c r="C1108" s="1" t="s">
-        <v>1761</v>
+        <v>791</v>
       </c>
     </row>
     <row r="1109" spans="1:3" x14ac:dyDescent="0.25">
@@ -18305,10 +18035,10 @@
         <v>0</v>
       </c>
       <c r="B1109" s="1" t="s">
-        <v>1762</v>
+        <v>1756</v>
       </c>
       <c r="C1109" s="1" t="s">
-        <v>1761</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1110" spans="1:3" x14ac:dyDescent="0.25">
@@ -18316,21 +18046,21 @@
         <v>0</v>
       </c>
       <c r="B1110" s="1" t="s">
-        <v>1763</v>
+        <v>1750</v>
       </c>
       <c r="C1110" s="1" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="1111" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1111" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1111" s="1" t="s">
-        <v>1764</v>
+        <v>1755</v>
       </c>
       <c r="C1111" s="1" t="s">
-        <v>1765</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="1112" spans="1:3" x14ac:dyDescent="0.25">
@@ -18338,10 +18068,10 @@
         <v>0</v>
       </c>
       <c r="B1112" s="1" t="s">
-        <v>1766</v>
+        <v>1752</v>
       </c>
       <c r="C1112" s="1" t="s">
-        <v>1767</v>
+        <v>834</v>
       </c>
     </row>
     <row r="1113" spans="1:3" x14ac:dyDescent="0.25">
@@ -18349,10 +18079,10 @@
         <v>0</v>
       </c>
       <c r="B1113" s="1" t="s">
-        <v>1768</v>
+        <v>1753</v>
       </c>
       <c r="C1113" s="1" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="1114" spans="1:3" x14ac:dyDescent="0.25">
@@ -18360,10 +18090,10 @@
         <v>0</v>
       </c>
       <c r="B1114" s="1" t="s">
-        <v>1769</v>
+        <v>1757</v>
       </c>
       <c r="C1114" s="1" t="s">
-        <v>1770</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1115" spans="1:3" x14ac:dyDescent="0.25">
@@ -18371,10 +18101,10 @@
         <v>0</v>
       </c>
       <c r="B1115" s="1" t="s">
-        <v>1771</v>
+        <v>1758</v>
       </c>
       <c r="C1115" s="1" t="s">
-        <v>204</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="1116" spans="1:3" x14ac:dyDescent="0.25">
@@ -18382,10 +18112,10 @@
         <v>0</v>
       </c>
       <c r="B1116" s="1" t="s">
-        <v>1772</v>
+        <v>1760</v>
       </c>
       <c r="C1116" s="1" t="s">
-        <v>1726</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="1117" spans="1:3" x14ac:dyDescent="0.25">
@@ -18393,10 +18123,10 @@
         <v>0</v>
       </c>
       <c r="B1117" s="1" t="s">
-        <v>1773</v>
+        <v>1761</v>
       </c>
       <c r="C1117" s="1" t="s">
-        <v>1774</v>
+        <v>289</v>
       </c>
     </row>
     <row r="1118" spans="1:3" x14ac:dyDescent="0.25">
@@ -18404,10 +18134,10 @@
         <v>0</v>
       </c>
       <c r="B1118" s="1" t="s">
-        <v>1775</v>
+        <v>1762</v>
       </c>
       <c r="C1118" s="1" t="s">
-        <v>1776</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="1119" spans="1:3" x14ac:dyDescent="0.25">
@@ -18415,10 +18145,10 @@
         <v>0</v>
       </c>
       <c r="B1119" s="1" t="s">
-        <v>1777</v>
+        <v>1760</v>
       </c>
       <c r="C1119" s="1" t="s">
-        <v>289</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="1120" spans="1:3" x14ac:dyDescent="0.25">
@@ -18426,10 +18156,10 @@
         <v>0</v>
       </c>
       <c r="B1120" s="1" t="s">
-        <v>1778</v>
+        <v>1764</v>
       </c>
       <c r="C1120" s="1" t="s">
-        <v>1779</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1121" spans="1:3" x14ac:dyDescent="0.25">
@@ -18437,10 +18167,10 @@
         <v>0</v>
       </c>
       <c r="B1121" s="1" t="s">
-        <v>1780</v>
+        <v>1765</v>
       </c>
       <c r="C1121" s="1" t="s">
-        <v>806</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1122" spans="1:3" x14ac:dyDescent="0.25">
@@ -18448,10 +18178,10 @@
         <v>0</v>
       </c>
       <c r="B1122" s="1" t="s">
-        <v>1781</v>
+        <v>1766</v>
       </c>
       <c r="C1122" s="1" t="s">
-        <v>1782</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1123" spans="1:3" x14ac:dyDescent="0.25">
@@ -18459,10 +18189,10 @@
         <v>0</v>
       </c>
       <c r="B1123" s="1" t="s">
-        <v>1783</v>
+        <v>1767</v>
       </c>
       <c r="C1123" s="1" t="s">
-        <v>393</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1124" spans="1:3" x14ac:dyDescent="0.25">
@@ -18470,10 +18200,10 @@
         <v>0</v>
       </c>
       <c r="B1124" s="1" t="s">
-        <v>1784</v>
+        <v>1768</v>
       </c>
       <c r="C1124" s="1" t="s">
-        <v>448</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1125" spans="1:3" x14ac:dyDescent="0.25">
@@ -18481,10 +18211,10 @@
         <v>0</v>
       </c>
       <c r="B1125" s="1" t="s">
-        <v>1785</v>
+        <v>1769</v>
       </c>
       <c r="C1125" s="1" t="s">
-        <v>241</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1126" spans="1:3" x14ac:dyDescent="0.25">
@@ -18492,10 +18222,10 @@
         <v>0</v>
       </c>
       <c r="B1126" s="1" t="s">
-        <v>1789</v>
+        <v>1770</v>
       </c>
       <c r="C1126" s="1" t="s">
-        <v>1786</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1127" spans="1:3" x14ac:dyDescent="0.25">
@@ -18503,21 +18233,21 @@
         <v>0</v>
       </c>
       <c r="B1127" s="1" t="s">
-        <v>1787</v>
+        <v>1771</v>
       </c>
       <c r="C1127" s="1" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="1128" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1128" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1128" s="1" t="s">
-        <v>1790</v>
+        <v>1772</v>
       </c>
       <c r="C1128" s="1" t="s">
-        <v>1791</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1129" spans="1:3" x14ac:dyDescent="0.25">
@@ -18525,10 +18255,10 @@
         <v>0</v>
       </c>
       <c r="B1129" s="1" t="s">
-        <v>1792</v>
+        <v>1773</v>
       </c>
       <c r="C1129" s="1" t="s">
-        <v>1793</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1130" spans="1:3" x14ac:dyDescent="0.25">
@@ -18536,10 +18266,10 @@
         <v>0</v>
       </c>
       <c r="B1130" s="1" t="s">
-        <v>1794</v>
+        <v>1774</v>
       </c>
       <c r="C1130" s="1" t="s">
-        <v>241</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1131" spans="1:3" x14ac:dyDescent="0.25">
@@ -18547,10 +18277,10 @@
         <v>0</v>
       </c>
       <c r="B1131" s="1" t="s">
-        <v>1795</v>
+        <v>1775</v>
       </c>
       <c r="C1131" s="1" t="s">
-        <v>1796</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1132" spans="1:3" x14ac:dyDescent="0.25">
@@ -18558,10 +18288,10 @@
         <v>0</v>
       </c>
       <c r="B1132" s="1" t="s">
-        <v>1797</v>
+        <v>1776</v>
       </c>
       <c r="C1132" s="1" t="s">
-        <v>528</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1133" spans="1:3" x14ac:dyDescent="0.25">
@@ -18569,10 +18299,10 @@
         <v>0</v>
       </c>
       <c r="B1133" s="1" t="s">
-        <v>1798</v>
+        <v>1777</v>
       </c>
       <c r="C1133" s="1" t="s">
-        <v>1799</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="1134" spans="1:3" x14ac:dyDescent="0.25">
@@ -18580,10 +18310,10 @@
         <v>0</v>
       </c>
       <c r="B1134" s="1" t="s">
-        <v>1800</v>
+        <v>1779</v>
       </c>
       <c r="C1134" s="1" t="s">
-        <v>889</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1135" spans="1:3" x14ac:dyDescent="0.25">
@@ -18591,10 +18321,10 @@
         <v>0</v>
       </c>
       <c r="B1135" s="1" t="s">
-        <v>1801</v>
+        <v>1780</v>
       </c>
       <c r="C1135" s="1" t="s">
-        <v>1802</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="1136" spans="1:3" x14ac:dyDescent="0.25">
@@ -18602,10 +18332,10 @@
         <v>0</v>
       </c>
       <c r="B1136" s="1" t="s">
-        <v>1803</v>
+        <v>1782</v>
       </c>
       <c r="C1136" s="1" t="s">
-        <v>728</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="1137" spans="1:3" x14ac:dyDescent="0.25">
@@ -18613,10 +18343,10 @@
         <v>0</v>
       </c>
       <c r="B1137" s="1" t="s">
-        <v>1804</v>
+        <v>1783</v>
       </c>
       <c r="C1137" s="1" t="s">
-        <v>791</v>
+        <v>298</v>
       </c>
     </row>
     <row r="1138" spans="1:3" x14ac:dyDescent="0.25">
@@ -18624,10 +18354,10 @@
         <v>0</v>
       </c>
       <c r="B1138" s="1" t="s">
-        <v>1805</v>
+        <v>1784</v>
       </c>
       <c r="C1138" s="1" t="s">
-        <v>1806</v>
+        <v>448</v>
       </c>
     </row>
     <row r="1139" spans="1:3" x14ac:dyDescent="0.25">
@@ -18635,10 +18365,10 @@
         <v>0</v>
       </c>
       <c r="B1139" s="1" t="s">
-        <v>1807</v>
+        <v>1785</v>
       </c>
       <c r="C1139" s="1" t="s">
-        <v>1808</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="1140" spans="1:3" x14ac:dyDescent="0.25">
@@ -18646,10 +18376,10 @@
         <v>0</v>
       </c>
       <c r="B1140" s="1" t="s">
-        <v>1809</v>
+        <v>1786</v>
       </c>
       <c r="C1140" s="1" t="s">
-        <v>1810</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="1141" spans="1:3" x14ac:dyDescent="0.25">
@@ -18657,10 +18387,10 @@
         <v>0</v>
       </c>
       <c r="B1141" s="1" t="s">
-        <v>1811</v>
+        <v>1787</v>
       </c>
       <c r="C1141" s="1" t="s">
-        <v>1812</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="1142" spans="1:3" x14ac:dyDescent="0.25">
@@ -18668,32 +18398,32 @@
         <v>0</v>
       </c>
       <c r="B1142" s="1" t="s">
-        <v>1813</v>
+        <v>1788</v>
       </c>
       <c r="C1142" s="1" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="1143" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1143" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1143" s="1" t="s">
-        <v>1815</v>
+        <v>1789</v>
       </c>
       <c r="C1143" s="1" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="1144" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1144" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1144" s="1" t="s">
-        <v>1817</v>
+        <v>1790</v>
       </c>
       <c r="C1144" s="1" t="s">
-        <v>1818</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="1145" spans="1:3" x14ac:dyDescent="0.25">
@@ -18701,10 +18431,10 @@
         <v>0</v>
       </c>
       <c r="B1145" s="1" t="s">
-        <v>1819</v>
+        <v>1792</v>
       </c>
       <c r="C1145" s="1" t="s">
-        <v>1820</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="1146" spans="1:3" x14ac:dyDescent="0.25">
@@ -18712,10 +18442,10 @@
         <v>0</v>
       </c>
       <c r="B1146" s="1" t="s">
-        <v>1821</v>
+        <v>1794</v>
       </c>
       <c r="C1146" s="1" t="s">
-        <v>1822</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="1147" spans="1:3" x14ac:dyDescent="0.25">
@@ -18723,10 +18453,10 @@
         <v>0</v>
       </c>
       <c r="B1147" s="1" t="s">
-        <v>1823</v>
+        <v>1795</v>
       </c>
       <c r="C1147" s="1" t="s">
-        <v>1818</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="1148" spans="1:3" x14ac:dyDescent="0.25">
@@ -18734,10 +18464,10 @@
         <v>0</v>
       </c>
       <c r="B1148" s="1" t="s">
-        <v>1824</v>
+        <v>1797</v>
       </c>
       <c r="C1148" s="1" t="s">
-        <v>1825</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="1149" spans="1:3" x14ac:dyDescent="0.25">
@@ -18745,10 +18475,10 @@
         <v>0</v>
       </c>
       <c r="B1149" s="1" t="s">
-        <v>1826</v>
+        <v>1798</v>
       </c>
       <c r="C1149" s="1" t="s">
-        <v>1827</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="1150" spans="1:3" x14ac:dyDescent="0.25">
@@ -18756,21 +18486,21 @@
         <v>0</v>
       </c>
       <c r="B1150" s="1" t="s">
-        <v>1828</v>
+        <v>1800</v>
       </c>
       <c r="C1150" s="1" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="1151" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1151" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1151" s="1" t="s">
-        <v>1829</v>
+        <v>1801</v>
       </c>
       <c r="C1151" s="1" t="s">
-        <v>1830</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1152" spans="1:3" x14ac:dyDescent="0.25">
@@ -18778,10 +18508,10 @@
         <v>0</v>
       </c>
       <c r="B1152" s="1" t="s">
-        <v>1831</v>
+        <v>1802</v>
       </c>
       <c r="C1152" s="1" t="s">
-        <v>1832</v>
+        <v>366</v>
       </c>
     </row>
     <row r="1153" spans="1:3" x14ac:dyDescent="0.25">
@@ -18789,10 +18519,10 @@
         <v>0</v>
       </c>
       <c r="B1153" s="1" t="s">
-        <v>1833</v>
+        <v>1803</v>
       </c>
       <c r="C1153" s="1" t="s">
-        <v>1521</v>
+        <v>791</v>
       </c>
     </row>
     <row r="1154" spans="1:3" x14ac:dyDescent="0.25">
@@ -18800,10 +18530,10 @@
         <v>0</v>
       </c>
       <c r="B1154" s="1" t="s">
-        <v>1834</v>
+        <v>1804</v>
       </c>
       <c r="C1154" s="1" t="s">
-        <v>1521</v>
+        <v>832</v>
       </c>
     </row>
     <row r="1155" spans="1:3" x14ac:dyDescent="0.25">
@@ -18811,21 +18541,21 @@
         <v>0</v>
       </c>
       <c r="B1155" s="1" t="s">
-        <v>1835</v>
+        <v>1805</v>
       </c>
       <c r="C1155" s="1" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="1156" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1156" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1156" s="1" t="s">
-        <v>1836</v>
+        <v>1807</v>
       </c>
       <c r="C1156" s="1" t="s">
-        <v>1837</v>
+        <v>770</v>
       </c>
     </row>
     <row r="1157" spans="1:3" x14ac:dyDescent="0.25">
@@ -18833,549 +18563,10 @@
         <v>0</v>
       </c>
       <c r="B1157" s="1" t="s">
-        <v>1838</v>
+        <v>1808</v>
       </c>
       <c r="C1157" s="1" t="s">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="1158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1158" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1158" s="1" t="s">
-        <v>1840</v>
-      </c>
-      <c r="C1158" s="1" t="s">
-        <v>1485</v>
-      </c>
-    </row>
-    <row r="1159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1159" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1159" s="1" t="s">
-        <v>1841</v>
-      </c>
-      <c r="C1159" s="1" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="1160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1160" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1160" s="1" t="s">
-        <v>1842</v>
-      </c>
-      <c r="C1160" s="1" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="1161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1161" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1161" s="1" t="s">
-        <v>1843</v>
-      </c>
-      <c r="C1161" s="1" t="s">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="1162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1162" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1162" s="1" t="s">
-        <v>1804</v>
-      </c>
-      <c r="C1162" s="1" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="1163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1163" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1163" s="1" t="s">
-        <v>1852</v>
-      </c>
-      <c r="C1163" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1164" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1164" s="1" t="s">
-        <v>1846</v>
-      </c>
-      <c r="C1164" s="1" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="1165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1165" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1165" s="1" t="s">
-        <v>1851</v>
-      </c>
-      <c r="C1165" s="1" t="s">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="1166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1166" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1166" s="1" t="s">
-        <v>1848</v>
-      </c>
-      <c r="C1166" s="1" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="1167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1167" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1167" s="1" t="s">
-        <v>1849</v>
-      </c>
-      <c r="C1167" s="1" t="s">
-        <v>1850</v>
-      </c>
-    </row>
-    <row r="1168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1168" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1168" s="1" t="s">
-        <v>1853</v>
-      </c>
-      <c r="C1168" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1169" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1169" s="1" t="s">
-        <v>1854</v>
-      </c>
-      <c r="C1169" s="1" t="s">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="1170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1170" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1170" s="1" t="s">
-        <v>1856</v>
-      </c>
-      <c r="C1170" s="1" t="s">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="1171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1171" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1171" s="1" t="s">
-        <v>1857</v>
-      </c>
-      <c r="C1171" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="1172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1172" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1172" s="1" t="s">
-        <v>1858</v>
-      </c>
-      <c r="C1172" s="1" t="s">
-        <v>1859</v>
-      </c>
-    </row>
-    <row r="1173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1173" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1173" s="1" t="s">
-        <v>1856</v>
-      </c>
-      <c r="C1173" s="1" t="s">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="1174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1174" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1174" s="1" t="s">
-        <v>1860</v>
-      </c>
-      <c r="C1174" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1175" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1175" s="1" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C1175" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1176" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1176" s="1" t="s">
-        <v>1862</v>
-      </c>
-      <c r="C1176" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1177" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1177" s="1" t="s">
-        <v>1863</v>
-      </c>
-      <c r="C1177" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1178" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1178" s="1" t="s">
-        <v>1864</v>
-      </c>
-      <c r="C1178" s="1" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="1179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1179" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1179" s="1" t="s">
-        <v>1865</v>
-      </c>
-      <c r="C1179" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1180" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1180" s="1" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C1180" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1181" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1181" s="1" t="s">
-        <v>1867</v>
-      </c>
-      <c r="C1181" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1182" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1182" s="1" t="s">
-        <v>1868</v>
-      </c>
-      <c r="C1182" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1183" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1183" s="1" t="s">
-        <v>1869</v>
-      </c>
-      <c r="C1183" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1184" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1184" s="1" t="s">
-        <v>1870</v>
-      </c>
-      <c r="C1184" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1185" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1185" s="1" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C1185" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1186" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1186" s="1" t="s">
-        <v>1872</v>
-      </c>
-      <c r="C1186" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1187" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1187" s="1" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C1187" s="1" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="1188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1188" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1188" s="1" t="s">
-        <v>1875</v>
-      </c>
-      <c r="C1188" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1189" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1189" s="1" t="s">
-        <v>1876</v>
-      </c>
-      <c r="C1189" s="1" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1190" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1190" s="1" t="s">
-        <v>1878</v>
-      </c>
-      <c r="C1190" s="1" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1191" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1191" s="1" t="s">
-        <v>1879</v>
-      </c>
-      <c r="C1191" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="1192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1192" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1192" s="1" t="s">
-        <v>1880</v>
-      </c>
-      <c r="C1192" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="1193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1193" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1193" s="1" t="s">
-        <v>1881</v>
-      </c>
-      <c r="C1193" s="1" t="s">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="1194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1194" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1194" s="1" t="s">
-        <v>1882</v>
-      </c>
-      <c r="C1194" s="1" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1195" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1195" s="1" t="s">
-        <v>1883</v>
-      </c>
-      <c r="C1195" s="1" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1196" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1196" s="1" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C1196" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="1197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1197" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1197" s="1" t="s">
-        <v>1885</v>
-      </c>
-      <c r="C1197" s="1" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="1198" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A1198" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1198" s="1" t="s">
-        <v>1886</v>
-      </c>
-      <c r="C1198" s="1" t="s">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="1199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1199" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1199" s="1" t="s">
-        <v>1888</v>
-      </c>
-      <c r="C1199" s="1" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="1200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1200" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1200" s="1" t="s">
-        <v>1890</v>
-      </c>
-      <c r="C1200" s="1" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="1201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1201" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1201" s="1" t="s">
-        <v>1891</v>
-      </c>
-      <c r="C1201" s="1" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="1202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1202" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1202" s="1" t="s">
-        <v>1893</v>
-      </c>
-      <c r="C1202" s="1" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="1203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1203" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1203" s="1" t="s">
-        <v>1894</v>
-      </c>
-      <c r="C1203" s="1" t="s">
-        <v>1895</v>
-      </c>
-    </row>
-    <row r="1204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1204" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1204" s="1" t="s">
-        <v>1896</v>
-      </c>
-      <c r="C1204" s="1" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="1205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1205" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1205" s="1" t="s">
-        <v>1897</v>
-      </c>
-      <c r="C1205" s="1" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="1206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1206" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1206" s="1" t="s">
-        <v>1898</v>
-      </c>
-      <c r="C1206" s="1" t="s">
-        <v>366</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added coil size to aromizers
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB9F26-E321-D343-89EB-D4C55D5314B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB5FBD-0089-A448-AE42-0E31E70F1689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3495" uniqueCount="1815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1827">
   <si>
     <t>cs</t>
   </si>
@@ -5484,6 +5484,42 @@
   </si>
   <si>
     <t>lab.mod.table.voltage</t>
+  </si>
+  <si>
+    <t>lab.atomizer.table.coilSize</t>
+  </si>
+  <si>
+    <t>lab.atomizer.coilMin.label</t>
+  </si>
+  <si>
+    <t>Minimální spirálka</t>
+  </si>
+  <si>
+    <t>lab.atomizer.coilMax.label</t>
+  </si>
+  <si>
+    <t>Maximální spirálka</t>
+  </si>
+  <si>
+    <t>lab.atomizer.coilMin.label.tooltip</t>
+  </si>
+  <si>
+    <t>Tento údaj říká nejmenší rozumnou spirálku, kterou lze do atomizéru osadit; primárně se jedná o doporučení, se kterým pak dále aplikace bude počítat, proto prosím udejte fyzikálně reálný údaj.</t>
+  </si>
+  <si>
+    <t>lab.atomizer.coilMax.label.tooltip</t>
+  </si>
+  <si>
+    <t>Maximální doporučení spirálka, kterou lze atomizér rozumně osadit. Tímto je míněno, že přestože by se do atomizéru dala nacpat nějaká extrémní prasárna, je to považováno za neobvyklé a na experimentování každého, nicméně pro běžnou věřejnost postačí rozumně přijatelný údaj (tzn. obvykle max 0.35, nejvýše 0.4).</t>
+  </si>
+  <si>
+    <t>lab.atomizer.preview.type</t>
+  </si>
+  <si>
+    <t>lab.atomizer.preview.coilSize</t>
+  </si>
+  <si>
+    <t>Doporučená spirálka</t>
   </si>
 </sst>
 </file>
@@ -5847,10 +5883,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1161"/>
+  <dimension ref="A1:C1168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1152" sqref="B1152"/>
+    <sheetView tabSelected="1" topLeftCell="A1150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1166" sqref="B1166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18629,6 +18665,83 @@
       </c>
       <c r="C1161" s="1" t="s">
         <v>1680</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1162" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C1162" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1163" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C1163" s="1" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1164" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C1164" s="1" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1165" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C1165" s="1" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A1166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1166" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C1166" s="1" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1167" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C1167" s="1" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1168" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C1168" s="1" t="s">
+        <v>1826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added magick to update data on background
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB5FBD-0089-A448-AE42-0E31E70F1689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC45FEA-9AC0-A246-ADBC-3FF0C3351F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3519" uniqueCount="1829">
   <si>
     <t>cs</t>
   </si>
@@ -5520,6 +5520,12 @@
   </si>
   <si>
     <t>Doporučená spirálka</t>
+  </si>
+  <si>
+    <t>job-service.PuffSmith\Updater\UpdaterJobService</t>
+  </si>
+  <si>
+    <t>Služba aktualizace dat</t>
   </si>
 </sst>
 </file>
@@ -5883,10 +5889,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1168"/>
+  <dimension ref="A1:C1169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1166" sqref="B1166"/>
+      <selection activeCell="B1165" sqref="B1165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18742,6 +18748,17 @@
       </c>
       <c r="C1168" s="1" t="s">
         <v>1826</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1169" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C1169" s="1" t="s">
+        <v>1828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added TC wire flag
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CE7FC5-CF14-4C9E-91BB-F8C9A71B7330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC0D9F4-4D74-4DF4-A490-2D980F061849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2145" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="2490" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3519" uniqueCount="1829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="1831">
   <si>
     <t>cs</t>
   </si>
@@ -5526,6 +5526,12 @@
   </si>
   <si>
     <t>Služba aktualizace dat</t>
+  </si>
+  <si>
+    <t>lab.wire.table.tc</t>
+  </si>
+  <si>
+    <t>Teplotní kontrola</t>
   </si>
 </sst>
 </file>
@@ -5889,10 +5895,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1169"/>
+  <dimension ref="A1:C1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1060" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1083" sqref="C1083"/>
+    <sheetView tabSelected="1" topLeftCell="A1159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1168" sqref="B1168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18759,6 +18765,17 @@
       </c>
       <c r="C1169" s="1" t="s">
         <v>1828</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1170" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1170" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C1170" s="1" t="s">
+        <v>1830</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Fixed somethings, improved build stuff, added dual coil support
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B5AFD1-D037-004D-9005-E2138AD6FFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FDE11-B8A1-8149-8C57-333BEF86467D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="1835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="1850">
   <si>
     <t>cs</t>
   </si>
@@ -5544,6 +5544,51 @@
   </si>
   <si>
     <t>Vyberte prosím drát; pokud není v seznamu, budete si jej muset pořídit v Obchodě.</t>
+  </si>
+  <si>
+    <t>lab.build.dual.label</t>
+  </si>
+  <si>
+    <t>Dual coil</t>
+  </si>
+  <si>
+    <t>lab.build.dualMode.label</t>
+  </si>
+  <si>
+    <t>Typ zapojení</t>
+  </si>
+  <si>
+    <t>lab.dual-coil.1</t>
+  </si>
+  <si>
+    <t>lab.dual-coil.2</t>
+  </si>
+  <si>
+    <t>Sériové</t>
+  </si>
+  <si>
+    <t>Paralelní</t>
+  </si>
+  <si>
+    <t>lab.build.dualMode.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte prosím režim zapojení spirálek.</t>
+  </si>
+  <si>
+    <t>lab.build.preview.dual</t>
+  </si>
+  <si>
+    <t>lab.build.preview.dualMode</t>
+  </si>
+  <si>
+    <t>Režim zapojení</t>
+  </si>
+  <si>
+    <t>lab.wire.tc.label</t>
+  </si>
+  <si>
+    <t>Teplotní kontrola</t>
   </si>
 </sst>
 </file>
@@ -5907,10 +5952,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1172"/>
+  <dimension ref="A1:C1180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1168" sqref="B1168"/>
+    <sheetView tabSelected="1" topLeftCell="A1162" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1176" sqref="B1176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18810,6 +18855,94 @@
       </c>
       <c r="C1172" s="1" t="s">
         <v>1834</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1173" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C1173" s="1" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1174" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1174" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C1174" s="1" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1175" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C1175" s="1" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1176" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C1176" s="1" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1177" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C1177" s="1" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1178" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1178" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C1178" s="1" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1179" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C1179" s="1" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1180" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C1180" s="1" t="s">
+        <v>1849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some little design improvements
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FDE11-B8A1-8149-8C57-333BEF86467D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA845593-EF53-E948-A156-0E8742E66764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="1850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1852">
   <si>
     <t>cs</t>
   </si>
@@ -5589,6 +5589,12 @@
   </si>
   <si>
     <t>Teplotní kontrola</t>
+  </si>
+  <si>
+    <t>lab.coil.common.tab</t>
+  </si>
+  <si>
+    <t>lab.coil.builds.tab</t>
   </si>
 </sst>
 </file>
@@ -5952,10 +5958,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1180"/>
+  <dimension ref="A1:C1182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1176" sqref="B1176"/>
+      <selection activeCell="B1177" sqref="B1177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18943,6 +18949,28 @@
       </c>
       <c r="C1180" s="1" t="s">
         <v>1849</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1181" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C1181" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1182" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1182" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C1182" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved build stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA845593-EF53-E948-A156-0E8742E66764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3443D7-0974-EE46-864F-A52AF70537FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="1854">
   <si>
     <t>cs</t>
   </si>
@@ -5595,6 +5595,12 @@
   </si>
   <si>
     <t>lab.coil.builds.tab</t>
+  </si>
+  <si>
+    <t>lab.build.table.dual</t>
+  </si>
+  <si>
+    <t>lab.build.table.dualMode</t>
   </si>
 </sst>
 </file>
@@ -5958,10 +5964,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1182"/>
+  <dimension ref="A1:C1184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1177" sqref="B1177"/>
+      <selection activeCell="B1174" sqref="B1174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18971,6 +18977,28 @@
       </c>
       <c r="C1182" s="1" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1183" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C1183" s="1" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1184" s="1" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C1184" s="1" t="s">
+        <v>1847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Initial support for nominal resistance of a coil
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3443D7-0974-EE46-864F-A52AF70537FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C24CAB8-8C9A-4B41-BB24-A2ED29EB4BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="1854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="1857">
   <si>
     <t>cs</t>
   </si>
@@ -5601,6 +5601,15 @@
   </si>
   <si>
     <t>lab.build.table.dualMode</t>
+  </si>
+  <si>
+    <t>lab.coil.table.nominalOhm</t>
+  </si>
+  <si>
+    <t>Nominální odpor</t>
+  </si>
+  <si>
+    <t>lab.coil.preview.nominalOhm</t>
   </si>
 </sst>
 </file>
@@ -5964,10 +5973,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1184"/>
+  <dimension ref="A1:C1186"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1174" sqref="B1174"/>
+      <selection activeCell="B1183" sqref="B1183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18999,6 +19008,28 @@
       </c>
       <c r="C1184" s="1" t="s">
         <v>1847</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1185" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C1185" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1186" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1186" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C1186" s="1" t="s">
+        <v>1855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Removed juiceflow from vape
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84888073-FB95-415B-810C-635BC9775B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBA0F0C-FBB3-44AB-AF4D-7CAE0AC271ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="2490" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="1861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="1862">
   <si>
     <t>cs</t>
   </si>
@@ -5622,6 +5622,9 @@
   </si>
   <si>
     <t>Omlouváme se, ale tento uživatel je již registrovaný.</t>
+  </si>
+  <si>
+    <t>Ohodnotit</t>
   </si>
 </sst>
 </file>
@@ -5987,8 +5990,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1189" sqref="B1189"/>
+    <sheetView tabSelected="1" topLeftCell="A784" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C807" sqref="A806:C807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14872,7 +14875,7 @@
         <v>1286</v>
       </c>
       <c r="C807" s="1" t="s">
-        <v>1287</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Common: Initial atomizer dual coil support
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBA0F0C-FBB3-44AB-AF4D-7CAE0AC271ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BB4E9-2803-4127-A590-3561FF747B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="2490" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="1862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3588" uniqueCount="1865">
   <si>
     <t>cs</t>
   </si>
@@ -5625,6 +5625,15 @@
   </si>
   <si>
     <t>Ohodnotit</t>
+  </si>
+  <si>
+    <t>lab.atomizer.dual.label</t>
+  </si>
+  <si>
+    <t>lab.wire.table.tc</t>
+  </si>
+  <si>
+    <t>lab.atomizer.preview.dual</t>
   </si>
 </sst>
 </file>
@@ -5988,10 +5997,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1189"/>
+  <dimension ref="A1:C1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A784" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C807" sqref="A806:C807"/>
+    <sheetView tabSelected="1" topLeftCell="A1170" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1188" sqref="B1188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19078,6 +19087,39 @@
       </c>
       <c r="C1189" s="1" t="s">
         <v>1860</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1190" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C1190" s="1" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1191" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C1191" s="1" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1192" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1192" s="1" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C1192" s="1" t="s">
+        <v>1836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Improved atomizer import
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/translations.xlsx
+++ b/upgrade/fixtures/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BB4E9-2803-4127-A590-3561FF747B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD06C7F8-B42E-4A05-8F59-BF5C4E88C506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="2490" windowWidth="33615" windowHeight="18390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3588" uniqueCount="1865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3591" uniqueCount="1866">
   <si>
     <t>cs</t>
   </si>
@@ -5634,6 +5634,9 @@
   </si>
   <si>
     <t>lab.atomizer.preview.dual</t>
+  </si>
+  <si>
+    <t>lab.atomizer.table.dual</t>
   </si>
 </sst>
 </file>
@@ -5997,10 +6000,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:C1192"/>
+  <dimension ref="A1:C1193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1170" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1188" sqref="B1188"/>
+      <selection activeCell="B1185" sqref="B1185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19119,6 +19122,17 @@
         <v>1864</v>
       </c>
       <c r="C1192" s="1" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1193" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C1193" s="1" t="s">
         <v>1836</v>
       </c>
     </row>

</xml_diff>